<commit_message>
Adding 23/12/2017 exercise data
</commit_message>
<xml_diff>
--- a/datasets/GymWorkouts.xlsx
+++ b/datasets/GymWorkouts.xlsx
@@ -12,7 +12,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="11640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="WeightTraining" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="821" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="848" uniqueCount="82">
   <si>
     <t>Exercise Date</t>
   </si>
@@ -264,6 +264,12 @@
   </si>
   <si>
     <t>ExerciseId</t>
+  </si>
+  <si>
+    <t>Saturday</t>
+  </si>
+  <si>
+    <t>V-up crunches with medicine ball</t>
   </si>
 </sst>
 </file>
@@ -618,11 +624,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K271"/>
+  <dimension ref="A1:K280"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L7" sqref="L7"/>
+      <pane ySplit="1" topLeftCell="A251" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B280" sqref="B280"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -634,7 +640,7 @@
     <col min="5" max="5" width="13.7265625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.7265625" customWidth="1"/>
     <col min="7" max="7" width="11.90625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8.7265625" style="1"/>
     <col min="10" max="10" width="4.81640625" style="3" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="8.7265625" style="3"/>
@@ -10126,6 +10132,321 @@
         <v>8</v>
       </c>
     </row>
+    <row r="272" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A272" s="3">
+        <v>271</v>
+      </c>
+      <c r="B272" s="3">
+        <v>33</v>
+      </c>
+      <c r="C272" s="2">
+        <v>43092</v>
+      </c>
+      <c r="D272">
+        <v>51</v>
+      </c>
+      <c r="E272" t="s">
+        <v>69</v>
+      </c>
+      <c r="F272">
+        <v>2017</v>
+      </c>
+      <c r="G272" t="s">
+        <v>80</v>
+      </c>
+      <c r="H272" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="I272" s="1">
+        <v>36</v>
+      </c>
+      <c r="J272" s="3">
+        <v>4</v>
+      </c>
+      <c r="K272" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="273" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A273" s="3">
+        <v>272</v>
+      </c>
+      <c r="B273" s="3">
+        <v>33</v>
+      </c>
+      <c r="C273" s="2">
+        <v>43092</v>
+      </c>
+      <c r="D273">
+        <v>51</v>
+      </c>
+      <c r="E273" t="s">
+        <v>69</v>
+      </c>
+      <c r="F273">
+        <v>2017</v>
+      </c>
+      <c r="G273" t="s">
+        <v>80</v>
+      </c>
+      <c r="H273" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I273" s="1">
+        <v>100</v>
+      </c>
+      <c r="J273" s="3">
+        <v>4</v>
+      </c>
+      <c r="K273" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="274" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A274" s="3">
+        <v>273</v>
+      </c>
+      <c r="B274" s="3">
+        <v>33</v>
+      </c>
+      <c r="C274" s="2">
+        <v>43092</v>
+      </c>
+      <c r="D274">
+        <v>51</v>
+      </c>
+      <c r="E274" t="s">
+        <v>69</v>
+      </c>
+      <c r="F274">
+        <v>2017</v>
+      </c>
+      <c r="G274" t="s">
+        <v>80</v>
+      </c>
+      <c r="H274" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="I274" s="1">
+        <v>100</v>
+      </c>
+      <c r="J274" s="3">
+        <v>5</v>
+      </c>
+      <c r="K274" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="275" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A275" s="3">
+        <v>274</v>
+      </c>
+      <c r="B275" s="3">
+        <v>33</v>
+      </c>
+      <c r="C275" s="2">
+        <v>43092</v>
+      </c>
+      <c r="D275">
+        <v>51</v>
+      </c>
+      <c r="E275" t="s">
+        <v>69</v>
+      </c>
+      <c r="F275">
+        <v>2017</v>
+      </c>
+      <c r="G275" t="s">
+        <v>80</v>
+      </c>
+      <c r="H275" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="I275" s="1">
+        <v>8</v>
+      </c>
+      <c r="J275" s="3">
+        <v>4</v>
+      </c>
+      <c r="K275" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="276" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A276" s="3">
+        <v>275</v>
+      </c>
+      <c r="B276" s="3">
+        <v>33</v>
+      </c>
+      <c r="C276" s="2">
+        <v>43092</v>
+      </c>
+      <c r="D276">
+        <v>51</v>
+      </c>
+      <c r="E276" t="s">
+        <v>69</v>
+      </c>
+      <c r="F276">
+        <v>2017</v>
+      </c>
+      <c r="G276" t="s">
+        <v>80</v>
+      </c>
+      <c r="H276" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I276" s="1">
+        <v>0</v>
+      </c>
+      <c r="J276" s="3">
+        <v>3</v>
+      </c>
+      <c r="K276" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="277" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A277" s="3">
+        <v>276</v>
+      </c>
+      <c r="B277" s="3">
+        <v>33</v>
+      </c>
+      <c r="C277" s="2">
+        <v>43092</v>
+      </c>
+      <c r="D277">
+        <v>51</v>
+      </c>
+      <c r="E277" t="s">
+        <v>69</v>
+      </c>
+      <c r="F277">
+        <v>2017</v>
+      </c>
+      <c r="G277" t="s">
+        <v>80</v>
+      </c>
+      <c r="H277" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="I277" s="1">
+        <v>8</v>
+      </c>
+      <c r="J277" s="3">
+        <v>4</v>
+      </c>
+      <c r="K277" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="278" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A278" s="3">
+        <v>277</v>
+      </c>
+      <c r="B278" s="3">
+        <v>33</v>
+      </c>
+      <c r="C278" s="2">
+        <v>43092</v>
+      </c>
+      <c r="D278">
+        <v>51</v>
+      </c>
+      <c r="E278" t="s">
+        <v>69</v>
+      </c>
+      <c r="F278">
+        <v>2017</v>
+      </c>
+      <c r="G278" t="s">
+        <v>80</v>
+      </c>
+      <c r="H278" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I278" s="1">
+        <v>0</v>
+      </c>
+      <c r="J278" s="3">
+        <v>4</v>
+      </c>
+      <c r="K278" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="279" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A279" s="3">
+        <v>278</v>
+      </c>
+      <c r="B279" s="3">
+        <v>33</v>
+      </c>
+      <c r="C279" s="2">
+        <v>43092</v>
+      </c>
+      <c r="D279">
+        <v>51</v>
+      </c>
+      <c r="E279" t="s">
+        <v>69</v>
+      </c>
+      <c r="F279">
+        <v>2017</v>
+      </c>
+      <c r="G279" t="s">
+        <v>80</v>
+      </c>
+      <c r="H279" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I279" s="1">
+        <v>0</v>
+      </c>
+      <c r="J279" s="3">
+        <v>4</v>
+      </c>
+      <c r="K279" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="280" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A280" s="3">
+        <v>279</v>
+      </c>
+      <c r="B280" s="3">
+        <v>33</v>
+      </c>
+      <c r="C280" s="2">
+        <v>43092</v>
+      </c>
+      <c r="D280">
+        <v>51</v>
+      </c>
+      <c r="E280" t="s">
+        <v>69</v>
+      </c>
+      <c r="F280">
+        <v>2017</v>
+      </c>
+      <c r="G280" t="s">
+        <v>80</v>
+      </c>
+      <c r="H280" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="I280" s="1">
+        <v>0</v>
+      </c>
+      <c r="J280" s="3">
+        <v>4</v>
+      </c>
+      <c r="K280" s="3">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updating CSV and XLSX workouts file
</commit_message>
<xml_diff>
--- a/datasets/GymWorkouts.xlsx
+++ b/datasets/GymWorkouts.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="848" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="875" uniqueCount="83">
   <si>
     <t>Exercise Date</t>
   </si>
@@ -270,6 +270,9 @@
   </si>
   <si>
     <t>V-up crunches with medicine ball</t>
+  </si>
+  <si>
+    <t>Seated Row</t>
   </si>
 </sst>
 </file>
@@ -624,11 +627,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K280"/>
+  <dimension ref="A1:K289"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A251" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B280" sqref="B280"/>
+      <pane ySplit="1" topLeftCell="A266" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H292" sqref="H292"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -10447,6 +10450,321 @@
         <v>10</v>
       </c>
     </row>
+    <row r="281" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A281" s="3">
+        <v>280</v>
+      </c>
+      <c r="B281" s="3">
+        <v>34</v>
+      </c>
+      <c r="C281" s="2">
+        <v>43093</v>
+      </c>
+      <c r="D281">
+        <v>51</v>
+      </c>
+      <c r="E281" t="s">
+        <v>69</v>
+      </c>
+      <c r="F281">
+        <v>2017</v>
+      </c>
+      <c r="G281" t="s">
+        <v>45</v>
+      </c>
+      <c r="H281" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I281" s="1">
+        <v>50</v>
+      </c>
+      <c r="J281" s="3">
+        <v>4</v>
+      </c>
+      <c r="K281" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="282" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A282" s="3">
+        <v>281</v>
+      </c>
+      <c r="B282" s="3">
+        <v>34</v>
+      </c>
+      <c r="C282" s="2">
+        <v>43093</v>
+      </c>
+      <c r="D282">
+        <v>51</v>
+      </c>
+      <c r="E282" t="s">
+        <v>69</v>
+      </c>
+      <c r="F282">
+        <v>2017</v>
+      </c>
+      <c r="G282" t="s">
+        <v>45</v>
+      </c>
+      <c r="H282" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I282" s="1">
+        <v>40</v>
+      </c>
+      <c r="J282" s="3">
+        <v>4</v>
+      </c>
+      <c r="K282" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="283" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A283" s="3">
+        <v>282</v>
+      </c>
+      <c r="B283" s="3">
+        <v>34</v>
+      </c>
+      <c r="C283" s="2">
+        <v>43093</v>
+      </c>
+      <c r="D283">
+        <v>51</v>
+      </c>
+      <c r="E283" t="s">
+        <v>69</v>
+      </c>
+      <c r="F283">
+        <v>2017</v>
+      </c>
+      <c r="G283" t="s">
+        <v>45</v>
+      </c>
+      <c r="H283" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I283" s="1">
+        <v>24</v>
+      </c>
+      <c r="J283" s="3">
+        <v>4</v>
+      </c>
+      <c r="K283" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="284" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A284" s="3">
+        <v>283</v>
+      </c>
+      <c r="B284" s="3">
+        <v>34</v>
+      </c>
+      <c r="C284" s="2">
+        <v>43093</v>
+      </c>
+      <c r="D284">
+        <v>51</v>
+      </c>
+      <c r="E284" t="s">
+        <v>69</v>
+      </c>
+      <c r="F284">
+        <v>2017</v>
+      </c>
+      <c r="G284" t="s">
+        <v>45</v>
+      </c>
+      <c r="H284" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I284" s="1">
+        <v>24</v>
+      </c>
+      <c r="J284" s="3">
+        <v>4</v>
+      </c>
+      <c r="K284" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="285" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A285" s="3">
+        <v>284</v>
+      </c>
+      <c r="B285" s="3">
+        <v>34</v>
+      </c>
+      <c r="C285" s="2">
+        <v>43093</v>
+      </c>
+      <c r="D285">
+        <v>51</v>
+      </c>
+      <c r="E285" t="s">
+        <v>69</v>
+      </c>
+      <c r="F285">
+        <v>2017</v>
+      </c>
+      <c r="G285" t="s">
+        <v>45</v>
+      </c>
+      <c r="H285" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="I285" s="1">
+        <v>34</v>
+      </c>
+      <c r="J285" s="3">
+        <v>4</v>
+      </c>
+      <c r="K285" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="286" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A286" s="3">
+        <v>285</v>
+      </c>
+      <c r="B286" s="3">
+        <v>34</v>
+      </c>
+      <c r="C286" s="2">
+        <v>43093</v>
+      </c>
+      <c r="D286">
+        <v>51</v>
+      </c>
+      <c r="E286" t="s">
+        <v>69</v>
+      </c>
+      <c r="F286">
+        <v>2017</v>
+      </c>
+      <c r="G286" t="s">
+        <v>45</v>
+      </c>
+      <c r="H286" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="I286" s="1">
+        <v>61</v>
+      </c>
+      <c r="J286" s="3">
+        <v>4</v>
+      </c>
+      <c r="K286" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="287" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A287" s="3">
+        <v>286</v>
+      </c>
+      <c r="B287" s="3">
+        <v>34</v>
+      </c>
+      <c r="C287" s="2">
+        <v>43093</v>
+      </c>
+      <c r="D287">
+        <v>51</v>
+      </c>
+      <c r="E287" t="s">
+        <v>69</v>
+      </c>
+      <c r="F287">
+        <v>2017</v>
+      </c>
+      <c r="G287" t="s">
+        <v>45</v>
+      </c>
+      <c r="H287" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="I287" s="1">
+        <v>8</v>
+      </c>
+      <c r="J287" s="3">
+        <v>3</v>
+      </c>
+      <c r="K287" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="288" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A288" s="3">
+        <v>287</v>
+      </c>
+      <c r="B288" s="3">
+        <v>34</v>
+      </c>
+      <c r="C288" s="2">
+        <v>43093</v>
+      </c>
+      <c r="D288">
+        <v>51</v>
+      </c>
+      <c r="E288" t="s">
+        <v>69</v>
+      </c>
+      <c r="F288">
+        <v>2017</v>
+      </c>
+      <c r="G288" t="s">
+        <v>45</v>
+      </c>
+      <c r="H288" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="I288" s="1">
+        <v>0</v>
+      </c>
+      <c r="J288" s="3">
+        <v>3</v>
+      </c>
+      <c r="K288" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="289" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A289" s="3">
+        <v>288</v>
+      </c>
+      <c r="B289" s="3">
+        <v>34</v>
+      </c>
+      <c r="C289" s="2">
+        <v>43093</v>
+      </c>
+      <c r="D289">
+        <v>51</v>
+      </c>
+      <c r="E289" t="s">
+        <v>69</v>
+      </c>
+      <c r="F289">
+        <v>2017</v>
+      </c>
+      <c r="G289" t="s">
+        <v>45</v>
+      </c>
+      <c r="H289" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="I289" s="1">
+        <v>10</v>
+      </c>
+      <c r="J289" s="3">
+        <v>3</v>
+      </c>
+      <c r="K289" s="3">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Adding workout data and preliminary weight file sheet
</commit_message>
<xml_diff>
--- a/datasets/GymWorkouts.xlsx
+++ b/datasets/GymWorkouts.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="875" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="929" uniqueCount="85">
   <si>
     <t>Exercise Date</t>
   </si>
@@ -273,6 +273,12 @@
   </si>
   <si>
     <t>Seated Row</t>
+  </si>
+  <si>
+    <t>Dumbell Chest Press</t>
+  </si>
+  <si>
+    <t>Sled Pushes</t>
   </si>
 </sst>
 </file>
@@ -627,11 +633,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K289"/>
+  <dimension ref="A1:K307"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A266" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H292" sqref="H292"/>
+      <pane ySplit="1" topLeftCell="A277" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C311" sqref="C311"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -10765,6 +10771,636 @@
         <v>20</v>
       </c>
     </row>
+    <row r="290" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A290" s="3">
+        <v>289</v>
+      </c>
+      <c r="B290" s="3">
+        <v>35</v>
+      </c>
+      <c r="C290" s="2">
+        <v>43096</v>
+      </c>
+      <c r="D290">
+        <v>52</v>
+      </c>
+      <c r="E290" t="s">
+        <v>69</v>
+      </c>
+      <c r="F290">
+        <v>2017</v>
+      </c>
+      <c r="G290" t="s">
+        <v>19</v>
+      </c>
+      <c r="H290" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I290" s="1">
+        <v>100</v>
+      </c>
+      <c r="J290" s="3">
+        <v>5</v>
+      </c>
+      <c r="K290" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="291" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A291" s="3">
+        <v>290</v>
+      </c>
+      <c r="B291" s="3">
+        <v>35</v>
+      </c>
+      <c r="C291" s="2">
+        <v>43096</v>
+      </c>
+      <c r="D291">
+        <v>52</v>
+      </c>
+      <c r="E291" t="s">
+        <v>69</v>
+      </c>
+      <c r="F291">
+        <v>2017</v>
+      </c>
+      <c r="G291" t="s">
+        <v>19</v>
+      </c>
+      <c r="H291" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I291" s="1">
+        <v>55</v>
+      </c>
+      <c r="J291" s="3">
+        <v>5</v>
+      </c>
+      <c r="K291" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="292" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A292" s="3">
+        <v>291</v>
+      </c>
+      <c r="B292" s="3">
+        <v>35</v>
+      </c>
+      <c r="C292" s="2">
+        <v>43096</v>
+      </c>
+      <c r="D292">
+        <v>52</v>
+      </c>
+      <c r="E292" t="s">
+        <v>69</v>
+      </c>
+      <c r="F292">
+        <v>2017</v>
+      </c>
+      <c r="G292" t="s">
+        <v>19</v>
+      </c>
+      <c r="H292" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I292" s="1">
+        <v>90</v>
+      </c>
+      <c r="J292" s="3">
+        <v>5</v>
+      </c>
+      <c r="K292" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="293" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A293" s="3">
+        <v>292</v>
+      </c>
+      <c r="B293" s="3">
+        <v>35</v>
+      </c>
+      <c r="C293" s="2">
+        <v>43096</v>
+      </c>
+      <c r="D293">
+        <v>52</v>
+      </c>
+      <c r="E293" t="s">
+        <v>69</v>
+      </c>
+      <c r="F293">
+        <v>2017</v>
+      </c>
+      <c r="G293" t="s">
+        <v>19</v>
+      </c>
+      <c r="H293" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I293" s="1">
+        <v>105</v>
+      </c>
+      <c r="J293" s="3">
+        <v>5</v>
+      </c>
+      <c r="K293" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="294" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A294" s="3">
+        <v>293</v>
+      </c>
+      <c r="B294" s="3">
+        <v>35</v>
+      </c>
+      <c r="C294" s="2">
+        <v>43096</v>
+      </c>
+      <c r="D294">
+        <v>52</v>
+      </c>
+      <c r="E294" t="s">
+        <v>69</v>
+      </c>
+      <c r="F294">
+        <v>2017</v>
+      </c>
+      <c r="G294" t="s">
+        <v>19</v>
+      </c>
+      <c r="H294" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I294" s="1">
+        <v>0</v>
+      </c>
+      <c r="J294" s="3">
+        <v>3</v>
+      </c>
+      <c r="K294" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="295" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A295" s="3">
+        <v>294</v>
+      </c>
+      <c r="B295" s="3">
+        <v>35</v>
+      </c>
+      <c r="C295" s="2">
+        <v>43096</v>
+      </c>
+      <c r="D295">
+        <v>52</v>
+      </c>
+      <c r="E295" t="s">
+        <v>69</v>
+      </c>
+      <c r="F295">
+        <v>2017</v>
+      </c>
+      <c r="G295" t="s">
+        <v>19</v>
+      </c>
+      <c r="H295" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I295" s="1">
+        <v>0</v>
+      </c>
+      <c r="J295" s="3">
+        <v>3</v>
+      </c>
+      <c r="K295" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="296" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A296" s="3">
+        <v>295</v>
+      </c>
+      <c r="B296" s="3">
+        <v>35</v>
+      </c>
+      <c r="C296" s="2">
+        <v>43096</v>
+      </c>
+      <c r="D296">
+        <v>52</v>
+      </c>
+      <c r="E296" t="s">
+        <v>69</v>
+      </c>
+      <c r="F296">
+        <v>2017</v>
+      </c>
+      <c r="G296" t="s">
+        <v>19</v>
+      </c>
+      <c r="H296" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="I296" s="1">
+        <v>10</v>
+      </c>
+      <c r="J296" s="3">
+        <v>3</v>
+      </c>
+      <c r="K296" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="297" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A297" s="3">
+        <v>296</v>
+      </c>
+      <c r="B297" s="3">
+        <v>35</v>
+      </c>
+      <c r="C297" s="2">
+        <v>43096</v>
+      </c>
+      <c r="D297">
+        <v>52</v>
+      </c>
+      <c r="E297" t="s">
+        <v>69</v>
+      </c>
+      <c r="F297">
+        <v>2017</v>
+      </c>
+      <c r="G297" t="s">
+        <v>19</v>
+      </c>
+      <c r="H297" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="I297" s="1">
+        <v>8</v>
+      </c>
+      <c r="J297" s="3">
+        <v>3</v>
+      </c>
+      <c r="K297" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="298" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A298" s="3">
+        <v>297</v>
+      </c>
+      <c r="B298" s="3">
+        <v>35</v>
+      </c>
+      <c r="C298" s="2">
+        <v>43097</v>
+      </c>
+      <c r="D298">
+        <v>52</v>
+      </c>
+      <c r="E298" t="s">
+        <v>69</v>
+      </c>
+      <c r="F298">
+        <v>2017</v>
+      </c>
+      <c r="G298" t="s">
+        <v>17</v>
+      </c>
+      <c r="H298" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I298" s="1">
+        <v>26</v>
+      </c>
+      <c r="J298" s="3">
+        <v>4</v>
+      </c>
+      <c r="K298" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="299" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A299" s="3">
+        <v>298</v>
+      </c>
+      <c r="B299" s="3">
+        <v>35</v>
+      </c>
+      <c r="C299" s="2">
+        <v>43097</v>
+      </c>
+      <c r="D299">
+        <v>52</v>
+      </c>
+      <c r="E299" t="s">
+        <v>69</v>
+      </c>
+      <c r="F299">
+        <v>2017</v>
+      </c>
+      <c r="G299" t="s">
+        <v>17</v>
+      </c>
+      <c r="H299" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I299" s="1">
+        <v>26</v>
+      </c>
+      <c r="J299" s="3">
+        <v>4</v>
+      </c>
+      <c r="K299" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="300" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A300" s="3">
+        <v>299</v>
+      </c>
+      <c r="B300" s="3">
+        <v>35</v>
+      </c>
+      <c r="C300" s="2">
+        <v>43097</v>
+      </c>
+      <c r="D300">
+        <v>52</v>
+      </c>
+      <c r="E300" t="s">
+        <v>69</v>
+      </c>
+      <c r="F300">
+        <v>2017</v>
+      </c>
+      <c r="G300" t="s">
+        <v>17</v>
+      </c>
+      <c r="H300" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="I300" s="1">
+        <v>26</v>
+      </c>
+      <c r="J300" s="3">
+        <v>4</v>
+      </c>
+      <c r="K300" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="301" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A301" s="3">
+        <v>300</v>
+      </c>
+      <c r="B301" s="3">
+        <v>35</v>
+      </c>
+      <c r="C301" s="2">
+        <v>43097</v>
+      </c>
+      <c r="D301">
+        <v>52</v>
+      </c>
+      <c r="E301" t="s">
+        <v>69</v>
+      </c>
+      <c r="F301">
+        <v>2017</v>
+      </c>
+      <c r="G301" t="s">
+        <v>17</v>
+      </c>
+      <c r="H301" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I301" s="1">
+        <v>32</v>
+      </c>
+      <c r="J301" s="3">
+        <v>4</v>
+      </c>
+      <c r="K301" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="302" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A302" s="3">
+        <v>301</v>
+      </c>
+      <c r="B302" s="3">
+        <v>35</v>
+      </c>
+      <c r="C302" s="2">
+        <v>43097</v>
+      </c>
+      <c r="D302">
+        <v>52</v>
+      </c>
+      <c r="E302" t="s">
+        <v>69</v>
+      </c>
+      <c r="F302">
+        <v>2017</v>
+      </c>
+      <c r="G302" t="s">
+        <v>17</v>
+      </c>
+      <c r="H302" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I302" s="1">
+        <v>32</v>
+      </c>
+      <c r="J302" s="3">
+        <v>4</v>
+      </c>
+      <c r="K302" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="303" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A303" s="3">
+        <v>302</v>
+      </c>
+      <c r="B303" s="3">
+        <v>35</v>
+      </c>
+      <c r="C303" s="2">
+        <v>43097</v>
+      </c>
+      <c r="D303">
+        <v>52</v>
+      </c>
+      <c r="E303" t="s">
+        <v>69</v>
+      </c>
+      <c r="F303">
+        <v>2017</v>
+      </c>
+      <c r="G303" t="s">
+        <v>17</v>
+      </c>
+      <c r="H303" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="I303" s="1">
+        <v>59</v>
+      </c>
+      <c r="J303" s="3">
+        <v>4</v>
+      </c>
+      <c r="K303" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="304" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A304" s="3">
+        <v>303</v>
+      </c>
+      <c r="B304" s="3">
+        <v>35</v>
+      </c>
+      <c r="C304" s="2">
+        <v>43097</v>
+      </c>
+      <c r="D304">
+        <v>52</v>
+      </c>
+      <c r="E304" t="s">
+        <v>69</v>
+      </c>
+      <c r="F304">
+        <v>2017</v>
+      </c>
+      <c r="G304" t="s">
+        <v>17</v>
+      </c>
+      <c r="H304" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="I304" s="1">
+        <v>66</v>
+      </c>
+      <c r="J304" s="3">
+        <v>4</v>
+      </c>
+      <c r="K304" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="305" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A305" s="3">
+        <v>304</v>
+      </c>
+      <c r="B305" s="3">
+        <v>35</v>
+      </c>
+      <c r="C305" s="2">
+        <v>43097</v>
+      </c>
+      <c r="D305">
+        <v>52</v>
+      </c>
+      <c r="E305" t="s">
+        <v>69</v>
+      </c>
+      <c r="F305">
+        <v>2017</v>
+      </c>
+      <c r="G305" t="s">
+        <v>17</v>
+      </c>
+      <c r="H305" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I305" s="1">
+        <v>0</v>
+      </c>
+      <c r="J305" s="3">
+        <v>4</v>
+      </c>
+      <c r="K305" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="306" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A306" s="3">
+        <v>305</v>
+      </c>
+      <c r="B306" s="3">
+        <v>35</v>
+      </c>
+      <c r="C306" s="2">
+        <v>43097</v>
+      </c>
+      <c r="D306">
+        <v>52</v>
+      </c>
+      <c r="E306" t="s">
+        <v>69</v>
+      </c>
+      <c r="F306">
+        <v>2017</v>
+      </c>
+      <c r="G306" t="s">
+        <v>17</v>
+      </c>
+      <c r="H306" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I306" s="1">
+        <v>0</v>
+      </c>
+      <c r="J306" s="3">
+        <v>4</v>
+      </c>
+      <c r="K306" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="307" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A307" s="3">
+        <v>306</v>
+      </c>
+      <c r="B307" s="3">
+        <v>35</v>
+      </c>
+      <c r="C307" s="2">
+        <v>43097</v>
+      </c>
+      <c r="D307">
+        <v>52</v>
+      </c>
+      <c r="E307" t="s">
+        <v>69</v>
+      </c>
+      <c r="F307">
+        <v>2017</v>
+      </c>
+      <c r="G307" t="s">
+        <v>17</v>
+      </c>
+      <c r="H307" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="I307" s="1">
+        <v>30</v>
+      </c>
+      <c r="J307" s="3">
+        <v>5</v>
+      </c>
+      <c r="K307" s="3">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Adding 29/12/2017 workout data
</commit_message>
<xml_diff>
--- a/datasets/GymWorkouts.xlsx
+++ b/datasets/GymWorkouts.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="929" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="947" uniqueCount="85">
   <si>
     <t>Exercise Date</t>
   </si>
@@ -633,11 +633,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K307"/>
+  <dimension ref="A1:K313"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A277" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C311" sqref="C311"/>
+      <pane ySplit="1" topLeftCell="A289" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A315" sqref="A315"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -11401,6 +11401,216 @@
         <v>4</v>
       </c>
     </row>
+    <row r="308" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A308" s="3">
+        <v>307</v>
+      </c>
+      <c r="B308" s="3">
+        <v>36</v>
+      </c>
+      <c r="C308" s="2">
+        <v>43098</v>
+      </c>
+      <c r="D308">
+        <v>52</v>
+      </c>
+      <c r="E308" t="s">
+        <v>69</v>
+      </c>
+      <c r="F308">
+        <v>2017</v>
+      </c>
+      <c r="G308" t="s">
+        <v>50</v>
+      </c>
+      <c r="H308" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I308" s="1">
+        <v>90</v>
+      </c>
+      <c r="J308" s="3">
+        <v>5</v>
+      </c>
+      <c r="K308" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="309" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A309" s="3">
+        <v>308</v>
+      </c>
+      <c r="B309" s="3">
+        <v>36</v>
+      </c>
+      <c r="C309" s="2">
+        <v>43098</v>
+      </c>
+      <c r="D309">
+        <v>52</v>
+      </c>
+      <c r="E309" t="s">
+        <v>69</v>
+      </c>
+      <c r="F309">
+        <v>2017</v>
+      </c>
+      <c r="G309" t="s">
+        <v>50</v>
+      </c>
+      <c r="H309" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I309" s="1">
+        <v>130</v>
+      </c>
+      <c r="J309" s="3">
+        <v>5</v>
+      </c>
+      <c r="K309" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="310" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A310" s="3">
+        <v>309</v>
+      </c>
+      <c r="B310" s="3">
+        <v>36</v>
+      </c>
+      <c r="C310" s="2">
+        <v>43098</v>
+      </c>
+      <c r="D310">
+        <v>52</v>
+      </c>
+      <c r="E310" t="s">
+        <v>69</v>
+      </c>
+      <c r="F310">
+        <v>2017</v>
+      </c>
+      <c r="G310" t="s">
+        <v>50</v>
+      </c>
+      <c r="H310" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I310" s="1">
+        <v>100</v>
+      </c>
+      <c r="J310" s="3">
+        <v>4</v>
+      </c>
+      <c r="K310" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="311" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A311" s="3">
+        <v>310</v>
+      </c>
+      <c r="B311" s="3">
+        <v>36</v>
+      </c>
+      <c r="C311" s="2">
+        <v>43098</v>
+      </c>
+      <c r="D311">
+        <v>52</v>
+      </c>
+      <c r="E311" t="s">
+        <v>69</v>
+      </c>
+      <c r="F311">
+        <v>2017</v>
+      </c>
+      <c r="G311" t="s">
+        <v>50</v>
+      </c>
+      <c r="H311" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I311" s="1">
+        <v>60</v>
+      </c>
+      <c r="J311" s="3">
+        <v>4</v>
+      </c>
+      <c r="K311" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="312" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A312" s="3">
+        <v>311</v>
+      </c>
+      <c r="B312" s="3">
+        <v>36</v>
+      </c>
+      <c r="C312" s="2">
+        <v>43098</v>
+      </c>
+      <c r="D312">
+        <v>52</v>
+      </c>
+      <c r="E312" t="s">
+        <v>69</v>
+      </c>
+      <c r="F312">
+        <v>2017</v>
+      </c>
+      <c r="G312" t="s">
+        <v>50</v>
+      </c>
+      <c r="H312" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I312" s="1">
+        <v>54</v>
+      </c>
+      <c r="J312" s="3">
+        <v>4</v>
+      </c>
+      <c r="K312" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="313" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A313" s="3">
+        <v>312</v>
+      </c>
+      <c r="B313" s="3">
+        <v>36</v>
+      </c>
+      <c r="C313" s="2">
+        <v>43098</v>
+      </c>
+      <c r="D313">
+        <v>52</v>
+      </c>
+      <c r="E313" t="s">
+        <v>69</v>
+      </c>
+      <c r="F313">
+        <v>2017</v>
+      </c>
+      <c r="G313" t="s">
+        <v>50</v>
+      </c>
+      <c r="H313" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I313" s="1">
+        <v>45</v>
+      </c>
+      <c r="J313" s="3">
+        <v>4</v>
+      </c>
+      <c r="K313" s="3">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Adding TrainingArea column to GymWorkouts sheet and updating documentation
</commit_message>
<xml_diff>
--- a/datasets/GymWorkouts.xlsx
+++ b/datasets/GymWorkouts.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="947" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1260" uniqueCount="93">
   <si>
     <t>Exercise Date</t>
   </si>
@@ -279,6 +279,30 @@
   </si>
   <si>
     <t>Sled Pushes</t>
+  </si>
+  <si>
+    <t>TrainingArea</t>
+  </si>
+  <si>
+    <t>Chest</t>
+  </si>
+  <si>
+    <t>Back</t>
+  </si>
+  <si>
+    <t>Legs</t>
+  </si>
+  <si>
+    <t>Core</t>
+  </si>
+  <si>
+    <t>Arms</t>
+  </si>
+  <si>
+    <t>Shoulders</t>
+  </si>
+  <si>
+    <t>Full</t>
   </si>
 </sst>
 </file>
@@ -633,11 +657,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K313"/>
+  <dimension ref="A1:L313"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A289" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A315" sqref="A315"/>
+      <pane ySplit="1" topLeftCell="A285" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L305" sqref="L305"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -656,7 +680,7 @@
     <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>79</v>
       </c>
@@ -690,8 +714,11 @@
       <c r="K1" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -725,8 +752,11 @@
       <c r="K2" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -760,8 +790,11 @@
       <c r="K3" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -795,8 +828,11 @@
       <c r="K4" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -830,8 +866,11 @@
       <c r="K5" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -865,8 +904,11 @@
       <c r="K6" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -900,8 +942,11 @@
       <c r="K7" s="3">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -935,8 +980,11 @@
       <c r="K8" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -970,8 +1018,11 @@
       <c r="K9" s="3">
         <v>15</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L9" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -1005,8 +1056,11 @@
       <c r="K10" s="3">
         <v>15</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L10" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -1040,8 +1094,11 @@
       <c r="K11" s="3">
         <v>15</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L11" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -1075,8 +1132,11 @@
       <c r="K12" s="3">
         <v>6</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L12" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -1110,8 +1170,11 @@
       <c r="K13" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L13" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -1145,8 +1208,11 @@
       <c r="K14" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L14" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -1180,8 +1246,11 @@
       <c r="K15" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L15" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -1215,8 +1284,11 @@
       <c r="K16" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L16" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -1250,8 +1322,11 @@
       <c r="K17" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L17" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -1285,8 +1360,11 @@
       <c r="K18" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L18" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -1320,8 +1398,11 @@
       <c r="K19" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L19" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -1355,8 +1436,11 @@
       <c r="K20" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L20" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -1390,8 +1474,11 @@
       <c r="K21" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L21" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -1425,8 +1512,11 @@
       <c r="K22" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L22" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -1460,8 +1550,11 @@
       <c r="K23" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L23" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A24" s="3">
         <v>23</v>
       </c>
@@ -1495,8 +1588,11 @@
       <c r="K24" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L24" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A25" s="3">
         <v>24</v>
       </c>
@@ -1530,8 +1626,11 @@
       <c r="K25" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L25" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A26" s="3">
         <v>25</v>
       </c>
@@ -1565,8 +1664,11 @@
       <c r="K26" s="3">
         <v>10</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L26" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A27" s="3">
         <v>26</v>
       </c>
@@ -1600,8 +1702,11 @@
       <c r="K27" s="3">
         <v>10</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L27" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A28" s="3">
         <v>27</v>
       </c>
@@ -1635,8 +1740,11 @@
       <c r="K28" s="3">
         <v>20</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L28" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A29" s="3">
         <v>28</v>
       </c>
@@ -1670,8 +1778,11 @@
       <c r="K29" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L29" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A30" s="3">
         <v>29</v>
       </c>
@@ -1705,8 +1816,11 @@
       <c r="K30" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L30" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A31" s="3">
         <v>30</v>
       </c>
@@ -1740,8 +1854,11 @@
       <c r="K31" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L31" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A32" s="3">
         <v>31</v>
       </c>
@@ -1775,8 +1892,11 @@
       <c r="K32" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L32" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A33" s="3">
         <v>32</v>
       </c>
@@ -1810,8 +1930,11 @@
       <c r="K33" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L33" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A34" s="3">
         <v>33</v>
       </c>
@@ -1845,8 +1968,11 @@
       <c r="K34" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L34" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A35" s="3">
         <v>34</v>
       </c>
@@ -1880,8 +2006,11 @@
       <c r="K35" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L35" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A36" s="3">
         <v>35</v>
       </c>
@@ -1915,8 +2044,11 @@
       <c r="K36" s="3">
         <v>10</v>
       </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L36" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A37" s="3">
         <v>36</v>
       </c>
@@ -1950,8 +2082,11 @@
       <c r="K37" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L37" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A38" s="3">
         <v>37</v>
       </c>
@@ -1985,8 +2120,11 @@
       <c r="K38" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L38" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A39" s="3">
         <v>38</v>
       </c>
@@ -2020,8 +2158,11 @@
       <c r="K39" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L39" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A40" s="3">
         <v>39</v>
       </c>
@@ -2055,8 +2196,11 @@
       <c r="K40" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L40" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A41" s="3">
         <v>40</v>
       </c>
@@ -2090,8 +2234,11 @@
       <c r="K41" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L41" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A42" s="3">
         <v>41</v>
       </c>
@@ -2125,8 +2272,11 @@
       <c r="K42" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L42" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A43" s="3">
         <v>42</v>
       </c>
@@ -2160,8 +2310,11 @@
       <c r="K43" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L43" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A44" s="3">
         <v>43</v>
       </c>
@@ -2195,8 +2348,11 @@
       <c r="K44" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L44" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A45" s="3">
         <v>44</v>
       </c>
@@ -2230,8 +2386,11 @@
       <c r="K45" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L45" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A46" s="3">
         <v>45</v>
       </c>
@@ -2265,8 +2424,11 @@
       <c r="K46" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L46" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A47" s="3">
         <v>46</v>
       </c>
@@ -2300,8 +2462,11 @@
       <c r="K47" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L47" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A48" s="3">
         <v>47</v>
       </c>
@@ -2335,8 +2500,11 @@
       <c r="K48" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L48" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A49" s="3">
         <v>48</v>
       </c>
@@ -2370,8 +2538,11 @@
       <c r="K49" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L49" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A50" s="3">
         <v>49</v>
       </c>
@@ -2405,8 +2576,11 @@
       <c r="K50" s="3">
         <v>10</v>
       </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L50" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A51" s="3">
         <v>50</v>
       </c>
@@ -2440,8 +2614,11 @@
       <c r="K51" s="3">
         <v>10</v>
       </c>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L51" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A52" s="3">
         <v>51</v>
       </c>
@@ -2475,8 +2652,11 @@
       <c r="K52" s="3">
         <v>10</v>
       </c>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L52" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A53" s="3">
         <v>52</v>
       </c>
@@ -2510,8 +2690,11 @@
       <c r="K53" s="3">
         <v>10</v>
       </c>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L53" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A54" s="3">
         <v>53</v>
       </c>
@@ -2545,8 +2728,11 @@
       <c r="K54" s="3">
         <v>10</v>
       </c>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L54" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A55" s="3">
         <v>54</v>
       </c>
@@ -2580,8 +2766,11 @@
       <c r="K55" s="3">
         <v>10</v>
       </c>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L55" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A56" s="3">
         <v>55</v>
       </c>
@@ -2615,8 +2804,11 @@
       <c r="K56" s="3">
         <v>10</v>
       </c>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L56" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A57" s="3">
         <v>56</v>
       </c>
@@ -2650,8 +2842,11 @@
       <c r="K57" s="3">
         <v>10</v>
       </c>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L57" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A58" s="3">
         <v>57</v>
       </c>
@@ -2685,8 +2880,11 @@
       <c r="K58" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L58" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A59" s="3">
         <v>58</v>
       </c>
@@ -2720,8 +2918,11 @@
       <c r="K59" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L59" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A60" s="3">
         <v>59</v>
       </c>
@@ -2755,8 +2956,11 @@
       <c r="K60" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L60" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A61" s="3">
         <v>60</v>
       </c>
@@ -2790,8 +2994,11 @@
       <c r="K61" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L61" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A62" s="3">
         <v>61</v>
       </c>
@@ -2825,8 +3032,11 @@
       <c r="K62" s="3">
         <v>10</v>
       </c>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L62" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A63" s="3">
         <v>62</v>
       </c>
@@ -2860,8 +3070,11 @@
       <c r="K63" s="3">
         <v>10</v>
       </c>
-    </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L63" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A64" s="3">
         <v>63</v>
       </c>
@@ -2895,8 +3108,11 @@
       <c r="K64" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L64" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A65" s="3">
         <v>64</v>
       </c>
@@ -2930,8 +3146,11 @@
       <c r="K65" s="3">
         <v>10</v>
       </c>
-    </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L65" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A66" s="3">
         <v>65</v>
       </c>
@@ -2965,8 +3184,11 @@
       <c r="K66" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L66" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A67" s="3">
         <v>66</v>
       </c>
@@ -3000,8 +3222,11 @@
       <c r="K67" s="3">
         <v>6</v>
       </c>
-    </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L67" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A68" s="3">
         <v>67</v>
       </c>
@@ -3035,8 +3260,11 @@
       <c r="K68" s="3">
         <v>6</v>
       </c>
-    </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L68" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A69" s="3">
         <v>68</v>
       </c>
@@ -3070,8 +3298,11 @@
       <c r="K69" s="3">
         <v>25</v>
       </c>
-    </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L69" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A70" s="3">
         <v>69</v>
       </c>
@@ -3105,8 +3336,11 @@
       <c r="K70" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L70" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A71" s="3">
         <v>70</v>
       </c>
@@ -3140,8 +3374,11 @@
       <c r="K71" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L71" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A72" s="3">
         <v>71</v>
       </c>
@@ -3175,8 +3412,11 @@
       <c r="K72" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L72" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A73" s="3">
         <v>72</v>
       </c>
@@ -3210,8 +3450,11 @@
       <c r="K73" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L73" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A74" s="3">
         <v>73</v>
       </c>
@@ -3245,8 +3488,11 @@
       <c r="K74" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L74" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A75" s="3">
         <v>74</v>
       </c>
@@ -3280,8 +3526,11 @@
       <c r="K75" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L75" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A76" s="3">
         <v>75</v>
       </c>
@@ -3315,8 +3564,11 @@
       <c r="K76" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L76" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A77" s="3">
         <v>76</v>
       </c>
@@ -3350,8 +3602,11 @@
       <c r="K77" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L77" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A78" s="3">
         <v>77</v>
       </c>
@@ -3385,8 +3640,11 @@
       <c r="K78" s="3">
         <v>10</v>
       </c>
-    </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L78" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A79" s="3">
         <v>78</v>
       </c>
@@ -3420,8 +3678,11 @@
       <c r="K79" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L79" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A80" s="3">
         <v>79</v>
       </c>
@@ -3455,8 +3716,11 @@
       <c r="K80" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L80" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A81" s="3">
         <v>80</v>
       </c>
@@ -3490,8 +3754,11 @@
       <c r="K81" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L81" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A82" s="3">
         <v>81</v>
       </c>
@@ -3525,8 +3792,11 @@
       <c r="K82" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L82" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A83" s="3">
         <v>82</v>
       </c>
@@ -3560,8 +3830,11 @@
       <c r="K83" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L83" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A84" s="3">
         <v>83</v>
       </c>
@@ -3595,8 +3868,11 @@
       <c r="K84" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L84" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A85" s="3">
         <v>84</v>
       </c>
@@ -3630,8 +3906,11 @@
       <c r="K85" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L85" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A86" s="3">
         <v>85</v>
       </c>
@@ -3665,8 +3944,11 @@
       <c r="K86" s="3">
         <v>20</v>
       </c>
-    </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L86" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A87" s="3">
         <v>86</v>
       </c>
@@ -3700,8 +3982,11 @@
       <c r="K87" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L87" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="88" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A88" s="3">
         <v>87</v>
       </c>
@@ -3735,8 +4020,11 @@
       <c r="K88" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L88" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="89" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A89" s="3">
         <v>88</v>
       </c>
@@ -3770,8 +4058,11 @@
       <c r="K89" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L89" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="90" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A90" s="3">
         <v>89</v>
       </c>
@@ -3805,8 +4096,11 @@
       <c r="K90" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L90" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="91" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A91" s="3">
         <v>90</v>
       </c>
@@ -3840,8 +4134,11 @@
       <c r="K91" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L91" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="92" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A92" s="3">
         <v>91</v>
       </c>
@@ -3875,8 +4172,11 @@
       <c r="K92" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L92" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="93" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A93" s="3">
         <v>92</v>
       </c>
@@ -3910,8 +4210,11 @@
       <c r="K93" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L93" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="94" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A94" s="3">
         <v>93</v>
       </c>
@@ -3945,8 +4248,11 @@
       <c r="K94" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L94" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="95" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A95" s="3">
         <v>94</v>
       </c>
@@ -3980,8 +4286,11 @@
       <c r="K95" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L95" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="96" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A96" s="3">
         <v>95</v>
       </c>
@@ -4015,8 +4324,11 @@
       <c r="K96" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L96" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="97" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A97" s="3">
         <v>96</v>
       </c>
@@ -4050,8 +4362,11 @@
       <c r="K97" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L97" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="98" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A98" s="3">
         <v>97</v>
       </c>
@@ -4085,8 +4400,11 @@
       <c r="K98" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L98" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="99" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A99" s="3">
         <v>98</v>
       </c>
@@ -4120,8 +4438,11 @@
       <c r="K99" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L99" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="100" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A100" s="3">
         <v>99</v>
       </c>
@@ -4155,8 +4476,11 @@
       <c r="K100" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L100" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="101" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A101" s="3">
         <v>100</v>
       </c>
@@ -4190,8 +4514,11 @@
       <c r="K101" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L101" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="102" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A102" s="3">
         <v>101</v>
       </c>
@@ -4225,8 +4552,11 @@
       <c r="K102" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L102" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="103" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A103" s="3">
         <v>102</v>
       </c>
@@ -4260,8 +4590,11 @@
       <c r="K103" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L103" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="104" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A104" s="3">
         <v>103</v>
       </c>
@@ -4295,8 +4628,11 @@
       <c r="K104" s="3">
         <v>10</v>
       </c>
-    </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L104" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="105" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A105" s="3">
         <v>104</v>
       </c>
@@ -4330,8 +4666,11 @@
       <c r="K105" s="3">
         <v>10</v>
       </c>
-    </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L105" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="106" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A106" s="3">
         <v>105</v>
       </c>
@@ -4365,8 +4704,11 @@
       <c r="K106" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L106" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="107" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A107" s="3">
         <v>106</v>
       </c>
@@ -4400,8 +4742,11 @@
       <c r="K107" s="3">
         <v>10</v>
       </c>
-    </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L107" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="108" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A108" s="3">
         <v>107</v>
       </c>
@@ -4435,8 +4780,11 @@
       <c r="K108" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L108" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="109" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A109" s="3">
         <v>108</v>
       </c>
@@ -4470,8 +4818,11 @@
       <c r="K109" s="3">
         <v>6</v>
       </c>
-    </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L109" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="110" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A110" s="3">
         <v>109</v>
       </c>
@@ -4505,8 +4856,11 @@
       <c r="K110" s="3">
         <v>6</v>
       </c>
-    </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L110" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="111" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A111" s="3">
         <v>110</v>
       </c>
@@ -4540,8 +4894,11 @@
       <c r="K111" s="3">
         <v>25</v>
       </c>
-    </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L111" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="112" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A112" s="3">
         <v>111</v>
       </c>
@@ -4575,8 +4932,11 @@
       <c r="K112" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L112" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="113" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A113" s="3">
         <v>112</v>
       </c>
@@ -4610,8 +4970,11 @@
       <c r="K113" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L113" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="114" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A114" s="3">
         <v>113</v>
       </c>
@@ -4645,8 +5008,11 @@
       <c r="K114" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L114" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="115" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A115" s="3">
         <v>114</v>
       </c>
@@ -4680,8 +5046,11 @@
       <c r="K115" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L115" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="116" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A116" s="3">
         <v>115</v>
       </c>
@@ -4715,8 +5084,11 @@
       <c r="K116" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L116" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="117" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A117" s="3">
         <v>116</v>
       </c>
@@ -4750,8 +5122,11 @@
       <c r="K117" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L117" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="118" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A118" s="3">
         <v>117</v>
       </c>
@@ -4785,8 +5160,11 @@
       <c r="K118" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L118" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="119" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A119" s="3">
         <v>118</v>
       </c>
@@ -4820,8 +5198,11 @@
       <c r="K119" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L119" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="120" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A120" s="3">
         <v>119</v>
       </c>
@@ -4855,8 +5236,11 @@
       <c r="K120" s="3">
         <v>10</v>
       </c>
-    </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L120" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="121" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A121" s="3">
         <v>120</v>
       </c>
@@ -4890,8 +5274,11 @@
       <c r="K121" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L121" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="122" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A122" s="3">
         <v>121</v>
       </c>
@@ -4925,8 +5312,11 @@
       <c r="K122" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L122" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="123" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A123" s="3">
         <v>122</v>
       </c>
@@ -4960,8 +5350,11 @@
       <c r="K123" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L123" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="124" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A124" s="3">
         <v>123</v>
       </c>
@@ -4995,8 +5388,11 @@
       <c r="K124" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L124" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="125" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A125" s="3">
         <v>124</v>
       </c>
@@ -5030,8 +5426,11 @@
       <c r="K125" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L125" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="126" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A126" s="3">
         <v>125</v>
       </c>
@@ -5065,8 +5464,11 @@
       <c r="K126" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L126" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="127" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A127" s="3">
         <v>126</v>
       </c>
@@ -5100,8 +5502,11 @@
       <c r="K127" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L127" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="128" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A128" s="3">
         <v>127</v>
       </c>
@@ -5135,8 +5540,11 @@
       <c r="K128" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L128" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="129" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A129" s="3">
         <v>128</v>
       </c>
@@ -5170,8 +5578,11 @@
       <c r="K129" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L129" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="130" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A130" s="3">
         <v>129</v>
       </c>
@@ -5205,8 +5616,11 @@
       <c r="K130" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L130" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="131" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A131" s="3">
         <v>130</v>
       </c>
@@ -5240,8 +5654,11 @@
       <c r="K131" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L131" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="132" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A132" s="3">
         <v>131</v>
       </c>
@@ -5275,8 +5692,11 @@
       <c r="K132" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L132" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="133" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A133" s="3">
         <v>132</v>
       </c>
@@ -5310,8 +5730,11 @@
       <c r="K133" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L133" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="134" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A134" s="3">
         <v>133</v>
       </c>
@@ -5345,8 +5768,11 @@
       <c r="K134" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L134" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="135" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A135" s="3">
         <v>134</v>
       </c>
@@ -5380,8 +5806,11 @@
       <c r="K135" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L135" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="136" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A136" s="3">
         <v>135</v>
       </c>
@@ -5415,8 +5844,11 @@
       <c r="K136" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="137" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L136" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="137" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A137" s="3">
         <v>136</v>
       </c>
@@ -5450,8 +5882,11 @@
       <c r="K137" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L137" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="138" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A138" s="3">
         <v>137</v>
       </c>
@@ -5485,8 +5920,11 @@
       <c r="K138" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L138" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="139" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A139" s="3">
         <v>138</v>
       </c>
@@ -5520,8 +5958,11 @@
       <c r="K139" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L139" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="140" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A140" s="3">
         <v>139</v>
       </c>
@@ -5555,8 +5996,11 @@
       <c r="K140" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="141" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L140" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="141" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A141" s="3">
         <v>140</v>
       </c>
@@ -5590,8 +6034,11 @@
       <c r="K141" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="142" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L141" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="142" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A142" s="3">
         <v>141</v>
       </c>
@@ -5625,8 +6072,11 @@
       <c r="K142" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="143" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L142" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="143" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A143" s="3">
         <v>142</v>
       </c>
@@ -5660,8 +6110,11 @@
       <c r="K143" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="144" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L143" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="144" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A144" s="3">
         <v>143</v>
       </c>
@@ -5695,8 +6148,11 @@
       <c r="K144" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="145" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L144" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="145" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A145" s="3">
         <v>144</v>
       </c>
@@ -5730,8 +6186,11 @@
       <c r="K145" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="146" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L145" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="146" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A146" s="3">
         <v>145</v>
       </c>
@@ -5765,8 +6224,11 @@
       <c r="K146" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="147" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L146" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="147" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A147" s="3">
         <v>146</v>
       </c>
@@ -5800,8 +6262,11 @@
       <c r="K147" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="148" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L147" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="148" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A148" s="3">
         <v>147</v>
       </c>
@@ -5835,8 +6300,11 @@
       <c r="K148" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="149" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L148" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="149" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A149" s="3">
         <v>148</v>
       </c>
@@ -5870,8 +6338,11 @@
       <c r="K149" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="150" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L149" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="150" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A150" s="3">
         <v>149</v>
       </c>
@@ -5905,8 +6376,11 @@
       <c r="K150" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="151" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L150" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="151" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A151" s="3">
         <v>150</v>
       </c>
@@ -5940,8 +6414,11 @@
       <c r="K151" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="152" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L151" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="152" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A152" s="3">
         <v>151</v>
       </c>
@@ -5975,8 +6452,11 @@
       <c r="K152" s="3">
         <v>10</v>
       </c>
-    </row>
-    <row r="153" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L152" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="153" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A153" s="3">
         <v>152</v>
       </c>
@@ -6010,8 +6490,11 @@
       <c r="K153" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="154" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L153" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="154" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A154" s="3">
         <v>153</v>
       </c>
@@ -6045,8 +6528,11 @@
       <c r="K154" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="155" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L154" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="155" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A155" s="3">
         <v>154</v>
       </c>
@@ -6080,8 +6566,11 @@
       <c r="K155" s="3">
         <v>6</v>
       </c>
-    </row>
-    <row r="156" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L155" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="156" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A156" s="3">
         <v>155</v>
       </c>
@@ -6115,8 +6604,11 @@
       <c r="K156" s="3">
         <v>10</v>
       </c>
-    </row>
-    <row r="157" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L156" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="157" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A157" s="3">
         <v>156</v>
       </c>
@@ -6150,8 +6642,11 @@
       <c r="K157" s="3">
         <v>10</v>
       </c>
-    </row>
-    <row r="158" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L157" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="158" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A158" s="3">
         <v>157</v>
       </c>
@@ -6185,8 +6680,11 @@
       <c r="K158" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="159" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L158" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="159" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A159" s="3">
         <v>158</v>
       </c>
@@ -6220,8 +6718,11 @@
       <c r="K159" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="160" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L159" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="160" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A160" s="3">
         <v>159</v>
       </c>
@@ -6255,8 +6756,11 @@
       <c r="K160" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="161" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L160" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="161" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A161" s="3">
         <v>160</v>
       </c>
@@ -6290,8 +6794,11 @@
       <c r="K161" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="162" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L161" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="162" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A162" s="3">
         <v>161</v>
       </c>
@@ -6325,8 +6832,11 @@
       <c r="K162" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="163" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L162" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="163" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A163" s="3">
         <v>162</v>
       </c>
@@ -6360,8 +6870,11 @@
       <c r="K163" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="164" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L163" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="164" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A164" s="3">
         <v>163</v>
       </c>
@@ -6395,8 +6908,11 @@
       <c r="K164" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="165" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L164" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="165" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A165" s="3">
         <v>164</v>
       </c>
@@ -6430,8 +6946,11 @@
       <c r="K165" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="166" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L165" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="166" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A166" s="3">
         <v>165</v>
       </c>
@@ -6465,8 +6984,11 @@
       <c r="K166" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="167" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L166" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="167" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A167" s="3">
         <v>166</v>
       </c>
@@ -6500,8 +7022,11 @@
       <c r="K167" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="168" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L167" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="168" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A168" s="3">
         <v>167</v>
       </c>
@@ -6535,8 +7060,11 @@
       <c r="K168" s="3">
         <v>10</v>
       </c>
-    </row>
-    <row r="169" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L168" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="169" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A169" s="3">
         <v>168</v>
       </c>
@@ -6570,8 +7098,11 @@
       <c r="K169" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="170" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L169" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="170" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A170" s="3">
         <v>169</v>
       </c>
@@ -6605,8 +7136,11 @@
       <c r="K170" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="171" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L170" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="171" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A171" s="3">
         <v>170</v>
       </c>
@@ -6640,8 +7174,11 @@
       <c r="K171" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="172" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L171" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="172" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A172" s="3">
         <v>171</v>
       </c>
@@ -6675,8 +7212,11 @@
       <c r="K172" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="173" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L172" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="173" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A173" s="3">
         <v>172</v>
       </c>
@@ -6710,8 +7250,11 @@
       <c r="K173" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="174" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L173" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="174" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A174" s="3">
         <v>173</v>
       </c>
@@ -6745,8 +7288,11 @@
       <c r="K174" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="175" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L174" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="175" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A175" s="3">
         <v>174</v>
       </c>
@@ -6780,8 +7326,11 @@
       <c r="K175" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="176" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L175" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="176" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A176" s="3">
         <v>175</v>
       </c>
@@ -6815,8 +7364,11 @@
       <c r="K176" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="177" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L176" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="177" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A177" s="3">
         <v>176</v>
       </c>
@@ -6850,8 +7402,11 @@
       <c r="K177" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="178" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L177" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="178" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A178" s="3">
         <v>177</v>
       </c>
@@ -6885,8 +7440,11 @@
       <c r="K178" s="3">
         <v>10</v>
       </c>
-    </row>
-    <row r="179" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L178" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="179" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A179" s="3">
         <v>178</v>
       </c>
@@ -6920,8 +7478,11 @@
       <c r="K179" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="180" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L179" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="180" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A180" s="3">
         <v>179</v>
       </c>
@@ -6955,8 +7516,11 @@
       <c r="K180" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="181" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L180" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="181" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A181" s="3">
         <v>180</v>
       </c>
@@ -6990,8 +7554,11 @@
       <c r="K181" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="182" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L181" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="182" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A182" s="3">
         <v>181</v>
       </c>
@@ -7025,8 +7592,11 @@
       <c r="K182" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="183" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L182" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="183" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A183" s="3">
         <v>182</v>
       </c>
@@ -7060,8 +7630,11 @@
       <c r="K183" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="184" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L183" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="184" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A184" s="3">
         <v>183</v>
       </c>
@@ -7095,8 +7668,11 @@
       <c r="K184" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="185" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L184" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="185" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A185" s="3">
         <v>184</v>
       </c>
@@ -7130,8 +7706,11 @@
       <c r="K185" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="186" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L185" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="186" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A186" s="3">
         <v>185</v>
       </c>
@@ -7165,8 +7744,11 @@
       <c r="K186" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="187" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L186" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="187" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A187" s="3">
         <v>186</v>
       </c>
@@ -7200,8 +7782,11 @@
       <c r="K187" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="188" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L187" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="188" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A188" s="3">
         <v>187</v>
       </c>
@@ -7235,8 +7820,11 @@
       <c r="K188" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="189" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L188" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="189" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A189" s="3">
         <v>188</v>
       </c>
@@ -7270,8 +7858,11 @@
       <c r="K189" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="190" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L189" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="190" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A190" s="3">
         <v>189</v>
       </c>
@@ -7305,8 +7896,11 @@
       <c r="K190" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="191" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L190" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="191" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A191" s="3">
         <v>190</v>
       </c>
@@ -7340,8 +7934,11 @@
       <c r="K191" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="192" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L191" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="192" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A192" s="3">
         <v>191</v>
       </c>
@@ -7375,8 +7972,11 @@
       <c r="K192" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="193" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L192" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="193" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A193" s="3">
         <v>192</v>
       </c>
@@ -7410,8 +8010,11 @@
       <c r="K193" s="3">
         <v>10</v>
       </c>
-    </row>
-    <row r="194" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L193" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="194" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A194" s="3">
         <v>193</v>
       </c>
@@ -7445,8 +8048,11 @@
       <c r="K194" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="195" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L194" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="195" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A195" s="3">
         <v>194</v>
       </c>
@@ -7480,8 +8086,11 @@
       <c r="K195" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="196" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L195" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="196" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A196" s="3">
         <v>195</v>
       </c>
@@ -7515,8 +8124,11 @@
       <c r="K196" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="197" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L196" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="197" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A197" s="3">
         <v>196</v>
       </c>
@@ -7550,8 +8162,11 @@
       <c r="K197" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="198" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L197" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="198" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A198" s="3">
         <v>197</v>
       </c>
@@ -7585,8 +8200,11 @@
       <c r="K198" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="199" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L198" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="199" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A199" s="3">
         <v>198</v>
       </c>
@@ -7620,8 +8238,11 @@
       <c r="K199" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="200" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L199" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="200" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A200" s="3">
         <v>199</v>
       </c>
@@ -7655,8 +8276,11 @@
       <c r="K200" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="201" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L200" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="201" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A201" s="3">
         <v>200</v>
       </c>
@@ -7690,8 +8314,11 @@
       <c r="K201" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="202" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L201" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="202" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A202" s="3">
         <v>201</v>
       </c>
@@ -7725,8 +8352,11 @@
       <c r="K202" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="203" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L202" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="203" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A203" s="3">
         <v>202</v>
       </c>
@@ -7760,8 +8390,11 @@
       <c r="K203" s="3">
         <v>10</v>
       </c>
-    </row>
-    <row r="204" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L203" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="204" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A204" s="3">
         <v>203</v>
       </c>
@@ -7795,8 +8428,11 @@
       <c r="K204" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="205" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L204" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="205" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A205" s="3">
         <v>204</v>
       </c>
@@ -7830,8 +8466,11 @@
       <c r="K205" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="206" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L205" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="206" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A206" s="3">
         <v>205</v>
       </c>
@@ -7865,8 +8504,11 @@
       <c r="K206" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="207" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L206" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="207" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A207" s="3">
         <v>206</v>
       </c>
@@ -7900,8 +8542,11 @@
       <c r="K207" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="208" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L207" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="208" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A208" s="3">
         <v>207</v>
       </c>
@@ -7935,8 +8580,11 @@
       <c r="K208" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="209" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L208" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="209" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A209" s="3">
         <v>208</v>
       </c>
@@ -7970,8 +8618,11 @@
       <c r="K209" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="210" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L209" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="210" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A210" s="3">
         <v>209</v>
       </c>
@@ -8005,8 +8656,11 @@
       <c r="K210" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="211" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L210" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="211" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A211" s="3">
         <v>210</v>
       </c>
@@ -8040,8 +8694,11 @@
       <c r="K211" s="3">
         <v>10</v>
       </c>
-    </row>
-    <row r="212" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L211" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="212" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A212" s="3">
         <v>211</v>
       </c>
@@ -8075,8 +8732,11 @@
       <c r="K212" s="3">
         <v>10</v>
       </c>
-    </row>
-    <row r="213" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L212" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="213" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A213" s="3">
         <v>212</v>
       </c>
@@ -8110,8 +8770,11 @@
       <c r="K213" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="214" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L213" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="214" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A214" s="3">
         <v>213</v>
       </c>
@@ -8145,8 +8808,11 @@
       <c r="K214" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="215" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L214" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="215" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A215" s="3">
         <v>214</v>
       </c>
@@ -8180,8 +8846,11 @@
       <c r="K215" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="216" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L215" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="216" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A216" s="3">
         <v>215</v>
       </c>
@@ -8215,8 +8884,11 @@
       <c r="K216" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="217" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L216" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="217" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A217" s="3">
         <v>216</v>
       </c>
@@ -8250,8 +8922,11 @@
       <c r="K217" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="218" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L217" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="218" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A218" s="3">
         <v>217</v>
       </c>
@@ -8285,8 +8960,11 @@
       <c r="K218" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="219" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L218" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="219" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A219" s="3">
         <v>218</v>
       </c>
@@ -8320,8 +8998,11 @@
       <c r="K219" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="220" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L219" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="220" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A220" s="3">
         <v>219</v>
       </c>
@@ -8355,8 +9036,11 @@
       <c r="K220" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="221" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L220" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="221" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A221" s="3">
         <v>220</v>
       </c>
@@ -8390,8 +9074,11 @@
       <c r="K221" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="222" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L221" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="222" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A222" s="3">
         <v>221</v>
       </c>
@@ -8425,8 +9112,11 @@
       <c r="K222" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="223" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L222" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="223" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A223" s="3">
         <v>222</v>
       </c>
@@ -8460,8 +9150,11 @@
       <c r="K223" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="224" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L223" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="224" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A224" s="3">
         <v>223</v>
       </c>
@@ -8495,8 +9188,11 @@
       <c r="K224" s="3">
         <v>10</v>
       </c>
-    </row>
-    <row r="225" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L224" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="225" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A225" s="3">
         <v>224</v>
       </c>
@@ -8530,8 +9226,11 @@
       <c r="K225" s="3">
         <v>10</v>
       </c>
-    </row>
-    <row r="226" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L225" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="226" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A226" s="3">
         <v>225</v>
       </c>
@@ -8565,8 +9264,11 @@
       <c r="K226" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="227" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L226" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="227" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A227" s="3">
         <v>226</v>
       </c>
@@ -8600,8 +9302,11 @@
       <c r="K227" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="228" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L227" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="228" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A228" s="3">
         <v>227</v>
       </c>
@@ -8635,8 +9340,11 @@
       <c r="K228" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="229" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L228" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="229" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A229" s="3">
         <v>228</v>
       </c>
@@ -8670,8 +9378,11 @@
       <c r="K229" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="230" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L229" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="230" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A230" s="3">
         <v>229</v>
       </c>
@@ -8705,8 +9416,11 @@
       <c r="K230" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="231" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L230" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="231" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A231" s="3">
         <v>230</v>
       </c>
@@ -8740,8 +9454,11 @@
       <c r="K231" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="232" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L231" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="232" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A232" s="3">
         <v>231</v>
       </c>
@@ -8775,8 +9492,11 @@
       <c r="K232" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="233" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L232" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="233" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A233" s="3">
         <v>232</v>
       </c>
@@ -8810,8 +9530,11 @@
       <c r="K233" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="234" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L233" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="234" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A234" s="3">
         <v>233</v>
       </c>
@@ -8845,8 +9568,11 @@
       <c r="K234" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="235" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L234" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="235" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A235" s="3">
         <v>234</v>
       </c>
@@ -8880,8 +9606,11 @@
       <c r="K235" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="236" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L235" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="236" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A236" s="3">
         <v>235</v>
       </c>
@@ -8915,8 +9644,11 @@
       <c r="K236" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="237" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L236" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="237" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A237" s="3">
         <v>236</v>
       </c>
@@ -8950,8 +9682,11 @@
       <c r="K237" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="238" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L237" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="238" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A238" s="3">
         <v>237</v>
       </c>
@@ -8985,8 +9720,11 @@
       <c r="K238" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="239" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L238" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="239" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A239" s="3">
         <v>238</v>
       </c>
@@ -9020,8 +9758,11 @@
       <c r="K239" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="240" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L239" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="240" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A240" s="3">
         <v>239</v>
       </c>
@@ -9055,8 +9796,11 @@
       <c r="K240" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="241" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L240" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="241" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A241" s="3">
         <v>240</v>
       </c>
@@ -9090,8 +9834,11 @@
       <c r="K241" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="242" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L241" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="242" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A242" s="3">
         <v>241</v>
       </c>
@@ -9125,8 +9872,11 @@
       <c r="K242" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="243" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L242" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="243" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A243" s="3">
         <v>242</v>
       </c>
@@ -9160,8 +9910,11 @@
       <c r="K243" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="244" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L243" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="244" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A244" s="3">
         <v>243</v>
       </c>
@@ -9195,8 +9948,11 @@
       <c r="K244" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="245" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L244" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="245" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A245" s="3">
         <v>244</v>
       </c>
@@ -9230,8 +9986,11 @@
       <c r="K245" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="246" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L245" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="246" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A246" s="3">
         <v>245</v>
       </c>
@@ -9265,8 +10024,11 @@
       <c r="K246" s="3">
         <v>10</v>
       </c>
-    </row>
-    <row r="247" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L246" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="247" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A247" s="3">
         <v>246</v>
       </c>
@@ -9300,8 +10062,11 @@
       <c r="K247" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="248" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L247" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="248" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A248" s="3">
         <v>247</v>
       </c>
@@ -9335,8 +10100,11 @@
       <c r="K248" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="249" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L248" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="249" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A249" s="3">
         <v>248</v>
       </c>
@@ -9370,8 +10138,11 @@
       <c r="K249" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="250" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L249" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="250" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A250" s="3">
         <v>249</v>
       </c>
@@ -9405,8 +10176,11 @@
       <c r="K250" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="251" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L250" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="251" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A251" s="3">
         <v>250</v>
       </c>
@@ -9440,8 +10214,11 @@
       <c r="K251" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="252" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L251" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="252" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A252" s="3">
         <v>251</v>
       </c>
@@ -9475,8 +10252,11 @@
       <c r="K252" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="253" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L252" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="253" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A253" s="3">
         <v>252</v>
       </c>
@@ -9510,8 +10290,11 @@
       <c r="K253" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="254" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L253" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="254" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A254" s="3">
         <v>253</v>
       </c>
@@ -9545,8 +10328,11 @@
       <c r="K254" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="255" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L254" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="255" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A255" s="3">
         <v>254</v>
       </c>
@@ -9580,8 +10366,11 @@
       <c r="K255" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="256" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L255" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="256" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A256" s="3">
         <v>255</v>
       </c>
@@ -9615,8 +10404,11 @@
       <c r="K256" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="257" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L256" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="257" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A257" s="3">
         <v>256</v>
       </c>
@@ -9650,8 +10442,11 @@
       <c r="K257" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="258" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L257" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="258" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A258" s="3">
         <v>257</v>
       </c>
@@ -9685,8 +10480,11 @@
       <c r="K258" s="3">
         <v>10</v>
       </c>
-    </row>
-    <row r="259" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L258" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="259" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A259" s="3">
         <v>258</v>
       </c>
@@ -9720,8 +10518,11 @@
       <c r="K259" s="3">
         <v>10</v>
       </c>
-    </row>
-    <row r="260" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L259" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="260" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A260" s="3">
         <v>259</v>
       </c>
@@ -9755,8 +10556,11 @@
       <c r="K260" s="3">
         <v>10</v>
       </c>
-    </row>
-    <row r="261" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L260" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="261" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A261" s="3">
         <v>260</v>
       </c>
@@ -9790,8 +10594,11 @@
       <c r="K261" s="3">
         <v>10</v>
       </c>
-    </row>
-    <row r="262" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L261" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="262" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A262" s="3">
         <v>261</v>
       </c>
@@ -9825,8 +10632,11 @@
       <c r="K262" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="263" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L262" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="263" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A263" s="3">
         <v>262</v>
       </c>
@@ -9860,8 +10670,11 @@
       <c r="K263" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="264" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L263" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="264" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A264" s="3">
         <v>263</v>
       </c>
@@ -9895,8 +10708,11 @@
       <c r="K264" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="265" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L264" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="265" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A265" s="3">
         <v>264</v>
       </c>
@@ -9930,8 +10746,11 @@
       <c r="K265" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="266" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L265" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="266" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A266" s="3">
         <v>265</v>
       </c>
@@ -9965,8 +10784,11 @@
       <c r="K266" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="267" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L266" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="267" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A267" s="3">
         <v>266</v>
       </c>
@@ -10000,8 +10822,11 @@
       <c r="K267" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="268" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L267" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="268" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A268" s="3">
         <v>267</v>
       </c>
@@ -10035,8 +10860,11 @@
       <c r="K268" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="269" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L268" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="269" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A269" s="3">
         <v>268</v>
       </c>
@@ -10070,8 +10898,11 @@
       <c r="K269" s="3">
         <v>10</v>
       </c>
-    </row>
-    <row r="270" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L269" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="270" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A270" s="3">
         <v>269</v>
       </c>
@@ -10105,8 +10936,11 @@
       <c r="K270" s="3">
         <v>10</v>
       </c>
-    </row>
-    <row r="271" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L270" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="271" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A271" s="3">
         <v>270</v>
       </c>
@@ -10140,8 +10974,11 @@
       <c r="K271" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="272" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L271" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="272" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A272" s="3">
         <v>271</v>
       </c>
@@ -10175,8 +11012,11 @@
       <c r="K272" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="273" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L272" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="273" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A273" s="3">
         <v>272</v>
       </c>
@@ -10210,8 +11050,11 @@
       <c r="K273" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="274" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L273" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="274" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A274" s="3">
         <v>273</v>
       </c>
@@ -10245,8 +11088,11 @@
       <c r="K274" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="275" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L274" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="275" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A275" s="3">
         <v>274</v>
       </c>
@@ -10280,8 +11126,11 @@
       <c r="K275" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="276" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L275" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="276" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A276" s="3">
         <v>275</v>
       </c>
@@ -10315,8 +11164,11 @@
       <c r="K276" s="3">
         <v>10</v>
       </c>
-    </row>
-    <row r="277" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L276" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="277" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A277" s="3">
         <v>276</v>
       </c>
@@ -10350,8 +11202,11 @@
       <c r="K277" s="3">
         <v>10</v>
       </c>
-    </row>
-    <row r="278" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L277" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="278" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A278" s="3">
         <v>277</v>
       </c>
@@ -10385,8 +11240,11 @@
       <c r="K278" s="3">
         <v>10</v>
       </c>
-    </row>
-    <row r="279" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L278" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="279" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A279" s="3">
         <v>278</v>
       </c>
@@ -10420,8 +11278,11 @@
       <c r="K279" s="3">
         <v>10</v>
       </c>
-    </row>
-    <row r="280" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L279" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="280" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A280" s="3">
         <v>279</v>
       </c>
@@ -10455,8 +11316,11 @@
       <c r="K280" s="3">
         <v>10</v>
       </c>
-    </row>
-    <row r="281" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L280" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="281" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A281" s="3">
         <v>280</v>
       </c>
@@ -10490,8 +11354,11 @@
       <c r="K281" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="282" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L281" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="282" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A282" s="3">
         <v>281</v>
       </c>
@@ -10525,8 +11392,11 @@
       <c r="K282" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="283" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L282" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="283" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A283" s="3">
         <v>282</v>
       </c>
@@ -10560,8 +11430,11 @@
       <c r="K283" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="284" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L283" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="284" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A284" s="3">
         <v>283</v>
       </c>
@@ -10595,8 +11468,11 @@
       <c r="K284" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="285" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L284" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="285" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A285" s="3">
         <v>284</v>
       </c>
@@ -10630,8 +11506,11 @@
       <c r="K285" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="286" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L285" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="286" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A286" s="3">
         <v>285</v>
       </c>
@@ -10665,8 +11544,11 @@
       <c r="K286" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="287" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L286" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="287" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A287" s="3">
         <v>286</v>
       </c>
@@ -10700,8 +11582,11 @@
       <c r="K287" s="3">
         <v>10</v>
       </c>
-    </row>
-    <row r="288" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L287" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="288" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A288" s="3">
         <v>287</v>
       </c>
@@ -10735,8 +11620,11 @@
       <c r="K288" s="3">
         <v>10</v>
       </c>
-    </row>
-    <row r="289" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L288" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="289" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A289" s="3">
         <v>288</v>
       </c>
@@ -10770,8 +11658,11 @@
       <c r="K289" s="3">
         <v>20</v>
       </c>
-    </row>
-    <row r="290" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L289" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="290" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A290" s="3">
         <v>289</v>
       </c>
@@ -10805,8 +11696,11 @@
       <c r="K290" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="291" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L290" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="291" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A291" s="3">
         <v>290</v>
       </c>
@@ -10840,8 +11734,11 @@
       <c r="K291" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="292" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L291" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="292" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A292" s="3">
         <v>291</v>
       </c>
@@ -10875,8 +11772,11 @@
       <c r="K292" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="293" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L292" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="293" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A293" s="3">
         <v>292</v>
       </c>
@@ -10910,8 +11810,11 @@
       <c r="K293" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="294" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L293" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="294" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A294" s="3">
         <v>293</v>
       </c>
@@ -10945,8 +11848,11 @@
       <c r="K294" s="3">
         <v>10</v>
       </c>
-    </row>
-    <row r="295" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L294" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="295" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A295" s="3">
         <v>294</v>
       </c>
@@ -10980,8 +11886,11 @@
       <c r="K295" s="3">
         <v>10</v>
       </c>
-    </row>
-    <row r="296" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L295" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="296" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A296" s="3">
         <v>295</v>
       </c>
@@ -11015,8 +11924,11 @@
       <c r="K296" s="3">
         <v>10</v>
       </c>
-    </row>
-    <row r="297" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L296" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="297" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A297" s="3">
         <v>296</v>
       </c>
@@ -11050,8 +11962,11 @@
       <c r="K297" s="3">
         <v>10</v>
       </c>
-    </row>
-    <row r="298" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L297" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="298" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A298" s="3">
         <v>297</v>
       </c>
@@ -11085,8 +12000,11 @@
       <c r="K298" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="299" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L298" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="299" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A299" s="3">
         <v>298</v>
       </c>
@@ -11120,8 +12038,11 @@
       <c r="K299" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="300" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L299" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="300" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A300" s="3">
         <v>299</v>
       </c>
@@ -11155,8 +12076,11 @@
       <c r="K300" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="301" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L300" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="301" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A301" s="3">
         <v>300</v>
       </c>
@@ -11190,8 +12114,11 @@
       <c r="K301" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="302" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L301" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="302" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A302" s="3">
         <v>301</v>
       </c>
@@ -11225,8 +12152,11 @@
       <c r="K302" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="303" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L302" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="303" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A303" s="3">
         <v>302</v>
       </c>
@@ -11260,8 +12190,11 @@
       <c r="K303" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="304" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L303" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="304" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A304" s="3">
         <v>303</v>
       </c>
@@ -11295,8 +12228,11 @@
       <c r="K304" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="305" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L304" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="305" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A305" s="3">
         <v>304</v>
       </c>
@@ -11330,8 +12266,11 @@
       <c r="K305" s="3">
         <v>10</v>
       </c>
-    </row>
-    <row r="306" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L305" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="306" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A306" s="3">
         <v>305</v>
       </c>
@@ -11365,8 +12304,11 @@
       <c r="K306" s="3">
         <v>10</v>
       </c>
-    </row>
-    <row r="307" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L306" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="307" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A307" s="3">
         <v>306</v>
       </c>
@@ -11400,8 +12342,11 @@
       <c r="K307" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="308" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L307" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="308" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A308" s="3">
         <v>307</v>
       </c>
@@ -11435,8 +12380,11 @@
       <c r="K308" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="309" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L308" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="309" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A309" s="3">
         <v>308</v>
       </c>
@@ -11470,8 +12418,11 @@
       <c r="K309" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="310" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L309" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="310" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A310" s="3">
         <v>309</v>
       </c>
@@ -11505,8 +12456,11 @@
       <c r="K310" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="311" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L310" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="311" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A311" s="3">
         <v>310</v>
       </c>
@@ -11540,8 +12494,11 @@
       <c r="K311" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="312" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L311" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="312" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A312" s="3">
         <v>311</v>
       </c>
@@ -11575,8 +12532,11 @@
       <c r="K312" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="313" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L312" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="313" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A313" s="3">
         <v>312</v>
       </c>
@@ -11609,6 +12569,9 @@
       </c>
       <c r="K313" s="3">
         <v>12</v>
+      </c>
+      <c r="L313" t="s">
+        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding updated gym workout data
</commit_message>
<xml_diff>
--- a/datasets/GymWorkouts.xlsx
+++ b/datasets/GymWorkouts.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1260" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1292" uniqueCount="94">
   <si>
     <t>Exercise Date</t>
   </si>
@@ -303,6 +303,9 @@
   </si>
   <si>
     <t>Full</t>
+  </si>
+  <si>
+    <t>January</t>
   </si>
 </sst>
 </file>
@@ -657,11 +660,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L313"/>
+  <dimension ref="A1:L321"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A285" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C289" sqref="C289"/>
+      <pane ySplit="1" topLeftCell="A292" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C322" sqref="C322"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -12574,6 +12577,310 @@
         <v>88</v>
       </c>
     </row>
+    <row r="314" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A314" s="3">
+        <v>313</v>
+      </c>
+      <c r="B314" s="3">
+        <v>37</v>
+      </c>
+      <c r="C314" s="2">
+        <v>43106</v>
+      </c>
+      <c r="D314">
+        <v>1</v>
+      </c>
+      <c r="E314" t="s">
+        <v>93</v>
+      </c>
+      <c r="F314">
+        <v>2018</v>
+      </c>
+      <c r="G314" t="s">
+        <v>80</v>
+      </c>
+      <c r="H314" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I314" s="1">
+        <v>95</v>
+      </c>
+      <c r="J314" s="3">
+        <v>5</v>
+      </c>
+      <c r="K314" s="3">
+        <v>5</v>
+      </c>
+      <c r="L314" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="315" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A315" s="3">
+        <v>314</v>
+      </c>
+      <c r="B315" s="3">
+        <v>37</v>
+      </c>
+      <c r="C315" s="2">
+        <v>43106</v>
+      </c>
+      <c r="D315">
+        <v>1</v>
+      </c>
+      <c r="E315" t="s">
+        <v>93</v>
+      </c>
+      <c r="F315">
+        <v>2018</v>
+      </c>
+      <c r="G315" t="s">
+        <v>80</v>
+      </c>
+      <c r="H315" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I315" s="1">
+        <v>85</v>
+      </c>
+      <c r="J315" s="3">
+        <v>5</v>
+      </c>
+      <c r="K315" s="3">
+        <v>5</v>
+      </c>
+      <c r="L315" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="316" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A316" s="3">
+        <v>315</v>
+      </c>
+      <c r="B316" s="3">
+        <v>37</v>
+      </c>
+      <c r="C316" s="2">
+        <v>43106</v>
+      </c>
+      <c r="D316">
+        <v>1</v>
+      </c>
+      <c r="E316" t="s">
+        <v>93</v>
+      </c>
+      <c r="F316">
+        <v>2018</v>
+      </c>
+      <c r="G316" t="s">
+        <v>80</v>
+      </c>
+      <c r="H316" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I316" s="1">
+        <v>26</v>
+      </c>
+      <c r="J316" s="3">
+        <v>4</v>
+      </c>
+      <c r="K316" s="3">
+        <v>8</v>
+      </c>
+      <c r="L316" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="317" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A317" s="3">
+        <v>316</v>
+      </c>
+      <c r="B317" s="3">
+        <v>37</v>
+      </c>
+      <c r="C317" s="2">
+        <v>43106</v>
+      </c>
+      <c r="D317">
+        <v>1</v>
+      </c>
+      <c r="E317" t="s">
+        <v>93</v>
+      </c>
+      <c r="F317">
+        <v>2018</v>
+      </c>
+      <c r="G317" t="s">
+        <v>80</v>
+      </c>
+      <c r="H317" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I317" s="1">
+        <v>26</v>
+      </c>
+      <c r="J317" s="3">
+        <v>4</v>
+      </c>
+      <c r="K317" s="3">
+        <v>8</v>
+      </c>
+      <c r="L317" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="318" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A318" s="3">
+        <v>317</v>
+      </c>
+      <c r="B318" s="3">
+        <v>37</v>
+      </c>
+      <c r="C318" s="2">
+        <v>43106</v>
+      </c>
+      <c r="D318">
+        <v>1</v>
+      </c>
+      <c r="E318" t="s">
+        <v>93</v>
+      </c>
+      <c r="F318">
+        <v>2018</v>
+      </c>
+      <c r="G318" t="s">
+        <v>80</v>
+      </c>
+      <c r="H318" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I318" s="1">
+        <v>86</v>
+      </c>
+      <c r="J318" s="3">
+        <v>4</v>
+      </c>
+      <c r="K318" s="3">
+        <v>8</v>
+      </c>
+      <c r="L318" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="319" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A319" s="3">
+        <v>318</v>
+      </c>
+      <c r="B319" s="3">
+        <v>37</v>
+      </c>
+      <c r="C319" s="2">
+        <v>43106</v>
+      </c>
+      <c r="D319">
+        <v>1</v>
+      </c>
+      <c r="E319" t="s">
+        <v>93</v>
+      </c>
+      <c r="F319">
+        <v>2018</v>
+      </c>
+      <c r="G319" t="s">
+        <v>80</v>
+      </c>
+      <c r="H319" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="I319" s="1">
+        <v>0</v>
+      </c>
+      <c r="J319" s="3">
+        <v>5</v>
+      </c>
+      <c r="K319" s="3">
+        <v>12</v>
+      </c>
+      <c r="L319" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="320" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A320" s="3">
+        <v>319</v>
+      </c>
+      <c r="B320" s="3">
+        <v>37</v>
+      </c>
+      <c r="C320" s="2">
+        <v>43106</v>
+      </c>
+      <c r="D320">
+        <v>1</v>
+      </c>
+      <c r="E320" t="s">
+        <v>93</v>
+      </c>
+      <c r="F320">
+        <v>2018</v>
+      </c>
+      <c r="G320" t="s">
+        <v>80</v>
+      </c>
+      <c r="H320" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="I320" s="1">
+        <v>10</v>
+      </c>
+      <c r="J320" s="3">
+        <v>4</v>
+      </c>
+      <c r="K320" s="3">
+        <v>12</v>
+      </c>
+      <c r="L320" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="321" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A321" s="3">
+        <v>320</v>
+      </c>
+      <c r="B321" s="3">
+        <v>37</v>
+      </c>
+      <c r="C321" s="2">
+        <v>43106</v>
+      </c>
+      <c r="D321">
+        <v>1</v>
+      </c>
+      <c r="E321" t="s">
+        <v>93</v>
+      </c>
+      <c r="F321">
+        <v>2018</v>
+      </c>
+      <c r="G321" t="s">
+        <v>80</v>
+      </c>
+      <c r="H321" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I321" s="1">
+        <v>105</v>
+      </c>
+      <c r="J321" s="3">
+        <v>5</v>
+      </c>
+      <c r="K321" s="3">
+        <v>5</v>
+      </c>
+      <c r="L321" t="s">
+        <v>87</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updating Gym workouts files
</commit_message>
<xml_diff>
--- a/datasets/GymWorkouts.xlsx
+++ b/datasets/GymWorkouts.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1292" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1376" uniqueCount="94">
   <si>
     <t>Exercise Date</t>
   </si>
@@ -660,11 +660,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L321"/>
+  <dimension ref="A1:L342"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A292" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C322" sqref="C322"/>
+      <pane ySplit="1" topLeftCell="A316" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C345" sqref="C345"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -12881,6 +12881,804 @@
         <v>87</v>
       </c>
     </row>
+    <row r="322" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A322" s="3">
+        <v>321</v>
+      </c>
+      <c r="B322" s="3">
+        <v>38</v>
+      </c>
+      <c r="C322" s="2">
+        <v>43107</v>
+      </c>
+      <c r="D322">
+        <v>1</v>
+      </c>
+      <c r="E322" t="s">
+        <v>93</v>
+      </c>
+      <c r="F322">
+        <v>2018</v>
+      </c>
+      <c r="G322" t="s">
+        <v>45</v>
+      </c>
+      <c r="H322" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I322" s="1">
+        <v>100</v>
+      </c>
+      <c r="J322" s="3">
+        <v>4</v>
+      </c>
+      <c r="K322" s="3">
+        <v>12</v>
+      </c>
+      <c r="L322" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="323" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A323" s="3">
+        <v>322</v>
+      </c>
+      <c r="B323" s="3">
+        <v>38</v>
+      </c>
+      <c r="C323" s="2">
+        <v>43107</v>
+      </c>
+      <c r="D323">
+        <v>1</v>
+      </c>
+      <c r="E323" t="s">
+        <v>93</v>
+      </c>
+      <c r="F323">
+        <v>2018</v>
+      </c>
+      <c r="G323" t="s">
+        <v>45</v>
+      </c>
+      <c r="H323" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I323" s="1">
+        <v>40</v>
+      </c>
+      <c r="J323" s="3">
+        <v>4</v>
+      </c>
+      <c r="K323" s="3">
+        <v>8</v>
+      </c>
+      <c r="L323" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="324" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A324" s="3">
+        <v>323</v>
+      </c>
+      <c r="B324" s="3">
+        <v>38</v>
+      </c>
+      <c r="C324" s="2">
+        <v>43107</v>
+      </c>
+      <c r="D324">
+        <v>1</v>
+      </c>
+      <c r="E324" t="s">
+        <v>93</v>
+      </c>
+      <c r="F324">
+        <v>2018</v>
+      </c>
+      <c r="G324" t="s">
+        <v>45</v>
+      </c>
+      <c r="H324" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I324" s="1">
+        <v>60</v>
+      </c>
+      <c r="J324" s="3">
+        <v>4</v>
+      </c>
+      <c r="K324" s="3">
+        <v>12</v>
+      </c>
+      <c r="L324" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="325" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A325" s="3">
+        <v>324</v>
+      </c>
+      <c r="B325" s="3">
+        <v>38</v>
+      </c>
+      <c r="C325" s="2">
+        <v>43107</v>
+      </c>
+      <c r="D325">
+        <v>1</v>
+      </c>
+      <c r="E325" t="s">
+        <v>93</v>
+      </c>
+      <c r="F325">
+        <v>2018</v>
+      </c>
+      <c r="G325" t="s">
+        <v>45</v>
+      </c>
+      <c r="H325" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I325" s="1">
+        <v>20</v>
+      </c>
+      <c r="J325" s="3">
+        <v>4</v>
+      </c>
+      <c r="K325" s="3">
+        <v>8</v>
+      </c>
+      <c r="L325" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="326" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A326" s="3">
+        <v>325</v>
+      </c>
+      <c r="B326" s="3">
+        <v>38</v>
+      </c>
+      <c r="C326" s="2">
+        <v>43107</v>
+      </c>
+      <c r="D326">
+        <v>1</v>
+      </c>
+      <c r="E326" t="s">
+        <v>93</v>
+      </c>
+      <c r="F326">
+        <v>2018</v>
+      </c>
+      <c r="G326" t="s">
+        <v>45</v>
+      </c>
+      <c r="H326" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I326" s="1">
+        <v>45</v>
+      </c>
+      <c r="J326" s="3">
+        <v>4</v>
+      </c>
+      <c r="K326" s="3">
+        <v>12</v>
+      </c>
+      <c r="L326" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="327" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A327" s="3">
+        <v>326</v>
+      </c>
+      <c r="B327" s="3">
+        <v>38</v>
+      </c>
+      <c r="C327" s="2">
+        <v>43107</v>
+      </c>
+      <c r="D327">
+        <v>1</v>
+      </c>
+      <c r="E327" t="s">
+        <v>93</v>
+      </c>
+      <c r="F327">
+        <v>2018</v>
+      </c>
+      <c r="G327" t="s">
+        <v>45</v>
+      </c>
+      <c r="H327" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="I327" s="1">
+        <v>30</v>
+      </c>
+      <c r="J327" s="3">
+        <v>4</v>
+      </c>
+      <c r="K327" s="3">
+        <v>8</v>
+      </c>
+      <c r="L327" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="328" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A328" s="3">
+        <v>327</v>
+      </c>
+      <c r="B328" s="3">
+        <v>38</v>
+      </c>
+      <c r="C328" s="2">
+        <v>43107</v>
+      </c>
+      <c r="D328">
+        <v>1</v>
+      </c>
+      <c r="E328" t="s">
+        <v>93</v>
+      </c>
+      <c r="F328">
+        <v>2018</v>
+      </c>
+      <c r="G328" t="s">
+        <v>45</v>
+      </c>
+      <c r="H328" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I328" s="1">
+        <v>52</v>
+      </c>
+      <c r="J328" s="3">
+        <v>4</v>
+      </c>
+      <c r="K328" s="3">
+        <v>12</v>
+      </c>
+      <c r="L328" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="329" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A329" s="3">
+        <v>328</v>
+      </c>
+      <c r="B329" s="3">
+        <v>38</v>
+      </c>
+      <c r="C329" s="2">
+        <v>43107</v>
+      </c>
+      <c r="D329">
+        <v>1</v>
+      </c>
+      <c r="E329" t="s">
+        <v>93</v>
+      </c>
+      <c r="F329">
+        <v>2018</v>
+      </c>
+      <c r="G329" t="s">
+        <v>45</v>
+      </c>
+      <c r="H329" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="I329" s="1">
+        <v>0</v>
+      </c>
+      <c r="J329" s="3">
+        <v>4</v>
+      </c>
+      <c r="K329" s="3">
+        <v>12</v>
+      </c>
+      <c r="L329" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="330" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A330" s="3">
+        <v>329</v>
+      </c>
+      <c r="B330" s="3">
+        <v>38</v>
+      </c>
+      <c r="C330" s="2">
+        <v>43107</v>
+      </c>
+      <c r="D330">
+        <v>1</v>
+      </c>
+      <c r="E330" t="s">
+        <v>93</v>
+      </c>
+      <c r="F330">
+        <v>2018</v>
+      </c>
+      <c r="G330" t="s">
+        <v>45</v>
+      </c>
+      <c r="H330" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I330" s="1">
+        <v>0</v>
+      </c>
+      <c r="J330" s="3">
+        <v>4</v>
+      </c>
+      <c r="K330" s="3">
+        <v>12</v>
+      </c>
+      <c r="L330" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="331" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A331" s="3">
+        <v>330</v>
+      </c>
+      <c r="B331" s="3">
+        <v>38</v>
+      </c>
+      <c r="C331" s="2">
+        <v>43107</v>
+      </c>
+      <c r="D331">
+        <v>1</v>
+      </c>
+      <c r="E331" t="s">
+        <v>93</v>
+      </c>
+      <c r="F331">
+        <v>2018</v>
+      </c>
+      <c r="G331" t="s">
+        <v>45</v>
+      </c>
+      <c r="H331" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I331" s="1">
+        <v>0</v>
+      </c>
+      <c r="J331" s="3">
+        <v>4</v>
+      </c>
+      <c r="K331" s="3">
+        <v>12</v>
+      </c>
+      <c r="L331" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="332" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A332" s="3">
+        <v>331</v>
+      </c>
+      <c r="B332" s="3">
+        <v>38</v>
+      </c>
+      <c r="C332" s="2">
+        <v>43107</v>
+      </c>
+      <c r="D332">
+        <v>1</v>
+      </c>
+      <c r="E332" t="s">
+        <v>93</v>
+      </c>
+      <c r="F332">
+        <v>2018</v>
+      </c>
+      <c r="G332" t="s">
+        <v>45</v>
+      </c>
+      <c r="H332" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I332" s="1">
+        <v>0</v>
+      </c>
+      <c r="J332" s="3">
+        <v>4</v>
+      </c>
+      <c r="K332" s="3">
+        <v>10</v>
+      </c>
+      <c r="L332" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="333" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A333" s="3">
+        <v>332</v>
+      </c>
+      <c r="B333" s="3">
+        <v>38</v>
+      </c>
+      <c r="C333" s="2">
+        <v>43107</v>
+      </c>
+      <c r="D333">
+        <v>1</v>
+      </c>
+      <c r="E333" t="s">
+        <v>93</v>
+      </c>
+      <c r="F333">
+        <v>2018</v>
+      </c>
+      <c r="G333" t="s">
+        <v>45</v>
+      </c>
+      <c r="H333" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="I333" s="1">
+        <v>25</v>
+      </c>
+      <c r="J333" s="3">
+        <v>5</v>
+      </c>
+      <c r="K333" s="3">
+        <v>2</v>
+      </c>
+      <c r="L333" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="334" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A334" s="3">
+        <v>333</v>
+      </c>
+      <c r="B334" s="3">
+        <v>39</v>
+      </c>
+      <c r="C334" s="2">
+        <v>43108</v>
+      </c>
+      <c r="D334">
+        <v>2</v>
+      </c>
+      <c r="E334" t="s">
+        <v>93</v>
+      </c>
+      <c r="F334">
+        <v>2018</v>
+      </c>
+      <c r="G334" t="s">
+        <v>18</v>
+      </c>
+      <c r="H334" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I334" s="1">
+        <v>80</v>
+      </c>
+      <c r="J334" s="3">
+        <v>5</v>
+      </c>
+      <c r="K334" s="3">
+        <v>5</v>
+      </c>
+      <c r="L334" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="335" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A335" s="3">
+        <v>334</v>
+      </c>
+      <c r="B335" s="3">
+        <v>39</v>
+      </c>
+      <c r="C335" s="2">
+        <v>43108</v>
+      </c>
+      <c r="D335">
+        <v>2</v>
+      </c>
+      <c r="E335" t="s">
+        <v>93</v>
+      </c>
+      <c r="F335">
+        <v>2018</v>
+      </c>
+      <c r="G335" t="s">
+        <v>18</v>
+      </c>
+      <c r="H335" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="I335" s="1">
+        <v>66</v>
+      </c>
+      <c r="J335" s="3">
+        <v>4</v>
+      </c>
+      <c r="K335" s="3">
+        <v>8</v>
+      </c>
+      <c r="L335" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="336" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A336" s="3">
+        <v>335</v>
+      </c>
+      <c r="B336" s="3">
+        <v>39</v>
+      </c>
+      <c r="C336" s="2">
+        <v>43108</v>
+      </c>
+      <c r="D336">
+        <v>2</v>
+      </c>
+      <c r="E336" t="s">
+        <v>93</v>
+      </c>
+      <c r="F336">
+        <v>2018</v>
+      </c>
+      <c r="G336" t="s">
+        <v>18</v>
+      </c>
+      <c r="H336" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I336" s="1">
+        <v>40</v>
+      </c>
+      <c r="J336" s="3">
+        <v>5</v>
+      </c>
+      <c r="K336" s="3">
+        <v>5</v>
+      </c>
+      <c r="L336" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="337" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A337" s="3">
+        <v>336</v>
+      </c>
+      <c r="B337" s="3">
+        <v>39</v>
+      </c>
+      <c r="C337" s="2">
+        <v>43108</v>
+      </c>
+      <c r="D337">
+        <v>2</v>
+      </c>
+      <c r="E337" t="s">
+        <v>93</v>
+      </c>
+      <c r="F337">
+        <v>2018</v>
+      </c>
+      <c r="G337" t="s">
+        <v>18</v>
+      </c>
+      <c r="H337" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="I337" s="1">
+        <v>0</v>
+      </c>
+      <c r="J337" s="3">
+        <v>5</v>
+      </c>
+      <c r="K337" s="3">
+        <v>12</v>
+      </c>
+      <c r="L337" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="338" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A338" s="3">
+        <v>337</v>
+      </c>
+      <c r="B338" s="3">
+        <v>39</v>
+      </c>
+      <c r="C338" s="2">
+        <v>43108</v>
+      </c>
+      <c r="D338">
+        <v>2</v>
+      </c>
+      <c r="E338" t="s">
+        <v>93</v>
+      </c>
+      <c r="F338">
+        <v>2018</v>
+      </c>
+      <c r="G338" t="s">
+        <v>18</v>
+      </c>
+      <c r="H338" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I338" s="1">
+        <v>0</v>
+      </c>
+      <c r="J338" s="3">
+        <v>4</v>
+      </c>
+      <c r="K338" s="3">
+        <v>12</v>
+      </c>
+      <c r="L338" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="339" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A339" s="3">
+        <v>338</v>
+      </c>
+      <c r="B339" s="3">
+        <v>39</v>
+      </c>
+      <c r="C339" s="2">
+        <v>43108</v>
+      </c>
+      <c r="D339">
+        <v>2</v>
+      </c>
+      <c r="E339" t="s">
+        <v>93</v>
+      </c>
+      <c r="F339">
+        <v>2018</v>
+      </c>
+      <c r="G339" t="s">
+        <v>18</v>
+      </c>
+      <c r="H339" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I339" s="1">
+        <v>0</v>
+      </c>
+      <c r="J339" s="3">
+        <v>4</v>
+      </c>
+      <c r="K339" s="3">
+        <v>10</v>
+      </c>
+      <c r="L339" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="340" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A340" s="3">
+        <v>339</v>
+      </c>
+      <c r="B340" s="3">
+        <v>39</v>
+      </c>
+      <c r="C340" s="2">
+        <v>43108</v>
+      </c>
+      <c r="D340">
+        <v>2</v>
+      </c>
+      <c r="E340" t="s">
+        <v>93</v>
+      </c>
+      <c r="F340">
+        <v>2018</v>
+      </c>
+      <c r="G340" t="s">
+        <v>18</v>
+      </c>
+      <c r="H340" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I340" s="1">
+        <v>0</v>
+      </c>
+      <c r="J340" s="3">
+        <v>4</v>
+      </c>
+      <c r="K340" s="3">
+        <v>10</v>
+      </c>
+      <c r="L340" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="341" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A341" s="3">
+        <v>340</v>
+      </c>
+      <c r="B341" s="3">
+        <v>39</v>
+      </c>
+      <c r="C341" s="2">
+        <v>43108</v>
+      </c>
+      <c r="D341">
+        <v>2</v>
+      </c>
+      <c r="E341" t="s">
+        <v>93</v>
+      </c>
+      <c r="F341">
+        <v>2018</v>
+      </c>
+      <c r="G341" t="s">
+        <v>18</v>
+      </c>
+      <c r="H341" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I341" s="1">
+        <v>0</v>
+      </c>
+      <c r="J341" s="3">
+        <v>4</v>
+      </c>
+      <c r="K341" s="3">
+        <v>10</v>
+      </c>
+      <c r="L341" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="342" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A342" s="3">
+        <v>341</v>
+      </c>
+      <c r="B342" s="3">
+        <v>39</v>
+      </c>
+      <c r="C342" s="2">
+        <v>43108</v>
+      </c>
+      <c r="D342">
+        <v>2</v>
+      </c>
+      <c r="E342" t="s">
+        <v>93</v>
+      </c>
+      <c r="F342">
+        <v>2018</v>
+      </c>
+      <c r="G342" t="s">
+        <v>18</v>
+      </c>
+      <c r="H342" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="I342" s="1">
+        <v>0</v>
+      </c>
+      <c r="J342" s="3">
+        <v>3</v>
+      </c>
+      <c r="K342" s="3">
+        <v>1</v>
+      </c>
+      <c r="L342" t="s">
+        <v>89</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updating Gym workouts for 10/01/2018
</commit_message>
<xml_diff>
--- a/datasets/GymWorkouts.xlsx
+++ b/datasets/GymWorkouts.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1376" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1420" uniqueCount="95">
   <si>
     <t>Exercise Date</t>
   </si>
@@ -306,6 +306,9 @@
   </si>
   <si>
     <t>January</t>
+  </si>
+  <si>
+    <t>Wall Squats</t>
   </si>
 </sst>
 </file>
@@ -660,11 +663,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L342"/>
+  <dimension ref="A1:L353"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A316" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C345" sqref="C345"/>
+      <pane ySplit="1" topLeftCell="A331" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M353" sqref="M353"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -13679,6 +13682,424 @@
         <v>89</v>
       </c>
     </row>
+    <row r="343" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A343" s="3">
+        <v>342</v>
+      </c>
+      <c r="B343" s="3">
+        <v>40</v>
+      </c>
+      <c r="C343" s="2">
+        <v>43110</v>
+      </c>
+      <c r="D343">
+        <v>2</v>
+      </c>
+      <c r="E343" t="s">
+        <v>93</v>
+      </c>
+      <c r="F343">
+        <v>2018</v>
+      </c>
+      <c r="G343" t="s">
+        <v>19</v>
+      </c>
+      <c r="H343" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="I343" s="1">
+        <v>32</v>
+      </c>
+      <c r="J343" s="3">
+        <v>4</v>
+      </c>
+      <c r="K343" s="3">
+        <v>12</v>
+      </c>
+      <c r="L343" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="344" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A344" s="3">
+        <v>343</v>
+      </c>
+      <c r="B344" s="3">
+        <v>40</v>
+      </c>
+      <c r="C344" s="2">
+        <v>43110</v>
+      </c>
+      <c r="D344">
+        <v>2</v>
+      </c>
+      <c r="E344" t="s">
+        <v>93</v>
+      </c>
+      <c r="F344">
+        <v>2018</v>
+      </c>
+      <c r="G344" t="s">
+        <v>19</v>
+      </c>
+      <c r="H344" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I344" s="1">
+        <v>102</v>
+      </c>
+      <c r="J344" s="3">
+        <v>4</v>
+      </c>
+      <c r="K344" s="3">
+        <v>8</v>
+      </c>
+      <c r="L344" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="345" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A345" s="3">
+        <v>344</v>
+      </c>
+      <c r="B345" s="3">
+        <v>40</v>
+      </c>
+      <c r="C345" s="2">
+        <v>43110</v>
+      </c>
+      <c r="D345">
+        <v>2</v>
+      </c>
+      <c r="E345" t="s">
+        <v>93</v>
+      </c>
+      <c r="F345">
+        <v>2018</v>
+      </c>
+      <c r="G345" t="s">
+        <v>19</v>
+      </c>
+      <c r="H345" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="I345" s="1">
+        <v>102</v>
+      </c>
+      <c r="J345" s="3">
+        <v>4</v>
+      </c>
+      <c r="K345" s="3">
+        <v>5</v>
+      </c>
+      <c r="L345" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="346" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A346" s="3">
+        <v>345</v>
+      </c>
+      <c r="B346" s="3">
+        <v>40</v>
+      </c>
+      <c r="C346" s="2">
+        <v>43110</v>
+      </c>
+      <c r="D346">
+        <v>2</v>
+      </c>
+      <c r="E346" t="s">
+        <v>93</v>
+      </c>
+      <c r="F346">
+        <v>2018</v>
+      </c>
+      <c r="G346" t="s">
+        <v>19</v>
+      </c>
+      <c r="H346" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I346" s="1">
+        <v>102</v>
+      </c>
+      <c r="J346" s="3">
+        <v>3</v>
+      </c>
+      <c r="K346" s="3">
+        <v>10</v>
+      </c>
+      <c r="L346" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="347" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A347" s="3">
+        <v>346</v>
+      </c>
+      <c r="B347" s="3">
+        <v>40</v>
+      </c>
+      <c r="C347" s="2">
+        <v>43110</v>
+      </c>
+      <c r="D347">
+        <v>2</v>
+      </c>
+      <c r="E347" t="s">
+        <v>93</v>
+      </c>
+      <c r="F347">
+        <v>2018</v>
+      </c>
+      <c r="G347" t="s">
+        <v>19</v>
+      </c>
+      <c r="H347" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="I347" s="1">
+        <v>0</v>
+      </c>
+      <c r="J347" s="3">
+        <v>5</v>
+      </c>
+      <c r="K347" s="3">
+        <v>10</v>
+      </c>
+      <c r="L347" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="348" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A348" s="3">
+        <v>347</v>
+      </c>
+      <c r="B348" s="3">
+        <v>40</v>
+      </c>
+      <c r="C348" s="2">
+        <v>43110</v>
+      </c>
+      <c r="D348">
+        <v>2</v>
+      </c>
+      <c r="E348" t="s">
+        <v>93</v>
+      </c>
+      <c r="F348">
+        <v>2018</v>
+      </c>
+      <c r="G348" t="s">
+        <v>19</v>
+      </c>
+      <c r="H348" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="I348" s="1">
+        <v>8</v>
+      </c>
+      <c r="J348" s="3">
+        <v>4</v>
+      </c>
+      <c r="K348" s="3">
+        <v>10</v>
+      </c>
+      <c r="L348" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="349" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A349" s="3">
+        <v>348</v>
+      </c>
+      <c r="B349" s="3">
+        <v>40</v>
+      </c>
+      <c r="C349" s="2">
+        <v>43110</v>
+      </c>
+      <c r="D349">
+        <v>2</v>
+      </c>
+      <c r="E349" t="s">
+        <v>93</v>
+      </c>
+      <c r="F349">
+        <v>2018</v>
+      </c>
+      <c r="G349" t="s">
+        <v>19</v>
+      </c>
+      <c r="H349" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="I349" s="1">
+        <v>0</v>
+      </c>
+      <c r="J349" s="3">
+        <v>4</v>
+      </c>
+      <c r="K349" s="3">
+        <v>30</v>
+      </c>
+      <c r="L349" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="350" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A350" s="3">
+        <v>349</v>
+      </c>
+      <c r="B350" s="3">
+        <v>40</v>
+      </c>
+      <c r="C350" s="2">
+        <v>43110</v>
+      </c>
+      <c r="D350">
+        <v>2</v>
+      </c>
+      <c r="E350" t="s">
+        <v>93</v>
+      </c>
+      <c r="F350">
+        <v>2018</v>
+      </c>
+      <c r="G350" t="s">
+        <v>19</v>
+      </c>
+      <c r="H350" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="I350" s="1">
+        <v>0</v>
+      </c>
+      <c r="J350" s="3">
+        <v>4</v>
+      </c>
+      <c r="K350" s="3">
+        <v>30</v>
+      </c>
+      <c r="L350" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="351" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A351" s="3">
+        <v>350</v>
+      </c>
+      <c r="B351" s="3">
+        <v>40</v>
+      </c>
+      <c r="C351" s="2">
+        <v>43110</v>
+      </c>
+      <c r="D351">
+        <v>2</v>
+      </c>
+      <c r="E351" t="s">
+        <v>93</v>
+      </c>
+      <c r="F351">
+        <v>2018</v>
+      </c>
+      <c r="G351" t="s">
+        <v>19</v>
+      </c>
+      <c r="H351" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I351" s="1">
+        <v>0</v>
+      </c>
+      <c r="J351" s="3">
+        <v>4</v>
+      </c>
+      <c r="K351" s="3">
+        <v>30</v>
+      </c>
+      <c r="L351" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="352" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A352" s="3">
+        <v>351</v>
+      </c>
+      <c r="B352" s="3">
+        <v>40</v>
+      </c>
+      <c r="C352" s="2">
+        <v>43110</v>
+      </c>
+      <c r="D352">
+        <v>2</v>
+      </c>
+      <c r="E352" t="s">
+        <v>93</v>
+      </c>
+      <c r="F352">
+        <v>2018</v>
+      </c>
+      <c r="G352" t="s">
+        <v>19</v>
+      </c>
+      <c r="H352" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="I352" s="1">
+        <v>0</v>
+      </c>
+      <c r="J352" s="3">
+        <v>4</v>
+      </c>
+      <c r="K352" s="3">
+        <v>30</v>
+      </c>
+      <c r="L352" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="353" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A353" s="3">
+        <v>352</v>
+      </c>
+      <c r="B353" s="3">
+        <v>40</v>
+      </c>
+      <c r="C353" s="2">
+        <v>43110</v>
+      </c>
+      <c r="D353">
+        <v>2</v>
+      </c>
+      <c r="E353" t="s">
+        <v>93</v>
+      </c>
+      <c r="F353">
+        <v>2018</v>
+      </c>
+      <c r="G353" t="s">
+        <v>19</v>
+      </c>
+      <c r="H353" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="I353" s="1">
+        <v>20</v>
+      </c>
+      <c r="J353" s="3">
+        <v>5</v>
+      </c>
+      <c r="K353" s="3">
+        <v>4</v>
+      </c>
+      <c r="L353" t="s">
+        <v>89</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Adding Gym Workout data
</commit_message>
<xml_diff>
--- a/datasets/GymWorkouts.xlsx
+++ b/datasets/GymWorkouts.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1420" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1652" uniqueCount="113">
   <si>
     <t>Exercise Date</t>
   </si>
@@ -309,6 +309,60 @@
   </si>
   <si>
     <t>Wall Squats</t>
+  </si>
+  <si>
+    <t>Dumbell Bench</t>
+  </si>
+  <si>
+    <t>Seated Bicep Curl</t>
+  </si>
+  <si>
+    <t>DB Bicep Curl</t>
+  </si>
+  <si>
+    <t>Reverse Crunch</t>
+  </si>
+  <si>
+    <t>Arnold Press</t>
+  </si>
+  <si>
+    <t>Walking Lunge</t>
+  </si>
+  <si>
+    <t>70% IRM Deadlift</t>
+  </si>
+  <si>
+    <t>80% IRM Deadlift</t>
+  </si>
+  <si>
+    <t>90% IRM Deadlift</t>
+  </si>
+  <si>
+    <t>Dumbell Rows</t>
+  </si>
+  <si>
+    <t>Upright Rows</t>
+  </si>
+  <si>
+    <t>Front raises</t>
+  </si>
+  <si>
+    <t>Rear delt flys</t>
+  </si>
+  <si>
+    <t>Goblet Squat</t>
+  </si>
+  <si>
+    <t>Barbell Lunge</t>
+  </si>
+  <si>
+    <t>60% 1RM Barbell Squat</t>
+  </si>
+  <si>
+    <t>70% 1RM Barbell Squat</t>
+  </si>
+  <si>
+    <t>80% 1RM Barbell Squat</t>
   </si>
 </sst>
 </file>
@@ -663,11 +717,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L353"/>
+  <dimension ref="A1:L411"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A331" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M353" sqref="M353"/>
+      <pane ySplit="1" topLeftCell="A388" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C415" sqref="C415"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -14100,6 +14154,2210 @@
         <v>89</v>
       </c>
     </row>
+    <row r="354" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A354" s="3">
+        <v>353</v>
+      </c>
+      <c r="B354" s="3">
+        <v>41</v>
+      </c>
+      <c r="C354" s="2">
+        <v>43111</v>
+      </c>
+      <c r="D354">
+        <v>2</v>
+      </c>
+      <c r="E354" t="s">
+        <v>93</v>
+      </c>
+      <c r="F354">
+        <v>2018</v>
+      </c>
+      <c r="G354" t="s">
+        <v>17</v>
+      </c>
+      <c r="H354" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I354" s="1">
+        <v>95</v>
+      </c>
+      <c r="J354" s="3">
+        <v>5</v>
+      </c>
+      <c r="K354" s="3">
+        <v>5</v>
+      </c>
+      <c r="L354" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="355" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A355" s="3">
+        <v>354</v>
+      </c>
+      <c r="B355" s="3">
+        <v>41</v>
+      </c>
+      <c r="C355" s="2">
+        <v>43111</v>
+      </c>
+      <c r="D355">
+        <v>2</v>
+      </c>
+      <c r="E355" t="s">
+        <v>93</v>
+      </c>
+      <c r="F355">
+        <v>2018</v>
+      </c>
+      <c r="G355" t="s">
+        <v>17</v>
+      </c>
+      <c r="H355" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I355" s="1">
+        <v>90</v>
+      </c>
+      <c r="J355" s="3">
+        <v>5</v>
+      </c>
+      <c r="K355" s="3">
+        <v>5</v>
+      </c>
+      <c r="L355" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="356" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A356" s="3">
+        <v>355</v>
+      </c>
+      <c r="B356" s="3">
+        <v>41</v>
+      </c>
+      <c r="C356" s="2">
+        <v>43111</v>
+      </c>
+      <c r="D356">
+        <v>2</v>
+      </c>
+      <c r="E356" t="s">
+        <v>93</v>
+      </c>
+      <c r="F356">
+        <v>2018</v>
+      </c>
+      <c r="G356" t="s">
+        <v>17</v>
+      </c>
+      <c r="H356" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="I356" s="1">
+        <v>32</v>
+      </c>
+      <c r="J356" s="3">
+        <v>5</v>
+      </c>
+      <c r="K356" s="3">
+        <v>8</v>
+      </c>
+      <c r="L356" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="357" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A357" s="3">
+        <v>356</v>
+      </c>
+      <c r="B357" s="3">
+        <v>41</v>
+      </c>
+      <c r="C357" s="2">
+        <v>43111</v>
+      </c>
+      <c r="D357">
+        <v>2</v>
+      </c>
+      <c r="E357" t="s">
+        <v>93</v>
+      </c>
+      <c r="F357">
+        <v>2018</v>
+      </c>
+      <c r="G357" t="s">
+        <v>17</v>
+      </c>
+      <c r="H357" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I357" s="1">
+        <v>95</v>
+      </c>
+      <c r="J357" s="3">
+        <v>5</v>
+      </c>
+      <c r="K357" s="3">
+        <v>5</v>
+      </c>
+      <c r="L357" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="358" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A358" s="3">
+        <v>357</v>
+      </c>
+      <c r="B358" s="3">
+        <v>41</v>
+      </c>
+      <c r="C358" s="2">
+        <v>43111</v>
+      </c>
+      <c r="D358">
+        <v>2</v>
+      </c>
+      <c r="E358" t="s">
+        <v>93</v>
+      </c>
+      <c r="F358">
+        <v>2018</v>
+      </c>
+      <c r="G358" t="s">
+        <v>17</v>
+      </c>
+      <c r="H358" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I358" s="1">
+        <v>26</v>
+      </c>
+      <c r="J358" s="3">
+        <v>4</v>
+      </c>
+      <c r="K358" s="3">
+        <v>8</v>
+      </c>
+      <c r="L358" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="359" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A359" s="3">
+        <v>358</v>
+      </c>
+      <c r="B359" s="3">
+        <v>41</v>
+      </c>
+      <c r="C359" s="2">
+        <v>43111</v>
+      </c>
+      <c r="D359">
+        <v>2</v>
+      </c>
+      <c r="E359" t="s">
+        <v>93</v>
+      </c>
+      <c r="F359">
+        <v>2018</v>
+      </c>
+      <c r="G359" t="s">
+        <v>17</v>
+      </c>
+      <c r="H359" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I359" s="1">
+        <v>26</v>
+      </c>
+      <c r="J359" s="3">
+        <v>4</v>
+      </c>
+      <c r="K359" s="3">
+        <v>8</v>
+      </c>
+      <c r="L359" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="360" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A360" s="3">
+        <v>359</v>
+      </c>
+      <c r="B360" s="3">
+        <v>41</v>
+      </c>
+      <c r="C360" s="2">
+        <v>43111</v>
+      </c>
+      <c r="D360">
+        <v>2</v>
+      </c>
+      <c r="E360" t="s">
+        <v>93</v>
+      </c>
+      <c r="F360">
+        <v>2018</v>
+      </c>
+      <c r="G360" t="s">
+        <v>17</v>
+      </c>
+      <c r="H360" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I360" s="1">
+        <v>0</v>
+      </c>
+      <c r="J360" s="3">
+        <v>3</v>
+      </c>
+      <c r="K360" s="3">
+        <v>20</v>
+      </c>
+      <c r="L360" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="361" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A361" s="3">
+        <v>360</v>
+      </c>
+      <c r="B361" s="3">
+        <v>41</v>
+      </c>
+      <c r="C361" s="2">
+        <v>43111</v>
+      </c>
+      <c r="D361">
+        <v>2</v>
+      </c>
+      <c r="E361" t="s">
+        <v>93</v>
+      </c>
+      <c r="F361">
+        <v>2018</v>
+      </c>
+      <c r="G361" t="s">
+        <v>17</v>
+      </c>
+      <c r="H361" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="I361" s="1">
+        <v>0</v>
+      </c>
+      <c r="J361" s="3">
+        <v>3</v>
+      </c>
+      <c r="K361" s="3">
+        <v>20</v>
+      </c>
+      <c r="L361" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="362" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A362" s="3">
+        <v>361</v>
+      </c>
+      <c r="B362" s="3">
+        <v>42</v>
+      </c>
+      <c r="C362" s="2">
+        <v>43113</v>
+      </c>
+      <c r="D362">
+        <v>2</v>
+      </c>
+      <c r="E362" t="s">
+        <v>93</v>
+      </c>
+      <c r="F362">
+        <v>2018</v>
+      </c>
+      <c r="G362" t="s">
+        <v>80</v>
+      </c>
+      <c r="H362" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I362" s="1">
+        <v>120</v>
+      </c>
+      <c r="J362" s="3">
+        <v>5</v>
+      </c>
+      <c r="K362" s="3">
+        <v>5</v>
+      </c>
+      <c r="L362" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="363" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A363" s="3">
+        <v>362</v>
+      </c>
+      <c r="B363" s="3">
+        <v>42</v>
+      </c>
+      <c r="C363" s="2">
+        <v>43113</v>
+      </c>
+      <c r="D363">
+        <v>2</v>
+      </c>
+      <c r="E363" t="s">
+        <v>93</v>
+      </c>
+      <c r="F363">
+        <v>2018</v>
+      </c>
+      <c r="G363" t="s">
+        <v>80</v>
+      </c>
+      <c r="H363" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I363" s="1">
+        <v>110</v>
+      </c>
+      <c r="J363" s="3">
+        <v>4</v>
+      </c>
+      <c r="K363" s="3">
+        <v>12</v>
+      </c>
+      <c r="L363" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="364" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A364" s="3">
+        <v>363</v>
+      </c>
+      <c r="B364" s="3">
+        <v>42</v>
+      </c>
+      <c r="C364" s="2">
+        <v>43113</v>
+      </c>
+      <c r="D364">
+        <v>2</v>
+      </c>
+      <c r="E364" t="s">
+        <v>93</v>
+      </c>
+      <c r="F364">
+        <v>2018</v>
+      </c>
+      <c r="G364" t="s">
+        <v>80</v>
+      </c>
+      <c r="H364" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I364" s="1">
+        <v>60</v>
+      </c>
+      <c r="J364" s="3">
+        <v>4</v>
+      </c>
+      <c r="K364" s="3">
+        <v>12</v>
+      </c>
+      <c r="L364" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="365" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A365" s="3">
+        <v>364</v>
+      </c>
+      <c r="B365" s="3">
+        <v>42</v>
+      </c>
+      <c r="C365" s="2">
+        <v>43113</v>
+      </c>
+      <c r="D365">
+        <v>2</v>
+      </c>
+      <c r="E365" t="s">
+        <v>93</v>
+      </c>
+      <c r="F365">
+        <v>2018</v>
+      </c>
+      <c r="G365" t="s">
+        <v>80</v>
+      </c>
+      <c r="H365" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I365" s="1">
+        <v>59</v>
+      </c>
+      <c r="J365" s="3">
+        <v>4</v>
+      </c>
+      <c r="K365" s="3">
+        <v>12</v>
+      </c>
+      <c r="L365" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="366" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A366" s="3">
+        <v>365</v>
+      </c>
+      <c r="B366" s="3">
+        <v>42</v>
+      </c>
+      <c r="C366" s="2">
+        <v>43113</v>
+      </c>
+      <c r="D366">
+        <v>2</v>
+      </c>
+      <c r="E366" t="s">
+        <v>93</v>
+      </c>
+      <c r="F366">
+        <v>2018</v>
+      </c>
+      <c r="G366" t="s">
+        <v>80</v>
+      </c>
+      <c r="H366" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I366" s="1">
+        <v>45</v>
+      </c>
+      <c r="J366" s="3">
+        <v>4</v>
+      </c>
+      <c r="K366" s="3">
+        <v>12</v>
+      </c>
+      <c r="L366" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="367" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A367" s="3">
+        <v>366</v>
+      </c>
+      <c r="B367" s="3">
+        <v>42</v>
+      </c>
+      <c r="C367" s="2">
+        <v>43113</v>
+      </c>
+      <c r="D367">
+        <v>2</v>
+      </c>
+      <c r="E367" t="s">
+        <v>93</v>
+      </c>
+      <c r="F367">
+        <v>2018</v>
+      </c>
+      <c r="G367" t="s">
+        <v>80</v>
+      </c>
+      <c r="H367" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I367" s="1">
+        <v>0</v>
+      </c>
+      <c r="J367" s="3">
+        <v>3</v>
+      </c>
+      <c r="K367" s="3">
+        <v>20</v>
+      </c>
+      <c r="L367" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="368" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A368" s="3">
+        <v>367</v>
+      </c>
+      <c r="B368" s="3">
+        <v>42</v>
+      </c>
+      <c r="C368" s="2">
+        <v>43113</v>
+      </c>
+      <c r="D368">
+        <v>2</v>
+      </c>
+      <c r="E368" t="s">
+        <v>93</v>
+      </c>
+      <c r="F368">
+        <v>2018</v>
+      </c>
+      <c r="G368" t="s">
+        <v>80</v>
+      </c>
+      <c r="H368" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="I368" s="1">
+        <v>0</v>
+      </c>
+      <c r="J368" s="3">
+        <v>3</v>
+      </c>
+      <c r="K368" s="3">
+        <v>20</v>
+      </c>
+      <c r="L368" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="369" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A369" s="3">
+        <v>368</v>
+      </c>
+      <c r="B369" s="3">
+        <v>42</v>
+      </c>
+      <c r="C369" s="2">
+        <v>43113</v>
+      </c>
+      <c r="D369">
+        <v>2</v>
+      </c>
+      <c r="E369" t="s">
+        <v>93</v>
+      </c>
+      <c r="F369">
+        <v>2018</v>
+      </c>
+      <c r="G369" t="s">
+        <v>80</v>
+      </c>
+      <c r="H369" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I369" s="1">
+        <v>0</v>
+      </c>
+      <c r="J369" s="3">
+        <v>4</v>
+      </c>
+      <c r="K369" s="3">
+        <v>10</v>
+      </c>
+      <c r="L369" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="370" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A370" s="3">
+        <v>369</v>
+      </c>
+      <c r="B370" s="3">
+        <v>43</v>
+      </c>
+      <c r="C370" s="2">
+        <v>43114</v>
+      </c>
+      <c r="D370">
+        <v>2</v>
+      </c>
+      <c r="E370" t="s">
+        <v>93</v>
+      </c>
+      <c r="F370">
+        <v>2018</v>
+      </c>
+      <c r="G370" t="s">
+        <v>45</v>
+      </c>
+      <c r="H370" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="I370" s="1">
+        <v>30</v>
+      </c>
+      <c r="J370" s="3">
+        <v>4</v>
+      </c>
+      <c r="K370" s="3">
+        <v>8</v>
+      </c>
+      <c r="L370" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="371" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A371" s="3">
+        <v>370</v>
+      </c>
+      <c r="B371" s="3">
+        <v>43</v>
+      </c>
+      <c r="C371" s="2">
+        <v>43114</v>
+      </c>
+      <c r="D371">
+        <v>2</v>
+      </c>
+      <c r="E371" t="s">
+        <v>93</v>
+      </c>
+      <c r="F371">
+        <v>2018</v>
+      </c>
+      <c r="G371" t="s">
+        <v>45</v>
+      </c>
+      <c r="H371" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I371" s="1">
+        <v>42</v>
+      </c>
+      <c r="J371" s="3">
+        <v>4</v>
+      </c>
+      <c r="K371" s="3">
+        <v>8</v>
+      </c>
+      <c r="L371" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="372" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A372" s="3">
+        <v>371</v>
+      </c>
+      <c r="B372" s="3">
+        <v>43</v>
+      </c>
+      <c r="C372" s="2">
+        <v>43114</v>
+      </c>
+      <c r="D372">
+        <v>2</v>
+      </c>
+      <c r="E372" t="s">
+        <v>93</v>
+      </c>
+      <c r="F372">
+        <v>2018</v>
+      </c>
+      <c r="G372" t="s">
+        <v>45</v>
+      </c>
+      <c r="H372" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="I372" s="1">
+        <v>30</v>
+      </c>
+      <c r="J372" s="3">
+        <v>4</v>
+      </c>
+      <c r="K372" s="3">
+        <v>8</v>
+      </c>
+      <c r="L372" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="373" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A373" s="3">
+        <v>372</v>
+      </c>
+      <c r="B373" s="3">
+        <v>43</v>
+      </c>
+      <c r="C373" s="2">
+        <v>43114</v>
+      </c>
+      <c r="D373">
+        <v>2</v>
+      </c>
+      <c r="E373" t="s">
+        <v>93</v>
+      </c>
+      <c r="F373">
+        <v>2018</v>
+      </c>
+      <c r="G373" t="s">
+        <v>45</v>
+      </c>
+      <c r="H373" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I373" s="1">
+        <v>35</v>
+      </c>
+      <c r="J373" s="3">
+        <v>4</v>
+      </c>
+      <c r="K373" s="3">
+        <v>8</v>
+      </c>
+      <c r="L373" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="374" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A374" s="3">
+        <v>373</v>
+      </c>
+      <c r="B374" s="3">
+        <v>43</v>
+      </c>
+      <c r="C374" s="2">
+        <v>43114</v>
+      </c>
+      <c r="D374">
+        <v>2</v>
+      </c>
+      <c r="E374" t="s">
+        <v>93</v>
+      </c>
+      <c r="F374">
+        <v>2018</v>
+      </c>
+      <c r="G374" t="s">
+        <v>45</v>
+      </c>
+      <c r="H374" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="I374" s="1">
+        <v>20</v>
+      </c>
+      <c r="J374" s="3">
+        <v>4</v>
+      </c>
+      <c r="K374" s="3">
+        <v>8</v>
+      </c>
+      <c r="L374" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="375" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A375" s="3">
+        <v>374</v>
+      </c>
+      <c r="B375" s="3">
+        <v>43</v>
+      </c>
+      <c r="C375" s="2">
+        <v>43114</v>
+      </c>
+      <c r="D375">
+        <v>2</v>
+      </c>
+      <c r="E375" t="s">
+        <v>93</v>
+      </c>
+      <c r="F375">
+        <v>2018</v>
+      </c>
+      <c r="G375" t="s">
+        <v>45</v>
+      </c>
+      <c r="H375" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I375" s="1">
+        <v>0</v>
+      </c>
+      <c r="J375" s="3">
+        <v>3</v>
+      </c>
+      <c r="K375" s="3">
+        <v>20</v>
+      </c>
+      <c r="L375" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="376" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A376" s="3">
+        <v>375</v>
+      </c>
+      <c r="B376" s="3">
+        <v>43</v>
+      </c>
+      <c r="C376" s="2">
+        <v>43114</v>
+      </c>
+      <c r="D376">
+        <v>2</v>
+      </c>
+      <c r="E376" t="s">
+        <v>93</v>
+      </c>
+      <c r="F376">
+        <v>2018</v>
+      </c>
+      <c r="G376" t="s">
+        <v>45</v>
+      </c>
+      <c r="H376" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I376" s="1">
+        <v>0</v>
+      </c>
+      <c r="J376" s="3">
+        <v>3</v>
+      </c>
+      <c r="K376" s="3">
+        <v>20</v>
+      </c>
+      <c r="L376" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="377" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A377" s="3">
+        <v>376</v>
+      </c>
+      <c r="B377" s="3">
+        <v>43</v>
+      </c>
+      <c r="C377" s="2">
+        <v>43114</v>
+      </c>
+      <c r="D377">
+        <v>2</v>
+      </c>
+      <c r="E377" t="s">
+        <v>93</v>
+      </c>
+      <c r="F377">
+        <v>2018</v>
+      </c>
+      <c r="G377" t="s">
+        <v>45</v>
+      </c>
+      <c r="H377" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="I377" s="1">
+        <v>0</v>
+      </c>
+      <c r="J377" s="3">
+        <v>3</v>
+      </c>
+      <c r="K377" s="3">
+        <v>20</v>
+      </c>
+      <c r="L377" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="378" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A378" s="3">
+        <v>377</v>
+      </c>
+      <c r="B378" s="3">
+        <v>44</v>
+      </c>
+      <c r="C378" s="2">
+        <v>43115</v>
+      </c>
+      <c r="D378">
+        <v>3</v>
+      </c>
+      <c r="E378" t="s">
+        <v>93</v>
+      </c>
+      <c r="F378">
+        <v>2018</v>
+      </c>
+      <c r="G378" t="s">
+        <v>18</v>
+      </c>
+      <c r="H378" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I378" s="1">
+        <v>80</v>
+      </c>
+      <c r="J378" s="3">
+        <v>4</v>
+      </c>
+      <c r="K378" s="3">
+        <v>10</v>
+      </c>
+      <c r="L378" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="379" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A379" s="3">
+        <v>378</v>
+      </c>
+      <c r="B379" s="3">
+        <v>44</v>
+      </c>
+      <c r="C379" s="2">
+        <v>43115</v>
+      </c>
+      <c r="D379">
+        <v>3</v>
+      </c>
+      <c r="E379" t="s">
+        <v>93</v>
+      </c>
+      <c r="F379">
+        <v>2018</v>
+      </c>
+      <c r="G379" t="s">
+        <v>18</v>
+      </c>
+      <c r="H379" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I379" s="1">
+        <v>40</v>
+      </c>
+      <c r="J379" s="3">
+        <v>4</v>
+      </c>
+      <c r="K379" s="3">
+        <v>8</v>
+      </c>
+      <c r="L379" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="380" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A380" s="3">
+        <v>379</v>
+      </c>
+      <c r="B380" s="3">
+        <v>44</v>
+      </c>
+      <c r="C380" s="2">
+        <v>43115</v>
+      </c>
+      <c r="D380">
+        <v>3</v>
+      </c>
+      <c r="E380" t="s">
+        <v>93</v>
+      </c>
+      <c r="F380">
+        <v>2018</v>
+      </c>
+      <c r="G380" t="s">
+        <v>18</v>
+      </c>
+      <c r="H380" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="I380" s="1">
+        <v>14</v>
+      </c>
+      <c r="J380" s="3">
+        <v>4</v>
+      </c>
+      <c r="K380" s="3">
+        <v>8</v>
+      </c>
+      <c r="L380" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="381" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A381" s="3">
+        <v>380</v>
+      </c>
+      <c r="B381" s="3">
+        <v>44</v>
+      </c>
+      <c r="C381" s="2">
+        <v>43115</v>
+      </c>
+      <c r="D381">
+        <v>3</v>
+      </c>
+      <c r="E381" t="s">
+        <v>93</v>
+      </c>
+      <c r="F381">
+        <v>2018</v>
+      </c>
+      <c r="G381" t="s">
+        <v>18</v>
+      </c>
+      <c r="H381" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I381" s="1">
+        <v>20</v>
+      </c>
+      <c r="J381" s="3">
+        <v>4</v>
+      </c>
+      <c r="K381" s="3">
+        <v>8</v>
+      </c>
+      <c r="L381" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="382" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A382" s="3">
+        <v>381</v>
+      </c>
+      <c r="B382" s="3">
+        <v>45</v>
+      </c>
+      <c r="C382" s="2">
+        <v>43117</v>
+      </c>
+      <c r="D382">
+        <v>3</v>
+      </c>
+      <c r="E382" t="s">
+        <v>93</v>
+      </c>
+      <c r="F382">
+        <v>2018</v>
+      </c>
+      <c r="G382" t="s">
+        <v>19</v>
+      </c>
+      <c r="H382" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="I382" s="1">
+        <v>14</v>
+      </c>
+      <c r="J382" s="3">
+        <v>2</v>
+      </c>
+      <c r="K382" s="3">
+        <v>10</v>
+      </c>
+      <c r="L382" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="383" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A383" s="3">
+        <v>382</v>
+      </c>
+      <c r="B383" s="3">
+        <v>45</v>
+      </c>
+      <c r="C383" s="2">
+        <v>43117</v>
+      </c>
+      <c r="D383">
+        <v>3</v>
+      </c>
+      <c r="E383" t="s">
+        <v>93</v>
+      </c>
+      <c r="F383">
+        <v>2018</v>
+      </c>
+      <c r="G383" t="s">
+        <v>19</v>
+      </c>
+      <c r="H383" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="I383" s="1">
+        <v>120</v>
+      </c>
+      <c r="J383" s="3">
+        <v>4</v>
+      </c>
+      <c r="K383" s="3">
+        <v>4</v>
+      </c>
+      <c r="L383" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="384" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A384" s="3">
+        <v>383</v>
+      </c>
+      <c r="B384" s="3">
+        <v>45</v>
+      </c>
+      <c r="C384" s="2">
+        <v>43117</v>
+      </c>
+      <c r="D384">
+        <v>3</v>
+      </c>
+      <c r="E384" t="s">
+        <v>93</v>
+      </c>
+      <c r="F384">
+        <v>2018</v>
+      </c>
+      <c r="G384" t="s">
+        <v>19</v>
+      </c>
+      <c r="H384" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="I384" s="1">
+        <v>130</v>
+      </c>
+      <c r="J384" s="3">
+        <v>3</v>
+      </c>
+      <c r="K384" s="3">
+        <v>3</v>
+      </c>
+      <c r="L384" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="385" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A385" s="3">
+        <v>384</v>
+      </c>
+      <c r="B385" s="3">
+        <v>45</v>
+      </c>
+      <c r="C385" s="2">
+        <v>43117</v>
+      </c>
+      <c r="D385">
+        <v>3</v>
+      </c>
+      <c r="E385" t="s">
+        <v>93</v>
+      </c>
+      <c r="F385">
+        <v>2018</v>
+      </c>
+      <c r="G385" t="s">
+        <v>19</v>
+      </c>
+      <c r="H385" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="I385" s="1">
+        <v>140</v>
+      </c>
+      <c r="J385" s="3">
+        <v>4</v>
+      </c>
+      <c r="K385" s="3">
+        <v>2</v>
+      </c>
+      <c r="L385" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="386" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A386" s="3">
+        <v>385</v>
+      </c>
+      <c r="B386" s="3">
+        <v>45</v>
+      </c>
+      <c r="C386" s="2">
+        <v>43117</v>
+      </c>
+      <c r="D386">
+        <v>3</v>
+      </c>
+      <c r="E386" t="s">
+        <v>93</v>
+      </c>
+      <c r="F386">
+        <v>2018</v>
+      </c>
+      <c r="G386" t="s">
+        <v>19</v>
+      </c>
+      <c r="H386" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="I386" s="1">
+        <v>22</v>
+      </c>
+      <c r="J386" s="3">
+        <v>3</v>
+      </c>
+      <c r="K386" s="3">
+        <v>24</v>
+      </c>
+      <c r="L386" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="387" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A387" s="3">
+        <v>386</v>
+      </c>
+      <c r="B387" s="3">
+        <v>45</v>
+      </c>
+      <c r="C387" s="2">
+        <v>43117</v>
+      </c>
+      <c r="D387">
+        <v>3</v>
+      </c>
+      <c r="E387" t="s">
+        <v>93</v>
+      </c>
+      <c r="F387">
+        <v>2018</v>
+      </c>
+      <c r="G387" t="s">
+        <v>19</v>
+      </c>
+      <c r="H387" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="I387" s="1">
+        <v>30</v>
+      </c>
+      <c r="J387" s="3">
+        <v>3</v>
+      </c>
+      <c r="K387" s="3">
+        <v>12</v>
+      </c>
+      <c r="L387" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="388" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A388" s="3">
+        <v>387</v>
+      </c>
+      <c r="B388" s="3">
+        <v>45</v>
+      </c>
+      <c r="C388" s="2">
+        <v>43117</v>
+      </c>
+      <c r="D388">
+        <v>3</v>
+      </c>
+      <c r="E388" t="s">
+        <v>93</v>
+      </c>
+      <c r="F388">
+        <v>2018</v>
+      </c>
+      <c r="G388" t="s">
+        <v>19</v>
+      </c>
+      <c r="H388" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I388" s="1">
+        <v>101</v>
+      </c>
+      <c r="J388" s="3">
+        <v>3</v>
+      </c>
+      <c r="K388" s="3">
+        <v>15</v>
+      </c>
+      <c r="L388" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="389" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A389" s="3">
+        <v>388</v>
+      </c>
+      <c r="B389" s="3">
+        <v>45</v>
+      </c>
+      <c r="C389" s="2">
+        <v>43117</v>
+      </c>
+      <c r="D389">
+        <v>3</v>
+      </c>
+      <c r="E389" t="s">
+        <v>93</v>
+      </c>
+      <c r="F389">
+        <v>2018</v>
+      </c>
+      <c r="G389" t="s">
+        <v>19</v>
+      </c>
+      <c r="H389" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="I389" s="1">
+        <v>0</v>
+      </c>
+      <c r="J389" s="3">
+        <v>3</v>
+      </c>
+      <c r="K389" s="3">
+        <v>30</v>
+      </c>
+      <c r="L389" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="390" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A390" s="3">
+        <v>389</v>
+      </c>
+      <c r="B390" s="3">
+        <v>45</v>
+      </c>
+      <c r="C390" s="2">
+        <v>43117</v>
+      </c>
+      <c r="D390">
+        <v>3</v>
+      </c>
+      <c r="E390" t="s">
+        <v>93</v>
+      </c>
+      <c r="F390">
+        <v>2018</v>
+      </c>
+      <c r="G390" t="s">
+        <v>19</v>
+      </c>
+      <c r="H390" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="I390" s="1">
+        <v>0</v>
+      </c>
+      <c r="J390" s="3">
+        <v>3</v>
+      </c>
+      <c r="K390" s="3">
+        <v>30</v>
+      </c>
+      <c r="L390" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="391" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A391" s="3">
+        <v>390</v>
+      </c>
+      <c r="B391" s="3">
+        <v>45</v>
+      </c>
+      <c r="C391" s="2">
+        <v>43117</v>
+      </c>
+      <c r="D391">
+        <v>3</v>
+      </c>
+      <c r="E391" t="s">
+        <v>93</v>
+      </c>
+      <c r="F391">
+        <v>2018</v>
+      </c>
+      <c r="G391" t="s">
+        <v>19</v>
+      </c>
+      <c r="H391" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I391" s="1">
+        <v>0</v>
+      </c>
+      <c r="J391" s="3">
+        <v>3</v>
+      </c>
+      <c r="K391" s="3">
+        <v>30</v>
+      </c>
+      <c r="L391" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="392" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A392" s="3">
+        <v>391</v>
+      </c>
+      <c r="B392" s="3">
+        <v>46</v>
+      </c>
+      <c r="C392" s="2">
+        <v>43118</v>
+      </c>
+      <c r="D392">
+        <v>3</v>
+      </c>
+      <c r="E392" t="s">
+        <v>93</v>
+      </c>
+      <c r="F392">
+        <v>2018</v>
+      </c>
+      <c r="G392" t="s">
+        <v>17</v>
+      </c>
+      <c r="H392" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I392" s="1">
+        <v>70</v>
+      </c>
+      <c r="J392" s="3">
+        <v>4</v>
+      </c>
+      <c r="K392" s="3">
+        <v>8</v>
+      </c>
+      <c r="L392" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="393" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A393" s="3">
+        <v>392</v>
+      </c>
+      <c r="B393" s="3">
+        <v>46</v>
+      </c>
+      <c r="C393" s="2">
+        <v>43118</v>
+      </c>
+      <c r="D393">
+        <v>3</v>
+      </c>
+      <c r="E393" t="s">
+        <v>93</v>
+      </c>
+      <c r="F393">
+        <v>2018</v>
+      </c>
+      <c r="G393" t="s">
+        <v>17</v>
+      </c>
+      <c r="H393" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I393" s="1">
+        <v>85</v>
+      </c>
+      <c r="J393" s="3">
+        <v>4</v>
+      </c>
+      <c r="K393" s="3">
+        <v>8</v>
+      </c>
+      <c r="L393" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="394" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A394" s="3">
+        <v>393</v>
+      </c>
+      <c r="B394" s="3">
+        <v>46</v>
+      </c>
+      <c r="C394" s="2">
+        <v>43118</v>
+      </c>
+      <c r="D394">
+        <v>3</v>
+      </c>
+      <c r="E394" t="s">
+        <v>93</v>
+      </c>
+      <c r="F394">
+        <v>2018</v>
+      </c>
+      <c r="G394" t="s">
+        <v>17</v>
+      </c>
+      <c r="H394" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I394" s="1">
+        <v>79</v>
+      </c>
+      <c r="J394" s="3">
+        <v>4</v>
+      </c>
+      <c r="K394" s="3">
+        <v>8</v>
+      </c>
+      <c r="L394" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="395" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A395" s="3">
+        <v>394</v>
+      </c>
+      <c r="B395" s="3">
+        <v>46</v>
+      </c>
+      <c r="C395" s="2">
+        <v>43118</v>
+      </c>
+      <c r="D395">
+        <v>3</v>
+      </c>
+      <c r="E395" t="s">
+        <v>93</v>
+      </c>
+      <c r="F395">
+        <v>2018</v>
+      </c>
+      <c r="G395" t="s">
+        <v>17</v>
+      </c>
+      <c r="H395" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I395" s="1">
+        <v>90</v>
+      </c>
+      <c r="J395" s="3">
+        <v>4</v>
+      </c>
+      <c r="K395" s="3">
+        <v>8</v>
+      </c>
+      <c r="L395" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="396" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A396" s="3">
+        <v>395</v>
+      </c>
+      <c r="B396" s="3">
+        <v>46</v>
+      </c>
+      <c r="C396" s="2">
+        <v>43118</v>
+      </c>
+      <c r="D396">
+        <v>3</v>
+      </c>
+      <c r="E396" t="s">
+        <v>93</v>
+      </c>
+      <c r="F396">
+        <v>2018</v>
+      </c>
+      <c r="G396" t="s">
+        <v>17</v>
+      </c>
+      <c r="H396" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="I396" s="1">
+        <v>8</v>
+      </c>
+      <c r="J396" s="3">
+        <v>3</v>
+      </c>
+      <c r="K396" s="3">
+        <v>12</v>
+      </c>
+      <c r="L396" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="397" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A397" s="3">
+        <v>396</v>
+      </c>
+      <c r="B397" s="3">
+        <v>46</v>
+      </c>
+      <c r="C397" s="2">
+        <v>43118</v>
+      </c>
+      <c r="D397">
+        <v>3</v>
+      </c>
+      <c r="E397" t="s">
+        <v>93</v>
+      </c>
+      <c r="F397">
+        <v>2018</v>
+      </c>
+      <c r="G397" t="s">
+        <v>17</v>
+      </c>
+      <c r="H397" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I397" s="1">
+        <v>8</v>
+      </c>
+      <c r="J397" s="3">
+        <v>3</v>
+      </c>
+      <c r="K397" s="3">
+        <v>12</v>
+      </c>
+      <c r="L397" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="398" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A398" s="3">
+        <v>397</v>
+      </c>
+      <c r="B398" s="3">
+        <v>46</v>
+      </c>
+      <c r="C398" s="2">
+        <v>43118</v>
+      </c>
+      <c r="D398">
+        <v>3</v>
+      </c>
+      <c r="E398" t="s">
+        <v>93</v>
+      </c>
+      <c r="F398">
+        <v>2018</v>
+      </c>
+      <c r="G398" t="s">
+        <v>17</v>
+      </c>
+      <c r="H398" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="I398" s="1">
+        <v>8</v>
+      </c>
+      <c r="J398" s="3">
+        <v>3</v>
+      </c>
+      <c r="K398" s="3">
+        <v>12</v>
+      </c>
+      <c r="L398" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="399" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A399" s="3">
+        <v>398</v>
+      </c>
+      <c r="B399" s="3">
+        <v>46</v>
+      </c>
+      <c r="C399" s="2">
+        <v>43118</v>
+      </c>
+      <c r="D399">
+        <v>3</v>
+      </c>
+      <c r="E399" t="s">
+        <v>93</v>
+      </c>
+      <c r="F399">
+        <v>2018</v>
+      </c>
+      <c r="G399" t="s">
+        <v>17</v>
+      </c>
+      <c r="H399" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="I399" s="1">
+        <v>0</v>
+      </c>
+      <c r="J399" s="3">
+        <v>3</v>
+      </c>
+      <c r="K399" s="3">
+        <v>30</v>
+      </c>
+      <c r="L399" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="400" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A400" s="3">
+        <v>399</v>
+      </c>
+      <c r="B400" s="3">
+        <v>46</v>
+      </c>
+      <c r="C400" s="2">
+        <v>43118</v>
+      </c>
+      <c r="D400">
+        <v>3</v>
+      </c>
+      <c r="E400" t="s">
+        <v>93</v>
+      </c>
+      <c r="F400">
+        <v>2018</v>
+      </c>
+      <c r="G400" t="s">
+        <v>17</v>
+      </c>
+      <c r="H400" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="I400" s="1">
+        <v>0</v>
+      </c>
+      <c r="J400" s="3">
+        <v>3</v>
+      </c>
+      <c r="K400" s="3">
+        <v>30</v>
+      </c>
+      <c r="L400" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="401" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A401" s="3">
+        <v>400</v>
+      </c>
+      <c r="B401" s="3">
+        <v>46</v>
+      </c>
+      <c r="C401" s="2">
+        <v>43118</v>
+      </c>
+      <c r="D401">
+        <v>3</v>
+      </c>
+      <c r="E401" t="s">
+        <v>93</v>
+      </c>
+      <c r="F401">
+        <v>2018</v>
+      </c>
+      <c r="G401" t="s">
+        <v>17</v>
+      </c>
+      <c r="H401" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I401" s="1">
+        <v>0</v>
+      </c>
+      <c r="J401" s="3">
+        <v>3</v>
+      </c>
+      <c r="K401" s="3">
+        <v>30</v>
+      </c>
+      <c r="L401" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="402" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A402" s="3">
+        <v>401</v>
+      </c>
+      <c r="B402" s="3">
+        <v>47</v>
+      </c>
+      <c r="C402" s="2">
+        <v>43119</v>
+      </c>
+      <c r="D402">
+        <v>3</v>
+      </c>
+      <c r="E402" t="s">
+        <v>93</v>
+      </c>
+      <c r="F402">
+        <v>2018</v>
+      </c>
+      <c r="G402" t="s">
+        <v>50</v>
+      </c>
+      <c r="H402" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="I402" s="1">
+        <v>0</v>
+      </c>
+      <c r="J402" s="3">
+        <v>3</v>
+      </c>
+      <c r="K402" s="3">
+        <v>60</v>
+      </c>
+      <c r="L402" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="403" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A403" s="3">
+        <v>402</v>
+      </c>
+      <c r="B403" s="3">
+        <v>47</v>
+      </c>
+      <c r="C403" s="2">
+        <v>43119</v>
+      </c>
+      <c r="D403">
+        <v>3</v>
+      </c>
+      <c r="E403" t="s">
+        <v>93</v>
+      </c>
+      <c r="F403">
+        <v>2018</v>
+      </c>
+      <c r="G403" t="s">
+        <v>50</v>
+      </c>
+      <c r="H403" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="I403" s="1">
+        <v>18</v>
+      </c>
+      <c r="J403" s="3">
+        <v>3</v>
+      </c>
+      <c r="K403" s="3">
+        <v>12</v>
+      </c>
+      <c r="L403" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="404" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A404" s="3">
+        <v>403</v>
+      </c>
+      <c r="B404" s="3">
+        <v>47</v>
+      </c>
+      <c r="C404" s="2">
+        <v>43119</v>
+      </c>
+      <c r="D404">
+        <v>3</v>
+      </c>
+      <c r="E404" t="s">
+        <v>93</v>
+      </c>
+      <c r="F404">
+        <v>2018</v>
+      </c>
+      <c r="G404" t="s">
+        <v>50</v>
+      </c>
+      <c r="H404" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="I404" s="1">
+        <v>14</v>
+      </c>
+      <c r="J404" s="3">
+        <v>3</v>
+      </c>
+      <c r="K404" s="3">
+        <v>12</v>
+      </c>
+      <c r="L404" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="405" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A405" s="3">
+        <v>404</v>
+      </c>
+      <c r="B405" s="3">
+        <v>47</v>
+      </c>
+      <c r="C405" s="2">
+        <v>43119</v>
+      </c>
+      <c r="D405">
+        <v>3</v>
+      </c>
+      <c r="E405" t="s">
+        <v>93</v>
+      </c>
+      <c r="F405">
+        <v>2018</v>
+      </c>
+      <c r="G405" t="s">
+        <v>50</v>
+      </c>
+      <c r="H405" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="I405" s="1">
+        <v>20</v>
+      </c>
+      <c r="J405" s="3">
+        <v>3</v>
+      </c>
+      <c r="K405" s="3">
+        <v>20</v>
+      </c>
+      <c r="L405" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="406" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A406" s="3">
+        <v>405</v>
+      </c>
+      <c r="B406" s="3">
+        <v>47</v>
+      </c>
+      <c r="C406" s="2">
+        <v>43119</v>
+      </c>
+      <c r="D406">
+        <v>3</v>
+      </c>
+      <c r="E406" t="s">
+        <v>93</v>
+      </c>
+      <c r="F406">
+        <v>2018</v>
+      </c>
+      <c r="G406" t="s">
+        <v>50</v>
+      </c>
+      <c r="H406" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="I406" s="1">
+        <v>60</v>
+      </c>
+      <c r="J406" s="3">
+        <v>3</v>
+      </c>
+      <c r="K406" s="3">
+        <v>8</v>
+      </c>
+      <c r="L406" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="407" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A407" s="3">
+        <v>406</v>
+      </c>
+      <c r="B407" s="3">
+        <v>47</v>
+      </c>
+      <c r="C407" s="2">
+        <v>43119</v>
+      </c>
+      <c r="D407">
+        <v>3</v>
+      </c>
+      <c r="E407" t="s">
+        <v>93</v>
+      </c>
+      <c r="F407">
+        <v>2018</v>
+      </c>
+      <c r="G407" t="s">
+        <v>50</v>
+      </c>
+      <c r="H407" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="I407" s="1">
+        <v>70</v>
+      </c>
+      <c r="J407" s="3">
+        <v>3</v>
+      </c>
+      <c r="K407" s="3">
+        <v>5</v>
+      </c>
+      <c r="L407" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="408" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A408" s="3">
+        <v>407</v>
+      </c>
+      <c r="B408" s="3">
+        <v>47</v>
+      </c>
+      <c r="C408" s="2">
+        <v>43119</v>
+      </c>
+      <c r="D408">
+        <v>3</v>
+      </c>
+      <c r="E408" t="s">
+        <v>93</v>
+      </c>
+      <c r="F408">
+        <v>2018</v>
+      </c>
+      <c r="G408" t="s">
+        <v>50</v>
+      </c>
+      <c r="H408" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="I408" s="1">
+        <v>80</v>
+      </c>
+      <c r="J408" s="3">
+        <v>2</v>
+      </c>
+      <c r="K408" s="3">
+        <v>3</v>
+      </c>
+      <c r="L408" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="409" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A409" s="3">
+        <v>408</v>
+      </c>
+      <c r="B409" s="3">
+        <v>47</v>
+      </c>
+      <c r="C409" s="2">
+        <v>43119</v>
+      </c>
+      <c r="D409">
+        <v>3</v>
+      </c>
+      <c r="E409" t="s">
+        <v>93</v>
+      </c>
+      <c r="F409">
+        <v>2018</v>
+      </c>
+      <c r="G409" t="s">
+        <v>50</v>
+      </c>
+      <c r="H409" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I409" s="1">
+        <v>0</v>
+      </c>
+      <c r="J409" s="3">
+        <v>3</v>
+      </c>
+      <c r="K409" s="3">
+        <v>30</v>
+      </c>
+      <c r="L409" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="410" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A410" s="3">
+        <v>409</v>
+      </c>
+      <c r="B410" s="3">
+        <v>47</v>
+      </c>
+      <c r="C410" s="2">
+        <v>43119</v>
+      </c>
+      <c r="D410">
+        <v>3</v>
+      </c>
+      <c r="E410" t="s">
+        <v>93</v>
+      </c>
+      <c r="F410">
+        <v>2018</v>
+      </c>
+      <c r="G410" t="s">
+        <v>50</v>
+      </c>
+      <c r="H410" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I410" s="1">
+        <v>0</v>
+      </c>
+      <c r="J410" s="3">
+        <v>3</v>
+      </c>
+      <c r="K410" s="3">
+        <v>20</v>
+      </c>
+      <c r="L410" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="411" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A411" s="3">
+        <v>410</v>
+      </c>
+      <c r="B411" s="3">
+        <v>47</v>
+      </c>
+      <c r="C411" s="2">
+        <v>43119</v>
+      </c>
+      <c r="D411">
+        <v>3</v>
+      </c>
+      <c r="E411" t="s">
+        <v>93</v>
+      </c>
+      <c r="F411">
+        <v>2018</v>
+      </c>
+      <c r="G411" t="s">
+        <v>50</v>
+      </c>
+      <c r="H411" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="I411" s="1">
+        <v>8</v>
+      </c>
+      <c r="J411" s="3">
+        <v>3</v>
+      </c>
+      <c r="K411" s="3">
+        <v>20</v>
+      </c>
+      <c r="L411" t="s">
+        <v>89</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Adding updated GymWorkout files 31/01/2018
</commit_message>
<xml_diff>
--- a/datasets/GymWorkouts.xlsx
+++ b/datasets/GymWorkouts.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1652" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1768" uniqueCount="119">
   <si>
     <t>Exercise Date</t>
   </si>
@@ -363,6 +363,24 @@
   </si>
   <si>
     <t>80% 1RM Barbell Squat</t>
+  </si>
+  <si>
+    <t>DB Bench Press</t>
+  </si>
+  <si>
+    <t>DB Pec Fly</t>
+  </si>
+  <si>
+    <t>Press up hold</t>
+  </si>
+  <si>
+    <t>Rugsack Squat</t>
+  </si>
+  <si>
+    <t>Rugsack Lunges</t>
+  </si>
+  <si>
+    <t>Rugsack Shoulder Raise</t>
   </si>
 </sst>
 </file>
@@ -717,11 +735,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L411"/>
+  <dimension ref="A1:L440"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A388" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C415" sqref="C415"/>
+      <pane ySplit="1" topLeftCell="A414" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C443" sqref="C443"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -16358,6 +16376,1108 @@
         <v>89</v>
       </c>
     </row>
+    <row r="412" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A412" s="3">
+        <v>411</v>
+      </c>
+      <c r="B412" s="3">
+        <v>48</v>
+      </c>
+      <c r="C412" s="2">
+        <v>43121</v>
+      </c>
+      <c r="D412">
+        <v>3</v>
+      </c>
+      <c r="E412" t="s">
+        <v>93</v>
+      </c>
+      <c r="F412">
+        <v>2018</v>
+      </c>
+      <c r="G412" t="s">
+        <v>45</v>
+      </c>
+      <c r="H412" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I412" s="1">
+        <v>0</v>
+      </c>
+      <c r="J412" s="3">
+        <v>3</v>
+      </c>
+      <c r="K412" s="3">
+        <v>12</v>
+      </c>
+      <c r="L412" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="413" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A413" s="3">
+        <v>412</v>
+      </c>
+      <c r="B413" s="3">
+        <v>48</v>
+      </c>
+      <c r="C413" s="2">
+        <v>43121</v>
+      </c>
+      <c r="D413">
+        <v>3</v>
+      </c>
+      <c r="E413" t="s">
+        <v>93</v>
+      </c>
+      <c r="F413">
+        <v>2018</v>
+      </c>
+      <c r="G413" t="s">
+        <v>45</v>
+      </c>
+      <c r="H413" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I413" s="1">
+        <v>102</v>
+      </c>
+      <c r="J413" s="3">
+        <v>3</v>
+      </c>
+      <c r="K413" s="3">
+        <v>12</v>
+      </c>
+      <c r="L413" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="414" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A414" s="3">
+        <v>413</v>
+      </c>
+      <c r="B414" s="3">
+        <v>48</v>
+      </c>
+      <c r="C414" s="2">
+        <v>43121</v>
+      </c>
+      <c r="D414">
+        <v>3</v>
+      </c>
+      <c r="E414" t="s">
+        <v>93</v>
+      </c>
+      <c r="F414">
+        <v>2018</v>
+      </c>
+      <c r="G414" t="s">
+        <v>45</v>
+      </c>
+      <c r="H414" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="I414" s="1">
+        <v>22</v>
+      </c>
+      <c r="J414" s="3">
+        <v>3</v>
+      </c>
+      <c r="K414" s="3">
+        <v>8</v>
+      </c>
+      <c r="L414" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="415" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A415" s="3">
+        <v>414</v>
+      </c>
+      <c r="B415" s="3">
+        <v>48</v>
+      </c>
+      <c r="C415" s="2">
+        <v>43121</v>
+      </c>
+      <c r="D415">
+        <v>3</v>
+      </c>
+      <c r="E415" t="s">
+        <v>93</v>
+      </c>
+      <c r="F415">
+        <v>2018</v>
+      </c>
+      <c r="G415" t="s">
+        <v>45</v>
+      </c>
+      <c r="H415" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="I415" s="1">
+        <v>22</v>
+      </c>
+      <c r="J415" s="3">
+        <v>3</v>
+      </c>
+      <c r="K415" s="3">
+        <v>8</v>
+      </c>
+      <c r="L415" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="416" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A416" s="3">
+        <v>415</v>
+      </c>
+      <c r="B416" s="3">
+        <v>48</v>
+      </c>
+      <c r="C416" s="2">
+        <v>43121</v>
+      </c>
+      <c r="D416">
+        <v>3</v>
+      </c>
+      <c r="E416" t="s">
+        <v>93</v>
+      </c>
+      <c r="F416">
+        <v>2018</v>
+      </c>
+      <c r="G416" t="s">
+        <v>45</v>
+      </c>
+      <c r="H416" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I416" s="1">
+        <v>0</v>
+      </c>
+      <c r="J416" s="3">
+        <v>3</v>
+      </c>
+      <c r="K416" s="3">
+        <v>12</v>
+      </c>
+      <c r="L416" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="417" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A417" s="3">
+        <v>416</v>
+      </c>
+      <c r="B417" s="3">
+        <v>48</v>
+      </c>
+      <c r="C417" s="2">
+        <v>43121</v>
+      </c>
+      <c r="D417">
+        <v>3</v>
+      </c>
+      <c r="E417" t="s">
+        <v>93</v>
+      </c>
+      <c r="F417">
+        <v>2018</v>
+      </c>
+      <c r="G417" t="s">
+        <v>45</v>
+      </c>
+      <c r="H417" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I417" s="1">
+        <v>0</v>
+      </c>
+      <c r="J417" s="3">
+        <v>3</v>
+      </c>
+      <c r="K417" s="3">
+        <v>20</v>
+      </c>
+      <c r="L417" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="418" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A418" s="3">
+        <v>417</v>
+      </c>
+      <c r="B418" s="3">
+        <v>48</v>
+      </c>
+      <c r="C418" s="2">
+        <v>43121</v>
+      </c>
+      <c r="D418">
+        <v>3</v>
+      </c>
+      <c r="E418" t="s">
+        <v>93</v>
+      </c>
+      <c r="F418">
+        <v>2018</v>
+      </c>
+      <c r="G418" t="s">
+        <v>45</v>
+      </c>
+      <c r="H418" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I418" s="1">
+        <v>0</v>
+      </c>
+      <c r="J418" s="3">
+        <v>3</v>
+      </c>
+      <c r="K418" s="3">
+        <v>12</v>
+      </c>
+      <c r="L418" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="419" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A419" s="3">
+        <v>418</v>
+      </c>
+      <c r="B419" s="3">
+        <v>48</v>
+      </c>
+      <c r="C419" s="2">
+        <v>43121</v>
+      </c>
+      <c r="D419">
+        <v>3</v>
+      </c>
+      <c r="E419" t="s">
+        <v>93</v>
+      </c>
+      <c r="F419">
+        <v>2018</v>
+      </c>
+      <c r="G419" t="s">
+        <v>45</v>
+      </c>
+      <c r="H419" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="I419" s="1">
+        <v>0</v>
+      </c>
+      <c r="J419" s="3">
+        <v>3</v>
+      </c>
+      <c r="K419" s="3">
+        <v>30</v>
+      </c>
+      <c r="L419" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="420" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A420" s="3">
+        <v>419</v>
+      </c>
+      <c r="B420" s="3">
+        <v>48</v>
+      </c>
+      <c r="C420" s="2">
+        <v>43121</v>
+      </c>
+      <c r="D420">
+        <v>3</v>
+      </c>
+      <c r="E420" t="s">
+        <v>93</v>
+      </c>
+      <c r="F420">
+        <v>2018</v>
+      </c>
+      <c r="G420" t="s">
+        <v>45</v>
+      </c>
+      <c r="H420" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="I420" s="1">
+        <v>0</v>
+      </c>
+      <c r="J420" s="3">
+        <v>3</v>
+      </c>
+      <c r="K420" s="3">
+        <v>30</v>
+      </c>
+      <c r="L420" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="421" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A421" s="3">
+        <v>420</v>
+      </c>
+      <c r="B421" s="3">
+        <v>48</v>
+      </c>
+      <c r="C421" s="2">
+        <v>43121</v>
+      </c>
+      <c r="D421">
+        <v>3</v>
+      </c>
+      <c r="E421" t="s">
+        <v>93</v>
+      </c>
+      <c r="F421">
+        <v>2018</v>
+      </c>
+      <c r="G421" t="s">
+        <v>45</v>
+      </c>
+      <c r="H421" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I421" s="1">
+        <v>0</v>
+      </c>
+      <c r="J421" s="3">
+        <v>3</v>
+      </c>
+      <c r="K421" s="3">
+        <v>30</v>
+      </c>
+      <c r="L421" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="422" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A422" s="3">
+        <v>421</v>
+      </c>
+      <c r="B422" s="3">
+        <v>49</v>
+      </c>
+      <c r="C422" s="2">
+        <v>43122</v>
+      </c>
+      <c r="D422">
+        <v>4</v>
+      </c>
+      <c r="E422" t="s">
+        <v>93</v>
+      </c>
+      <c r="F422">
+        <v>2018</v>
+      </c>
+      <c r="G422" t="s">
+        <v>18</v>
+      </c>
+      <c r="H422" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I422" s="1">
+        <v>82.5</v>
+      </c>
+      <c r="J422" s="3">
+        <v>4</v>
+      </c>
+      <c r="K422" s="3">
+        <v>10</v>
+      </c>
+      <c r="L422" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="423" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A423" s="3">
+        <v>422</v>
+      </c>
+      <c r="B423" s="3">
+        <v>49</v>
+      </c>
+      <c r="C423" s="2">
+        <v>43122</v>
+      </c>
+      <c r="D423">
+        <v>5</v>
+      </c>
+      <c r="E423" t="s">
+        <v>93</v>
+      </c>
+      <c r="F423">
+        <v>2018</v>
+      </c>
+      <c r="G423" t="s">
+        <v>18</v>
+      </c>
+      <c r="H423" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I423" s="1">
+        <v>40</v>
+      </c>
+      <c r="J423" s="3">
+        <v>4</v>
+      </c>
+      <c r="K423" s="3">
+        <v>8</v>
+      </c>
+      <c r="L423" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="424" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A424" s="3">
+        <v>423</v>
+      </c>
+      <c r="B424" s="3">
+        <v>49</v>
+      </c>
+      <c r="C424" s="2">
+        <v>43122</v>
+      </c>
+      <c r="D424">
+        <v>5</v>
+      </c>
+      <c r="E424" t="s">
+        <v>93</v>
+      </c>
+      <c r="F424">
+        <v>2018</v>
+      </c>
+      <c r="G424" t="s">
+        <v>18</v>
+      </c>
+      <c r="H424" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="I424" s="1">
+        <v>14</v>
+      </c>
+      <c r="J424" s="3">
+        <v>4</v>
+      </c>
+      <c r="K424" s="3">
+        <v>8</v>
+      </c>
+      <c r="L424" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="425" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A425" s="3">
+        <v>424</v>
+      </c>
+      <c r="B425" s="3">
+        <v>49</v>
+      </c>
+      <c r="C425" s="2">
+        <v>43122</v>
+      </c>
+      <c r="D425">
+        <v>5</v>
+      </c>
+      <c r="E425" t="s">
+        <v>93</v>
+      </c>
+      <c r="F425">
+        <v>2018</v>
+      </c>
+      <c r="G425" t="s">
+        <v>18</v>
+      </c>
+      <c r="H425" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I425" s="1">
+        <v>22</v>
+      </c>
+      <c r="J425" s="3">
+        <v>4</v>
+      </c>
+      <c r="K425" s="3">
+        <v>8</v>
+      </c>
+      <c r="L425" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="426" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A426" s="3">
+        <v>425</v>
+      </c>
+      <c r="B426" s="3">
+        <v>49</v>
+      </c>
+      <c r="C426" s="2">
+        <v>43122</v>
+      </c>
+      <c r="D426">
+        <v>5</v>
+      </c>
+      <c r="E426" t="s">
+        <v>93</v>
+      </c>
+      <c r="F426">
+        <v>2018</v>
+      </c>
+      <c r="G426" t="s">
+        <v>18</v>
+      </c>
+      <c r="H426" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I426" s="1">
+        <v>30</v>
+      </c>
+      <c r="J426" s="3">
+        <v>4</v>
+      </c>
+      <c r="K426" s="3">
+        <v>8</v>
+      </c>
+      <c r="L426" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="427" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A427" s="3">
+        <v>426</v>
+      </c>
+      <c r="B427" s="3">
+        <v>49</v>
+      </c>
+      <c r="C427" s="2">
+        <v>43122</v>
+      </c>
+      <c r="D427">
+        <v>5</v>
+      </c>
+      <c r="E427" t="s">
+        <v>93</v>
+      </c>
+      <c r="F427">
+        <v>2018</v>
+      </c>
+      <c r="G427" t="s">
+        <v>18</v>
+      </c>
+      <c r="H427" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I427" s="1">
+        <v>14</v>
+      </c>
+      <c r="J427" s="3">
+        <v>4</v>
+      </c>
+      <c r="K427" s="3">
+        <v>8</v>
+      </c>
+      <c r="L427" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="428" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A428" s="3">
+        <v>427</v>
+      </c>
+      <c r="B428" s="3">
+        <v>49</v>
+      </c>
+      <c r="C428" s="2">
+        <v>43122</v>
+      </c>
+      <c r="D428">
+        <v>5</v>
+      </c>
+      <c r="E428" t="s">
+        <v>93</v>
+      </c>
+      <c r="F428">
+        <v>2018</v>
+      </c>
+      <c r="G428" t="s">
+        <v>18</v>
+      </c>
+      <c r="H428" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I428" s="1">
+        <v>101</v>
+      </c>
+      <c r="J428" s="3">
+        <v>3</v>
+      </c>
+      <c r="K428" s="3">
+        <v>10</v>
+      </c>
+      <c r="L428" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="429" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A429" s="3">
+        <v>428</v>
+      </c>
+      <c r="B429" s="3">
+        <v>49</v>
+      </c>
+      <c r="C429" s="2">
+        <v>43122</v>
+      </c>
+      <c r="D429">
+        <v>5</v>
+      </c>
+      <c r="E429" t="s">
+        <v>93</v>
+      </c>
+      <c r="F429">
+        <v>2018</v>
+      </c>
+      <c r="G429" t="s">
+        <v>18</v>
+      </c>
+      <c r="H429" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I429" s="1">
+        <v>101</v>
+      </c>
+      <c r="J429" s="3">
+        <v>3</v>
+      </c>
+      <c r="K429" s="3">
+        <v>10</v>
+      </c>
+      <c r="L429" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="430" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A430" s="3">
+        <v>429</v>
+      </c>
+      <c r="B430" s="3">
+        <v>49</v>
+      </c>
+      <c r="C430" s="2">
+        <v>43122</v>
+      </c>
+      <c r="D430">
+        <v>5</v>
+      </c>
+      <c r="E430" t="s">
+        <v>93</v>
+      </c>
+      <c r="F430">
+        <v>2018</v>
+      </c>
+      <c r="G430" t="s">
+        <v>18</v>
+      </c>
+      <c r="H430" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="I430" s="1">
+        <v>101</v>
+      </c>
+      <c r="J430" s="3">
+        <v>1</v>
+      </c>
+      <c r="K430" s="3">
+        <v>53</v>
+      </c>
+      <c r="L430" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="431" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A431" s="3">
+        <v>430</v>
+      </c>
+      <c r="B431" s="3">
+        <v>50</v>
+      </c>
+      <c r="C431" s="2">
+        <v>43131</v>
+      </c>
+      <c r="D431">
+        <v>6</v>
+      </c>
+      <c r="E431" t="s">
+        <v>93</v>
+      </c>
+      <c r="F431">
+        <v>2018</v>
+      </c>
+      <c r="G431" t="s">
+        <v>19</v>
+      </c>
+      <c r="H431" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="I431" s="1">
+        <v>101</v>
+      </c>
+      <c r="J431" s="3">
+        <v>5</v>
+      </c>
+      <c r="K431" s="3">
+        <v>10</v>
+      </c>
+      <c r="L431" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="432" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A432" s="3">
+        <v>431</v>
+      </c>
+      <c r="B432" s="3">
+        <v>50</v>
+      </c>
+      <c r="C432" s="2">
+        <v>43131</v>
+      </c>
+      <c r="D432">
+        <v>7</v>
+      </c>
+      <c r="E432" t="s">
+        <v>93</v>
+      </c>
+      <c r="F432">
+        <v>2018</v>
+      </c>
+      <c r="G432" t="s">
+        <v>19</v>
+      </c>
+      <c r="H432" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I432" s="1">
+        <v>101</v>
+      </c>
+      <c r="J432" s="3">
+        <v>5</v>
+      </c>
+      <c r="K432" s="3">
+        <v>10</v>
+      </c>
+      <c r="L432" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="433" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A433" s="3">
+        <v>432</v>
+      </c>
+      <c r="B433" s="3">
+        <v>50</v>
+      </c>
+      <c r="C433" s="2">
+        <v>43131</v>
+      </c>
+      <c r="D433">
+        <v>7</v>
+      </c>
+      <c r="E433" t="s">
+        <v>93</v>
+      </c>
+      <c r="F433">
+        <v>2018</v>
+      </c>
+      <c r="G433" t="s">
+        <v>19</v>
+      </c>
+      <c r="H433" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="I433" s="1">
+        <v>20</v>
+      </c>
+      <c r="J433" s="3">
+        <v>5</v>
+      </c>
+      <c r="K433" s="3">
+        <v>10</v>
+      </c>
+      <c r="L433" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="434" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A434" s="3">
+        <v>433</v>
+      </c>
+      <c r="B434" s="3">
+        <v>50</v>
+      </c>
+      <c r="C434" s="2">
+        <v>43131</v>
+      </c>
+      <c r="D434">
+        <v>7</v>
+      </c>
+      <c r="E434" t="s">
+        <v>93</v>
+      </c>
+      <c r="F434">
+        <v>2018</v>
+      </c>
+      <c r="G434" t="s">
+        <v>19</v>
+      </c>
+      <c r="H434" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="I434" s="1">
+        <v>20</v>
+      </c>
+      <c r="J434" s="3">
+        <v>5</v>
+      </c>
+      <c r="K434" s="3">
+        <v>20</v>
+      </c>
+      <c r="L434" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="435" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A435" s="3">
+        <v>434</v>
+      </c>
+      <c r="B435" s="3">
+        <v>50</v>
+      </c>
+      <c r="C435" s="2">
+        <v>43131</v>
+      </c>
+      <c r="D435">
+        <v>7</v>
+      </c>
+      <c r="E435" t="s">
+        <v>93</v>
+      </c>
+      <c r="F435">
+        <v>2018</v>
+      </c>
+      <c r="G435" t="s">
+        <v>19</v>
+      </c>
+      <c r="H435" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="I435" s="1">
+        <v>20</v>
+      </c>
+      <c r="J435" s="3">
+        <v>5</v>
+      </c>
+      <c r="K435" s="3">
+        <v>10</v>
+      </c>
+      <c r="L435" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="436" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A436" s="3">
+        <v>435</v>
+      </c>
+      <c r="B436" s="3">
+        <v>50</v>
+      </c>
+      <c r="C436" s="2">
+        <v>43131</v>
+      </c>
+      <c r="D436">
+        <v>7</v>
+      </c>
+      <c r="E436" t="s">
+        <v>93</v>
+      </c>
+      <c r="F436">
+        <v>2018</v>
+      </c>
+      <c r="G436" t="s">
+        <v>19</v>
+      </c>
+      <c r="H436" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I436" s="1">
+        <v>0</v>
+      </c>
+      <c r="J436" s="3">
+        <v>5</v>
+      </c>
+      <c r="K436" s="3">
+        <v>10</v>
+      </c>
+      <c r="L436" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="437" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A437" s="3">
+        <v>436</v>
+      </c>
+      <c r="B437" s="3">
+        <v>50</v>
+      </c>
+      <c r="C437" s="2">
+        <v>43131</v>
+      </c>
+      <c r="D437">
+        <v>7</v>
+      </c>
+      <c r="E437" t="s">
+        <v>93</v>
+      </c>
+      <c r="F437">
+        <v>2018</v>
+      </c>
+      <c r="G437" t="s">
+        <v>19</v>
+      </c>
+      <c r="H437" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I437" s="1">
+        <v>0</v>
+      </c>
+      <c r="J437" s="3">
+        <v>5</v>
+      </c>
+      <c r="K437" s="3">
+        <v>10</v>
+      </c>
+      <c r="L437" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="438" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A438" s="3">
+        <v>437</v>
+      </c>
+      <c r="B438" s="3">
+        <v>50</v>
+      </c>
+      <c r="C438" s="2">
+        <v>43131</v>
+      </c>
+      <c r="D438">
+        <v>7</v>
+      </c>
+      <c r="E438" t="s">
+        <v>93</v>
+      </c>
+      <c r="F438">
+        <v>2018</v>
+      </c>
+      <c r="G438" t="s">
+        <v>19</v>
+      </c>
+      <c r="H438" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="I438" s="1">
+        <v>0</v>
+      </c>
+      <c r="J438" s="3">
+        <v>5</v>
+      </c>
+      <c r="K438" s="3">
+        <v>30</v>
+      </c>
+      <c r="L438" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="439" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A439" s="3">
+        <v>438</v>
+      </c>
+      <c r="B439" s="3">
+        <v>50</v>
+      </c>
+      <c r="C439" s="2">
+        <v>43131</v>
+      </c>
+      <c r="D439">
+        <v>7</v>
+      </c>
+      <c r="E439" t="s">
+        <v>93</v>
+      </c>
+      <c r="F439">
+        <v>2018</v>
+      </c>
+      <c r="G439" t="s">
+        <v>19</v>
+      </c>
+      <c r="H439" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="I439" s="1">
+        <v>0</v>
+      </c>
+      <c r="J439" s="3">
+        <v>5</v>
+      </c>
+      <c r="K439" s="3">
+        <v>30</v>
+      </c>
+      <c r="L439" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="440" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A440" s="3">
+        <v>439</v>
+      </c>
+      <c r="B440" s="3">
+        <v>50</v>
+      </c>
+      <c r="C440" s="2">
+        <v>43131</v>
+      </c>
+      <c r="D440">
+        <v>7</v>
+      </c>
+      <c r="E440" t="s">
+        <v>93</v>
+      </c>
+      <c r="F440">
+        <v>2018</v>
+      </c>
+      <c r="G440" t="s">
+        <v>19</v>
+      </c>
+      <c r="H440" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I440" s="1">
+        <v>0</v>
+      </c>
+      <c r="J440" s="3">
+        <v>5</v>
+      </c>
+      <c r="K440" s="3">
+        <v>30</v>
+      </c>
+      <c r="L440" t="s">
+        <v>89</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Adding updated GymWorkout data 11/02/2018
</commit_message>
<xml_diff>
--- a/datasets/GymWorkouts.xlsx
+++ b/datasets/GymWorkouts.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1768" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1976" uniqueCount="128">
   <si>
     <t>Exercise Date</t>
   </si>
@@ -382,6 +382,33 @@
   <si>
     <t>Rugsack Shoulder Raise</t>
   </si>
+  <si>
+    <t>February</t>
+  </si>
+  <si>
+    <t>Chest Press</t>
+  </si>
+  <si>
+    <t>Barbell Pull Down</t>
+  </si>
+  <si>
+    <t>Press-up hold</t>
+  </si>
+  <si>
+    <t>MTS Ab Crunch</t>
+  </si>
+  <si>
+    <t>Raised leg circles</t>
+  </si>
+  <si>
+    <t>Scissors</t>
+  </si>
+  <si>
+    <t>Knee-Pull ins</t>
+  </si>
+  <si>
+    <t>Flitter Kicks</t>
+  </si>
 </sst>
 </file>
 
@@ -735,11 +762,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L440"/>
+  <dimension ref="A1:L492"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A414" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C443" sqref="C443"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A463" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C489" sqref="C489"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -17478,6 +17505,1982 @@
         <v>89</v>
       </c>
     </row>
+    <row r="441" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A441" s="3">
+        <v>440</v>
+      </c>
+      <c r="B441" s="3">
+        <v>51</v>
+      </c>
+      <c r="C441" s="2">
+        <v>43133</v>
+      </c>
+      <c r="D441">
+        <v>7</v>
+      </c>
+      <c r="E441" t="s">
+        <v>119</v>
+      </c>
+      <c r="F441">
+        <v>2018</v>
+      </c>
+      <c r="G441" t="s">
+        <v>50</v>
+      </c>
+      <c r="H441" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="I441" s="1">
+        <v>80</v>
+      </c>
+      <c r="J441" s="3">
+        <v>5</v>
+      </c>
+      <c r="K441" s="3">
+        <v>10</v>
+      </c>
+      <c r="L441" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="442" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A442" s="3">
+        <v>441</v>
+      </c>
+      <c r="B442" s="3">
+        <v>51</v>
+      </c>
+      <c r="C442" s="2">
+        <v>43133</v>
+      </c>
+      <c r="D442">
+        <v>7</v>
+      </c>
+      <c r="E442" t="s">
+        <v>119</v>
+      </c>
+      <c r="F442">
+        <v>2018</v>
+      </c>
+      <c r="G442" t="s">
+        <v>50</v>
+      </c>
+      <c r="H442" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="I442" s="1">
+        <v>80</v>
+      </c>
+      <c r="J442" s="3">
+        <v>5</v>
+      </c>
+      <c r="K442" s="3">
+        <v>10</v>
+      </c>
+      <c r="L442" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="443" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A443" s="3">
+        <v>442</v>
+      </c>
+      <c r="B443" s="3">
+        <v>51</v>
+      </c>
+      <c r="C443" s="2">
+        <v>43133</v>
+      </c>
+      <c r="D443">
+        <v>7</v>
+      </c>
+      <c r="E443" t="s">
+        <v>119</v>
+      </c>
+      <c r="F443">
+        <v>2018</v>
+      </c>
+      <c r="G443" t="s">
+        <v>50</v>
+      </c>
+      <c r="H443" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I443" s="1">
+        <v>40</v>
+      </c>
+      <c r="J443" s="3">
+        <v>5</v>
+      </c>
+      <c r="K443" s="3">
+        <v>10</v>
+      </c>
+      <c r="L443" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="444" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A444" s="3">
+        <v>443</v>
+      </c>
+      <c r="B444" s="3">
+        <v>51</v>
+      </c>
+      <c r="C444" s="2">
+        <v>43133</v>
+      </c>
+      <c r="D444">
+        <v>7</v>
+      </c>
+      <c r="E444" t="s">
+        <v>119</v>
+      </c>
+      <c r="F444">
+        <v>2018</v>
+      </c>
+      <c r="G444" t="s">
+        <v>50</v>
+      </c>
+      <c r="H444" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I444" s="1">
+        <v>80</v>
+      </c>
+      <c r="J444" s="3">
+        <v>5</v>
+      </c>
+      <c r="K444" s="3">
+        <v>10</v>
+      </c>
+      <c r="L444" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="445" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A445" s="3">
+        <v>444</v>
+      </c>
+      <c r="B445" s="3">
+        <v>51</v>
+      </c>
+      <c r="C445" s="2">
+        <v>43133</v>
+      </c>
+      <c r="D445">
+        <v>7</v>
+      </c>
+      <c r="E445" t="s">
+        <v>119</v>
+      </c>
+      <c r="F445">
+        <v>2018</v>
+      </c>
+      <c r="G445" t="s">
+        <v>50</v>
+      </c>
+      <c r="H445" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="I445" s="1">
+        <v>0</v>
+      </c>
+      <c r="J445" s="3">
+        <v>5</v>
+      </c>
+      <c r="K445" s="3">
+        <v>30</v>
+      </c>
+      <c r="L445" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="446" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A446" s="3">
+        <v>445</v>
+      </c>
+      <c r="B446" s="3">
+        <v>51</v>
+      </c>
+      <c r="C446" s="2">
+        <v>43133</v>
+      </c>
+      <c r="D446">
+        <v>7</v>
+      </c>
+      <c r="E446" t="s">
+        <v>119</v>
+      </c>
+      <c r="F446">
+        <v>2018</v>
+      </c>
+      <c r="G446" t="s">
+        <v>50</v>
+      </c>
+      <c r="H446" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="I446" s="1">
+        <v>0</v>
+      </c>
+      <c r="J446" s="3">
+        <v>5</v>
+      </c>
+      <c r="K446" s="3">
+        <v>30</v>
+      </c>
+      <c r="L446" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="447" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A447" s="3">
+        <v>446</v>
+      </c>
+      <c r="B447" s="3">
+        <v>51</v>
+      </c>
+      <c r="C447" s="2">
+        <v>43133</v>
+      </c>
+      <c r="D447">
+        <v>7</v>
+      </c>
+      <c r="E447" t="s">
+        <v>119</v>
+      </c>
+      <c r="F447">
+        <v>2018</v>
+      </c>
+      <c r="G447" t="s">
+        <v>50</v>
+      </c>
+      <c r="H447" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I447" s="1">
+        <v>0</v>
+      </c>
+      <c r="J447" s="3">
+        <v>5</v>
+      </c>
+      <c r="K447" s="3">
+        <v>30</v>
+      </c>
+      <c r="L447" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="448" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A448" s="3">
+        <v>447</v>
+      </c>
+      <c r="B448" s="3">
+        <v>52</v>
+      </c>
+      <c r="C448" s="2">
+        <v>43136</v>
+      </c>
+      <c r="D448">
+        <v>8</v>
+      </c>
+      <c r="E448" t="s">
+        <v>119</v>
+      </c>
+      <c r="F448">
+        <v>2018</v>
+      </c>
+      <c r="G448" t="s">
+        <v>18</v>
+      </c>
+      <c r="H448" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I448" s="1">
+        <v>83.6</v>
+      </c>
+      <c r="J448" s="3">
+        <v>4</v>
+      </c>
+      <c r="K448" s="3">
+        <v>8</v>
+      </c>
+      <c r="L448" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="449" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A449" s="3">
+        <v>448</v>
+      </c>
+      <c r="B449" s="3">
+        <v>52</v>
+      </c>
+      <c r="C449" s="2">
+        <v>43136</v>
+      </c>
+      <c r="D449">
+        <v>8</v>
+      </c>
+      <c r="E449" t="s">
+        <v>119</v>
+      </c>
+      <c r="F449">
+        <v>2018</v>
+      </c>
+      <c r="G449" t="s">
+        <v>18</v>
+      </c>
+      <c r="H449" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I449" s="1">
+        <v>44.8</v>
+      </c>
+      <c r="J449" s="3">
+        <v>5</v>
+      </c>
+      <c r="K449" s="3">
+        <v>5</v>
+      </c>
+      <c r="L449" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="450" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A450" s="3">
+        <v>449</v>
+      </c>
+      <c r="B450" s="3">
+        <v>52</v>
+      </c>
+      <c r="C450" s="2">
+        <v>43136</v>
+      </c>
+      <c r="D450">
+        <v>8</v>
+      </c>
+      <c r="E450" t="s">
+        <v>119</v>
+      </c>
+      <c r="F450">
+        <v>2018</v>
+      </c>
+      <c r="G450" t="s">
+        <v>18</v>
+      </c>
+      <c r="H450" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="I450" s="1">
+        <v>18</v>
+      </c>
+      <c r="J450" s="3">
+        <v>4</v>
+      </c>
+      <c r="K450" s="3">
+        <v>5</v>
+      </c>
+      <c r="L450" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="451" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A451" s="3">
+        <v>450</v>
+      </c>
+      <c r="B451" s="3">
+        <v>52</v>
+      </c>
+      <c r="C451" s="2">
+        <v>43136</v>
+      </c>
+      <c r="D451">
+        <v>8</v>
+      </c>
+      <c r="E451" t="s">
+        <v>119</v>
+      </c>
+      <c r="F451">
+        <v>2018</v>
+      </c>
+      <c r="G451" t="s">
+        <v>18</v>
+      </c>
+      <c r="H451" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I451" s="1">
+        <v>22</v>
+      </c>
+      <c r="J451" s="3">
+        <v>4</v>
+      </c>
+      <c r="K451" s="3">
+        <v>8</v>
+      </c>
+      <c r="L451" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="452" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A452" s="3">
+        <v>451</v>
+      </c>
+      <c r="B452" s="3">
+        <v>52</v>
+      </c>
+      <c r="C452" s="2">
+        <v>43136</v>
+      </c>
+      <c r="D452">
+        <v>8</v>
+      </c>
+      <c r="E452" t="s">
+        <v>119</v>
+      </c>
+      <c r="F452">
+        <v>2018</v>
+      </c>
+      <c r="G452" t="s">
+        <v>18</v>
+      </c>
+      <c r="H452" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I452" s="1">
+        <v>19.5</v>
+      </c>
+      <c r="J452" s="3">
+        <v>4</v>
+      </c>
+      <c r="K452" s="3">
+        <v>8</v>
+      </c>
+      <c r="L452" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="453" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A453" s="3">
+        <v>452</v>
+      </c>
+      <c r="B453" s="3">
+        <v>52</v>
+      </c>
+      <c r="C453" s="2">
+        <v>43136</v>
+      </c>
+      <c r="D453">
+        <v>8</v>
+      </c>
+      <c r="E453" t="s">
+        <v>119</v>
+      </c>
+      <c r="F453">
+        <v>2018</v>
+      </c>
+      <c r="G453" t="s">
+        <v>18</v>
+      </c>
+      <c r="H453" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I453" s="1">
+        <v>15</v>
+      </c>
+      <c r="J453" s="3">
+        <v>4</v>
+      </c>
+      <c r="K453" s="3">
+        <v>8</v>
+      </c>
+      <c r="L453" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="454" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A454" s="3">
+        <v>453</v>
+      </c>
+      <c r="B454" s="3">
+        <v>52</v>
+      </c>
+      <c r="C454" s="2">
+        <v>43136</v>
+      </c>
+      <c r="D454">
+        <v>8</v>
+      </c>
+      <c r="E454" t="s">
+        <v>119</v>
+      </c>
+      <c r="F454">
+        <v>2018</v>
+      </c>
+      <c r="G454" t="s">
+        <v>18</v>
+      </c>
+      <c r="H454" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I454" s="1">
+        <v>101</v>
+      </c>
+      <c r="J454" s="3">
+        <v>4</v>
+      </c>
+      <c r="K454" s="3">
+        <v>5</v>
+      </c>
+      <c r="L454" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="455" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A455" s="3">
+        <v>454</v>
+      </c>
+      <c r="B455" s="3">
+        <v>52</v>
+      </c>
+      <c r="C455" s="2">
+        <v>43136</v>
+      </c>
+      <c r="D455">
+        <v>8</v>
+      </c>
+      <c r="E455" t="s">
+        <v>119</v>
+      </c>
+      <c r="F455">
+        <v>2018</v>
+      </c>
+      <c r="G455" t="s">
+        <v>18</v>
+      </c>
+      <c r="H455" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="I455" s="1">
+        <v>0</v>
+      </c>
+      <c r="J455" s="3">
+        <v>1</v>
+      </c>
+      <c r="K455" s="3">
+        <v>45</v>
+      </c>
+      <c r="L455" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="456" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A456" s="3">
+        <v>455</v>
+      </c>
+      <c r="B456" s="3">
+        <v>53</v>
+      </c>
+      <c r="C456" s="2">
+        <v>43137</v>
+      </c>
+      <c r="D456">
+        <v>8</v>
+      </c>
+      <c r="E456" t="s">
+        <v>119</v>
+      </c>
+      <c r="F456">
+        <v>2018</v>
+      </c>
+      <c r="G456" t="s">
+        <v>74</v>
+      </c>
+      <c r="H456" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="I456" s="1">
+        <v>0</v>
+      </c>
+      <c r="J456" s="3">
+        <v>2</v>
+      </c>
+      <c r="K456" s="3">
+        <v>30</v>
+      </c>
+      <c r="L456" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="457" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A457" s="3">
+        <v>456</v>
+      </c>
+      <c r="B457" s="3">
+        <v>53</v>
+      </c>
+      <c r="C457" s="2">
+        <v>43137</v>
+      </c>
+      <c r="D457">
+        <v>8</v>
+      </c>
+      <c r="E457" t="s">
+        <v>119</v>
+      </c>
+      <c r="F457">
+        <v>2018</v>
+      </c>
+      <c r="G457" t="s">
+        <v>74</v>
+      </c>
+      <c r="H457" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="I457" s="1">
+        <v>0</v>
+      </c>
+      <c r="J457" s="3">
+        <v>2</v>
+      </c>
+      <c r="K457" s="3">
+        <v>10</v>
+      </c>
+      <c r="L457" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="458" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A458" s="3">
+        <v>457</v>
+      </c>
+      <c r="B458" s="3">
+        <v>53</v>
+      </c>
+      <c r="C458" s="2">
+        <v>43137</v>
+      </c>
+      <c r="D458">
+        <v>8</v>
+      </c>
+      <c r="E458" t="s">
+        <v>119</v>
+      </c>
+      <c r="F458">
+        <v>2018</v>
+      </c>
+      <c r="G458" t="s">
+        <v>74</v>
+      </c>
+      <c r="H458" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="I458" s="1">
+        <v>120</v>
+      </c>
+      <c r="J458" s="3">
+        <v>4</v>
+      </c>
+      <c r="K458" s="3">
+        <v>4</v>
+      </c>
+      <c r="L458" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="459" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A459" s="3">
+        <v>458</v>
+      </c>
+      <c r="B459" s="3">
+        <v>53</v>
+      </c>
+      <c r="C459" s="2">
+        <v>43137</v>
+      </c>
+      <c r="D459">
+        <v>8</v>
+      </c>
+      <c r="E459" t="s">
+        <v>119</v>
+      </c>
+      <c r="F459">
+        <v>2018</v>
+      </c>
+      <c r="G459" t="s">
+        <v>74</v>
+      </c>
+      <c r="H459" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="I459" s="1">
+        <v>125</v>
+      </c>
+      <c r="J459" s="3">
+        <v>3</v>
+      </c>
+      <c r="K459" s="3">
+        <v>3</v>
+      </c>
+      <c r="L459" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="460" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A460" s="3">
+        <v>459</v>
+      </c>
+      <c r="B460" s="3">
+        <v>53</v>
+      </c>
+      <c r="C460" s="2">
+        <v>43137</v>
+      </c>
+      <c r="D460">
+        <v>8</v>
+      </c>
+      <c r="E460" t="s">
+        <v>119</v>
+      </c>
+      <c r="F460">
+        <v>2018</v>
+      </c>
+      <c r="G460" t="s">
+        <v>74</v>
+      </c>
+      <c r="H460" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="I460" s="1">
+        <v>130</v>
+      </c>
+      <c r="J460" s="3">
+        <v>2</v>
+      </c>
+      <c r="K460" s="3">
+        <v>3</v>
+      </c>
+      <c r="L460" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="461" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A461" s="3">
+        <v>460</v>
+      </c>
+      <c r="B461" s="3">
+        <v>53</v>
+      </c>
+      <c r="C461" s="2">
+        <v>43137</v>
+      </c>
+      <c r="D461">
+        <v>8</v>
+      </c>
+      <c r="E461" t="s">
+        <v>119</v>
+      </c>
+      <c r="F461">
+        <v>2018</v>
+      </c>
+      <c r="G461" t="s">
+        <v>74</v>
+      </c>
+      <c r="H461" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="I461" s="1">
+        <v>24</v>
+      </c>
+      <c r="J461" s="3">
+        <v>3</v>
+      </c>
+      <c r="K461" s="3">
+        <v>12</v>
+      </c>
+      <c r="L461" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="462" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A462" s="3">
+        <v>461</v>
+      </c>
+      <c r="B462" s="3">
+        <v>53</v>
+      </c>
+      <c r="C462" s="2">
+        <v>43137</v>
+      </c>
+      <c r="D462">
+        <v>8</v>
+      </c>
+      <c r="E462" t="s">
+        <v>119</v>
+      </c>
+      <c r="F462">
+        <v>2018</v>
+      </c>
+      <c r="G462" t="s">
+        <v>74</v>
+      </c>
+      <c r="H462" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="I462" s="1">
+        <v>25</v>
+      </c>
+      <c r="J462" s="3">
+        <v>3</v>
+      </c>
+      <c r="K462" s="3">
+        <v>12</v>
+      </c>
+      <c r="L462" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="463" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A463" s="3">
+        <v>462</v>
+      </c>
+      <c r="B463" s="3">
+        <v>54</v>
+      </c>
+      <c r="C463" s="2">
+        <v>43139</v>
+      </c>
+      <c r="D463">
+        <v>8</v>
+      </c>
+      <c r="E463" t="s">
+        <v>119</v>
+      </c>
+      <c r="F463">
+        <v>2018</v>
+      </c>
+      <c r="G463" t="s">
+        <v>17</v>
+      </c>
+      <c r="H463" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I463" s="1">
+        <v>90</v>
+      </c>
+      <c r="J463" s="3">
+        <v>5</v>
+      </c>
+      <c r="K463" s="3">
+        <v>5</v>
+      </c>
+      <c r="L463" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="464" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A464" s="3">
+        <v>463</v>
+      </c>
+      <c r="B464" s="3">
+        <v>54</v>
+      </c>
+      <c r="C464" s="2">
+        <v>43139</v>
+      </c>
+      <c r="D464">
+        <v>8</v>
+      </c>
+      <c r="E464" t="s">
+        <v>119</v>
+      </c>
+      <c r="F464">
+        <v>2018</v>
+      </c>
+      <c r="G464" t="s">
+        <v>17</v>
+      </c>
+      <c r="H464" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I464" s="1">
+        <v>85</v>
+      </c>
+      <c r="J464" s="3">
+        <v>5</v>
+      </c>
+      <c r="K464" s="3">
+        <v>5</v>
+      </c>
+      <c r="L464" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="465" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A465" s="3">
+        <v>464</v>
+      </c>
+      <c r="B465" s="3">
+        <v>54</v>
+      </c>
+      <c r="C465" s="2">
+        <v>43139</v>
+      </c>
+      <c r="D465">
+        <v>8</v>
+      </c>
+      <c r="E465" t="s">
+        <v>119</v>
+      </c>
+      <c r="F465">
+        <v>2018</v>
+      </c>
+      <c r="G465" t="s">
+        <v>17</v>
+      </c>
+      <c r="H465" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I465" s="1">
+        <v>75</v>
+      </c>
+      <c r="J465" s="3">
+        <v>5</v>
+      </c>
+      <c r="K465" s="3">
+        <v>5</v>
+      </c>
+      <c r="L465" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="466" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A466" s="3">
+        <v>465</v>
+      </c>
+      <c r="B466" s="3">
+        <v>54</v>
+      </c>
+      <c r="C466" s="2">
+        <v>43139</v>
+      </c>
+      <c r="D466">
+        <v>8</v>
+      </c>
+      <c r="E466" t="s">
+        <v>119</v>
+      </c>
+      <c r="F466">
+        <v>2018</v>
+      </c>
+      <c r="G466" t="s">
+        <v>17</v>
+      </c>
+      <c r="H466" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I466" s="1">
+        <v>65</v>
+      </c>
+      <c r="J466" s="3">
+        <v>5</v>
+      </c>
+      <c r="K466" s="3">
+        <v>5</v>
+      </c>
+      <c r="L466" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="467" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A467" s="3">
+        <v>466</v>
+      </c>
+      <c r="B467" s="3">
+        <v>54</v>
+      </c>
+      <c r="C467" s="2">
+        <v>43139</v>
+      </c>
+      <c r="D467">
+        <v>8</v>
+      </c>
+      <c r="E467" t="s">
+        <v>119</v>
+      </c>
+      <c r="F467">
+        <v>2018</v>
+      </c>
+      <c r="G467" t="s">
+        <v>17</v>
+      </c>
+      <c r="H467" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="I467" s="1">
+        <v>5</v>
+      </c>
+      <c r="J467" s="3">
+        <v>3</v>
+      </c>
+      <c r="K467" s="3">
+        <v>20</v>
+      </c>
+      <c r="L467" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="468" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A468" s="3">
+        <v>467</v>
+      </c>
+      <c r="B468" s="3">
+        <v>54</v>
+      </c>
+      <c r="C468" s="2">
+        <v>43139</v>
+      </c>
+      <c r="D468">
+        <v>8</v>
+      </c>
+      <c r="E468" t="s">
+        <v>119</v>
+      </c>
+      <c r="F468">
+        <v>2018</v>
+      </c>
+      <c r="G468" t="s">
+        <v>17</v>
+      </c>
+      <c r="H468" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="I468" s="1">
+        <v>0</v>
+      </c>
+      <c r="J468" s="3">
+        <v>3</v>
+      </c>
+      <c r="K468" s="3">
+        <v>20</v>
+      </c>
+      <c r="L468" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="469" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A469" s="3">
+        <v>468</v>
+      </c>
+      <c r="B469" s="3">
+        <v>54</v>
+      </c>
+      <c r="C469" s="2">
+        <v>43139</v>
+      </c>
+      <c r="D469">
+        <v>8</v>
+      </c>
+      <c r="E469" t="s">
+        <v>119</v>
+      </c>
+      <c r="F469">
+        <v>2018</v>
+      </c>
+      <c r="G469" t="s">
+        <v>17</v>
+      </c>
+      <c r="H469" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="I469" s="1">
+        <v>8</v>
+      </c>
+      <c r="J469" s="3">
+        <v>3</v>
+      </c>
+      <c r="K469" s="3">
+        <v>20</v>
+      </c>
+      <c r="L469" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="470" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A470" s="3">
+        <v>469</v>
+      </c>
+      <c r="B470" s="3">
+        <v>55</v>
+      </c>
+      <c r="C470" s="2">
+        <v>43140</v>
+      </c>
+      <c r="D470">
+        <v>8</v>
+      </c>
+      <c r="E470" t="s">
+        <v>119</v>
+      </c>
+      <c r="F470">
+        <v>2018</v>
+      </c>
+      <c r="G470" t="s">
+        <v>50</v>
+      </c>
+      <c r="H470" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="I470" s="1">
+        <v>0</v>
+      </c>
+      <c r="J470" s="3">
+        <v>3</v>
+      </c>
+      <c r="K470" s="3">
+        <v>30</v>
+      </c>
+      <c r="L470" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="471" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A471" s="3">
+        <v>470</v>
+      </c>
+      <c r="B471" s="3">
+        <v>55</v>
+      </c>
+      <c r="C471" s="2">
+        <v>43140</v>
+      </c>
+      <c r="D471">
+        <v>8</v>
+      </c>
+      <c r="E471" t="s">
+        <v>119</v>
+      </c>
+      <c r="F471">
+        <v>2018</v>
+      </c>
+      <c r="G471" t="s">
+        <v>50</v>
+      </c>
+      <c r="H471" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="I471" s="1">
+        <v>20</v>
+      </c>
+      <c r="J471" s="3">
+        <v>3</v>
+      </c>
+      <c r="K471" s="3">
+        <v>12</v>
+      </c>
+      <c r="L471" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="472" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A472" s="3">
+        <v>471</v>
+      </c>
+      <c r="B472" s="3">
+        <v>55</v>
+      </c>
+      <c r="C472" s="2">
+        <v>43140</v>
+      </c>
+      <c r="D472">
+        <v>8</v>
+      </c>
+      <c r="E472" t="s">
+        <v>119</v>
+      </c>
+      <c r="F472">
+        <v>2018</v>
+      </c>
+      <c r="G472" t="s">
+        <v>50</v>
+      </c>
+      <c r="H472" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="I472" s="1">
+        <v>60</v>
+      </c>
+      <c r="J472" s="3">
+        <v>3</v>
+      </c>
+      <c r="K472" s="3">
+        <v>8</v>
+      </c>
+      <c r="L472" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="473" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A473" s="3">
+        <v>472</v>
+      </c>
+      <c r="B473" s="3">
+        <v>55</v>
+      </c>
+      <c r="C473" s="2">
+        <v>43140</v>
+      </c>
+      <c r="D473">
+        <v>8</v>
+      </c>
+      <c r="E473" t="s">
+        <v>119</v>
+      </c>
+      <c r="F473">
+        <v>2018</v>
+      </c>
+      <c r="G473" t="s">
+        <v>50</v>
+      </c>
+      <c r="H473" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="I473" s="1">
+        <v>70</v>
+      </c>
+      <c r="J473" s="3">
+        <v>3</v>
+      </c>
+      <c r="K473" s="3">
+        <v>5</v>
+      </c>
+      <c r="L473" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="474" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A474" s="3">
+        <v>473</v>
+      </c>
+      <c r="B474" s="3">
+        <v>55</v>
+      </c>
+      <c r="C474" s="2">
+        <v>43140</v>
+      </c>
+      <c r="D474">
+        <v>8</v>
+      </c>
+      <c r="E474" t="s">
+        <v>119</v>
+      </c>
+      <c r="F474">
+        <v>2018</v>
+      </c>
+      <c r="G474" t="s">
+        <v>50</v>
+      </c>
+      <c r="H474" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="I474" s="1">
+        <v>80</v>
+      </c>
+      <c r="J474" s="3">
+        <v>2</v>
+      </c>
+      <c r="K474" s="3">
+        <v>3</v>
+      </c>
+      <c r="L474" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="475" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A475" s="3">
+        <v>474</v>
+      </c>
+      <c r="B475" s="3">
+        <v>55</v>
+      </c>
+      <c r="C475" s="2">
+        <v>43140</v>
+      </c>
+      <c r="D475">
+        <v>8</v>
+      </c>
+      <c r="E475" t="s">
+        <v>119</v>
+      </c>
+      <c r="F475">
+        <v>2018</v>
+      </c>
+      <c r="G475" t="s">
+        <v>50</v>
+      </c>
+      <c r="H475" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="I475" s="1">
+        <v>30</v>
+      </c>
+      <c r="J475" s="3">
+        <v>3</v>
+      </c>
+      <c r="K475" s="3">
+        <v>12</v>
+      </c>
+      <c r="L475" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="476" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A476" s="3">
+        <v>475</v>
+      </c>
+      <c r="B476" s="3">
+        <v>55</v>
+      </c>
+      <c r="C476" s="2">
+        <v>43140</v>
+      </c>
+      <c r="D476">
+        <v>8</v>
+      </c>
+      <c r="E476" t="s">
+        <v>119</v>
+      </c>
+      <c r="F476">
+        <v>2018</v>
+      </c>
+      <c r="G476" t="s">
+        <v>50</v>
+      </c>
+      <c r="H476" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I476" s="1">
+        <v>0</v>
+      </c>
+      <c r="J476" s="3">
+        <v>4</v>
+      </c>
+      <c r="K476" s="3">
+        <v>8</v>
+      </c>
+      <c r="L476" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="477" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A477" s="3">
+        <v>476</v>
+      </c>
+      <c r="B477" s="3">
+        <v>55</v>
+      </c>
+      <c r="C477" s="2">
+        <v>43140</v>
+      </c>
+      <c r="D477">
+        <v>8</v>
+      </c>
+      <c r="E477" t="s">
+        <v>119</v>
+      </c>
+      <c r="F477">
+        <v>2018</v>
+      </c>
+      <c r="G477" t="s">
+        <v>50</v>
+      </c>
+      <c r="H477" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I477" s="1">
+        <v>0</v>
+      </c>
+      <c r="J477" s="3">
+        <v>4</v>
+      </c>
+      <c r="K477" s="3">
+        <v>12</v>
+      </c>
+      <c r="L477" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="478" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A478" s="3">
+        <v>477</v>
+      </c>
+      <c r="B478" s="3">
+        <v>55</v>
+      </c>
+      <c r="C478" s="2">
+        <v>43140</v>
+      </c>
+      <c r="D478">
+        <v>8</v>
+      </c>
+      <c r="E478" t="s">
+        <v>119</v>
+      </c>
+      <c r="F478">
+        <v>2018</v>
+      </c>
+      <c r="G478" t="s">
+        <v>50</v>
+      </c>
+      <c r="H478" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I478" s="1">
+        <v>0</v>
+      </c>
+      <c r="J478" s="3">
+        <v>4</v>
+      </c>
+      <c r="K478" s="3">
+        <v>12</v>
+      </c>
+      <c r="L478" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="479" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A479" s="3">
+        <v>478</v>
+      </c>
+      <c r="B479" s="3">
+        <v>56</v>
+      </c>
+      <c r="C479" s="2">
+        <v>43142</v>
+      </c>
+      <c r="D479">
+        <v>8</v>
+      </c>
+      <c r="E479" t="s">
+        <v>119</v>
+      </c>
+      <c r="F479">
+        <v>2018</v>
+      </c>
+      <c r="G479" t="s">
+        <v>45</v>
+      </c>
+      <c r="H479" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I479" s="1">
+        <v>80</v>
+      </c>
+      <c r="J479" s="3">
+        <v>4</v>
+      </c>
+      <c r="K479" s="3">
+        <v>10</v>
+      </c>
+      <c r="L479" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="480" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A480" s="3">
+        <v>479</v>
+      </c>
+      <c r="B480" s="3">
+        <v>56</v>
+      </c>
+      <c r="C480" s="2">
+        <v>43142</v>
+      </c>
+      <c r="D480">
+        <v>8</v>
+      </c>
+      <c r="E480" t="s">
+        <v>119</v>
+      </c>
+      <c r="F480">
+        <v>2018</v>
+      </c>
+      <c r="G480" t="s">
+        <v>45</v>
+      </c>
+      <c r="H480" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I480" s="1">
+        <v>40</v>
+      </c>
+      <c r="J480" s="3">
+        <v>4</v>
+      </c>
+      <c r="K480" s="3">
+        <v>8</v>
+      </c>
+      <c r="L480" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="481" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A481" s="3">
+        <v>480</v>
+      </c>
+      <c r="B481" s="3">
+        <v>56</v>
+      </c>
+      <c r="C481" s="2">
+        <v>43142</v>
+      </c>
+      <c r="D481">
+        <v>8</v>
+      </c>
+      <c r="E481" t="s">
+        <v>119</v>
+      </c>
+      <c r="F481">
+        <v>2018</v>
+      </c>
+      <c r="G481" t="s">
+        <v>45</v>
+      </c>
+      <c r="H481" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I481" s="1">
+        <v>30</v>
+      </c>
+      <c r="J481" s="3">
+        <v>4</v>
+      </c>
+      <c r="K481" s="3">
+        <v>8</v>
+      </c>
+      <c r="L481" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="482" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A482" s="3">
+        <v>481</v>
+      </c>
+      <c r="B482" s="3">
+        <v>56</v>
+      </c>
+      <c r="C482" s="2">
+        <v>43142</v>
+      </c>
+      <c r="D482">
+        <v>8</v>
+      </c>
+      <c r="E482" t="s">
+        <v>119</v>
+      </c>
+      <c r="F482">
+        <v>2018</v>
+      </c>
+      <c r="G482" t="s">
+        <v>45</v>
+      </c>
+      <c r="H482" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I482" s="1">
+        <v>35</v>
+      </c>
+      <c r="J482" s="3">
+        <v>4</v>
+      </c>
+      <c r="K482" s="3">
+        <v>8</v>
+      </c>
+      <c r="L482" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="483" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A483" s="3">
+        <v>482</v>
+      </c>
+      <c r="B483" s="3">
+        <v>56</v>
+      </c>
+      <c r="C483" s="2">
+        <v>43142</v>
+      </c>
+      <c r="D483">
+        <v>8</v>
+      </c>
+      <c r="E483" t="s">
+        <v>119</v>
+      </c>
+      <c r="F483">
+        <v>2018</v>
+      </c>
+      <c r="G483" t="s">
+        <v>45</v>
+      </c>
+      <c r="H483" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I483" s="1">
+        <v>17.5</v>
+      </c>
+      <c r="J483" s="3">
+        <v>4</v>
+      </c>
+      <c r="K483" s="3">
+        <v>8</v>
+      </c>
+      <c r="L483" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="484" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A484" s="3">
+        <v>483</v>
+      </c>
+      <c r="B484" s="3">
+        <v>56</v>
+      </c>
+      <c r="C484" s="2">
+        <v>43142</v>
+      </c>
+      <c r="D484">
+        <v>8</v>
+      </c>
+      <c r="E484" t="s">
+        <v>119</v>
+      </c>
+      <c r="F484">
+        <v>2018</v>
+      </c>
+      <c r="G484" t="s">
+        <v>45</v>
+      </c>
+      <c r="H484" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I484" s="1">
+        <v>30</v>
+      </c>
+      <c r="J484" s="3">
+        <v>4</v>
+      </c>
+      <c r="K484" s="3">
+        <v>8</v>
+      </c>
+      <c r="L484" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="485" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A485" s="3">
+        <v>484</v>
+      </c>
+      <c r="B485" s="3">
+        <v>56</v>
+      </c>
+      <c r="C485" s="2">
+        <v>43142</v>
+      </c>
+      <c r="D485">
+        <v>8</v>
+      </c>
+      <c r="E485" t="s">
+        <v>119</v>
+      </c>
+      <c r="F485">
+        <v>2018</v>
+      </c>
+      <c r="G485" t="s">
+        <v>45</v>
+      </c>
+      <c r="H485" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I485" s="1">
+        <v>25</v>
+      </c>
+      <c r="J485" s="3">
+        <v>4</v>
+      </c>
+      <c r="K485" s="3">
+        <v>8</v>
+      </c>
+      <c r="L485" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="486" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A486" s="3">
+        <v>485</v>
+      </c>
+      <c r="B486" s="3">
+        <v>56</v>
+      </c>
+      <c r="C486" s="2">
+        <v>43142</v>
+      </c>
+      <c r="D486">
+        <v>8</v>
+      </c>
+      <c r="E486" t="s">
+        <v>119</v>
+      </c>
+      <c r="F486">
+        <v>2018</v>
+      </c>
+      <c r="G486" t="s">
+        <v>45</v>
+      </c>
+      <c r="H486" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I486" s="1">
+        <v>25</v>
+      </c>
+      <c r="J486" s="3">
+        <v>4</v>
+      </c>
+      <c r="K486" s="3">
+        <v>8</v>
+      </c>
+      <c r="L486" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="487" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A487" s="3">
+        <v>486</v>
+      </c>
+      <c r="B487" s="3">
+        <v>56</v>
+      </c>
+      <c r="C487" s="2">
+        <v>43142</v>
+      </c>
+      <c r="D487">
+        <v>8</v>
+      </c>
+      <c r="E487" t="s">
+        <v>119</v>
+      </c>
+      <c r="F487">
+        <v>2018</v>
+      </c>
+      <c r="G487" t="s">
+        <v>45</v>
+      </c>
+      <c r="H487" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I487" s="1">
+        <v>0</v>
+      </c>
+      <c r="J487" s="3">
+        <v>3</v>
+      </c>
+      <c r="K487" s="3">
+        <v>10</v>
+      </c>
+      <c r="L487" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="488" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A488" s="3">
+        <v>487</v>
+      </c>
+      <c r="B488" s="3">
+        <v>56</v>
+      </c>
+      <c r="C488" s="2">
+        <v>43142</v>
+      </c>
+      <c r="D488">
+        <v>8</v>
+      </c>
+      <c r="E488" t="s">
+        <v>119</v>
+      </c>
+      <c r="F488">
+        <v>2018</v>
+      </c>
+      <c r="G488" t="s">
+        <v>45</v>
+      </c>
+      <c r="H488" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="I488" s="1">
+        <v>0</v>
+      </c>
+      <c r="J488" s="3">
+        <v>3</v>
+      </c>
+      <c r="K488" s="3">
+        <v>10</v>
+      </c>
+      <c r="L488" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="489" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A489" s="3">
+        <v>488</v>
+      </c>
+      <c r="B489" s="3">
+        <v>56</v>
+      </c>
+      <c r="C489" s="2">
+        <v>43142</v>
+      </c>
+      <c r="D489">
+        <v>8</v>
+      </c>
+      <c r="E489" t="s">
+        <v>119</v>
+      </c>
+      <c r="F489">
+        <v>2018</v>
+      </c>
+      <c r="G489" t="s">
+        <v>45</v>
+      </c>
+      <c r="H489" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="I489" s="1">
+        <v>0</v>
+      </c>
+      <c r="J489" s="3">
+        <v>3</v>
+      </c>
+      <c r="K489" s="3">
+        <v>12</v>
+      </c>
+      <c r="L489" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="490" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A490" s="3">
+        <v>489</v>
+      </c>
+      <c r="B490" s="3">
+        <v>56</v>
+      </c>
+      <c r="C490" s="2">
+        <v>43142</v>
+      </c>
+      <c r="D490">
+        <v>8</v>
+      </c>
+      <c r="E490" t="s">
+        <v>119</v>
+      </c>
+      <c r="F490">
+        <v>2018</v>
+      </c>
+      <c r="G490" t="s">
+        <v>45</v>
+      </c>
+      <c r="H490" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="I490" s="1">
+        <v>0</v>
+      </c>
+      <c r="J490" s="3">
+        <v>3</v>
+      </c>
+      <c r="K490" s="3">
+        <v>10</v>
+      </c>
+      <c r="L490" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="491" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A491" s="3">
+        <v>490</v>
+      </c>
+      <c r="B491" s="3">
+        <v>56</v>
+      </c>
+      <c r="C491" s="2">
+        <v>43142</v>
+      </c>
+      <c r="D491">
+        <v>8</v>
+      </c>
+      <c r="E491" t="s">
+        <v>119</v>
+      </c>
+      <c r="F491">
+        <v>2018</v>
+      </c>
+      <c r="G491" t="s">
+        <v>45</v>
+      </c>
+      <c r="H491" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="I491" s="1">
+        <v>0</v>
+      </c>
+      <c r="J491" s="3">
+        <v>3</v>
+      </c>
+      <c r="K491" s="3">
+        <v>20</v>
+      </c>
+      <c r="L491" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="492" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A492" s="3">
+        <v>491</v>
+      </c>
+      <c r="B492" s="3">
+        <v>56</v>
+      </c>
+      <c r="C492" s="2">
+        <v>43142</v>
+      </c>
+      <c r="D492">
+        <v>8</v>
+      </c>
+      <c r="E492" t="s">
+        <v>119</v>
+      </c>
+      <c r="F492">
+        <v>2018</v>
+      </c>
+      <c r="G492" t="s">
+        <v>45</v>
+      </c>
+      <c r="H492" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="I492" s="1">
+        <v>0</v>
+      </c>
+      <c r="J492" s="3">
+        <v>3</v>
+      </c>
+      <c r="K492" s="3">
+        <v>10</v>
+      </c>
+      <c r="L492" t="s">
+        <v>89</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updating 25/02/2108 GymWorkouts log
</commit_message>
<xml_diff>
--- a/datasets/GymWorkouts.xlsx
+++ b/datasets/GymWorkouts.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1976" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2200" uniqueCount="128">
   <si>
     <t>Exercise Date</t>
   </si>
@@ -762,11 +762,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L492"/>
+  <dimension ref="A1:L548"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A463" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C489" sqref="C489"/>
+      <pane ySplit="1" topLeftCell="A524" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C550" sqref="C550"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -19481,6 +19481,2134 @@
         <v>89</v>
       </c>
     </row>
+    <row r="493" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A493" s="3">
+        <v>492</v>
+      </c>
+      <c r="B493" s="3">
+        <v>57</v>
+      </c>
+      <c r="C493" s="2">
+        <v>43145</v>
+      </c>
+      <c r="D493">
+        <v>9</v>
+      </c>
+      <c r="E493" t="s">
+        <v>119</v>
+      </c>
+      <c r="F493">
+        <v>2018</v>
+      </c>
+      <c r="G493" t="s">
+        <v>19</v>
+      </c>
+      <c r="H493" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I493" s="1">
+        <v>75</v>
+      </c>
+      <c r="J493" s="3">
+        <v>5</v>
+      </c>
+      <c r="K493" s="3">
+        <v>5</v>
+      </c>
+      <c r="L493" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="494" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A494" s="3">
+        <v>493</v>
+      </c>
+      <c r="B494" s="3">
+        <v>57</v>
+      </c>
+      <c r="C494" s="2">
+        <v>43145</v>
+      </c>
+      <c r="D494">
+        <v>9</v>
+      </c>
+      <c r="E494" t="s">
+        <v>119</v>
+      </c>
+      <c r="F494">
+        <v>2018</v>
+      </c>
+      <c r="G494" t="s">
+        <v>19</v>
+      </c>
+      <c r="H494" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I494" s="1">
+        <v>90</v>
+      </c>
+      <c r="J494" s="3">
+        <v>5</v>
+      </c>
+      <c r="K494" s="3">
+        <v>5</v>
+      </c>
+      <c r="L494" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="495" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A495" s="3">
+        <v>494</v>
+      </c>
+      <c r="B495" s="3">
+        <v>57</v>
+      </c>
+      <c r="C495" s="2">
+        <v>43145</v>
+      </c>
+      <c r="D495">
+        <v>9</v>
+      </c>
+      <c r="E495" t="s">
+        <v>119</v>
+      </c>
+      <c r="F495">
+        <v>2018</v>
+      </c>
+      <c r="G495" t="s">
+        <v>19</v>
+      </c>
+      <c r="H495" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I495" s="1">
+        <v>35</v>
+      </c>
+      <c r="J495" s="3">
+        <v>4</v>
+      </c>
+      <c r="K495" s="3">
+        <v>8</v>
+      </c>
+      <c r="L495" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="496" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A496" s="3">
+        <v>495</v>
+      </c>
+      <c r="B496" s="3">
+        <v>57</v>
+      </c>
+      <c r="C496" s="2">
+        <v>43145</v>
+      </c>
+      <c r="D496">
+        <v>9</v>
+      </c>
+      <c r="E496" t="s">
+        <v>119</v>
+      </c>
+      <c r="F496">
+        <v>2018</v>
+      </c>
+      <c r="G496" t="s">
+        <v>19</v>
+      </c>
+      <c r="H496" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I496" s="1">
+        <v>40</v>
+      </c>
+      <c r="J496" s="3">
+        <v>4</v>
+      </c>
+      <c r="K496" s="3">
+        <v>8</v>
+      </c>
+      <c r="L496" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="497" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A497" s="3">
+        <v>496</v>
+      </c>
+      <c r="B497" s="3">
+        <v>57</v>
+      </c>
+      <c r="C497" s="2">
+        <v>43145</v>
+      </c>
+      <c r="D497">
+        <v>9</v>
+      </c>
+      <c r="E497" t="s">
+        <v>119</v>
+      </c>
+      <c r="F497">
+        <v>2018</v>
+      </c>
+      <c r="G497" t="s">
+        <v>19</v>
+      </c>
+      <c r="H497" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="I497" s="1">
+        <v>10</v>
+      </c>
+      <c r="J497" s="3">
+        <v>3</v>
+      </c>
+      <c r="K497" s="3">
+        <v>20</v>
+      </c>
+      <c r="L497" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="498" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A498" s="3">
+        <v>497</v>
+      </c>
+      <c r="B498" s="3">
+        <v>57</v>
+      </c>
+      <c r="C498" s="2">
+        <v>43145</v>
+      </c>
+      <c r="D498">
+        <v>9</v>
+      </c>
+      <c r="E498" t="s">
+        <v>119</v>
+      </c>
+      <c r="F498">
+        <v>2018</v>
+      </c>
+      <c r="G498" t="s">
+        <v>19</v>
+      </c>
+      <c r="H498" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="I498" s="1">
+        <v>0</v>
+      </c>
+      <c r="J498" s="3">
+        <v>3</v>
+      </c>
+      <c r="K498" s="3">
+        <v>30</v>
+      </c>
+      <c r="L498" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="499" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A499" s="3">
+        <v>498</v>
+      </c>
+      <c r="B499" s="3">
+        <v>57</v>
+      </c>
+      <c r="C499" s="2">
+        <v>43145</v>
+      </c>
+      <c r="D499">
+        <v>9</v>
+      </c>
+      <c r="E499" t="s">
+        <v>119</v>
+      </c>
+      <c r="F499">
+        <v>2018</v>
+      </c>
+      <c r="G499" t="s">
+        <v>19</v>
+      </c>
+      <c r="H499" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="I499" s="1">
+        <v>0</v>
+      </c>
+      <c r="J499" s="3">
+        <v>3</v>
+      </c>
+      <c r="K499" s="3">
+        <v>30</v>
+      </c>
+      <c r="L499" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="500" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A500" s="3">
+        <v>499</v>
+      </c>
+      <c r="B500" s="3">
+        <v>57</v>
+      </c>
+      <c r="C500" s="2">
+        <v>43145</v>
+      </c>
+      <c r="D500">
+        <v>9</v>
+      </c>
+      <c r="E500" t="s">
+        <v>119</v>
+      </c>
+      <c r="F500">
+        <v>2018</v>
+      </c>
+      <c r="G500" t="s">
+        <v>19</v>
+      </c>
+      <c r="H500" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I500" s="1">
+        <v>0</v>
+      </c>
+      <c r="J500" s="3">
+        <v>3</v>
+      </c>
+      <c r="K500" s="3">
+        <v>30</v>
+      </c>
+      <c r="L500" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="501" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A501" s="3">
+        <v>500</v>
+      </c>
+      <c r="B501" s="3">
+        <v>58</v>
+      </c>
+      <c r="C501" s="2">
+        <v>43149</v>
+      </c>
+      <c r="D501">
+        <v>9</v>
+      </c>
+      <c r="E501" t="s">
+        <v>119</v>
+      </c>
+      <c r="F501">
+        <v>2018</v>
+      </c>
+      <c r="G501" t="s">
+        <v>45</v>
+      </c>
+      <c r="H501" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I501" s="1">
+        <v>25</v>
+      </c>
+      <c r="J501" s="3">
+        <v>4</v>
+      </c>
+      <c r="K501" s="3">
+        <v>8</v>
+      </c>
+      <c r="L501" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="502" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A502" s="3">
+        <v>501</v>
+      </c>
+      <c r="B502" s="3">
+        <v>58</v>
+      </c>
+      <c r="C502" s="2">
+        <v>43149</v>
+      </c>
+      <c r="D502">
+        <v>9</v>
+      </c>
+      <c r="E502" t="s">
+        <v>119</v>
+      </c>
+      <c r="F502">
+        <v>2018</v>
+      </c>
+      <c r="G502" t="s">
+        <v>45</v>
+      </c>
+      <c r="H502" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I502" s="1">
+        <v>25</v>
+      </c>
+      <c r="J502" s="3">
+        <v>4</v>
+      </c>
+      <c r="K502" s="3">
+        <v>8</v>
+      </c>
+      <c r="L502" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="503" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A503" s="3">
+        <v>502</v>
+      </c>
+      <c r="B503" s="3">
+        <v>58</v>
+      </c>
+      <c r="C503" s="2">
+        <v>43149</v>
+      </c>
+      <c r="D503">
+        <v>9</v>
+      </c>
+      <c r="E503" t="s">
+        <v>119</v>
+      </c>
+      <c r="F503">
+        <v>2018</v>
+      </c>
+      <c r="G503" t="s">
+        <v>45</v>
+      </c>
+      <c r="H503" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I503" s="1">
+        <v>97</v>
+      </c>
+      <c r="J503" s="3">
+        <v>4</v>
+      </c>
+      <c r="K503" s="3">
+        <v>8</v>
+      </c>
+      <c r="L503" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="504" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A504" s="3">
+        <v>503</v>
+      </c>
+      <c r="B504" s="3">
+        <v>58</v>
+      </c>
+      <c r="C504" s="2">
+        <v>43149</v>
+      </c>
+      <c r="D504">
+        <v>9</v>
+      </c>
+      <c r="E504" t="s">
+        <v>119</v>
+      </c>
+      <c r="F504">
+        <v>2018</v>
+      </c>
+      <c r="G504" t="s">
+        <v>45</v>
+      </c>
+      <c r="H504" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I504" s="1">
+        <v>102</v>
+      </c>
+      <c r="J504" s="3">
+        <v>4</v>
+      </c>
+      <c r="K504" s="3">
+        <v>8</v>
+      </c>
+      <c r="L504" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="505" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A505" s="3">
+        <v>504</v>
+      </c>
+      <c r="B505" s="3">
+        <v>58</v>
+      </c>
+      <c r="C505" s="2">
+        <v>43149</v>
+      </c>
+      <c r="D505">
+        <v>9</v>
+      </c>
+      <c r="E505" t="s">
+        <v>119</v>
+      </c>
+      <c r="F505">
+        <v>2018</v>
+      </c>
+      <c r="G505" t="s">
+        <v>45</v>
+      </c>
+      <c r="H505" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="I505" s="1">
+        <v>30</v>
+      </c>
+      <c r="J505" s="3">
+        <v>3</v>
+      </c>
+      <c r="K505" s="3">
+        <v>20</v>
+      </c>
+      <c r="L505" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="506" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A506" s="3">
+        <v>505</v>
+      </c>
+      <c r="B506" s="3">
+        <v>58</v>
+      </c>
+      <c r="C506" s="2">
+        <v>43149</v>
+      </c>
+      <c r="D506">
+        <v>9</v>
+      </c>
+      <c r="E506" t="s">
+        <v>119</v>
+      </c>
+      <c r="F506">
+        <v>2018</v>
+      </c>
+      <c r="G506" t="s">
+        <v>45</v>
+      </c>
+      <c r="H506" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I506" s="1">
+        <v>0</v>
+      </c>
+      <c r="J506" s="3">
+        <v>3</v>
+      </c>
+      <c r="K506" s="3">
+        <v>10</v>
+      </c>
+      <c r="L506" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="507" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A507" s="3">
+        <v>506</v>
+      </c>
+      <c r="B507" s="3">
+        <v>58</v>
+      </c>
+      <c r="C507" s="2">
+        <v>43149</v>
+      </c>
+      <c r="D507">
+        <v>9</v>
+      </c>
+      <c r="E507" t="s">
+        <v>119</v>
+      </c>
+      <c r="F507">
+        <v>2018</v>
+      </c>
+      <c r="G507" t="s">
+        <v>45</v>
+      </c>
+      <c r="H507" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="I507" s="1">
+        <v>0</v>
+      </c>
+      <c r="J507" s="3">
+        <v>3</v>
+      </c>
+      <c r="K507" s="3">
+        <v>10</v>
+      </c>
+      <c r="L507" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="508" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A508" s="3">
+        <v>507</v>
+      </c>
+      <c r="B508" s="3">
+        <v>58</v>
+      </c>
+      <c r="C508" s="2">
+        <v>43149</v>
+      </c>
+      <c r="D508">
+        <v>9</v>
+      </c>
+      <c r="E508" t="s">
+        <v>119</v>
+      </c>
+      <c r="F508">
+        <v>2018</v>
+      </c>
+      <c r="G508" t="s">
+        <v>45</v>
+      </c>
+      <c r="H508" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="I508" s="1">
+        <v>0</v>
+      </c>
+      <c r="J508" s="3">
+        <v>3</v>
+      </c>
+      <c r="K508" s="3">
+        <v>12</v>
+      </c>
+      <c r="L508" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="509" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A509" s="3">
+        <v>508</v>
+      </c>
+      <c r="B509" s="3">
+        <v>58</v>
+      </c>
+      <c r="C509" s="2">
+        <v>43149</v>
+      </c>
+      <c r="D509">
+        <v>9</v>
+      </c>
+      <c r="E509" t="s">
+        <v>119</v>
+      </c>
+      <c r="F509">
+        <v>2018</v>
+      </c>
+      <c r="G509" t="s">
+        <v>45</v>
+      </c>
+      <c r="H509" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="I509" s="1">
+        <v>0</v>
+      </c>
+      <c r="J509" s="3">
+        <v>3</v>
+      </c>
+      <c r="K509" s="3">
+        <v>10</v>
+      </c>
+      <c r="L509" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="510" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A510" s="3">
+        <v>509</v>
+      </c>
+      <c r="B510" s="3">
+        <v>58</v>
+      </c>
+      <c r="C510" s="2">
+        <v>43149</v>
+      </c>
+      <c r="D510">
+        <v>9</v>
+      </c>
+      <c r="E510" t="s">
+        <v>119</v>
+      </c>
+      <c r="F510">
+        <v>2018</v>
+      </c>
+      <c r="G510" t="s">
+        <v>45</v>
+      </c>
+      <c r="H510" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="I510" s="1">
+        <v>0</v>
+      </c>
+      <c r="J510" s="3">
+        <v>3</v>
+      </c>
+      <c r="K510" s="3">
+        <v>20</v>
+      </c>
+      <c r="L510" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="511" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A511" s="3">
+        <v>510</v>
+      </c>
+      <c r="B511" s="3">
+        <v>59</v>
+      </c>
+      <c r="C511" s="2">
+        <v>43150</v>
+      </c>
+      <c r="D511">
+        <v>10</v>
+      </c>
+      <c r="E511" t="s">
+        <v>119</v>
+      </c>
+      <c r="F511">
+        <v>2018</v>
+      </c>
+      <c r="G511" t="s">
+        <v>18</v>
+      </c>
+      <c r="H511" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I511" s="1">
+        <v>75</v>
+      </c>
+      <c r="J511" s="3">
+        <v>4</v>
+      </c>
+      <c r="K511" s="3">
+        <v>8</v>
+      </c>
+      <c r="L511" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="512" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A512" s="3">
+        <v>511</v>
+      </c>
+      <c r="B512" s="3">
+        <v>59</v>
+      </c>
+      <c r="C512" s="2">
+        <v>43150</v>
+      </c>
+      <c r="D512">
+        <v>10</v>
+      </c>
+      <c r="E512" t="s">
+        <v>119</v>
+      </c>
+      <c r="F512">
+        <v>2018</v>
+      </c>
+      <c r="G512" t="s">
+        <v>18</v>
+      </c>
+      <c r="H512" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I512" s="1">
+        <v>80</v>
+      </c>
+      <c r="J512" s="3">
+        <v>4</v>
+      </c>
+      <c r="K512" s="3">
+        <v>8</v>
+      </c>
+      <c r="L512" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="513" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A513" s="3">
+        <v>512</v>
+      </c>
+      <c r="B513" s="3">
+        <v>59</v>
+      </c>
+      <c r="C513" s="2">
+        <v>43150</v>
+      </c>
+      <c r="D513">
+        <v>10</v>
+      </c>
+      <c r="E513" t="s">
+        <v>119</v>
+      </c>
+      <c r="F513">
+        <v>2018</v>
+      </c>
+      <c r="G513" t="s">
+        <v>18</v>
+      </c>
+      <c r="H513" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I513" s="1">
+        <v>45</v>
+      </c>
+      <c r="J513" s="3">
+        <v>4</v>
+      </c>
+      <c r="K513" s="3">
+        <v>8</v>
+      </c>
+      <c r="L513" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="514" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A514" s="3">
+        <v>513</v>
+      </c>
+      <c r="B514" s="3">
+        <v>59</v>
+      </c>
+      <c r="C514" s="2">
+        <v>43150</v>
+      </c>
+      <c r="D514">
+        <v>10</v>
+      </c>
+      <c r="E514" t="s">
+        <v>119</v>
+      </c>
+      <c r="F514">
+        <v>2018</v>
+      </c>
+      <c r="G514" t="s">
+        <v>18</v>
+      </c>
+      <c r="H514" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I514" s="1">
+        <v>0</v>
+      </c>
+      <c r="J514" s="3">
+        <v>3</v>
+      </c>
+      <c r="K514" s="3">
+        <v>10</v>
+      </c>
+      <c r="L514" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="515" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A515" s="3">
+        <v>514</v>
+      </c>
+      <c r="B515" s="3">
+        <v>59</v>
+      </c>
+      <c r="C515" s="2">
+        <v>43150</v>
+      </c>
+      <c r="D515">
+        <v>10</v>
+      </c>
+      <c r="E515" t="s">
+        <v>119</v>
+      </c>
+      <c r="F515">
+        <v>2018</v>
+      </c>
+      <c r="G515" t="s">
+        <v>18</v>
+      </c>
+      <c r="H515" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="I515" s="1">
+        <v>0</v>
+      </c>
+      <c r="J515" s="3">
+        <v>3</v>
+      </c>
+      <c r="K515" s="3">
+        <v>10</v>
+      </c>
+      <c r="L515" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="516" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A516" s="3">
+        <v>515</v>
+      </c>
+      <c r="B516" s="3">
+        <v>59</v>
+      </c>
+      <c r="C516" s="2">
+        <v>43150</v>
+      </c>
+      <c r="D516">
+        <v>10</v>
+      </c>
+      <c r="E516" t="s">
+        <v>119</v>
+      </c>
+      <c r="F516">
+        <v>2018</v>
+      </c>
+      <c r="G516" t="s">
+        <v>18</v>
+      </c>
+      <c r="H516" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="I516" s="1">
+        <v>0</v>
+      </c>
+      <c r="J516" s="3">
+        <v>3</v>
+      </c>
+      <c r="K516" s="3">
+        <v>12</v>
+      </c>
+      <c r="L516" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="517" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A517" s="3">
+        <v>516</v>
+      </c>
+      <c r="B517" s="3">
+        <v>59</v>
+      </c>
+      <c r="C517" s="2">
+        <v>43150</v>
+      </c>
+      <c r="D517">
+        <v>10</v>
+      </c>
+      <c r="E517" t="s">
+        <v>119</v>
+      </c>
+      <c r="F517">
+        <v>2018</v>
+      </c>
+      <c r="G517" t="s">
+        <v>18</v>
+      </c>
+      <c r="H517" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="I517" s="1">
+        <v>0</v>
+      </c>
+      <c r="J517" s="3">
+        <v>3</v>
+      </c>
+      <c r="K517" s="3">
+        <v>10</v>
+      </c>
+      <c r="L517" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="518" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A518" s="3">
+        <v>517</v>
+      </c>
+      <c r="B518" s="3">
+        <v>59</v>
+      </c>
+      <c r="C518" s="2">
+        <v>43150</v>
+      </c>
+      <c r="D518">
+        <v>10</v>
+      </c>
+      <c r="E518" t="s">
+        <v>119</v>
+      </c>
+      <c r="F518">
+        <v>2018</v>
+      </c>
+      <c r="G518" t="s">
+        <v>18</v>
+      </c>
+      <c r="H518" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="I518" s="1">
+        <v>0</v>
+      </c>
+      <c r="J518" s="3">
+        <v>3</v>
+      </c>
+      <c r="K518" s="3">
+        <v>20</v>
+      </c>
+      <c r="L518" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="519" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A519" s="3">
+        <v>518</v>
+      </c>
+      <c r="B519" s="3">
+        <v>60</v>
+      </c>
+      <c r="C519" s="2">
+        <v>43151</v>
+      </c>
+      <c r="D519">
+        <v>10</v>
+      </c>
+      <c r="E519" t="s">
+        <v>119</v>
+      </c>
+      <c r="F519">
+        <v>2018</v>
+      </c>
+      <c r="G519" t="s">
+        <v>74</v>
+      </c>
+      <c r="H519" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="I519" s="1">
+        <v>0</v>
+      </c>
+      <c r="J519" s="3">
+        <v>2</v>
+      </c>
+      <c r="K519" s="3">
+        <v>30</v>
+      </c>
+      <c r="L519" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="520" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A520" s="3">
+        <v>519</v>
+      </c>
+      <c r="B520" s="3">
+        <v>60</v>
+      </c>
+      <c r="C520" s="2">
+        <v>43151</v>
+      </c>
+      <c r="D520">
+        <v>10</v>
+      </c>
+      <c r="E520" t="s">
+        <v>119</v>
+      </c>
+      <c r="F520">
+        <v>2018</v>
+      </c>
+      <c r="G520" t="s">
+        <v>74</v>
+      </c>
+      <c r="H520" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="I520" s="1">
+        <v>0</v>
+      </c>
+      <c r="J520" s="3">
+        <v>2</v>
+      </c>
+      <c r="K520" s="3">
+        <v>10</v>
+      </c>
+      <c r="L520" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="521" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A521" s="3">
+        <v>520</v>
+      </c>
+      <c r="B521" s="3">
+        <v>60</v>
+      </c>
+      <c r="C521" s="2">
+        <v>43151</v>
+      </c>
+      <c r="D521">
+        <v>10</v>
+      </c>
+      <c r="E521" t="s">
+        <v>119</v>
+      </c>
+      <c r="F521">
+        <v>2018</v>
+      </c>
+      <c r="G521" t="s">
+        <v>74</v>
+      </c>
+      <c r="H521" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="I521" s="1">
+        <v>120</v>
+      </c>
+      <c r="J521" s="3">
+        <v>4</v>
+      </c>
+      <c r="K521" s="3">
+        <v>4</v>
+      </c>
+      <c r="L521" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="522" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A522" s="3">
+        <v>521</v>
+      </c>
+      <c r="B522" s="3">
+        <v>60</v>
+      </c>
+      <c r="C522" s="2">
+        <v>43151</v>
+      </c>
+      <c r="D522">
+        <v>10</v>
+      </c>
+      <c r="E522" t="s">
+        <v>119</v>
+      </c>
+      <c r="F522">
+        <v>2018</v>
+      </c>
+      <c r="G522" t="s">
+        <v>74</v>
+      </c>
+      <c r="H522" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="I522" s="1">
+        <v>130</v>
+      </c>
+      <c r="J522" s="3">
+        <v>3</v>
+      </c>
+      <c r="K522" s="3">
+        <v>3</v>
+      </c>
+      <c r="L522" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="523" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A523" s="3">
+        <v>522</v>
+      </c>
+      <c r="B523" s="3">
+        <v>60</v>
+      </c>
+      <c r="C523" s="2">
+        <v>43151</v>
+      </c>
+      <c r="D523">
+        <v>10</v>
+      </c>
+      <c r="E523" t="s">
+        <v>119</v>
+      </c>
+      <c r="F523">
+        <v>2018</v>
+      </c>
+      <c r="G523" t="s">
+        <v>74</v>
+      </c>
+      <c r="H523" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="I523" s="1">
+        <v>140</v>
+      </c>
+      <c r="J523" s="3">
+        <v>2</v>
+      </c>
+      <c r="K523" s="3">
+        <v>2</v>
+      </c>
+      <c r="L523" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="524" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A524" s="3">
+        <v>523</v>
+      </c>
+      <c r="B524" s="3">
+        <v>60</v>
+      </c>
+      <c r="C524" s="2">
+        <v>43151</v>
+      </c>
+      <c r="D524">
+        <v>10</v>
+      </c>
+      <c r="E524" t="s">
+        <v>119</v>
+      </c>
+      <c r="F524">
+        <v>2018</v>
+      </c>
+      <c r="G524" t="s">
+        <v>74</v>
+      </c>
+      <c r="H524" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="I524" s="1">
+        <v>27.5</v>
+      </c>
+      <c r="J524" s="3">
+        <v>3</v>
+      </c>
+      <c r="K524" s="3">
+        <v>12</v>
+      </c>
+      <c r="L524" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="525" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A525" s="3">
+        <v>524</v>
+      </c>
+      <c r="B525" s="3">
+        <v>60</v>
+      </c>
+      <c r="C525" s="2">
+        <v>43151</v>
+      </c>
+      <c r="D525">
+        <v>10</v>
+      </c>
+      <c r="E525" t="s">
+        <v>119</v>
+      </c>
+      <c r="F525">
+        <v>2018</v>
+      </c>
+      <c r="G525" t="s">
+        <v>74</v>
+      </c>
+      <c r="H525" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="I525" s="1">
+        <v>25</v>
+      </c>
+      <c r="J525" s="3">
+        <v>3</v>
+      </c>
+      <c r="K525" s="3">
+        <v>12</v>
+      </c>
+      <c r="L525" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="526" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A526" s="3">
+        <v>525</v>
+      </c>
+      <c r="B526" s="3">
+        <v>60</v>
+      </c>
+      <c r="C526" s="2">
+        <v>43151</v>
+      </c>
+      <c r="D526">
+        <v>10</v>
+      </c>
+      <c r="E526" t="s">
+        <v>119</v>
+      </c>
+      <c r="F526">
+        <v>2018</v>
+      </c>
+      <c r="G526" t="s">
+        <v>74</v>
+      </c>
+      <c r="H526" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="I526" s="1">
+        <v>0</v>
+      </c>
+      <c r="J526" s="3">
+        <v>3</v>
+      </c>
+      <c r="K526" s="3">
+        <v>45</v>
+      </c>
+      <c r="L526" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="527" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A527" s="3">
+        <v>526</v>
+      </c>
+      <c r="B527" s="3">
+        <v>60</v>
+      </c>
+      <c r="C527" s="2">
+        <v>43151</v>
+      </c>
+      <c r="D527">
+        <v>10</v>
+      </c>
+      <c r="E527" t="s">
+        <v>119</v>
+      </c>
+      <c r="F527">
+        <v>2018</v>
+      </c>
+      <c r="G527" t="s">
+        <v>74</v>
+      </c>
+      <c r="H527" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="I527" s="1">
+        <v>0</v>
+      </c>
+      <c r="J527" s="3">
+        <v>3</v>
+      </c>
+      <c r="K527" s="3">
+        <v>30</v>
+      </c>
+      <c r="L527" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="528" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A528" s="3">
+        <v>527</v>
+      </c>
+      <c r="B528" s="3">
+        <v>60</v>
+      </c>
+      <c r="C528" s="2">
+        <v>43151</v>
+      </c>
+      <c r="D528">
+        <v>10</v>
+      </c>
+      <c r="E528" t="s">
+        <v>119</v>
+      </c>
+      <c r="F528">
+        <v>2018</v>
+      </c>
+      <c r="G528" t="s">
+        <v>74</v>
+      </c>
+      <c r="H528" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I528" s="1">
+        <v>0</v>
+      </c>
+      <c r="J528" s="3">
+        <v>3</v>
+      </c>
+      <c r="K528" s="3">
+        <v>30</v>
+      </c>
+      <c r="L528" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="529" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A529" s="3">
+        <v>528</v>
+      </c>
+      <c r="B529" s="3">
+        <v>61</v>
+      </c>
+      <c r="C529" s="2">
+        <v>43153</v>
+      </c>
+      <c r="D529">
+        <v>10</v>
+      </c>
+      <c r="E529" t="s">
+        <v>119</v>
+      </c>
+      <c r="F529">
+        <v>2018</v>
+      </c>
+      <c r="G529" t="s">
+        <v>17</v>
+      </c>
+      <c r="H529" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I529" s="1">
+        <v>85</v>
+      </c>
+      <c r="J529" s="3">
+        <v>4</v>
+      </c>
+      <c r="K529" s="3">
+        <v>8</v>
+      </c>
+      <c r="L529" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="530" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A530" s="3">
+        <v>529</v>
+      </c>
+      <c r="B530" s="3">
+        <v>61</v>
+      </c>
+      <c r="C530" s="2">
+        <v>43153</v>
+      </c>
+      <c r="D530">
+        <v>10</v>
+      </c>
+      <c r="E530" t="s">
+        <v>119</v>
+      </c>
+      <c r="F530">
+        <v>2018</v>
+      </c>
+      <c r="G530" t="s">
+        <v>17</v>
+      </c>
+      <c r="H530" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I530" s="1">
+        <v>25</v>
+      </c>
+      <c r="J530" s="3">
+        <v>4</v>
+      </c>
+      <c r="K530" s="3">
+        <v>8</v>
+      </c>
+      <c r="L530" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="531" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A531" s="3">
+        <v>530</v>
+      </c>
+      <c r="B531" s="3">
+        <v>61</v>
+      </c>
+      <c r="C531" s="2">
+        <v>43153</v>
+      </c>
+      <c r="D531">
+        <v>10</v>
+      </c>
+      <c r="E531" t="s">
+        <v>119</v>
+      </c>
+      <c r="F531">
+        <v>2018</v>
+      </c>
+      <c r="G531" t="s">
+        <v>17</v>
+      </c>
+      <c r="H531" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I531" s="1">
+        <v>25</v>
+      </c>
+      <c r="J531" s="3">
+        <v>4</v>
+      </c>
+      <c r="K531" s="3">
+        <v>8</v>
+      </c>
+      <c r="L531" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="532" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A532" s="3">
+        <v>531</v>
+      </c>
+      <c r="B532" s="3">
+        <v>61</v>
+      </c>
+      <c r="C532" s="2">
+        <v>43153</v>
+      </c>
+      <c r="D532">
+        <v>10</v>
+      </c>
+      <c r="E532" t="s">
+        <v>119</v>
+      </c>
+      <c r="F532">
+        <v>2018</v>
+      </c>
+      <c r="G532" t="s">
+        <v>17</v>
+      </c>
+      <c r="H532" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I532" s="1">
+        <v>40</v>
+      </c>
+      <c r="J532" s="3">
+        <v>4</v>
+      </c>
+      <c r="K532" s="3">
+        <v>8</v>
+      </c>
+      <c r="L532" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="533" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A533" s="3">
+        <v>532</v>
+      </c>
+      <c r="B533" s="3">
+        <v>61</v>
+      </c>
+      <c r="C533" s="2">
+        <v>43153</v>
+      </c>
+      <c r="D533">
+        <v>10</v>
+      </c>
+      <c r="E533" t="s">
+        <v>119</v>
+      </c>
+      <c r="F533">
+        <v>2018</v>
+      </c>
+      <c r="G533" t="s">
+        <v>17</v>
+      </c>
+      <c r="H533" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I533" s="1">
+        <v>35</v>
+      </c>
+      <c r="J533" s="3">
+        <v>4</v>
+      </c>
+      <c r="K533" s="3">
+        <v>8</v>
+      </c>
+      <c r="L533" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="534" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A534" s="3">
+        <v>533</v>
+      </c>
+      <c r="B534" s="3">
+        <v>61</v>
+      </c>
+      <c r="C534" s="2">
+        <v>43153</v>
+      </c>
+      <c r="D534">
+        <v>10</v>
+      </c>
+      <c r="E534" t="s">
+        <v>119</v>
+      </c>
+      <c r="F534">
+        <v>2018</v>
+      </c>
+      <c r="G534" t="s">
+        <v>17</v>
+      </c>
+      <c r="H534" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I534" s="1">
+        <v>95</v>
+      </c>
+      <c r="J534" s="3">
+        <v>4</v>
+      </c>
+      <c r="K534" s="3">
+        <v>8</v>
+      </c>
+      <c r="L534" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="535" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A535" s="3">
+        <v>534</v>
+      </c>
+      <c r="B535" s="3">
+        <v>61</v>
+      </c>
+      <c r="C535" s="2">
+        <v>43153</v>
+      </c>
+      <c r="D535">
+        <v>10</v>
+      </c>
+      <c r="E535" t="s">
+        <v>119</v>
+      </c>
+      <c r="F535">
+        <v>2018</v>
+      </c>
+      <c r="G535" t="s">
+        <v>17</v>
+      </c>
+      <c r="H535" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I535" s="1">
+        <v>97</v>
+      </c>
+      <c r="J535" s="3">
+        <v>4</v>
+      </c>
+      <c r="K535" s="3">
+        <v>8</v>
+      </c>
+      <c r="L535" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="536" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A536" s="3">
+        <v>535</v>
+      </c>
+      <c r="B536" s="3">
+        <v>61</v>
+      </c>
+      <c r="C536" s="2">
+        <v>43153</v>
+      </c>
+      <c r="D536">
+        <v>10</v>
+      </c>
+      <c r="E536" t="s">
+        <v>119</v>
+      </c>
+      <c r="F536">
+        <v>2018</v>
+      </c>
+      <c r="G536" t="s">
+        <v>17</v>
+      </c>
+      <c r="H536" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="I536" s="1">
+        <v>10</v>
+      </c>
+      <c r="J536" s="3">
+        <v>3</v>
+      </c>
+      <c r="K536" s="3">
+        <v>20</v>
+      </c>
+      <c r="L536" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="537" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A537" s="3">
+        <v>536</v>
+      </c>
+      <c r="B537" s="3">
+        <v>61</v>
+      </c>
+      <c r="C537" s="2">
+        <v>43153</v>
+      </c>
+      <c r="D537">
+        <v>10</v>
+      </c>
+      <c r="E537" t="s">
+        <v>119</v>
+      </c>
+      <c r="F537">
+        <v>2018</v>
+      </c>
+      <c r="G537" t="s">
+        <v>17</v>
+      </c>
+      <c r="H537" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="I537" s="1">
+        <v>0</v>
+      </c>
+      <c r="J537" s="3">
+        <v>3</v>
+      </c>
+      <c r="K537" s="3">
+        <v>20</v>
+      </c>
+      <c r="L537" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="538" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A538" s="3">
+        <v>537</v>
+      </c>
+      <c r="B538" s="3">
+        <v>61</v>
+      </c>
+      <c r="C538" s="2">
+        <v>43153</v>
+      </c>
+      <c r="D538">
+        <v>10</v>
+      </c>
+      <c r="E538" t="s">
+        <v>119</v>
+      </c>
+      <c r="F538">
+        <v>2018</v>
+      </c>
+      <c r="G538" t="s">
+        <v>17</v>
+      </c>
+      <c r="H538" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I538" s="1">
+        <v>0</v>
+      </c>
+      <c r="J538" s="3">
+        <v>3</v>
+      </c>
+      <c r="K538" s="3">
+        <v>10</v>
+      </c>
+      <c r="L538" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="539" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A539" s="3">
+        <v>538</v>
+      </c>
+      <c r="B539" s="3">
+        <v>61</v>
+      </c>
+      <c r="C539" s="2">
+        <v>43153</v>
+      </c>
+      <c r="D539">
+        <v>10</v>
+      </c>
+      <c r="E539" t="s">
+        <v>119</v>
+      </c>
+      <c r="F539">
+        <v>2018</v>
+      </c>
+      <c r="G539" t="s">
+        <v>17</v>
+      </c>
+      <c r="H539" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I539" s="1">
+        <v>0</v>
+      </c>
+      <c r="J539" s="3">
+        <v>3</v>
+      </c>
+      <c r="K539" s="3">
+        <v>10</v>
+      </c>
+      <c r="L539" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="540" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A540" s="3">
+        <v>539</v>
+      </c>
+      <c r="B540" s="3">
+        <v>62</v>
+      </c>
+      <c r="C540" s="2">
+        <v>43155</v>
+      </c>
+      <c r="D540">
+        <v>10</v>
+      </c>
+      <c r="E540" t="s">
+        <v>119</v>
+      </c>
+      <c r="F540">
+        <v>2018</v>
+      </c>
+      <c r="G540" t="s">
+        <v>80</v>
+      </c>
+      <c r="H540" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I540" s="1">
+        <v>100</v>
+      </c>
+      <c r="J540" s="3">
+        <v>4</v>
+      </c>
+      <c r="K540" s="3">
+        <v>8</v>
+      </c>
+      <c r="L540" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="541" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A541" s="3">
+        <v>540</v>
+      </c>
+      <c r="B541" s="3">
+        <v>62</v>
+      </c>
+      <c r="C541" s="2">
+        <v>43155</v>
+      </c>
+      <c r="D541">
+        <v>10</v>
+      </c>
+      <c r="E541" t="s">
+        <v>119</v>
+      </c>
+      <c r="F541">
+        <v>2018</v>
+      </c>
+      <c r="G541" t="s">
+        <v>80</v>
+      </c>
+      <c r="H541" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I541" s="1">
+        <v>60</v>
+      </c>
+      <c r="J541" s="3">
+        <v>4</v>
+      </c>
+      <c r="K541" s="3">
+        <v>8</v>
+      </c>
+      <c r="L541" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="542" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A542" s="3">
+        <v>541</v>
+      </c>
+      <c r="B542" s="3">
+        <v>62</v>
+      </c>
+      <c r="C542" s="2">
+        <v>43155</v>
+      </c>
+      <c r="D542">
+        <v>10</v>
+      </c>
+      <c r="E542" t="s">
+        <v>119</v>
+      </c>
+      <c r="F542">
+        <v>2018</v>
+      </c>
+      <c r="G542" t="s">
+        <v>80</v>
+      </c>
+      <c r="H542" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="I542" s="1">
+        <v>80</v>
+      </c>
+      <c r="J542" s="3">
+        <v>4</v>
+      </c>
+      <c r="K542" s="3">
+        <v>8</v>
+      </c>
+      <c r="L542" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="543" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A543" s="3">
+        <v>542</v>
+      </c>
+      <c r="B543" s="3">
+        <v>62</v>
+      </c>
+      <c r="C543" s="2">
+        <v>43155</v>
+      </c>
+      <c r="D543">
+        <v>10</v>
+      </c>
+      <c r="E543" t="s">
+        <v>119</v>
+      </c>
+      <c r="F543">
+        <v>2018</v>
+      </c>
+      <c r="G543" t="s">
+        <v>80</v>
+      </c>
+      <c r="H543" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I543" s="1">
+        <v>30</v>
+      </c>
+      <c r="J543" s="3">
+        <v>4</v>
+      </c>
+      <c r="K543" s="3">
+        <v>8</v>
+      </c>
+      <c r="L543" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="544" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A544" s="3">
+        <v>543</v>
+      </c>
+      <c r="B544" s="3">
+        <v>62</v>
+      </c>
+      <c r="C544" s="2">
+        <v>43155</v>
+      </c>
+      <c r="D544">
+        <v>10</v>
+      </c>
+      <c r="E544" t="s">
+        <v>119</v>
+      </c>
+      <c r="F544">
+        <v>2018</v>
+      </c>
+      <c r="G544" t="s">
+        <v>80</v>
+      </c>
+      <c r="H544" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I544" s="1">
+        <v>0</v>
+      </c>
+      <c r="J544" s="3">
+        <v>4</v>
+      </c>
+      <c r="K544" s="3">
+        <v>10</v>
+      </c>
+      <c r="L544" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="545" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A545" s="3">
+        <v>544</v>
+      </c>
+      <c r="B545" s="3">
+        <v>62</v>
+      </c>
+      <c r="C545" s="2">
+        <v>43155</v>
+      </c>
+      <c r="D545">
+        <v>10</v>
+      </c>
+      <c r="E545" t="s">
+        <v>119</v>
+      </c>
+      <c r="F545">
+        <v>2018</v>
+      </c>
+      <c r="G545" t="s">
+        <v>80</v>
+      </c>
+      <c r="H545" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="I545" s="1">
+        <v>0</v>
+      </c>
+      <c r="J545" s="3">
+        <v>4</v>
+      </c>
+      <c r="K545" s="3">
+        <v>10</v>
+      </c>
+      <c r="L545" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="546" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A546" s="3">
+        <v>545</v>
+      </c>
+      <c r="B546" s="3">
+        <v>62</v>
+      </c>
+      <c r="C546" s="2">
+        <v>43155</v>
+      </c>
+      <c r="D546">
+        <v>10</v>
+      </c>
+      <c r="E546" t="s">
+        <v>119</v>
+      </c>
+      <c r="F546">
+        <v>2018</v>
+      </c>
+      <c r="G546" t="s">
+        <v>80</v>
+      </c>
+      <c r="H546" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="I546" s="1">
+        <v>0</v>
+      </c>
+      <c r="J546" s="3">
+        <v>4</v>
+      </c>
+      <c r="K546" s="3">
+        <v>12</v>
+      </c>
+      <c r="L546" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="547" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A547" s="3">
+        <v>546</v>
+      </c>
+      <c r="B547" s="3">
+        <v>62</v>
+      </c>
+      <c r="C547" s="2">
+        <v>43155</v>
+      </c>
+      <c r="D547">
+        <v>10</v>
+      </c>
+      <c r="E547" t="s">
+        <v>119</v>
+      </c>
+      <c r="F547">
+        <v>2018</v>
+      </c>
+      <c r="G547" t="s">
+        <v>80</v>
+      </c>
+      <c r="H547" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="I547" s="1">
+        <v>0</v>
+      </c>
+      <c r="J547" s="3">
+        <v>4</v>
+      </c>
+      <c r="K547" s="3">
+        <v>10</v>
+      </c>
+      <c r="L547" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="548" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A548" s="3">
+        <v>547</v>
+      </c>
+      <c r="B548" s="3">
+        <v>62</v>
+      </c>
+      <c r="C548" s="2">
+        <v>43155</v>
+      </c>
+      <c r="D548">
+        <v>10</v>
+      </c>
+      <c r="E548" t="s">
+        <v>119</v>
+      </c>
+      <c r="F548">
+        <v>2018</v>
+      </c>
+      <c r="G548" t="s">
+        <v>80</v>
+      </c>
+      <c r="H548" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="I548" s="1">
+        <v>0</v>
+      </c>
+      <c r="J548" s="3">
+        <v>4</v>
+      </c>
+      <c r="K548" s="3">
+        <v>20</v>
+      </c>
+      <c r="L548" t="s">
+        <v>89</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Adding updated GymWorkout data 11/03/2018
</commit_message>
<xml_diff>
--- a/datasets/GymWorkouts.xlsx
+++ b/datasets/GymWorkouts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Will\Documents\Data Science\My Projects\My Data Project\mydata\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E5A1EBD-926F-426E-9D12-C6544F854417}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD507199-0694-4875-8FDF-18167370F04C}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="11640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2484" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2524" uniqueCount="131">
   <si>
     <t>Exercise Date</t>
   </si>
@@ -772,11 +772,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L619"/>
+  <dimension ref="A1:L629"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A590" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C620" sqref="C620"/>
+      <pane ySplit="1" topLeftCell="A601" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A611" sqref="A611:A629"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -24317,6 +24317,386 @@
         <v>89</v>
       </c>
     </row>
+    <row r="620" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A620" s="3">
+        <v>619</v>
+      </c>
+      <c r="B620" s="3">
+        <v>71</v>
+      </c>
+      <c r="C620" s="2">
+        <v>43170</v>
+      </c>
+      <c r="D620">
+        <v>12</v>
+      </c>
+      <c r="E620" t="s">
+        <v>128</v>
+      </c>
+      <c r="F620">
+        <v>2018</v>
+      </c>
+      <c r="G620" t="s">
+        <v>45</v>
+      </c>
+      <c r="H620" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I620" s="1">
+        <v>88</v>
+      </c>
+      <c r="J620" s="3">
+        <v>4</v>
+      </c>
+      <c r="K620" s="3">
+        <v>12</v>
+      </c>
+      <c r="L620" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="621" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A621" s="3">
+        <v>620</v>
+      </c>
+      <c r="B621" s="3">
+        <v>71</v>
+      </c>
+      <c r="C621" s="2">
+        <v>43170</v>
+      </c>
+      <c r="D621">
+        <v>12</v>
+      </c>
+      <c r="E621" t="s">
+        <v>128</v>
+      </c>
+      <c r="F621">
+        <v>2018</v>
+      </c>
+      <c r="G621" t="s">
+        <v>45</v>
+      </c>
+      <c r="H621" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I621" s="1">
+        <v>100</v>
+      </c>
+      <c r="J621" s="3">
+        <v>4</v>
+      </c>
+      <c r="K621" s="3">
+        <v>8</v>
+      </c>
+      <c r="L621" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="622" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A622" s="3">
+        <v>621</v>
+      </c>
+      <c r="B622" s="3">
+        <v>71</v>
+      </c>
+      <c r="C622" s="2">
+        <v>43170</v>
+      </c>
+      <c r="D622">
+        <v>12</v>
+      </c>
+      <c r="E622" t="s">
+        <v>128</v>
+      </c>
+      <c r="F622">
+        <v>2018</v>
+      </c>
+      <c r="G622" t="s">
+        <v>45</v>
+      </c>
+      <c r="H622" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I622" s="1">
+        <v>60</v>
+      </c>
+      <c r="J622" s="3">
+        <v>3</v>
+      </c>
+      <c r="K622" s="3">
+        <v>12</v>
+      </c>
+      <c r="L622" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="623" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A623" s="3">
+        <v>622</v>
+      </c>
+      <c r="B623" s="3">
+        <v>71</v>
+      </c>
+      <c r="C623" s="2">
+        <v>43170</v>
+      </c>
+      <c r="D623">
+        <v>12</v>
+      </c>
+      <c r="E623" t="s">
+        <v>128</v>
+      </c>
+      <c r="F623">
+        <v>2018</v>
+      </c>
+      <c r="G623" t="s">
+        <v>45</v>
+      </c>
+      <c r="H623" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I623" s="1">
+        <v>65</v>
+      </c>
+      <c r="J623" s="3">
+        <v>3</v>
+      </c>
+      <c r="K623" s="3">
+        <v>12</v>
+      </c>
+      <c r="L623" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="624" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A624" s="3">
+        <v>623</v>
+      </c>
+      <c r="B624" s="3">
+        <v>71</v>
+      </c>
+      <c r="C624" s="2">
+        <v>43170</v>
+      </c>
+      <c r="D624">
+        <v>12</v>
+      </c>
+      <c r="E624" t="s">
+        <v>128</v>
+      </c>
+      <c r="F624">
+        <v>2018</v>
+      </c>
+      <c r="G624" t="s">
+        <v>45</v>
+      </c>
+      <c r="H624" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="I624" s="1">
+        <v>90</v>
+      </c>
+      <c r="J624" s="3">
+        <v>4</v>
+      </c>
+      <c r="K624" s="3">
+        <v>8</v>
+      </c>
+      <c r="L624" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="625" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A625" s="3">
+        <v>624</v>
+      </c>
+      <c r="B625" s="3">
+        <v>71</v>
+      </c>
+      <c r="C625" s="2">
+        <v>43170</v>
+      </c>
+      <c r="D625">
+        <v>12</v>
+      </c>
+      <c r="E625" t="s">
+        <v>128</v>
+      </c>
+      <c r="F625">
+        <v>2018</v>
+      </c>
+      <c r="G625" t="s">
+        <v>45</v>
+      </c>
+      <c r="H625" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I625" s="1">
+        <v>0</v>
+      </c>
+      <c r="J625" s="3">
+        <v>4</v>
+      </c>
+      <c r="K625" s="3">
+        <v>10</v>
+      </c>
+      <c r="L625" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="626" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A626" s="3">
+        <v>625</v>
+      </c>
+      <c r="B626" s="3">
+        <v>71</v>
+      </c>
+      <c r="C626" s="2">
+        <v>43170</v>
+      </c>
+      <c r="D626">
+        <v>12</v>
+      </c>
+      <c r="E626" t="s">
+        <v>128</v>
+      </c>
+      <c r="F626">
+        <v>2018</v>
+      </c>
+      <c r="G626" t="s">
+        <v>45</v>
+      </c>
+      <c r="H626" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="I626" s="1">
+        <v>0</v>
+      </c>
+      <c r="J626" s="3">
+        <v>4</v>
+      </c>
+      <c r="K626" s="3">
+        <v>10</v>
+      </c>
+      <c r="L626" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="627" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A627" s="3">
+        <v>626</v>
+      </c>
+      <c r="B627" s="3">
+        <v>71</v>
+      </c>
+      <c r="C627" s="2">
+        <v>43170</v>
+      </c>
+      <c r="D627">
+        <v>12</v>
+      </c>
+      <c r="E627" t="s">
+        <v>128</v>
+      </c>
+      <c r="F627">
+        <v>2018</v>
+      </c>
+      <c r="G627" t="s">
+        <v>45</v>
+      </c>
+      <c r="H627" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="I627" s="1">
+        <v>0</v>
+      </c>
+      <c r="J627" s="3">
+        <v>4</v>
+      </c>
+      <c r="K627" s="3">
+        <v>12</v>
+      </c>
+      <c r="L627" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="628" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A628" s="3">
+        <v>627</v>
+      </c>
+      <c r="B628" s="3">
+        <v>71</v>
+      </c>
+      <c r="C628" s="2">
+        <v>43170</v>
+      </c>
+      <c r="D628">
+        <v>12</v>
+      </c>
+      <c r="E628" t="s">
+        <v>128</v>
+      </c>
+      <c r="F628">
+        <v>2018</v>
+      </c>
+      <c r="G628" t="s">
+        <v>45</v>
+      </c>
+      <c r="H628" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="I628" s="1">
+        <v>0</v>
+      </c>
+      <c r="J628" s="3">
+        <v>4</v>
+      </c>
+      <c r="K628" s="3">
+        <v>10</v>
+      </c>
+      <c r="L628" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="629" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A629" s="3">
+        <v>628</v>
+      </c>
+      <c r="B629" s="3">
+        <v>71</v>
+      </c>
+      <c r="C629" s="2">
+        <v>43170</v>
+      </c>
+      <c r="D629">
+        <v>12</v>
+      </c>
+      <c r="E629" t="s">
+        <v>128</v>
+      </c>
+      <c r="F629">
+        <v>2018</v>
+      </c>
+      <c r="G629" t="s">
+        <v>45</v>
+      </c>
+      <c r="H629" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="I629" s="1">
+        <v>0</v>
+      </c>
+      <c r="J629" s="3">
+        <v>4</v>
+      </c>
+      <c r="K629" s="3">
+        <v>20</v>
+      </c>
+      <c r="L629" t="s">
+        <v>89</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updating GymWorkouts file 18/03/2018
</commit_message>
<xml_diff>
--- a/datasets/GymWorkouts.xlsx
+++ b/datasets/GymWorkouts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Will\Documents\Data Science\My Projects\My Data Project\mydata\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9B76A3E-688E-4254-BC20-2E2AFC07EDBD}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82DE8CEB-CAA4-44C4-96DB-B93F83475158}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="11640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2523" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2695" uniqueCount="130">
   <si>
     <t>Exercise Date</t>
   </si>
@@ -769,11 +769,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K629"/>
+  <dimension ref="A1:K672"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A605" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D1" sqref="D1:D1048576"/>
+      <pane ySplit="1" topLeftCell="A645" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C674" sqref="C674"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -22806,6 +22806,1511 @@
         <v>88</v>
       </c>
     </row>
+    <row r="630" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A630" s="3">
+        <v>629</v>
+      </c>
+      <c r="B630" s="3">
+        <v>72</v>
+      </c>
+      <c r="C630" s="2">
+        <v>43171</v>
+      </c>
+      <c r="D630" t="s">
+        <v>127</v>
+      </c>
+      <c r="E630">
+        <v>2018</v>
+      </c>
+      <c r="F630" t="s">
+        <v>17</v>
+      </c>
+      <c r="G630" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H630" s="1">
+        <v>80</v>
+      </c>
+      <c r="I630" s="3">
+        <v>4</v>
+      </c>
+      <c r="J630" s="3">
+        <v>8</v>
+      </c>
+      <c r="K630" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="631" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A631" s="3">
+        <v>630</v>
+      </c>
+      <c r="B631" s="3">
+        <v>72</v>
+      </c>
+      <c r="C631" s="2">
+        <v>43171</v>
+      </c>
+      <c r="D631" t="s">
+        <v>127</v>
+      </c>
+      <c r="E631">
+        <v>2018</v>
+      </c>
+      <c r="F631" t="s">
+        <v>17</v>
+      </c>
+      <c r="G631" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H631" s="1">
+        <v>45</v>
+      </c>
+      <c r="I631" s="3">
+        <v>4</v>
+      </c>
+      <c r="J631" s="3">
+        <v>8</v>
+      </c>
+      <c r="K631" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="632" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A632" s="3">
+        <v>631</v>
+      </c>
+      <c r="B632" s="3">
+        <v>72</v>
+      </c>
+      <c r="C632" s="2">
+        <v>43171</v>
+      </c>
+      <c r="D632" t="s">
+        <v>127</v>
+      </c>
+      <c r="E632">
+        <v>2018</v>
+      </c>
+      <c r="F632" t="s">
+        <v>17</v>
+      </c>
+      <c r="G632" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H632" s="1">
+        <v>80</v>
+      </c>
+      <c r="I632" s="3">
+        <v>4</v>
+      </c>
+      <c r="J632" s="3">
+        <v>8</v>
+      </c>
+      <c r="K632" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="633" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A633" s="3">
+        <v>632</v>
+      </c>
+      <c r="B633" s="3">
+        <v>72</v>
+      </c>
+      <c r="C633" s="2">
+        <v>43171</v>
+      </c>
+      <c r="D633" t="s">
+        <v>127</v>
+      </c>
+      <c r="E633">
+        <v>2018</v>
+      </c>
+      <c r="F633" t="s">
+        <v>17</v>
+      </c>
+      <c r="G633" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="H633" s="1">
+        <v>25</v>
+      </c>
+      <c r="I633" s="3">
+        <v>3</v>
+      </c>
+      <c r="J633" s="3">
+        <v>12</v>
+      </c>
+      <c r="K633" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="634" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A634" s="3">
+        <v>633</v>
+      </c>
+      <c r="B634" s="3">
+        <v>72</v>
+      </c>
+      <c r="C634" s="2">
+        <v>43171</v>
+      </c>
+      <c r="D634" t="s">
+        <v>127</v>
+      </c>
+      <c r="E634">
+        <v>2018</v>
+      </c>
+      <c r="F634" t="s">
+        <v>17</v>
+      </c>
+      <c r="G634" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H634" s="1">
+        <v>0</v>
+      </c>
+      <c r="I634" s="3">
+        <v>5</v>
+      </c>
+      <c r="J634" s="3">
+        <v>30</v>
+      </c>
+      <c r="K634" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="635" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A635" s="3">
+        <v>634</v>
+      </c>
+      <c r="B635" s="3">
+        <v>72</v>
+      </c>
+      <c r="C635" s="2">
+        <v>43171</v>
+      </c>
+      <c r="D635" t="s">
+        <v>127</v>
+      </c>
+      <c r="E635">
+        <v>2018</v>
+      </c>
+      <c r="F635" t="s">
+        <v>17</v>
+      </c>
+      <c r="G635" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H635" s="1">
+        <v>0</v>
+      </c>
+      <c r="I635" s="3">
+        <v>5</v>
+      </c>
+      <c r="J635" s="3">
+        <v>30</v>
+      </c>
+      <c r="K635" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="636" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A636" s="3">
+        <v>635</v>
+      </c>
+      <c r="B636" s="3">
+        <v>72</v>
+      </c>
+      <c r="C636" s="2">
+        <v>43171</v>
+      </c>
+      <c r="D636" t="s">
+        <v>127</v>
+      </c>
+      <c r="E636">
+        <v>2018</v>
+      </c>
+      <c r="F636" t="s">
+        <v>17</v>
+      </c>
+      <c r="G636" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H636" s="1">
+        <v>0</v>
+      </c>
+      <c r="I636" s="3">
+        <v>5</v>
+      </c>
+      <c r="J636" s="3">
+        <v>30</v>
+      </c>
+      <c r="K636" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="637" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A637" s="3">
+        <v>636</v>
+      </c>
+      <c r="B637" s="3">
+        <v>73</v>
+      </c>
+      <c r="C637" s="2">
+        <v>43172</v>
+      </c>
+      <c r="D637" t="s">
+        <v>127</v>
+      </c>
+      <c r="E637">
+        <v>2018</v>
+      </c>
+      <c r="F637" t="s">
+        <v>73</v>
+      </c>
+      <c r="G637" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H637" s="1">
+        <v>35</v>
+      </c>
+      <c r="I637" s="3">
+        <v>4</v>
+      </c>
+      <c r="J637" s="3">
+        <v>8</v>
+      </c>
+      <c r="K637" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="638" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A638" s="3">
+        <v>637</v>
+      </c>
+      <c r="B638" s="3">
+        <v>73</v>
+      </c>
+      <c r="C638" s="2">
+        <v>43172</v>
+      </c>
+      <c r="D638" t="s">
+        <v>127</v>
+      </c>
+      <c r="E638">
+        <v>2018</v>
+      </c>
+      <c r="F638" t="s">
+        <v>73</v>
+      </c>
+      <c r="G638" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H638" s="1">
+        <v>15</v>
+      </c>
+      <c r="I638" s="3">
+        <v>4</v>
+      </c>
+      <c r="J638" s="3">
+        <v>8</v>
+      </c>
+      <c r="K638" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="639" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A639" s="3">
+        <v>638</v>
+      </c>
+      <c r="B639" s="3">
+        <v>73</v>
+      </c>
+      <c r="C639" s="2">
+        <v>43172</v>
+      </c>
+      <c r="D639" t="s">
+        <v>127</v>
+      </c>
+      <c r="E639">
+        <v>2018</v>
+      </c>
+      <c r="F639" t="s">
+        <v>73</v>
+      </c>
+      <c r="G639" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H639" s="1">
+        <v>30</v>
+      </c>
+      <c r="I639" s="3">
+        <v>4</v>
+      </c>
+      <c r="J639" s="3">
+        <v>8</v>
+      </c>
+      <c r="K639" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="640" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A640" s="3">
+        <v>639</v>
+      </c>
+      <c r="B640" s="3">
+        <v>73</v>
+      </c>
+      <c r="C640" s="2">
+        <v>43172</v>
+      </c>
+      <c r="D640" t="s">
+        <v>127</v>
+      </c>
+      <c r="E640">
+        <v>2018</v>
+      </c>
+      <c r="F640" t="s">
+        <v>73</v>
+      </c>
+      <c r="G640" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H640" s="1">
+        <v>40</v>
+      </c>
+      <c r="I640" s="3">
+        <v>4</v>
+      </c>
+      <c r="J640" s="3">
+        <v>8</v>
+      </c>
+      <c r="K640" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="641" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A641" s="3">
+        <v>640</v>
+      </c>
+      <c r="B641" s="3">
+        <v>73</v>
+      </c>
+      <c r="C641" s="2">
+        <v>43172</v>
+      </c>
+      <c r="D641" t="s">
+        <v>127</v>
+      </c>
+      <c r="E641">
+        <v>2018</v>
+      </c>
+      <c r="F641" t="s">
+        <v>73</v>
+      </c>
+      <c r="G641" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="H641" s="1">
+        <v>94</v>
+      </c>
+      <c r="I641" s="3">
+        <v>4</v>
+      </c>
+      <c r="J641" s="3">
+        <v>8</v>
+      </c>
+      <c r="K641" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="642" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A642" s="3">
+        <v>641</v>
+      </c>
+      <c r="B642" s="3">
+        <v>73</v>
+      </c>
+      <c r="C642" s="2">
+        <v>43172</v>
+      </c>
+      <c r="D642" t="s">
+        <v>127</v>
+      </c>
+      <c r="E642">
+        <v>2018</v>
+      </c>
+      <c r="F642" t="s">
+        <v>73</v>
+      </c>
+      <c r="G642" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H642" s="1">
+        <v>0</v>
+      </c>
+      <c r="I642" s="3">
+        <v>4</v>
+      </c>
+      <c r="J642" s="3">
+        <v>10</v>
+      </c>
+      <c r="K642" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="643" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A643" s="3">
+        <v>642</v>
+      </c>
+      <c r="B643" s="3">
+        <v>73</v>
+      </c>
+      <c r="C643" s="2">
+        <v>43172</v>
+      </c>
+      <c r="D643" t="s">
+        <v>127</v>
+      </c>
+      <c r="E643">
+        <v>2018</v>
+      </c>
+      <c r="F643" t="s">
+        <v>73</v>
+      </c>
+      <c r="G643" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="H643" s="1">
+        <v>0</v>
+      </c>
+      <c r="I643" s="3">
+        <v>4</v>
+      </c>
+      <c r="J643" s="3">
+        <v>10</v>
+      </c>
+      <c r="K643" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="644" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A644" s="3">
+        <v>643</v>
+      </c>
+      <c r="B644" s="3">
+        <v>73</v>
+      </c>
+      <c r="C644" s="2">
+        <v>43172</v>
+      </c>
+      <c r="D644" t="s">
+        <v>127</v>
+      </c>
+      <c r="E644">
+        <v>2018</v>
+      </c>
+      <c r="F644" t="s">
+        <v>73</v>
+      </c>
+      <c r="G644" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="H644" s="1">
+        <v>0</v>
+      </c>
+      <c r="I644" s="3">
+        <v>4</v>
+      </c>
+      <c r="J644" s="3">
+        <v>12</v>
+      </c>
+      <c r="K644" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="645" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A645" s="3">
+        <v>644</v>
+      </c>
+      <c r="B645" s="3">
+        <v>73</v>
+      </c>
+      <c r="C645" s="2">
+        <v>43172</v>
+      </c>
+      <c r="D645" t="s">
+        <v>127</v>
+      </c>
+      <c r="E645">
+        <v>2018</v>
+      </c>
+      <c r="F645" t="s">
+        <v>73</v>
+      </c>
+      <c r="G645" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="H645" s="1">
+        <v>0</v>
+      </c>
+      <c r="I645" s="3">
+        <v>4</v>
+      </c>
+      <c r="J645" s="3">
+        <v>10</v>
+      </c>
+      <c r="K645" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="646" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A646" s="3">
+        <v>645</v>
+      </c>
+      <c r="B646" s="3">
+        <v>73</v>
+      </c>
+      <c r="C646" s="2">
+        <v>43172</v>
+      </c>
+      <c r="D646" t="s">
+        <v>127</v>
+      </c>
+      <c r="E646">
+        <v>2018</v>
+      </c>
+      <c r="F646" t="s">
+        <v>73</v>
+      </c>
+      <c r="G646" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="H646" s="1">
+        <v>0</v>
+      </c>
+      <c r="I646" s="3">
+        <v>4</v>
+      </c>
+      <c r="J646" s="3">
+        <v>20</v>
+      </c>
+      <c r="K646" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="647" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A647" s="3">
+        <v>646</v>
+      </c>
+      <c r="B647" s="3">
+        <v>74</v>
+      </c>
+      <c r="C647" s="2">
+        <v>43174</v>
+      </c>
+      <c r="D647" t="s">
+        <v>127</v>
+      </c>
+      <c r="E647">
+        <v>2018</v>
+      </c>
+      <c r="F647" t="s">
+        <v>16</v>
+      </c>
+      <c r="G647" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H647" s="1">
+        <v>90</v>
+      </c>
+      <c r="I647" s="3">
+        <v>5</v>
+      </c>
+      <c r="J647" s="3">
+        <v>5</v>
+      </c>
+      <c r="K647" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="648" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A648" s="3">
+        <v>647</v>
+      </c>
+      <c r="B648" s="3">
+        <v>74</v>
+      </c>
+      <c r="C648" s="2">
+        <v>43174</v>
+      </c>
+      <c r="D648" t="s">
+        <v>127</v>
+      </c>
+      <c r="E648">
+        <v>2018</v>
+      </c>
+      <c r="F648" t="s">
+        <v>16</v>
+      </c>
+      <c r="G648" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="H648" s="1">
+        <v>40</v>
+      </c>
+      <c r="I648" s="3">
+        <v>3</v>
+      </c>
+      <c r="J648" s="3">
+        <v>20</v>
+      </c>
+      <c r="K648" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="649" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A649" s="3">
+        <v>648</v>
+      </c>
+      <c r="B649" s="3">
+        <v>74</v>
+      </c>
+      <c r="C649" s="2">
+        <v>43174</v>
+      </c>
+      <c r="D649" t="s">
+        <v>127</v>
+      </c>
+      <c r="E649">
+        <v>2018</v>
+      </c>
+      <c r="F649" t="s">
+        <v>16</v>
+      </c>
+      <c r="G649" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="H649" s="1">
+        <v>25</v>
+      </c>
+      <c r="I649" s="3">
+        <v>3</v>
+      </c>
+      <c r="J649" s="3">
+        <v>12</v>
+      </c>
+      <c r="K649" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="650" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A650" s="3">
+        <v>649</v>
+      </c>
+      <c r="B650" s="3">
+        <v>74</v>
+      </c>
+      <c r="C650" s="2">
+        <v>43174</v>
+      </c>
+      <c r="D650" t="s">
+        <v>127</v>
+      </c>
+      <c r="E650">
+        <v>2018</v>
+      </c>
+      <c r="F650" t="s">
+        <v>16</v>
+      </c>
+      <c r="G650" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H650" s="1">
+        <v>100</v>
+      </c>
+      <c r="I650" s="3">
+        <v>4</v>
+      </c>
+      <c r="J650" s="3">
+        <v>8</v>
+      </c>
+      <c r="K650" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="651" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A651" s="3">
+        <v>650</v>
+      </c>
+      <c r="B651" s="3">
+        <v>74</v>
+      </c>
+      <c r="C651" s="2">
+        <v>43174</v>
+      </c>
+      <c r="D651" t="s">
+        <v>127</v>
+      </c>
+      <c r="E651">
+        <v>2018</v>
+      </c>
+      <c r="F651" t="s">
+        <v>16</v>
+      </c>
+      <c r="G651" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="H651" s="1">
+        <v>10</v>
+      </c>
+      <c r="I651" s="3">
+        <v>3</v>
+      </c>
+      <c r="J651" s="3">
+        <v>20</v>
+      </c>
+      <c r="K651" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="652" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A652" s="3">
+        <v>651</v>
+      </c>
+      <c r="B652" s="3">
+        <v>74</v>
+      </c>
+      <c r="C652" s="2">
+        <v>43174</v>
+      </c>
+      <c r="D652" t="s">
+        <v>127</v>
+      </c>
+      <c r="E652">
+        <v>2018</v>
+      </c>
+      <c r="F652" t="s">
+        <v>16</v>
+      </c>
+      <c r="G652" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="H652" s="1">
+        <v>0</v>
+      </c>
+      <c r="I652" s="3">
+        <v>3</v>
+      </c>
+      <c r="J652" s="3">
+        <v>20</v>
+      </c>
+      <c r="K652" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="653" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A653" s="3">
+        <v>652</v>
+      </c>
+      <c r="B653" s="3">
+        <v>75</v>
+      </c>
+      <c r="C653" s="2">
+        <v>43176</v>
+      </c>
+      <c r="D653" t="s">
+        <v>127</v>
+      </c>
+      <c r="E653">
+        <v>2018</v>
+      </c>
+      <c r="F653" t="s">
+        <v>79</v>
+      </c>
+      <c r="G653" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H653" s="1">
+        <v>72.5</v>
+      </c>
+      <c r="I653" s="3">
+        <v>4</v>
+      </c>
+      <c r="J653" s="3">
+        <v>8</v>
+      </c>
+      <c r="K653" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="654" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A654" s="3">
+        <v>653</v>
+      </c>
+      <c r="B654" s="3">
+        <v>75</v>
+      </c>
+      <c r="C654" s="2">
+        <v>43176</v>
+      </c>
+      <c r="D654" t="s">
+        <v>127</v>
+      </c>
+      <c r="E654">
+        <v>2018</v>
+      </c>
+      <c r="F654" t="s">
+        <v>79</v>
+      </c>
+      <c r="G654" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="H654" s="1">
+        <v>30</v>
+      </c>
+      <c r="I654" s="3">
+        <v>4</v>
+      </c>
+      <c r="J654" s="3">
+        <v>8</v>
+      </c>
+      <c r="K654" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="655" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A655" s="3">
+        <v>654</v>
+      </c>
+      <c r="B655" s="3">
+        <v>75</v>
+      </c>
+      <c r="C655" s="2">
+        <v>43176</v>
+      </c>
+      <c r="D655" t="s">
+        <v>127</v>
+      </c>
+      <c r="E655">
+        <v>2018</v>
+      </c>
+      <c r="F655" t="s">
+        <v>79</v>
+      </c>
+      <c r="G655" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H655" s="1">
+        <v>25</v>
+      </c>
+      <c r="I655" s="3">
+        <v>4</v>
+      </c>
+      <c r="J655" s="3">
+        <v>8</v>
+      </c>
+      <c r="K655" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="656" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A656" s="3">
+        <v>655</v>
+      </c>
+      <c r="B656" s="3">
+        <v>75</v>
+      </c>
+      <c r="C656" s="2">
+        <v>43176</v>
+      </c>
+      <c r="D656" t="s">
+        <v>127</v>
+      </c>
+      <c r="E656">
+        <v>2018</v>
+      </c>
+      <c r="F656" t="s">
+        <v>79</v>
+      </c>
+      <c r="G656" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H656" s="1">
+        <v>25</v>
+      </c>
+      <c r="I656" s="3">
+        <v>4</v>
+      </c>
+      <c r="J656" s="3">
+        <v>8</v>
+      </c>
+      <c r="K656" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="657" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A657" s="3">
+        <v>656</v>
+      </c>
+      <c r="B657" s="3">
+        <v>75</v>
+      </c>
+      <c r="C657" s="2">
+        <v>43176</v>
+      </c>
+      <c r="D657" t="s">
+        <v>127</v>
+      </c>
+      <c r="E657">
+        <v>2018</v>
+      </c>
+      <c r="F657" t="s">
+        <v>79</v>
+      </c>
+      <c r="G657" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="H657" s="1">
+        <v>7.5</v>
+      </c>
+      <c r="I657" s="3">
+        <v>4</v>
+      </c>
+      <c r="J657" s="3">
+        <v>8</v>
+      </c>
+      <c r="K657" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="658" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A658" s="3">
+        <v>657</v>
+      </c>
+      <c r="B658" s="3">
+        <v>75</v>
+      </c>
+      <c r="C658" s="2">
+        <v>43176</v>
+      </c>
+      <c r="D658" t="s">
+        <v>127</v>
+      </c>
+      <c r="E658">
+        <v>2018</v>
+      </c>
+      <c r="F658" t="s">
+        <v>79</v>
+      </c>
+      <c r="G658" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H658" s="1">
+        <v>7.5</v>
+      </c>
+      <c r="I658" s="3">
+        <v>4</v>
+      </c>
+      <c r="J658" s="3">
+        <v>8</v>
+      </c>
+      <c r="K658" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="659" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A659" s="3">
+        <v>658</v>
+      </c>
+      <c r="B659" s="3">
+        <v>75</v>
+      </c>
+      <c r="C659" s="2">
+        <v>43176</v>
+      </c>
+      <c r="D659" t="s">
+        <v>127</v>
+      </c>
+      <c r="E659">
+        <v>2018</v>
+      </c>
+      <c r="F659" t="s">
+        <v>79</v>
+      </c>
+      <c r="G659" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="H659" s="1">
+        <v>7.5</v>
+      </c>
+      <c r="I659" s="3">
+        <v>4</v>
+      </c>
+      <c r="J659" s="3">
+        <v>8</v>
+      </c>
+      <c r="K659" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="660" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A660" s="3">
+        <v>659</v>
+      </c>
+      <c r="B660" s="3">
+        <v>75</v>
+      </c>
+      <c r="C660" s="2">
+        <v>43176</v>
+      </c>
+      <c r="D660" t="s">
+        <v>127</v>
+      </c>
+      <c r="E660">
+        <v>2018</v>
+      </c>
+      <c r="F660" t="s">
+        <v>79</v>
+      </c>
+      <c r="G660" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H660" s="1">
+        <v>0</v>
+      </c>
+      <c r="I660" s="3">
+        <v>4</v>
+      </c>
+      <c r="J660" s="3">
+        <v>30</v>
+      </c>
+      <c r="K660" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="661" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A661" s="3">
+        <v>660</v>
+      </c>
+      <c r="B661" s="3">
+        <v>75</v>
+      </c>
+      <c r="C661" s="2">
+        <v>43176</v>
+      </c>
+      <c r="D661" t="s">
+        <v>127</v>
+      </c>
+      <c r="E661">
+        <v>2018</v>
+      </c>
+      <c r="F661" t="s">
+        <v>79</v>
+      </c>
+      <c r="G661" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="H661" s="1">
+        <v>0</v>
+      </c>
+      <c r="I661" s="3">
+        <v>4</v>
+      </c>
+      <c r="J661" s="3">
+        <v>10</v>
+      </c>
+      <c r="K661" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="662" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A662" s="3">
+        <v>661</v>
+      </c>
+      <c r="B662" s="3">
+        <v>75</v>
+      </c>
+      <c r="C662" s="2">
+        <v>43176</v>
+      </c>
+      <c r="D662" t="s">
+        <v>127</v>
+      </c>
+      <c r="E662">
+        <v>2018</v>
+      </c>
+      <c r="F662" t="s">
+        <v>79</v>
+      </c>
+      <c r="G662" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="H662" s="1">
+        <v>0</v>
+      </c>
+      <c r="I662" s="3">
+        <v>4</v>
+      </c>
+      <c r="J662" s="3">
+        <v>10</v>
+      </c>
+      <c r="K662" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="663" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A663" s="3">
+        <v>662</v>
+      </c>
+      <c r="B663" s="3">
+        <v>76</v>
+      </c>
+      <c r="C663" s="2">
+        <v>43177</v>
+      </c>
+      <c r="D663" t="s">
+        <v>127</v>
+      </c>
+      <c r="E663">
+        <v>2018</v>
+      </c>
+      <c r="F663" t="s">
+        <v>44</v>
+      </c>
+      <c r="G663" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="H663" s="1">
+        <v>10</v>
+      </c>
+      <c r="I663" s="3">
+        <v>4</v>
+      </c>
+      <c r="J663" s="3">
+        <v>20</v>
+      </c>
+      <c r="K663" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="664" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A664" s="3">
+        <v>663</v>
+      </c>
+      <c r="B664" s="3">
+        <v>76</v>
+      </c>
+      <c r="C664" s="2">
+        <v>43177</v>
+      </c>
+      <c r="D664" t="s">
+        <v>127</v>
+      </c>
+      <c r="E664">
+        <v>2018</v>
+      </c>
+      <c r="F664" t="s">
+        <v>44</v>
+      </c>
+      <c r="G664" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="H664" s="1">
+        <v>0</v>
+      </c>
+      <c r="I664" s="3">
+        <v>4</v>
+      </c>
+      <c r="J664" s="3">
+        <v>20</v>
+      </c>
+      <c r="K664" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="665" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A665" s="3">
+        <v>664</v>
+      </c>
+      <c r="B665" s="3">
+        <v>76</v>
+      </c>
+      <c r="C665" s="2">
+        <v>43177</v>
+      </c>
+      <c r="D665" t="s">
+        <v>127</v>
+      </c>
+      <c r="E665">
+        <v>2018</v>
+      </c>
+      <c r="F665" t="s">
+        <v>44</v>
+      </c>
+      <c r="G665" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H665" s="1">
+        <v>0</v>
+      </c>
+      <c r="I665" s="3">
+        <v>4</v>
+      </c>
+      <c r="J665" s="3">
+        <v>30</v>
+      </c>
+      <c r="K665" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="666" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A666" s="3">
+        <v>665</v>
+      </c>
+      <c r="B666" s="3">
+        <v>76</v>
+      </c>
+      <c r="C666" s="2">
+        <v>43177</v>
+      </c>
+      <c r="D666" t="s">
+        <v>127</v>
+      </c>
+      <c r="E666">
+        <v>2018</v>
+      </c>
+      <c r="F666" t="s">
+        <v>44</v>
+      </c>
+      <c r="G666" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H666" s="1">
+        <v>0</v>
+      </c>
+      <c r="I666" s="3">
+        <v>4</v>
+      </c>
+      <c r="J666" s="3">
+        <v>30</v>
+      </c>
+      <c r="K666" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="667" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A667" s="3">
+        <v>666</v>
+      </c>
+      <c r="B667" s="3">
+        <v>76</v>
+      </c>
+      <c r="C667" s="2">
+        <v>43177</v>
+      </c>
+      <c r="D667" t="s">
+        <v>127</v>
+      </c>
+      <c r="E667">
+        <v>2018</v>
+      </c>
+      <c r="F667" t="s">
+        <v>44</v>
+      </c>
+      <c r="G667" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H667" s="1">
+        <v>0</v>
+      </c>
+      <c r="I667" s="3">
+        <v>4</v>
+      </c>
+      <c r="J667" s="3">
+        <v>30</v>
+      </c>
+      <c r="K667" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="668" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A668" s="3">
+        <v>667</v>
+      </c>
+      <c r="B668" s="3">
+        <v>76</v>
+      </c>
+      <c r="C668" s="2">
+        <v>43177</v>
+      </c>
+      <c r="D668" t="s">
+        <v>127</v>
+      </c>
+      <c r="E668">
+        <v>2018</v>
+      </c>
+      <c r="F668" t="s">
+        <v>44</v>
+      </c>
+      <c r="G668" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H668" s="1">
+        <v>0</v>
+      </c>
+      <c r="I668" s="3">
+        <v>4</v>
+      </c>
+      <c r="J668" s="3">
+        <v>15</v>
+      </c>
+      <c r="K668" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="669" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A669" s="3">
+        <v>668</v>
+      </c>
+      <c r="B669" s="3">
+        <v>76</v>
+      </c>
+      <c r="C669" s="2">
+        <v>43177</v>
+      </c>
+      <c r="D669" t="s">
+        <v>127</v>
+      </c>
+      <c r="E669">
+        <v>2018</v>
+      </c>
+      <c r="F669" t="s">
+        <v>44</v>
+      </c>
+      <c r="G669" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="H669" s="1">
+        <v>0</v>
+      </c>
+      <c r="I669" s="3">
+        <v>4</v>
+      </c>
+      <c r="J669" s="3">
+        <v>12</v>
+      </c>
+      <c r="K669" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="670" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A670" s="3">
+        <v>669</v>
+      </c>
+      <c r="B670" s="3">
+        <v>76</v>
+      </c>
+      <c r="C670" s="2">
+        <v>43177</v>
+      </c>
+      <c r="D670" t="s">
+        <v>127</v>
+      </c>
+      <c r="E670">
+        <v>2018</v>
+      </c>
+      <c r="F670" t="s">
+        <v>44</v>
+      </c>
+      <c r="G670" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="H670" s="1">
+        <v>0</v>
+      </c>
+      <c r="I670" s="3">
+        <v>4</v>
+      </c>
+      <c r="J670" s="3">
+        <v>12</v>
+      </c>
+      <c r="K670" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="671" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A671" s="3">
+        <v>670</v>
+      </c>
+      <c r="B671" s="3">
+        <v>76</v>
+      </c>
+      <c r="C671" s="2">
+        <v>43177</v>
+      </c>
+      <c r="D671" t="s">
+        <v>127</v>
+      </c>
+      <c r="E671">
+        <v>2018</v>
+      </c>
+      <c r="F671" t="s">
+        <v>44</v>
+      </c>
+      <c r="G671" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="H671" s="1">
+        <v>0</v>
+      </c>
+      <c r="I671" s="3">
+        <v>4</v>
+      </c>
+      <c r="J671" s="3">
+        <v>12</v>
+      </c>
+      <c r="K671" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="672" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A672" s="3">
+        <v>671</v>
+      </c>
+      <c r="B672" s="3">
+        <v>76</v>
+      </c>
+      <c r="C672" s="2">
+        <v>43177</v>
+      </c>
+      <c r="D672" t="s">
+        <v>127</v>
+      </c>
+      <c r="E672">
+        <v>2018</v>
+      </c>
+      <c r="F672" t="s">
+        <v>44</v>
+      </c>
+      <c r="G672" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="H672" s="1">
+        <v>0</v>
+      </c>
+      <c r="I672" s="3">
+        <v>4</v>
+      </c>
+      <c r="J672" s="3">
+        <v>20</v>
+      </c>
+      <c r="K672" t="s">
+        <v>88</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updating GymWorkouts file 25/03/2018
</commit_message>
<xml_diff>
--- a/datasets/GymWorkouts.xlsx
+++ b/datasets/GymWorkouts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Will\Documents\Data Science\My Projects\My Data Project\mydata\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82DE8CEB-CAA4-44C4-96DB-B93F83475158}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BE59F7B-0A13-4015-9B4C-6200CDD40903}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="11640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2695" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2799" uniqueCount="130">
   <si>
     <t>Exercise Date</t>
   </si>
@@ -769,11 +769,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K672"/>
+  <dimension ref="A1:K698"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A645" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C674" sqref="C674"/>
+      <pane ySplit="1" topLeftCell="A676" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C701" sqref="C701"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -24311,6 +24311,916 @@
         <v>88</v>
       </c>
     </row>
+    <row r="673" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A673" s="3">
+        <v>672</v>
+      </c>
+      <c r="B673" s="3">
+        <v>77</v>
+      </c>
+      <c r="C673" s="2">
+        <v>43178</v>
+      </c>
+      <c r="D673" t="s">
+        <v>127</v>
+      </c>
+      <c r="E673">
+        <v>2018</v>
+      </c>
+      <c r="F673" t="s">
+        <v>17</v>
+      </c>
+      <c r="G673" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H673" s="1">
+        <v>105</v>
+      </c>
+      <c r="I673" s="3">
+        <v>4</v>
+      </c>
+      <c r="J673" s="3">
+        <v>8</v>
+      </c>
+      <c r="K673" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="674" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A674" s="3">
+        <v>673</v>
+      </c>
+      <c r="B674" s="3">
+        <v>77</v>
+      </c>
+      <c r="C674" s="2">
+        <v>43178</v>
+      </c>
+      <c r="D674" t="s">
+        <v>127</v>
+      </c>
+      <c r="E674">
+        <v>2018</v>
+      </c>
+      <c r="F674" t="s">
+        <v>17</v>
+      </c>
+      <c r="G674" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="H674" s="1">
+        <v>30</v>
+      </c>
+      <c r="I674" s="3">
+        <v>3</v>
+      </c>
+      <c r="J674" s="3">
+        <v>12</v>
+      </c>
+      <c r="K674" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="675" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A675" s="3">
+        <v>674</v>
+      </c>
+      <c r="B675" s="3">
+        <v>77</v>
+      </c>
+      <c r="C675" s="2">
+        <v>43178</v>
+      </c>
+      <c r="D675" t="s">
+        <v>127</v>
+      </c>
+      <c r="E675">
+        <v>2018</v>
+      </c>
+      <c r="F675" t="s">
+        <v>17</v>
+      </c>
+      <c r="G675" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H675" s="1">
+        <v>35</v>
+      </c>
+      <c r="I675" s="3">
+        <v>4</v>
+      </c>
+      <c r="J675" s="3">
+        <v>8</v>
+      </c>
+      <c r="K675" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="676" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A676" s="3">
+        <v>675</v>
+      </c>
+      <c r="B676" s="3">
+        <v>77</v>
+      </c>
+      <c r="C676" s="2">
+        <v>43178</v>
+      </c>
+      <c r="D676" t="s">
+        <v>127</v>
+      </c>
+      <c r="E676">
+        <v>2018</v>
+      </c>
+      <c r="F676" t="s">
+        <v>17</v>
+      </c>
+      <c r="G676" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="H676" s="1">
+        <v>80</v>
+      </c>
+      <c r="I676" s="3">
+        <v>4</v>
+      </c>
+      <c r="J676" s="3">
+        <v>8</v>
+      </c>
+      <c r="K676" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="677" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A677" s="3">
+        <v>676</v>
+      </c>
+      <c r="B677" s="3">
+        <v>78</v>
+      </c>
+      <c r="C677" s="2">
+        <v>43180</v>
+      </c>
+      <c r="D677" t="s">
+        <v>127</v>
+      </c>
+      <c r="E677">
+        <v>2018</v>
+      </c>
+      <c r="F677" t="s">
+        <v>18</v>
+      </c>
+      <c r="G677" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H677" s="1">
+        <v>72.5</v>
+      </c>
+      <c r="I677" s="3">
+        <v>4</v>
+      </c>
+      <c r="J677" s="3">
+        <v>8</v>
+      </c>
+      <c r="K677" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="678" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A678" s="3">
+        <v>677</v>
+      </c>
+      <c r="B678" s="3">
+        <v>78</v>
+      </c>
+      <c r="C678" s="2">
+        <v>43180</v>
+      </c>
+      <c r="D678" t="s">
+        <v>127</v>
+      </c>
+      <c r="E678">
+        <v>2018</v>
+      </c>
+      <c r="F678" t="s">
+        <v>18</v>
+      </c>
+      <c r="G678" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H678" s="1">
+        <v>80</v>
+      </c>
+      <c r="I678" s="3">
+        <v>5</v>
+      </c>
+      <c r="J678" s="3">
+        <v>8</v>
+      </c>
+      <c r="K678" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="679" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A679" s="3">
+        <v>678</v>
+      </c>
+      <c r="B679" s="3">
+        <v>78</v>
+      </c>
+      <c r="C679" s="2">
+        <v>43180</v>
+      </c>
+      <c r="D679" t="s">
+        <v>127</v>
+      </c>
+      <c r="E679">
+        <v>2018</v>
+      </c>
+      <c r="F679" t="s">
+        <v>18</v>
+      </c>
+      <c r="G679" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H679" s="1">
+        <v>40</v>
+      </c>
+      <c r="I679" s="3">
+        <v>4</v>
+      </c>
+      <c r="J679" s="3">
+        <v>8</v>
+      </c>
+      <c r="K679" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="680" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A680" s="3">
+        <v>679</v>
+      </c>
+      <c r="B680" s="3">
+        <v>78</v>
+      </c>
+      <c r="C680" s="2">
+        <v>43180</v>
+      </c>
+      <c r="D680" t="s">
+        <v>127</v>
+      </c>
+      <c r="E680">
+        <v>2018</v>
+      </c>
+      <c r="F680" t="s">
+        <v>18</v>
+      </c>
+      <c r="G680" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H680" s="1">
+        <v>80</v>
+      </c>
+      <c r="I680" s="3">
+        <v>5</v>
+      </c>
+      <c r="J680" s="3">
+        <v>5</v>
+      </c>
+      <c r="K680" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="681" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A681" s="3">
+        <v>680</v>
+      </c>
+      <c r="B681" s="3">
+        <v>79</v>
+      </c>
+      <c r="C681" s="2">
+        <v>43182</v>
+      </c>
+      <c r="D681" t="s">
+        <v>127</v>
+      </c>
+      <c r="E681">
+        <v>2018</v>
+      </c>
+      <c r="F681" t="s">
+        <v>49</v>
+      </c>
+      <c r="G681" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H681" s="1">
+        <v>25</v>
+      </c>
+      <c r="I681" s="3">
+        <v>4</v>
+      </c>
+      <c r="J681" s="3">
+        <v>8</v>
+      </c>
+      <c r="K681" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="682" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A682" s="3">
+        <v>681</v>
+      </c>
+      <c r="B682" s="3">
+        <v>79</v>
+      </c>
+      <c r="C682" s="2">
+        <v>43182</v>
+      </c>
+      <c r="D682" t="s">
+        <v>127</v>
+      </c>
+      <c r="E682">
+        <v>2018</v>
+      </c>
+      <c r="F682" t="s">
+        <v>49</v>
+      </c>
+      <c r="G682" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H682" s="1">
+        <v>25</v>
+      </c>
+      <c r="I682" s="3">
+        <v>4</v>
+      </c>
+      <c r="J682" s="3">
+        <v>8</v>
+      </c>
+      <c r="K682" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="683" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A683" s="3">
+        <v>682</v>
+      </c>
+      <c r="B683" s="3">
+        <v>79</v>
+      </c>
+      <c r="C683" s="2">
+        <v>43182</v>
+      </c>
+      <c r="D683" t="s">
+        <v>127</v>
+      </c>
+      <c r="E683">
+        <v>2018</v>
+      </c>
+      <c r="F683" t="s">
+        <v>49</v>
+      </c>
+      <c r="G683" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H683" s="1">
+        <v>42.5</v>
+      </c>
+      <c r="I683" s="3">
+        <v>4</v>
+      </c>
+      <c r="J683" s="3">
+        <v>8</v>
+      </c>
+      <c r="K683" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="684" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A684" s="3">
+        <v>683</v>
+      </c>
+      <c r="B684" s="3">
+        <v>79</v>
+      </c>
+      <c r="C684" s="2">
+        <v>43182</v>
+      </c>
+      <c r="D684" t="s">
+        <v>127</v>
+      </c>
+      <c r="E684">
+        <v>2018</v>
+      </c>
+      <c r="F684" t="s">
+        <v>49</v>
+      </c>
+      <c r="G684" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H684" s="1">
+        <v>17.5</v>
+      </c>
+      <c r="I684" s="3">
+        <v>4</v>
+      </c>
+      <c r="J684" s="3">
+        <v>8</v>
+      </c>
+      <c r="K684" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="685" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A685" s="3">
+        <v>684</v>
+      </c>
+      <c r="B685" s="3">
+        <v>79</v>
+      </c>
+      <c r="C685" s="2">
+        <v>43182</v>
+      </c>
+      <c r="D685" t="s">
+        <v>127</v>
+      </c>
+      <c r="E685">
+        <v>2018</v>
+      </c>
+      <c r="F685" t="s">
+        <v>49</v>
+      </c>
+      <c r="G685" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H685" s="1">
+        <v>0</v>
+      </c>
+      <c r="I685" s="3">
+        <v>4</v>
+      </c>
+      <c r="J685" s="3">
+        <v>15</v>
+      </c>
+      <c r="K685" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="686" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A686" s="3">
+        <v>685</v>
+      </c>
+      <c r="B686" s="3">
+        <v>79</v>
+      </c>
+      <c r="C686" s="2">
+        <v>43182</v>
+      </c>
+      <c r="D686" t="s">
+        <v>127</v>
+      </c>
+      <c r="E686">
+        <v>2018</v>
+      </c>
+      <c r="F686" t="s">
+        <v>49</v>
+      </c>
+      <c r="G686" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="H686" s="1">
+        <v>0</v>
+      </c>
+      <c r="I686" s="3">
+        <v>4</v>
+      </c>
+      <c r="J686" s="3">
+        <v>12</v>
+      </c>
+      <c r="K686" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="687" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A687" s="3">
+        <v>686</v>
+      </c>
+      <c r="B687" s="3">
+        <v>79</v>
+      </c>
+      <c r="C687" s="2">
+        <v>43182</v>
+      </c>
+      <c r="D687" t="s">
+        <v>127</v>
+      </c>
+      <c r="E687">
+        <v>2018</v>
+      </c>
+      <c r="F687" t="s">
+        <v>49</v>
+      </c>
+      <c r="G687" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="H687" s="1">
+        <v>0</v>
+      </c>
+      <c r="I687" s="3">
+        <v>4</v>
+      </c>
+      <c r="J687" s="3">
+        <v>12</v>
+      </c>
+      <c r="K687" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="688" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A688" s="3">
+        <v>687</v>
+      </c>
+      <c r="B688" s="3">
+        <v>79</v>
+      </c>
+      <c r="C688" s="2">
+        <v>43182</v>
+      </c>
+      <c r="D688" t="s">
+        <v>127</v>
+      </c>
+      <c r="E688">
+        <v>2018</v>
+      </c>
+      <c r="F688" t="s">
+        <v>49</v>
+      </c>
+      <c r="G688" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="H688" s="1">
+        <v>0</v>
+      </c>
+      <c r="I688" s="3">
+        <v>4</v>
+      </c>
+      <c r="J688" s="3">
+        <v>12</v>
+      </c>
+      <c r="K688" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="689" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A689" s="3">
+        <v>688</v>
+      </c>
+      <c r="B689" s="3">
+        <v>79</v>
+      </c>
+      <c r="C689" s="2">
+        <v>43182</v>
+      </c>
+      <c r="D689" t="s">
+        <v>127</v>
+      </c>
+      <c r="E689">
+        <v>2018</v>
+      </c>
+      <c r="F689" t="s">
+        <v>49</v>
+      </c>
+      <c r="G689" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="H689" s="1">
+        <v>0</v>
+      </c>
+      <c r="I689" s="3">
+        <v>4</v>
+      </c>
+      <c r="J689" s="3">
+        <v>20</v>
+      </c>
+      <c r="K689" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="690" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A690" s="3">
+        <v>689</v>
+      </c>
+      <c r="B690" s="3">
+        <v>80</v>
+      </c>
+      <c r="C690" s="2">
+        <v>43184</v>
+      </c>
+      <c r="D690" t="s">
+        <v>127</v>
+      </c>
+      <c r="E690">
+        <v>2018</v>
+      </c>
+      <c r="F690" t="s">
+        <v>44</v>
+      </c>
+      <c r="G690" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H690" s="1">
+        <v>85</v>
+      </c>
+      <c r="I690" s="3">
+        <v>5</v>
+      </c>
+      <c r="J690" s="3">
+        <v>5</v>
+      </c>
+      <c r="K690" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="691" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A691" s="3">
+        <v>690</v>
+      </c>
+      <c r="B691" s="3">
+        <v>80</v>
+      </c>
+      <c r="C691" s="2">
+        <v>43184</v>
+      </c>
+      <c r="D691" t="s">
+        <v>127</v>
+      </c>
+      <c r="E691">
+        <v>2018</v>
+      </c>
+      <c r="F691" t="s">
+        <v>44</v>
+      </c>
+      <c r="G691" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H691" s="1">
+        <v>50</v>
+      </c>
+      <c r="I691" s="3">
+        <v>5</v>
+      </c>
+      <c r="J691" s="3">
+        <v>5</v>
+      </c>
+      <c r="K691" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="692" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A692" s="3">
+        <v>691</v>
+      </c>
+      <c r="B692" s="3">
+        <v>80</v>
+      </c>
+      <c r="C692" s="2">
+        <v>43184</v>
+      </c>
+      <c r="D692" t="s">
+        <v>127</v>
+      </c>
+      <c r="E692">
+        <v>2018</v>
+      </c>
+      <c r="F692" t="s">
+        <v>44</v>
+      </c>
+      <c r="G692" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H692" s="1">
+        <v>90</v>
+      </c>
+      <c r="I692" s="3">
+        <v>5</v>
+      </c>
+      <c r="J692" s="3">
+        <v>5</v>
+      </c>
+      <c r="K692" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="693" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A693" s="3">
+        <v>692</v>
+      </c>
+      <c r="B693" s="3">
+        <v>80</v>
+      </c>
+      <c r="C693" s="2">
+        <v>43184</v>
+      </c>
+      <c r="D693" t="s">
+        <v>127</v>
+      </c>
+      <c r="E693">
+        <v>2018</v>
+      </c>
+      <c r="F693" t="s">
+        <v>44</v>
+      </c>
+      <c r="G693" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H693" s="1">
+        <v>93.8</v>
+      </c>
+      <c r="I693" s="3">
+        <v>4</v>
+      </c>
+      <c r="J693" s="3">
+        <v>5</v>
+      </c>
+      <c r="K693" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="694" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A694" s="3">
+        <v>693</v>
+      </c>
+      <c r="B694" s="3">
+        <v>80</v>
+      </c>
+      <c r="C694" s="2">
+        <v>43184</v>
+      </c>
+      <c r="D694" t="s">
+        <v>127</v>
+      </c>
+      <c r="E694">
+        <v>2018</v>
+      </c>
+      <c r="F694" t="s">
+        <v>44</v>
+      </c>
+      <c r="G694" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="H694" s="1">
+        <v>30</v>
+      </c>
+      <c r="I694" s="3">
+        <v>3</v>
+      </c>
+      <c r="J694" s="3">
+        <v>12</v>
+      </c>
+      <c r="K694" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="695" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A695" s="3">
+        <v>694</v>
+      </c>
+      <c r="B695" s="3">
+        <v>80</v>
+      </c>
+      <c r="C695" s="2">
+        <v>43184</v>
+      </c>
+      <c r="D695" t="s">
+        <v>127</v>
+      </c>
+      <c r="E695">
+        <v>2018</v>
+      </c>
+      <c r="F695" t="s">
+        <v>44</v>
+      </c>
+      <c r="G695" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H695" s="1">
+        <v>30</v>
+      </c>
+      <c r="I695" s="3">
+        <v>3</v>
+      </c>
+      <c r="J695" s="3">
+        <v>12</v>
+      </c>
+      <c r="K695" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="696" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A696" s="3">
+        <v>695</v>
+      </c>
+      <c r="B696" s="3">
+        <v>80</v>
+      </c>
+      <c r="C696" s="2">
+        <v>43184</v>
+      </c>
+      <c r="D696" t="s">
+        <v>127</v>
+      </c>
+      <c r="E696">
+        <v>2018</v>
+      </c>
+      <c r="F696" t="s">
+        <v>44</v>
+      </c>
+      <c r="G696" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H696" s="1">
+        <v>0</v>
+      </c>
+      <c r="I696" s="3">
+        <v>3</v>
+      </c>
+      <c r="J696" s="3">
+        <v>30</v>
+      </c>
+      <c r="K696" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="697" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A697" s="3">
+        <v>696</v>
+      </c>
+      <c r="B697" s="3">
+        <v>80</v>
+      </c>
+      <c r="C697" s="2">
+        <v>43184</v>
+      </c>
+      <c r="D697" t="s">
+        <v>127</v>
+      </c>
+      <c r="E697">
+        <v>2018</v>
+      </c>
+      <c r="F697" t="s">
+        <v>44</v>
+      </c>
+      <c r="G697" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="H697" s="1">
+        <v>0</v>
+      </c>
+      <c r="I697" s="3">
+        <v>3</v>
+      </c>
+      <c r="J697" s="3">
+        <v>12</v>
+      </c>
+      <c r="K697" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="698" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A698" s="3">
+        <v>697</v>
+      </c>
+      <c r="B698" s="3">
+        <v>80</v>
+      </c>
+      <c r="C698" s="2">
+        <v>43184</v>
+      </c>
+      <c r="D698" t="s">
+        <v>127</v>
+      </c>
+      <c r="E698">
+        <v>2018</v>
+      </c>
+      <c r="F698" t="s">
+        <v>44</v>
+      </c>
+      <c r="G698" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H698" s="1">
+        <v>0</v>
+      </c>
+      <c r="I698" s="3">
+        <v>3</v>
+      </c>
+      <c r="J698" s="3">
+        <v>15</v>
+      </c>
+      <c r="K698" t="s">
+        <v>88</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updating GymWorkouts file 08/04/2018
</commit_message>
<xml_diff>
--- a/datasets/GymWorkouts.xlsx
+++ b/datasets/GymWorkouts.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Will\Documents\Data Science\My Projects\My Data Project\mydata\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{747886B9-3EE8-443F-BB41-684343AAB5DE}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3F4B733-527E-4714-B77F-0CB1CFB9B826}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="11640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2927" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3055" uniqueCount="134">
   <si>
     <t>Exercise Date</t>
   </si>
@@ -425,6 +425,9 @@
   <si>
     <t>April</t>
   </si>
+  <si>
+    <t>Leg Press</t>
+  </si>
 </sst>
 </file>
 
@@ -778,11 +781,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K730"/>
+  <dimension ref="A1:K762"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A703" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A711" sqref="A711:A730"/>
+      <pane ySplit="1" topLeftCell="A739" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C764" sqref="C764"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -26350,6 +26353,1126 @@
         <v>88</v>
       </c>
     </row>
+    <row r="731" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A731" s="3">
+        <v>730</v>
+      </c>
+      <c r="B731" s="3">
+        <v>85</v>
+      </c>
+      <c r="C731" s="2">
+        <v>43192</v>
+      </c>
+      <c r="D731" t="s">
+        <v>132</v>
+      </c>
+      <c r="E731">
+        <v>2018</v>
+      </c>
+      <c r="F731" t="s">
+        <v>17</v>
+      </c>
+      <c r="G731" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H731" s="1">
+        <v>85</v>
+      </c>
+      <c r="I731" s="3">
+        <v>5</v>
+      </c>
+      <c r="J731" s="3">
+        <v>5</v>
+      </c>
+      <c r="K731" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="732" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A732" s="3">
+        <v>731</v>
+      </c>
+      <c r="B732" s="3">
+        <v>85</v>
+      </c>
+      <c r="C732" s="2">
+        <v>43192</v>
+      </c>
+      <c r="D732" t="s">
+        <v>132</v>
+      </c>
+      <c r="E732">
+        <v>2018</v>
+      </c>
+      <c r="F732" t="s">
+        <v>17</v>
+      </c>
+      <c r="G732" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H732" s="1">
+        <v>50</v>
+      </c>
+      <c r="I732" s="3">
+        <v>5</v>
+      </c>
+      <c r="J732" s="3">
+        <v>5</v>
+      </c>
+      <c r="K732" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="733" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A733" s="3">
+        <v>732</v>
+      </c>
+      <c r="B733" s="3">
+        <v>85</v>
+      </c>
+      <c r="C733" s="2">
+        <v>43192</v>
+      </c>
+      <c r="D733" t="s">
+        <v>132</v>
+      </c>
+      <c r="E733">
+        <v>2018</v>
+      </c>
+      <c r="F733" t="s">
+        <v>17</v>
+      </c>
+      <c r="G733" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H733" s="1">
+        <v>90</v>
+      </c>
+      <c r="I733" s="3">
+        <v>5</v>
+      </c>
+      <c r="J733" s="3">
+        <v>5</v>
+      </c>
+      <c r="K733" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="734" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A734" s="3">
+        <v>733</v>
+      </c>
+      <c r="B734" s="3">
+        <v>85</v>
+      </c>
+      <c r="C734" s="2">
+        <v>43192</v>
+      </c>
+      <c r="D734" t="s">
+        <v>132</v>
+      </c>
+      <c r="E734">
+        <v>2018</v>
+      </c>
+      <c r="F734" t="s">
+        <v>17</v>
+      </c>
+      <c r="G734" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H734" s="1">
+        <v>93</v>
+      </c>
+      <c r="I734" s="3">
+        <v>5</v>
+      </c>
+      <c r="J734" s="3">
+        <v>5</v>
+      </c>
+      <c r="K734" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="735" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A735" s="3">
+        <v>734</v>
+      </c>
+      <c r="B735" s="3">
+        <v>85</v>
+      </c>
+      <c r="C735" s="2">
+        <v>43192</v>
+      </c>
+      <c r="D735" t="s">
+        <v>132</v>
+      </c>
+      <c r="E735">
+        <v>2018</v>
+      </c>
+      <c r="F735" t="s">
+        <v>17</v>
+      </c>
+      <c r="G735" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H735" s="1">
+        <v>30</v>
+      </c>
+      <c r="I735" s="3">
+        <v>4</v>
+      </c>
+      <c r="J735" s="3">
+        <v>12</v>
+      </c>
+      <c r="K735" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="736" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A736" s="3">
+        <v>735</v>
+      </c>
+      <c r="B736" s="3">
+        <v>85</v>
+      </c>
+      <c r="C736" s="2">
+        <v>43192</v>
+      </c>
+      <c r="D736" t="s">
+        <v>132</v>
+      </c>
+      <c r="E736">
+        <v>2018</v>
+      </c>
+      <c r="F736" t="s">
+        <v>17</v>
+      </c>
+      <c r="G736" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="H736" s="1">
+        <v>30</v>
+      </c>
+      <c r="I736" s="3">
+        <v>4</v>
+      </c>
+      <c r="J736" s="3">
+        <v>12</v>
+      </c>
+      <c r="K736" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="737" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A737" s="3">
+        <v>736</v>
+      </c>
+      <c r="B737" s="3">
+        <v>86</v>
+      </c>
+      <c r="C737" s="2">
+        <v>43194</v>
+      </c>
+      <c r="D737" t="s">
+        <v>132</v>
+      </c>
+      <c r="E737">
+        <v>2018</v>
+      </c>
+      <c r="F737" t="s">
+        <v>18</v>
+      </c>
+      <c r="G737" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H737" s="1">
+        <v>125</v>
+      </c>
+      <c r="I737" s="3">
+        <v>5</v>
+      </c>
+      <c r="J737" s="3">
+        <v>5</v>
+      </c>
+      <c r="K737" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="738" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A738" s="3">
+        <v>737</v>
+      </c>
+      <c r="B738" s="3">
+        <v>86</v>
+      </c>
+      <c r="C738" s="2">
+        <v>43194</v>
+      </c>
+      <c r="D738" t="s">
+        <v>132</v>
+      </c>
+      <c r="E738">
+        <v>2018</v>
+      </c>
+      <c r="F738" t="s">
+        <v>18</v>
+      </c>
+      <c r="G738" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H738" s="1">
+        <v>70</v>
+      </c>
+      <c r="I738" s="3">
+        <v>4</v>
+      </c>
+      <c r="J738" s="3">
+        <v>8</v>
+      </c>
+      <c r="K738" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="739" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A739" s="3">
+        <v>738</v>
+      </c>
+      <c r="B739" s="3">
+        <v>86</v>
+      </c>
+      <c r="C739" s="2">
+        <v>43194</v>
+      </c>
+      <c r="D739" t="s">
+        <v>132</v>
+      </c>
+      <c r="E739">
+        <v>2018</v>
+      </c>
+      <c r="F739" t="s">
+        <v>18</v>
+      </c>
+      <c r="G739" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H739" s="1">
+        <v>70</v>
+      </c>
+      <c r="I739" s="3">
+        <v>4</v>
+      </c>
+      <c r="J739" s="3">
+        <v>8</v>
+      </c>
+      <c r="K739" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="740" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A740" s="3">
+        <v>739</v>
+      </c>
+      <c r="B740" s="3">
+        <v>86</v>
+      </c>
+      <c r="C740" s="2">
+        <v>43194</v>
+      </c>
+      <c r="D740" t="s">
+        <v>132</v>
+      </c>
+      <c r="E740">
+        <v>2018</v>
+      </c>
+      <c r="F740" t="s">
+        <v>18</v>
+      </c>
+      <c r="G740" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="H740" s="1">
+        <v>150</v>
+      </c>
+      <c r="I740" s="3">
+        <v>4</v>
+      </c>
+      <c r="J740" s="3">
+        <v>8</v>
+      </c>
+      <c r="K740" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="741" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A741" s="3">
+        <v>740</v>
+      </c>
+      <c r="B741" s="3">
+        <v>87</v>
+      </c>
+      <c r="C741" s="2">
+        <v>43195</v>
+      </c>
+      <c r="D741" t="s">
+        <v>132</v>
+      </c>
+      <c r="E741">
+        <v>2018</v>
+      </c>
+      <c r="F741" t="s">
+        <v>16</v>
+      </c>
+      <c r="G741" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H741" s="1">
+        <v>120</v>
+      </c>
+      <c r="I741" s="3">
+        <v>5</v>
+      </c>
+      <c r="J741" s="3">
+        <v>5</v>
+      </c>
+      <c r="K741" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="742" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A742" s="3">
+        <v>741</v>
+      </c>
+      <c r="B742" s="3">
+        <v>87</v>
+      </c>
+      <c r="C742" s="2">
+        <v>43195</v>
+      </c>
+      <c r="D742" t="s">
+        <v>132</v>
+      </c>
+      <c r="E742">
+        <v>2018</v>
+      </c>
+      <c r="F742" t="s">
+        <v>16</v>
+      </c>
+      <c r="G742" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H742" s="1">
+        <v>42.5</v>
+      </c>
+      <c r="I742" s="3">
+        <v>4</v>
+      </c>
+      <c r="J742" s="3">
+        <v>8</v>
+      </c>
+      <c r="K742" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="743" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A743" s="3">
+        <v>742</v>
+      </c>
+      <c r="B743" s="3">
+        <v>87</v>
+      </c>
+      <c r="C743" s="2">
+        <v>43195</v>
+      </c>
+      <c r="D743" t="s">
+        <v>132</v>
+      </c>
+      <c r="E743">
+        <v>2018</v>
+      </c>
+      <c r="F743" t="s">
+        <v>16</v>
+      </c>
+      <c r="G743" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H743" s="1">
+        <v>17.5</v>
+      </c>
+      <c r="I743" s="3">
+        <v>4</v>
+      </c>
+      <c r="J743" s="3">
+        <v>8</v>
+      </c>
+      <c r="K743" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="744" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A744" s="3">
+        <v>743</v>
+      </c>
+      <c r="B744" s="3">
+        <v>87</v>
+      </c>
+      <c r="C744" s="2">
+        <v>43195</v>
+      </c>
+      <c r="D744" t="s">
+        <v>132</v>
+      </c>
+      <c r="E744">
+        <v>2018</v>
+      </c>
+      <c r="F744" t="s">
+        <v>16</v>
+      </c>
+      <c r="G744" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="H744" s="1">
+        <v>80</v>
+      </c>
+      <c r="I744" s="3">
+        <v>4</v>
+      </c>
+      <c r="J744" s="3">
+        <v>8</v>
+      </c>
+      <c r="K744" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="745" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A745" s="3">
+        <v>744</v>
+      </c>
+      <c r="B745" s="3">
+        <v>87</v>
+      </c>
+      <c r="C745" s="2">
+        <v>43195</v>
+      </c>
+      <c r="D745" t="s">
+        <v>132</v>
+      </c>
+      <c r="E745">
+        <v>2018</v>
+      </c>
+      <c r="F745" t="s">
+        <v>16</v>
+      </c>
+      <c r="G745" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H745" s="1">
+        <v>0</v>
+      </c>
+      <c r="I745" s="3">
+        <v>4</v>
+      </c>
+      <c r="J745" s="3">
+        <v>30</v>
+      </c>
+      <c r="K745" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="746" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A746" s="3">
+        <v>745</v>
+      </c>
+      <c r="B746" s="3">
+        <v>87</v>
+      </c>
+      <c r="C746" s="2">
+        <v>43195</v>
+      </c>
+      <c r="D746" t="s">
+        <v>132</v>
+      </c>
+      <c r="E746">
+        <v>2018</v>
+      </c>
+      <c r="F746" t="s">
+        <v>16</v>
+      </c>
+      <c r="G746" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H746" s="1">
+        <v>0</v>
+      </c>
+      <c r="I746" s="3">
+        <v>4</v>
+      </c>
+      <c r="J746" s="3">
+        <v>30</v>
+      </c>
+      <c r="K746" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="747" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A747" s="3">
+        <v>746</v>
+      </c>
+      <c r="B747" s="3">
+        <v>87</v>
+      </c>
+      <c r="C747" s="2">
+        <v>43195</v>
+      </c>
+      <c r="D747" t="s">
+        <v>132</v>
+      </c>
+      <c r="E747">
+        <v>2018</v>
+      </c>
+      <c r="F747" t="s">
+        <v>16</v>
+      </c>
+      <c r="G747" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H747" s="1">
+        <v>0</v>
+      </c>
+      <c r="I747" s="3">
+        <v>4</v>
+      </c>
+      <c r="J747" s="3">
+        <v>30</v>
+      </c>
+      <c r="K747" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="748" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A748" s="3">
+        <v>747</v>
+      </c>
+      <c r="B748" s="3">
+        <v>88</v>
+      </c>
+      <c r="C748" s="2">
+        <v>43197</v>
+      </c>
+      <c r="D748" t="s">
+        <v>132</v>
+      </c>
+      <c r="E748">
+        <v>2018</v>
+      </c>
+      <c r="F748" t="s">
+        <v>79</v>
+      </c>
+      <c r="G748" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H748" s="1">
+        <v>75</v>
+      </c>
+      <c r="I748" s="3">
+        <v>5</v>
+      </c>
+      <c r="J748" s="3">
+        <v>5</v>
+      </c>
+      <c r="K748" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="749" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A749" s="3">
+        <v>748</v>
+      </c>
+      <c r="B749" s="3">
+        <v>88</v>
+      </c>
+      <c r="C749" s="2">
+        <v>43197</v>
+      </c>
+      <c r="D749" t="s">
+        <v>132</v>
+      </c>
+      <c r="E749">
+        <v>2018</v>
+      </c>
+      <c r="F749" t="s">
+        <v>79</v>
+      </c>
+      <c r="G749" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H749" s="1">
+        <v>120</v>
+      </c>
+      <c r="I749" s="3">
+        <v>5</v>
+      </c>
+      <c r="J749" s="3">
+        <v>5</v>
+      </c>
+      <c r="K749" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="750" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A750" s="3">
+        <v>749</v>
+      </c>
+      <c r="B750" s="3">
+        <v>88</v>
+      </c>
+      <c r="C750" s="2">
+        <v>43197</v>
+      </c>
+      <c r="D750" t="s">
+        <v>132</v>
+      </c>
+      <c r="E750">
+        <v>2018</v>
+      </c>
+      <c r="F750" t="s">
+        <v>79</v>
+      </c>
+      <c r="G750" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H750" s="1">
+        <v>30</v>
+      </c>
+      <c r="I750" s="3">
+        <v>5</v>
+      </c>
+      <c r="J750" s="3">
+        <v>5</v>
+      </c>
+      <c r="K750" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="751" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A751" s="3">
+        <v>750</v>
+      </c>
+      <c r="B751" s="3">
+        <v>88</v>
+      </c>
+      <c r="C751" s="2">
+        <v>43197</v>
+      </c>
+      <c r="D751" t="s">
+        <v>132</v>
+      </c>
+      <c r="E751">
+        <v>2018</v>
+      </c>
+      <c r="F751" t="s">
+        <v>79</v>
+      </c>
+      <c r="G751" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H751" s="1">
+        <v>30</v>
+      </c>
+      <c r="I751" s="3">
+        <v>5</v>
+      </c>
+      <c r="J751" s="3">
+        <v>5</v>
+      </c>
+      <c r="K751" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="752" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A752" s="3">
+        <v>751</v>
+      </c>
+      <c r="B752" s="3">
+        <v>88</v>
+      </c>
+      <c r="C752" s="2">
+        <v>43197</v>
+      </c>
+      <c r="D752" t="s">
+        <v>132</v>
+      </c>
+      <c r="E752">
+        <v>2018</v>
+      </c>
+      <c r="F752" t="s">
+        <v>79</v>
+      </c>
+      <c r="G752" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H752" s="1">
+        <v>0</v>
+      </c>
+      <c r="I752" s="3">
+        <v>4</v>
+      </c>
+      <c r="J752" s="3">
+        <v>12</v>
+      </c>
+      <c r="K752" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="753" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A753" s="3">
+        <v>752</v>
+      </c>
+      <c r="B753" s="3">
+        <v>88</v>
+      </c>
+      <c r="C753" s="2">
+        <v>43197</v>
+      </c>
+      <c r="D753" t="s">
+        <v>132</v>
+      </c>
+      <c r="E753">
+        <v>2018</v>
+      </c>
+      <c r="F753" t="s">
+        <v>79</v>
+      </c>
+      <c r="G753" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="H753" s="1">
+        <v>0</v>
+      </c>
+      <c r="I753" s="3">
+        <v>4</v>
+      </c>
+      <c r="J753" s="3">
+        <v>10</v>
+      </c>
+      <c r="K753" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="754" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A754" s="3">
+        <v>753</v>
+      </c>
+      <c r="B754" s="3">
+        <v>88</v>
+      </c>
+      <c r="C754" s="2">
+        <v>43197</v>
+      </c>
+      <c r="D754" t="s">
+        <v>132</v>
+      </c>
+      <c r="E754">
+        <v>2018</v>
+      </c>
+      <c r="F754" t="s">
+        <v>79</v>
+      </c>
+      <c r="G754" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="H754" s="1">
+        <v>0</v>
+      </c>
+      <c r="I754" s="3">
+        <v>4</v>
+      </c>
+      <c r="J754" s="3">
+        <v>12</v>
+      </c>
+      <c r="K754" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="755" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A755" s="3">
+        <v>754</v>
+      </c>
+      <c r="B755" s="3">
+        <v>88</v>
+      </c>
+      <c r="C755" s="2">
+        <v>43197</v>
+      </c>
+      <c r="D755" t="s">
+        <v>132</v>
+      </c>
+      <c r="E755">
+        <v>2018</v>
+      </c>
+      <c r="F755" t="s">
+        <v>79</v>
+      </c>
+      <c r="G755" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="H755" s="1">
+        <v>0</v>
+      </c>
+      <c r="I755" s="3">
+        <v>4</v>
+      </c>
+      <c r="J755" s="3">
+        <v>10</v>
+      </c>
+      <c r="K755" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="756" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A756" s="3">
+        <v>755</v>
+      </c>
+      <c r="B756" s="3">
+        <v>88</v>
+      </c>
+      <c r="C756" s="2">
+        <v>43197</v>
+      </c>
+      <c r="D756" t="s">
+        <v>132</v>
+      </c>
+      <c r="E756">
+        <v>2018</v>
+      </c>
+      <c r="F756" t="s">
+        <v>79</v>
+      </c>
+      <c r="G756" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="H756" s="1">
+        <v>0</v>
+      </c>
+      <c r="I756" s="3">
+        <v>4</v>
+      </c>
+      <c r="J756" s="3">
+        <v>20</v>
+      </c>
+      <c r="K756" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="757" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A757" s="3">
+        <v>756</v>
+      </c>
+      <c r="B757" s="3">
+        <v>89</v>
+      </c>
+      <c r="C757" s="2">
+        <v>43198</v>
+      </c>
+      <c r="D757" t="s">
+        <v>132</v>
+      </c>
+      <c r="E757">
+        <v>2018</v>
+      </c>
+      <c r="F757" t="s">
+        <v>44</v>
+      </c>
+      <c r="G757" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H757" s="1">
+        <v>85</v>
+      </c>
+      <c r="I757" s="3">
+        <v>5</v>
+      </c>
+      <c r="J757" s="3">
+        <v>5</v>
+      </c>
+      <c r="K757" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="758" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A758" s="3">
+        <v>757</v>
+      </c>
+      <c r="B758" s="3">
+        <v>89</v>
+      </c>
+      <c r="C758" s="2">
+        <v>43198</v>
+      </c>
+      <c r="D758" t="s">
+        <v>132</v>
+      </c>
+      <c r="E758">
+        <v>2018</v>
+      </c>
+      <c r="F758" t="s">
+        <v>44</v>
+      </c>
+      <c r="G758" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H758" s="1">
+        <v>50</v>
+      </c>
+      <c r="I758" s="3">
+        <v>5</v>
+      </c>
+      <c r="J758" s="3">
+        <v>5</v>
+      </c>
+      <c r="K758" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="759" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A759" s="3">
+        <v>758</v>
+      </c>
+      <c r="B759" s="3">
+        <v>89</v>
+      </c>
+      <c r="C759" s="2">
+        <v>43198</v>
+      </c>
+      <c r="D759" t="s">
+        <v>132</v>
+      </c>
+      <c r="E759">
+        <v>2018</v>
+      </c>
+      <c r="F759" t="s">
+        <v>44</v>
+      </c>
+      <c r="G759" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H759" s="1">
+        <v>95</v>
+      </c>
+      <c r="I759" s="3">
+        <v>5</v>
+      </c>
+      <c r="J759" s="3">
+        <v>5</v>
+      </c>
+      <c r="K759" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="760" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A760" s="3">
+        <v>759</v>
+      </c>
+      <c r="B760" s="3">
+        <v>89</v>
+      </c>
+      <c r="C760" s="2">
+        <v>43198</v>
+      </c>
+      <c r="D760" t="s">
+        <v>132</v>
+      </c>
+      <c r="E760">
+        <v>2018</v>
+      </c>
+      <c r="F760" t="s">
+        <v>44</v>
+      </c>
+      <c r="G760" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H760" s="1">
+        <v>93</v>
+      </c>
+      <c r="I760" s="3">
+        <v>5</v>
+      </c>
+      <c r="J760" s="3">
+        <v>5</v>
+      </c>
+      <c r="K760" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="761" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A761" s="3">
+        <v>760</v>
+      </c>
+      <c r="B761" s="3">
+        <v>89</v>
+      </c>
+      <c r="C761" s="2">
+        <v>43198</v>
+      </c>
+      <c r="D761" t="s">
+        <v>132</v>
+      </c>
+      <c r="E761">
+        <v>2018</v>
+      </c>
+      <c r="F761" t="s">
+        <v>44</v>
+      </c>
+      <c r="G761" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="H761" s="1">
+        <v>30</v>
+      </c>
+      <c r="I761" s="3">
+        <v>4</v>
+      </c>
+      <c r="J761" s="3">
+        <v>12</v>
+      </c>
+      <c r="K761" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="762" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A762" s="3">
+        <v>761</v>
+      </c>
+      <c r="B762" s="3">
+        <v>89</v>
+      </c>
+      <c r="C762" s="2">
+        <v>43198</v>
+      </c>
+      <c r="D762" t="s">
+        <v>132</v>
+      </c>
+      <c r="E762">
+        <v>2018</v>
+      </c>
+      <c r="F762" t="s">
+        <v>44</v>
+      </c>
+      <c r="G762" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H762" s="1">
+        <v>35</v>
+      </c>
+      <c r="I762" s="3">
+        <v>4</v>
+      </c>
+      <c r="J762" s="3">
+        <v>8</v>
+      </c>
+      <c r="K762" t="s">
+        <v>89</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updating GymWorkouts file 22/04/2018
</commit_message>
<xml_diff>
--- a/datasets/GymWorkouts.xlsx
+++ b/datasets/GymWorkouts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Will\Documents\Data Science\My Projects\My Data Project\mydata\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3F4B733-527E-4714-B77F-0CB1CFB9B826}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2DE5D87-4E23-4AEC-B530-28CA9D6180E2}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="11640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3055" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3183" uniqueCount="135">
   <si>
     <t>Exercise Date</t>
   </si>
@@ -428,6 +428,9 @@
   <si>
     <t>Leg Press</t>
   </si>
+  <si>
+    <t>Kettlebell Squat</t>
+  </si>
 </sst>
 </file>
 
@@ -781,11 +784,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K762"/>
+  <dimension ref="A1:K794"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A739" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C764" sqref="C764"/>
+      <pane ySplit="1" topLeftCell="A775" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C788" sqref="C788"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -27473,6 +27476,1126 @@
         <v>89</v>
       </c>
     </row>
+    <row r="763" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A763" s="3">
+        <v>762</v>
+      </c>
+      <c r="B763" s="3">
+        <v>90</v>
+      </c>
+      <c r="C763" s="2">
+        <v>43200</v>
+      </c>
+      <c r="D763" t="s">
+        <v>132</v>
+      </c>
+      <c r="E763">
+        <v>2018</v>
+      </c>
+      <c r="F763" t="s">
+        <v>73</v>
+      </c>
+      <c r="G763" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H763" s="1">
+        <v>85</v>
+      </c>
+      <c r="I763" s="3">
+        <v>5</v>
+      </c>
+      <c r="J763" s="3">
+        <v>5</v>
+      </c>
+      <c r="K763" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="764" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A764" s="3">
+        <v>763</v>
+      </c>
+      <c r="B764" s="3">
+        <v>90</v>
+      </c>
+      <c r="C764" s="2">
+        <v>43200</v>
+      </c>
+      <c r="D764" t="s">
+        <v>132</v>
+      </c>
+      <c r="E764">
+        <v>2018</v>
+      </c>
+      <c r="F764" t="s">
+        <v>73</v>
+      </c>
+      <c r="G764" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H764" s="1">
+        <v>108</v>
+      </c>
+      <c r="I764" s="3">
+        <v>4</v>
+      </c>
+      <c r="J764" s="3">
+        <v>8</v>
+      </c>
+      <c r="K764" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="765" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A765" s="3">
+        <v>764</v>
+      </c>
+      <c r="B765" s="3">
+        <v>90</v>
+      </c>
+      <c r="C765" s="2">
+        <v>43200</v>
+      </c>
+      <c r="D765" t="s">
+        <v>132</v>
+      </c>
+      <c r="E765">
+        <v>2018</v>
+      </c>
+      <c r="F765" t="s">
+        <v>73</v>
+      </c>
+      <c r="G765" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H765" s="1">
+        <v>75</v>
+      </c>
+      <c r="I765" s="3">
+        <v>4</v>
+      </c>
+      <c r="J765" s="3">
+        <v>8</v>
+      </c>
+      <c r="K765" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="766" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A766" s="3">
+        <v>765</v>
+      </c>
+      <c r="B766" s="3">
+        <v>90</v>
+      </c>
+      <c r="C766" s="2">
+        <v>43200</v>
+      </c>
+      <c r="D766" t="s">
+        <v>132</v>
+      </c>
+      <c r="E766">
+        <v>2018</v>
+      </c>
+      <c r="F766" t="s">
+        <v>73</v>
+      </c>
+      <c r="G766" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H766" s="1">
+        <v>65</v>
+      </c>
+      <c r="I766" s="3">
+        <v>4</v>
+      </c>
+      <c r="J766" s="3">
+        <v>8</v>
+      </c>
+      <c r="K766" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="767" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A767" s="3">
+        <v>766</v>
+      </c>
+      <c r="B767" s="3">
+        <v>91</v>
+      </c>
+      <c r="C767" s="2">
+        <v>43206</v>
+      </c>
+      <c r="D767" t="s">
+        <v>132</v>
+      </c>
+      <c r="E767">
+        <v>2018</v>
+      </c>
+      <c r="F767" t="s">
+        <v>17</v>
+      </c>
+      <c r="G767" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="H767" s="1">
+        <v>15</v>
+      </c>
+      <c r="I767" s="3">
+        <v>4</v>
+      </c>
+      <c r="J767" s="3">
+        <v>12</v>
+      </c>
+      <c r="K767" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="768" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A768" s="3">
+        <v>767</v>
+      </c>
+      <c r="B768" s="3">
+        <v>91</v>
+      </c>
+      <c r="C768" s="2">
+        <v>43206</v>
+      </c>
+      <c r="D768" t="s">
+        <v>132</v>
+      </c>
+      <c r="E768">
+        <v>2018</v>
+      </c>
+      <c r="F768" t="s">
+        <v>17</v>
+      </c>
+      <c r="G768" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="H768" s="1">
+        <v>0</v>
+      </c>
+      <c r="I768" s="3">
+        <v>4</v>
+      </c>
+      <c r="J768" s="3">
+        <v>12</v>
+      </c>
+      <c r="K768" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="769" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A769" s="3">
+        <v>768</v>
+      </c>
+      <c r="B769" s="3">
+        <v>91</v>
+      </c>
+      <c r="C769" s="2">
+        <v>43206</v>
+      </c>
+      <c r="D769" t="s">
+        <v>132</v>
+      </c>
+      <c r="E769">
+        <v>2018</v>
+      </c>
+      <c r="F769" t="s">
+        <v>17</v>
+      </c>
+      <c r="G769" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H769" s="1">
+        <v>0</v>
+      </c>
+      <c r="I769" s="3">
+        <v>4</v>
+      </c>
+      <c r="J769" s="3">
+        <v>12</v>
+      </c>
+      <c r="K769" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="770" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A770" s="3">
+        <v>769</v>
+      </c>
+      <c r="B770" s="3">
+        <v>91</v>
+      </c>
+      <c r="C770" s="2">
+        <v>43206</v>
+      </c>
+      <c r="D770" t="s">
+        <v>132</v>
+      </c>
+      <c r="E770">
+        <v>2018</v>
+      </c>
+      <c r="F770" t="s">
+        <v>17</v>
+      </c>
+      <c r="G770" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="H770" s="1">
+        <v>0</v>
+      </c>
+      <c r="I770" s="3">
+        <v>4</v>
+      </c>
+      <c r="J770" s="3">
+        <v>10</v>
+      </c>
+      <c r="K770" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="771" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A771" s="3">
+        <v>770</v>
+      </c>
+      <c r="B771" s="3">
+        <v>91</v>
+      </c>
+      <c r="C771" s="2">
+        <v>43206</v>
+      </c>
+      <c r="D771" t="s">
+        <v>132</v>
+      </c>
+      <c r="E771">
+        <v>2018</v>
+      </c>
+      <c r="F771" t="s">
+        <v>17</v>
+      </c>
+      <c r="G771" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="H771" s="1">
+        <v>0</v>
+      </c>
+      <c r="I771" s="3">
+        <v>4</v>
+      </c>
+      <c r="J771" s="3">
+        <v>10</v>
+      </c>
+      <c r="K771" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="772" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A772" s="3">
+        <v>771</v>
+      </c>
+      <c r="B772" s="3">
+        <v>91</v>
+      </c>
+      <c r="C772" s="2">
+        <v>43206</v>
+      </c>
+      <c r="D772" t="s">
+        <v>132</v>
+      </c>
+      <c r="E772">
+        <v>2018</v>
+      </c>
+      <c r="F772" t="s">
+        <v>17</v>
+      </c>
+      <c r="G772" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="H772" s="1">
+        <v>0</v>
+      </c>
+      <c r="I772" s="3">
+        <v>4</v>
+      </c>
+      <c r="J772" s="3">
+        <v>12</v>
+      </c>
+      <c r="K772" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="773" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A773" s="3">
+        <v>772</v>
+      </c>
+      <c r="B773" s="3">
+        <v>91</v>
+      </c>
+      <c r="C773" s="2">
+        <v>43206</v>
+      </c>
+      <c r="D773" t="s">
+        <v>132</v>
+      </c>
+      <c r="E773">
+        <v>2018</v>
+      </c>
+      <c r="F773" t="s">
+        <v>17</v>
+      </c>
+      <c r="G773" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="H773" s="1">
+        <v>0</v>
+      </c>
+      <c r="I773" s="3">
+        <v>4</v>
+      </c>
+      <c r="J773" s="3">
+        <v>20</v>
+      </c>
+      <c r="K773" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="774" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A774" s="3">
+        <v>773</v>
+      </c>
+      <c r="B774" s="3">
+        <v>92</v>
+      </c>
+      <c r="C774" s="2">
+        <v>43207</v>
+      </c>
+      <c r="D774" t="s">
+        <v>132</v>
+      </c>
+      <c r="E774">
+        <v>2018</v>
+      </c>
+      <c r="F774" t="s">
+        <v>73</v>
+      </c>
+      <c r="G774" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H774" s="1">
+        <v>75</v>
+      </c>
+      <c r="I774" s="3">
+        <v>5</v>
+      </c>
+      <c r="J774" s="3">
+        <v>5</v>
+      </c>
+      <c r="K774" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="775" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A775" s="3">
+        <v>774</v>
+      </c>
+      <c r="B775" s="3">
+        <v>92</v>
+      </c>
+      <c r="C775" s="2">
+        <v>43207</v>
+      </c>
+      <c r="D775" t="s">
+        <v>132</v>
+      </c>
+      <c r="E775">
+        <v>2018</v>
+      </c>
+      <c r="F775" t="s">
+        <v>73</v>
+      </c>
+      <c r="G775" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H775" s="1">
+        <v>30</v>
+      </c>
+      <c r="I775" s="3">
+        <v>4</v>
+      </c>
+      <c r="J775" s="3">
+        <v>12</v>
+      </c>
+      <c r="K775" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="776" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A776" s="3">
+        <v>775</v>
+      </c>
+      <c r="B776" s="3">
+        <v>92</v>
+      </c>
+      <c r="C776" s="2">
+        <v>43207</v>
+      </c>
+      <c r="D776" t="s">
+        <v>132</v>
+      </c>
+      <c r="E776">
+        <v>2018</v>
+      </c>
+      <c r="F776" t="s">
+        <v>73</v>
+      </c>
+      <c r="G776" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="H776" s="1">
+        <v>30</v>
+      </c>
+      <c r="I776" s="3">
+        <v>4</v>
+      </c>
+      <c r="J776" s="3">
+        <v>12</v>
+      </c>
+      <c r="K776" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="777" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A777" s="3">
+        <v>776</v>
+      </c>
+      <c r="B777" s="3">
+        <v>92</v>
+      </c>
+      <c r="C777" s="2">
+        <v>43207</v>
+      </c>
+      <c r="D777" t="s">
+        <v>132</v>
+      </c>
+      <c r="E777">
+        <v>2018</v>
+      </c>
+      <c r="F777" t="s">
+        <v>73</v>
+      </c>
+      <c r="G777" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="H777" s="1">
+        <v>80</v>
+      </c>
+      <c r="I777" s="3">
+        <v>4</v>
+      </c>
+      <c r="J777" s="3">
+        <v>8</v>
+      </c>
+      <c r="K777" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="778" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A778" s="3">
+        <v>777</v>
+      </c>
+      <c r="B778" s="3">
+        <v>93</v>
+      </c>
+      <c r="C778" s="2">
+        <v>43209</v>
+      </c>
+      <c r="D778" t="s">
+        <v>132</v>
+      </c>
+      <c r="E778">
+        <v>2018</v>
+      </c>
+      <c r="F778" t="s">
+        <v>16</v>
+      </c>
+      <c r="G778" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H778" s="1">
+        <v>120</v>
+      </c>
+      <c r="I778" s="3">
+        <v>4</v>
+      </c>
+      <c r="J778" s="3">
+        <v>5</v>
+      </c>
+      <c r="K778" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="779" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A779" s="3">
+        <v>778</v>
+      </c>
+      <c r="B779" s="3">
+        <v>93</v>
+      </c>
+      <c r="C779" s="2">
+        <v>43209</v>
+      </c>
+      <c r="D779" t="s">
+        <v>132</v>
+      </c>
+      <c r="E779">
+        <v>2018</v>
+      </c>
+      <c r="F779" t="s">
+        <v>16</v>
+      </c>
+      <c r="G779" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="H779" s="1">
+        <v>40</v>
+      </c>
+      <c r="I779" s="3">
+        <v>4</v>
+      </c>
+      <c r="J779" s="3">
+        <v>12</v>
+      </c>
+      <c r="K779" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="780" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A780" s="3">
+        <v>779</v>
+      </c>
+      <c r="B780" s="3">
+        <v>93</v>
+      </c>
+      <c r="C780" s="2">
+        <v>43209</v>
+      </c>
+      <c r="D780" t="s">
+        <v>132</v>
+      </c>
+      <c r="E780">
+        <v>2018</v>
+      </c>
+      <c r="F780" t="s">
+        <v>16</v>
+      </c>
+      <c r="G780" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H780" s="1">
+        <v>155</v>
+      </c>
+      <c r="I780" s="3">
+        <v>4</v>
+      </c>
+      <c r="J780" s="3">
+        <v>8</v>
+      </c>
+      <c r="K780" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="781" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A781" s="3">
+        <v>780</v>
+      </c>
+      <c r="B781" s="3">
+        <v>93</v>
+      </c>
+      <c r="C781" s="2">
+        <v>43209</v>
+      </c>
+      <c r="D781" t="s">
+        <v>132</v>
+      </c>
+      <c r="E781">
+        <v>2018</v>
+      </c>
+      <c r="F781" t="s">
+        <v>16</v>
+      </c>
+      <c r="G781" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="H781" s="1">
+        <v>28</v>
+      </c>
+      <c r="I781" s="3">
+        <v>4</v>
+      </c>
+      <c r="J781" s="3">
+        <v>8</v>
+      </c>
+      <c r="K781" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="782" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A782" s="3">
+        <v>781</v>
+      </c>
+      <c r="B782" s="3">
+        <v>93</v>
+      </c>
+      <c r="C782" s="2">
+        <v>43209</v>
+      </c>
+      <c r="D782" t="s">
+        <v>132</v>
+      </c>
+      <c r="E782">
+        <v>2018</v>
+      </c>
+      <c r="F782" t="s">
+        <v>16</v>
+      </c>
+      <c r="G782" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="H782" s="1">
+        <v>24</v>
+      </c>
+      <c r="I782" s="3">
+        <v>4</v>
+      </c>
+      <c r="J782" s="3">
+        <v>30</v>
+      </c>
+      <c r="K782" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="783" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A783" s="3">
+        <v>782</v>
+      </c>
+      <c r="B783" s="3">
+        <v>94</v>
+      </c>
+      <c r="C783" s="2">
+        <v>43210</v>
+      </c>
+      <c r="D783" t="s">
+        <v>132</v>
+      </c>
+      <c r="E783">
+        <v>2018</v>
+      </c>
+      <c r="F783" t="s">
+        <v>49</v>
+      </c>
+      <c r="G783" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H783" s="1">
+        <v>42.5</v>
+      </c>
+      <c r="I783" s="3">
+        <v>4</v>
+      </c>
+      <c r="J783" s="3">
+        <v>8</v>
+      </c>
+      <c r="K783" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="784" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A784" s="3">
+        <v>783</v>
+      </c>
+      <c r="B784" s="3">
+        <v>94</v>
+      </c>
+      <c r="C784" s="2">
+        <v>43210</v>
+      </c>
+      <c r="D784" t="s">
+        <v>132</v>
+      </c>
+      <c r="E784">
+        <v>2018</v>
+      </c>
+      <c r="F784" t="s">
+        <v>49</v>
+      </c>
+      <c r="G784" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H784" s="1">
+        <v>17.5</v>
+      </c>
+      <c r="I784" s="3">
+        <v>4</v>
+      </c>
+      <c r="J784" s="3">
+        <v>8</v>
+      </c>
+      <c r="K784" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="785" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A785" s="3">
+        <v>784</v>
+      </c>
+      <c r="B785" s="3">
+        <v>94</v>
+      </c>
+      <c r="C785" s="2">
+        <v>43210</v>
+      </c>
+      <c r="D785" t="s">
+        <v>132</v>
+      </c>
+      <c r="E785">
+        <v>2018</v>
+      </c>
+      <c r="F785" t="s">
+        <v>49</v>
+      </c>
+      <c r="G785" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H785" s="1">
+        <v>30</v>
+      </c>
+      <c r="I785" s="3">
+        <v>4</v>
+      </c>
+      <c r="J785" s="3">
+        <v>8</v>
+      </c>
+      <c r="K785" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="786" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A786" s="3">
+        <v>785</v>
+      </c>
+      <c r="B786" s="3">
+        <v>94</v>
+      </c>
+      <c r="C786" s="2">
+        <v>43210</v>
+      </c>
+      <c r="D786" t="s">
+        <v>132</v>
+      </c>
+      <c r="E786">
+        <v>2018</v>
+      </c>
+      <c r="F786" t="s">
+        <v>49</v>
+      </c>
+      <c r="G786" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="H786" s="1">
+        <v>10</v>
+      </c>
+      <c r="I786" s="3">
+        <v>4</v>
+      </c>
+      <c r="J786" s="3">
+        <v>8</v>
+      </c>
+      <c r="K786" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="787" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A787" s="3">
+        <v>786</v>
+      </c>
+      <c r="B787" s="3">
+        <v>94</v>
+      </c>
+      <c r="C787" s="2">
+        <v>43210</v>
+      </c>
+      <c r="D787" t="s">
+        <v>132</v>
+      </c>
+      <c r="E787">
+        <v>2018</v>
+      </c>
+      <c r="F787" t="s">
+        <v>49</v>
+      </c>
+      <c r="G787" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H787" s="1">
+        <v>10</v>
+      </c>
+      <c r="I787" s="3">
+        <v>4</v>
+      </c>
+      <c r="J787" s="3">
+        <v>8</v>
+      </c>
+      <c r="K787" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="788" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A788" s="3">
+        <v>787</v>
+      </c>
+      <c r="B788" s="3">
+        <v>94</v>
+      </c>
+      <c r="C788" s="2">
+        <v>43210</v>
+      </c>
+      <c r="D788" t="s">
+        <v>132</v>
+      </c>
+      <c r="E788">
+        <v>2018</v>
+      </c>
+      <c r="F788" t="s">
+        <v>49</v>
+      </c>
+      <c r="G788" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="H788" s="1">
+        <v>10</v>
+      </c>
+      <c r="I788" s="3">
+        <v>4</v>
+      </c>
+      <c r="J788" s="3">
+        <v>8</v>
+      </c>
+      <c r="K788" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="789" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A789" s="3">
+        <v>788</v>
+      </c>
+      <c r="B789" s="3">
+        <v>95</v>
+      </c>
+      <c r="C789" s="2">
+        <v>43211</v>
+      </c>
+      <c r="D789" t="s">
+        <v>132</v>
+      </c>
+      <c r="E789">
+        <v>2018</v>
+      </c>
+      <c r="F789" t="s">
+        <v>79</v>
+      </c>
+      <c r="G789" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H789" s="1">
+        <v>85</v>
+      </c>
+      <c r="I789" s="3">
+        <v>5</v>
+      </c>
+      <c r="J789" s="3">
+        <v>5</v>
+      </c>
+      <c r="K789" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="790" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A790" s="3">
+        <v>789</v>
+      </c>
+      <c r="B790" s="3">
+        <v>95</v>
+      </c>
+      <c r="C790" s="2">
+        <v>43211</v>
+      </c>
+      <c r="D790" t="s">
+        <v>132</v>
+      </c>
+      <c r="E790">
+        <v>2018</v>
+      </c>
+      <c r="F790" t="s">
+        <v>79</v>
+      </c>
+      <c r="G790" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H790" s="1">
+        <v>50</v>
+      </c>
+      <c r="I790" s="3">
+        <v>5</v>
+      </c>
+      <c r="J790" s="3">
+        <v>5</v>
+      </c>
+      <c r="K790" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="791" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A791" s="3">
+        <v>790</v>
+      </c>
+      <c r="B791" s="3">
+        <v>95</v>
+      </c>
+      <c r="C791" s="2">
+        <v>43211</v>
+      </c>
+      <c r="D791" t="s">
+        <v>132</v>
+      </c>
+      <c r="E791">
+        <v>2018</v>
+      </c>
+      <c r="F791" t="s">
+        <v>79</v>
+      </c>
+      <c r="G791" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H791" s="1">
+        <v>95</v>
+      </c>
+      <c r="I791" s="3">
+        <v>5</v>
+      </c>
+      <c r="J791" s="3">
+        <v>5</v>
+      </c>
+      <c r="K791" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="792" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A792" s="3">
+        <v>791</v>
+      </c>
+      <c r="B792" s="3">
+        <v>95</v>
+      </c>
+      <c r="C792" s="2">
+        <v>43211</v>
+      </c>
+      <c r="D792" t="s">
+        <v>132</v>
+      </c>
+      <c r="E792">
+        <v>2018</v>
+      </c>
+      <c r="F792" t="s">
+        <v>79</v>
+      </c>
+      <c r="G792" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H792" s="1">
+        <v>94</v>
+      </c>
+      <c r="I792" s="3">
+        <v>4</v>
+      </c>
+      <c r="J792" s="3">
+        <v>5</v>
+      </c>
+      <c r="K792" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="793" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A793" s="3">
+        <v>792</v>
+      </c>
+      <c r="B793" s="3">
+        <v>95</v>
+      </c>
+      <c r="C793" s="2">
+        <v>43211</v>
+      </c>
+      <c r="D793" t="s">
+        <v>132</v>
+      </c>
+      <c r="E793">
+        <v>2018</v>
+      </c>
+      <c r="F793" t="s">
+        <v>79</v>
+      </c>
+      <c r="G793" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H793" s="1">
+        <v>35</v>
+      </c>
+      <c r="I793" s="3">
+        <v>4</v>
+      </c>
+      <c r="J793" s="3">
+        <v>8</v>
+      </c>
+      <c r="K793" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="794" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A794" s="3">
+        <v>793</v>
+      </c>
+      <c r="B794" s="3">
+        <v>95</v>
+      </c>
+      <c r="C794" s="2">
+        <v>43211</v>
+      </c>
+      <c r="D794" t="s">
+        <v>132</v>
+      </c>
+      <c r="E794">
+        <v>2018</v>
+      </c>
+      <c r="F794" t="s">
+        <v>79</v>
+      </c>
+      <c r="G794" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="H794" s="1">
+        <v>35</v>
+      </c>
+      <c r="I794" s="3">
+        <v>4</v>
+      </c>
+      <c r="J794" s="3">
+        <v>8</v>
+      </c>
+      <c r="K794" t="s">
+        <v>90</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updating GymWorkouts files 29/04/2018
</commit_message>
<xml_diff>
--- a/datasets/GymWorkouts.xlsx
+++ b/datasets/GymWorkouts.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Will\Documents\Data Science\My Projects\My Data Project\mydata\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2DE5D87-4E23-4AEC-B530-28CA9D6180E2}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65F1A110-4807-47B0-BE59-8F79AFFE5012}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="11640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3183" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3279" uniqueCount="136">
   <si>
     <t>Exercise Date</t>
   </si>
@@ -431,6 +431,9 @@
   <si>
     <t>Kettlebell Squat</t>
   </si>
+  <si>
+    <t>Row (machine)</t>
+  </si>
 </sst>
 </file>
 
@@ -784,11 +787,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K794"/>
+  <dimension ref="A1:K818"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A775" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C788" sqref="C788"/>
+      <pane ySplit="1" topLeftCell="A795" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A819" sqref="A819"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -28596,6 +28599,846 @@
         <v>90</v>
       </c>
     </row>
+    <row r="795" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A795" s="3">
+        <v>794</v>
+      </c>
+      <c r="B795" s="3">
+        <v>96</v>
+      </c>
+      <c r="C795" s="2">
+        <v>43213</v>
+      </c>
+      <c r="D795" t="s">
+        <v>132</v>
+      </c>
+      <c r="E795">
+        <v>2018</v>
+      </c>
+      <c r="F795" t="s">
+        <v>17</v>
+      </c>
+      <c r="G795" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H795" s="1">
+        <v>25</v>
+      </c>
+      <c r="I795" s="3">
+        <v>4</v>
+      </c>
+      <c r="J795" s="3">
+        <v>8</v>
+      </c>
+      <c r="K795" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="796" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A796" s="3">
+        <v>795</v>
+      </c>
+      <c r="B796" s="3">
+        <v>96</v>
+      </c>
+      <c r="C796" s="2">
+        <v>43213</v>
+      </c>
+      <c r="D796" t="s">
+        <v>132</v>
+      </c>
+      <c r="E796">
+        <v>2018</v>
+      </c>
+      <c r="F796" t="s">
+        <v>17</v>
+      </c>
+      <c r="G796" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H796" s="1">
+        <v>25</v>
+      </c>
+      <c r="I796" s="3">
+        <v>4</v>
+      </c>
+      <c r="J796" s="3">
+        <v>8</v>
+      </c>
+      <c r="K796" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="797" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A797" s="3">
+        <v>796</v>
+      </c>
+      <c r="B797" s="3">
+        <v>96</v>
+      </c>
+      <c r="C797" s="2">
+        <v>43213</v>
+      </c>
+      <c r="D797" t="s">
+        <v>132</v>
+      </c>
+      <c r="E797">
+        <v>2018</v>
+      </c>
+      <c r="F797" t="s">
+        <v>17</v>
+      </c>
+      <c r="G797" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H797" s="1">
+        <v>108</v>
+      </c>
+      <c r="I797" s="3">
+        <v>4</v>
+      </c>
+      <c r="J797" s="3">
+        <v>8</v>
+      </c>
+      <c r="K797" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="798" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A798" s="3">
+        <v>797</v>
+      </c>
+      <c r="B798" s="3">
+        <v>96</v>
+      </c>
+      <c r="C798" s="2">
+        <v>43213</v>
+      </c>
+      <c r="D798" t="s">
+        <v>132</v>
+      </c>
+      <c r="E798">
+        <v>2018</v>
+      </c>
+      <c r="F798" t="s">
+        <v>17</v>
+      </c>
+      <c r="G798" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="H798" s="1">
+        <v>30</v>
+      </c>
+      <c r="I798" s="3">
+        <v>4</v>
+      </c>
+      <c r="J798" s="3">
+        <v>8</v>
+      </c>
+      <c r="K798" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="799" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A799" s="3">
+        <v>798</v>
+      </c>
+      <c r="B799" s="3">
+        <v>96</v>
+      </c>
+      <c r="C799" s="2">
+        <v>43213</v>
+      </c>
+      <c r="D799" t="s">
+        <v>132</v>
+      </c>
+      <c r="E799">
+        <v>2018</v>
+      </c>
+      <c r="F799" t="s">
+        <v>17</v>
+      </c>
+      <c r="G799" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H799" s="1">
+        <v>0</v>
+      </c>
+      <c r="I799" s="3">
+        <v>4</v>
+      </c>
+      <c r="J799" s="3">
+        <v>10</v>
+      </c>
+      <c r="K799" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="800" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A800" s="3">
+        <v>799</v>
+      </c>
+      <c r="B800" s="3">
+        <v>96</v>
+      </c>
+      <c r="C800" s="2">
+        <v>43213</v>
+      </c>
+      <c r="D800" t="s">
+        <v>132</v>
+      </c>
+      <c r="E800">
+        <v>2018</v>
+      </c>
+      <c r="F800" t="s">
+        <v>17</v>
+      </c>
+      <c r="G800" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H800" s="1">
+        <v>0</v>
+      </c>
+      <c r="I800" s="3">
+        <v>4</v>
+      </c>
+      <c r="J800" s="3">
+        <v>30</v>
+      </c>
+      <c r="K800" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="801" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A801" s="3">
+        <v>800</v>
+      </c>
+      <c r="B801" s="3">
+        <v>97</v>
+      </c>
+      <c r="C801" s="2">
+        <v>43215</v>
+      </c>
+      <c r="D801" t="s">
+        <v>132</v>
+      </c>
+      <c r="E801">
+        <v>2018</v>
+      </c>
+      <c r="F801" t="s">
+        <v>18</v>
+      </c>
+      <c r="G801" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H801" s="1">
+        <v>110</v>
+      </c>
+      <c r="I801" s="3">
+        <v>4</v>
+      </c>
+      <c r="J801" s="3">
+        <v>8</v>
+      </c>
+      <c r="K801" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="802" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A802" s="3">
+        <v>801</v>
+      </c>
+      <c r="B802" s="3">
+        <v>97</v>
+      </c>
+      <c r="C802" s="2">
+        <v>43215</v>
+      </c>
+      <c r="D802" t="s">
+        <v>132</v>
+      </c>
+      <c r="E802">
+        <v>2018</v>
+      </c>
+      <c r="F802" t="s">
+        <v>18</v>
+      </c>
+      <c r="G802" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H802" s="1">
+        <v>35</v>
+      </c>
+      <c r="I802" s="3">
+        <v>4</v>
+      </c>
+      <c r="J802" s="3">
+        <v>8</v>
+      </c>
+      <c r="K802" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="803" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A803" s="3">
+        <v>802</v>
+      </c>
+      <c r="B803" s="3">
+        <v>97</v>
+      </c>
+      <c r="C803" s="2">
+        <v>43215</v>
+      </c>
+      <c r="D803" t="s">
+        <v>132</v>
+      </c>
+      <c r="E803">
+        <v>2018</v>
+      </c>
+      <c r="F803" t="s">
+        <v>18</v>
+      </c>
+      <c r="G803" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="H803" s="1">
+        <v>60</v>
+      </c>
+      <c r="I803" s="3">
+        <v>4</v>
+      </c>
+      <c r="J803" s="3">
+        <v>8</v>
+      </c>
+      <c r="K803" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="804" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A804" s="3">
+        <v>803</v>
+      </c>
+      <c r="B804" s="3">
+        <v>97</v>
+      </c>
+      <c r="C804" s="2">
+        <v>43215</v>
+      </c>
+      <c r="D804" t="s">
+        <v>132</v>
+      </c>
+      <c r="E804">
+        <v>2018</v>
+      </c>
+      <c r="F804" t="s">
+        <v>18</v>
+      </c>
+      <c r="G804" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="H804" s="1">
+        <v>15</v>
+      </c>
+      <c r="I804" s="3">
+        <v>4</v>
+      </c>
+      <c r="J804" s="3">
+        <v>12</v>
+      </c>
+      <c r="K804" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="805" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A805" s="3">
+        <v>804</v>
+      </c>
+      <c r="B805" s="3">
+        <v>97</v>
+      </c>
+      <c r="C805" s="2">
+        <v>43215</v>
+      </c>
+      <c r="D805" t="s">
+        <v>132</v>
+      </c>
+      <c r="E805">
+        <v>2018</v>
+      </c>
+      <c r="F805" t="s">
+        <v>18</v>
+      </c>
+      <c r="G805" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H805" s="1">
+        <v>0</v>
+      </c>
+      <c r="I805" s="3">
+        <v>3</v>
+      </c>
+      <c r="J805" s="3">
+        <v>12</v>
+      </c>
+      <c r="K805" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="806" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A806" s="3">
+        <v>805</v>
+      </c>
+      <c r="B806" s="3">
+        <v>97</v>
+      </c>
+      <c r="C806" s="2">
+        <v>43215</v>
+      </c>
+      <c r="D806" t="s">
+        <v>132</v>
+      </c>
+      <c r="E806">
+        <v>2018</v>
+      </c>
+      <c r="F806" t="s">
+        <v>18</v>
+      </c>
+      <c r="G806" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="H806" s="1">
+        <v>0</v>
+      </c>
+      <c r="I806" s="3">
+        <v>3</v>
+      </c>
+      <c r="J806" s="3">
+        <v>10</v>
+      </c>
+      <c r="K806" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="807" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A807" s="3">
+        <v>806</v>
+      </c>
+      <c r="B807" s="3">
+        <v>97</v>
+      </c>
+      <c r="C807" s="2">
+        <v>43215</v>
+      </c>
+      <c r="D807" t="s">
+        <v>132</v>
+      </c>
+      <c r="E807">
+        <v>2018</v>
+      </c>
+      <c r="F807" t="s">
+        <v>18</v>
+      </c>
+      <c r="G807" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="H807" s="1">
+        <v>0</v>
+      </c>
+      <c r="I807" s="3">
+        <v>3</v>
+      </c>
+      <c r="J807" s="3">
+        <v>12</v>
+      </c>
+      <c r="K807" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="808" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A808" s="3">
+        <v>807</v>
+      </c>
+      <c r="B808" s="3">
+        <v>97</v>
+      </c>
+      <c r="C808" s="2">
+        <v>43215</v>
+      </c>
+      <c r="D808" t="s">
+        <v>132</v>
+      </c>
+      <c r="E808">
+        <v>2018</v>
+      </c>
+      <c r="F808" t="s">
+        <v>18</v>
+      </c>
+      <c r="G808" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="H808" s="1">
+        <v>0</v>
+      </c>
+      <c r="I808" s="3">
+        <v>3</v>
+      </c>
+      <c r="J808" s="3">
+        <v>10</v>
+      </c>
+      <c r="K808" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="809" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A809" s="3">
+        <v>808</v>
+      </c>
+      <c r="B809" s="3">
+        <v>97</v>
+      </c>
+      <c r="C809" s="2">
+        <v>43215</v>
+      </c>
+      <c r="D809" t="s">
+        <v>132</v>
+      </c>
+      <c r="E809">
+        <v>2018</v>
+      </c>
+      <c r="F809" t="s">
+        <v>18</v>
+      </c>
+      <c r="G809" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="H809" s="1">
+        <v>0</v>
+      </c>
+      <c r="I809" s="3">
+        <v>3</v>
+      </c>
+      <c r="J809" s="3">
+        <v>20</v>
+      </c>
+      <c r="K809" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="810" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A810" s="3">
+        <v>809</v>
+      </c>
+      <c r="B810" s="3">
+        <v>98</v>
+      </c>
+      <c r="C810" s="2">
+        <v>43216</v>
+      </c>
+      <c r="D810" t="s">
+        <v>132</v>
+      </c>
+      <c r="E810">
+        <v>2018</v>
+      </c>
+      <c r="F810" t="s">
+        <v>16</v>
+      </c>
+      <c r="G810" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H810" s="1">
+        <v>85</v>
+      </c>
+      <c r="I810" s="3">
+        <v>5</v>
+      </c>
+      <c r="J810" s="3">
+        <v>5</v>
+      </c>
+      <c r="K810" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="811" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A811" s="3">
+        <v>810</v>
+      </c>
+      <c r="B811" s="3">
+        <v>98</v>
+      </c>
+      <c r="C811" s="2">
+        <v>43216</v>
+      </c>
+      <c r="D811" t="s">
+        <v>132</v>
+      </c>
+      <c r="E811">
+        <v>2018</v>
+      </c>
+      <c r="F811" t="s">
+        <v>16</v>
+      </c>
+      <c r="G811" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H811" s="1">
+        <v>50</v>
+      </c>
+      <c r="I811" s="3">
+        <v>5</v>
+      </c>
+      <c r="J811" s="3">
+        <v>5</v>
+      </c>
+      <c r="K811" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="812" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A812" s="3">
+        <v>811</v>
+      </c>
+      <c r="B812" s="3">
+        <v>98</v>
+      </c>
+      <c r="C812" s="2">
+        <v>43216</v>
+      </c>
+      <c r="D812" t="s">
+        <v>132</v>
+      </c>
+      <c r="E812">
+        <v>2018</v>
+      </c>
+      <c r="F812" t="s">
+        <v>16</v>
+      </c>
+      <c r="G812" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H812" s="1">
+        <v>100</v>
+      </c>
+      <c r="I812" s="3">
+        <v>5</v>
+      </c>
+      <c r="J812" s="3">
+        <v>5</v>
+      </c>
+      <c r="K812" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="813" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A813" s="3">
+        <v>812</v>
+      </c>
+      <c r="B813" s="3">
+        <v>98</v>
+      </c>
+      <c r="C813" s="2">
+        <v>43216</v>
+      </c>
+      <c r="D813" t="s">
+        <v>132</v>
+      </c>
+      <c r="E813">
+        <v>2018</v>
+      </c>
+      <c r="F813" t="s">
+        <v>16</v>
+      </c>
+      <c r="G813" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="H813" s="1">
+        <v>30</v>
+      </c>
+      <c r="I813" s="3">
+        <v>4</v>
+      </c>
+      <c r="J813" s="3">
+        <v>12</v>
+      </c>
+      <c r="K813" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="814" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A814" s="3">
+        <v>813</v>
+      </c>
+      <c r="B814" s="3">
+        <v>98</v>
+      </c>
+      <c r="C814" s="2">
+        <v>43216</v>
+      </c>
+      <c r="D814" t="s">
+        <v>132</v>
+      </c>
+      <c r="E814">
+        <v>2018</v>
+      </c>
+      <c r="F814" t="s">
+        <v>16</v>
+      </c>
+      <c r="G814" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="H814" s="1">
+        <v>0</v>
+      </c>
+      <c r="I814" s="3">
+        <v>1</v>
+      </c>
+      <c r="J814" s="3">
+        <v>60</v>
+      </c>
+      <c r="K814" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="815" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A815" s="3">
+        <v>814</v>
+      </c>
+      <c r="B815" s="3">
+        <v>99</v>
+      </c>
+      <c r="C815" s="2">
+        <v>43219</v>
+      </c>
+      <c r="D815" t="s">
+        <v>132</v>
+      </c>
+      <c r="E815">
+        <v>2018</v>
+      </c>
+      <c r="F815" t="s">
+        <v>44</v>
+      </c>
+      <c r="G815" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H815" s="1">
+        <v>130</v>
+      </c>
+      <c r="I815" s="3">
+        <v>5</v>
+      </c>
+      <c r="J815" s="3">
+        <v>3</v>
+      </c>
+      <c r="K815" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="816" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A816" s="3">
+        <v>815</v>
+      </c>
+      <c r="B816" s="3">
+        <v>99</v>
+      </c>
+      <c r="C816" s="2">
+        <v>43219</v>
+      </c>
+      <c r="D816" t="s">
+        <v>132</v>
+      </c>
+      <c r="E816">
+        <v>2018</v>
+      </c>
+      <c r="F816" t="s">
+        <v>44</v>
+      </c>
+      <c r="G816" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="H816" s="1">
+        <v>40</v>
+      </c>
+      <c r="I816" s="3">
+        <v>3</v>
+      </c>
+      <c r="J816" s="3">
+        <v>8</v>
+      </c>
+      <c r="K816" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="817" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A817" s="3">
+        <v>816</v>
+      </c>
+      <c r="B817" s="3">
+        <v>99</v>
+      </c>
+      <c r="C817" s="2">
+        <v>43219</v>
+      </c>
+      <c r="D817" t="s">
+        <v>132</v>
+      </c>
+      <c r="E817">
+        <v>2018</v>
+      </c>
+      <c r="F817" t="s">
+        <v>44</v>
+      </c>
+      <c r="G817" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H817" s="1">
+        <v>70</v>
+      </c>
+      <c r="I817" s="3">
+        <v>3</v>
+      </c>
+      <c r="J817" s="3">
+        <v>8</v>
+      </c>
+      <c r="K817" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="818" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A818" s="3">
+        <v>817</v>
+      </c>
+      <c r="B818" s="3">
+        <v>99</v>
+      </c>
+      <c r="C818" s="2">
+        <v>43219</v>
+      </c>
+      <c r="D818" t="s">
+        <v>132</v>
+      </c>
+      <c r="E818">
+        <v>2018</v>
+      </c>
+      <c r="F818" t="s">
+        <v>44</v>
+      </c>
+      <c r="G818" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="H818" s="1">
+        <v>120</v>
+      </c>
+      <c r="I818" s="3">
+        <v>3</v>
+      </c>
+      <c r="J818" s="3">
+        <v>6</v>
+      </c>
+      <c r="K818" t="s">
+        <v>87</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updating GymWorkouts file 06/05/2018
</commit_message>
<xml_diff>
--- a/datasets/GymWorkouts.xlsx
+++ b/datasets/GymWorkouts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Will\Documents\Data Science\My Projects\My Data Project\mydata\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65F1A110-4807-47B0-BE59-8F79AFFE5012}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{554EA8EF-D7F9-4C6F-A403-316A3CD37E07}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="11640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3279" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3411" uniqueCount="140">
   <si>
     <t>Exercise Date</t>
   </si>
@@ -434,6 +434,18 @@
   <si>
     <t>Row (machine)</t>
   </si>
+  <si>
+    <t>Laying down tricep curl</t>
+  </si>
+  <si>
+    <t>May</t>
+  </si>
+  <si>
+    <t>Left Situp</t>
+  </si>
+  <si>
+    <t>Right Situp</t>
+  </si>
 </sst>
 </file>
 
@@ -787,11 +799,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K818"/>
+  <dimension ref="A1:K851"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A795" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A819" sqref="A819"/>
+      <pane ySplit="1" topLeftCell="A828" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A852" sqref="A852"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -29439,6 +29451,1161 @@
         <v>87</v>
       </c>
     </row>
+    <row r="819" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A819" s="3">
+        <v>818</v>
+      </c>
+      <c r="B819" s="3">
+        <v>100</v>
+      </c>
+      <c r="C819" s="2">
+        <v>43220</v>
+      </c>
+      <c r="D819" t="s">
+        <v>132</v>
+      </c>
+      <c r="E819">
+        <v>2018</v>
+      </c>
+      <c r="F819" t="s">
+        <v>17</v>
+      </c>
+      <c r="G819" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H819" s="1">
+        <v>40</v>
+      </c>
+      <c r="I819" s="3">
+        <v>4</v>
+      </c>
+      <c r="J819" s="3">
+        <v>8</v>
+      </c>
+      <c r="K819" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="820" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A820" s="3">
+        <v>819</v>
+      </c>
+      <c r="B820" s="3">
+        <v>100</v>
+      </c>
+      <c r="C820" s="2">
+        <v>43220</v>
+      </c>
+      <c r="D820" t="s">
+        <v>132</v>
+      </c>
+      <c r="E820">
+        <v>2018</v>
+      </c>
+      <c r="F820" t="s">
+        <v>17</v>
+      </c>
+      <c r="G820" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="H820" s="1">
+        <v>30</v>
+      </c>
+      <c r="I820" s="3">
+        <v>4</v>
+      </c>
+      <c r="J820" s="3">
+        <v>8</v>
+      </c>
+      <c r="K820" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="821" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A821" s="3">
+        <v>820</v>
+      </c>
+      <c r="B821" s="3">
+        <v>100</v>
+      </c>
+      <c r="C821" s="2">
+        <v>43220</v>
+      </c>
+      <c r="D821" t="s">
+        <v>132</v>
+      </c>
+      <c r="E821">
+        <v>2018</v>
+      </c>
+      <c r="F821" t="s">
+        <v>17</v>
+      </c>
+      <c r="G821" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H821" s="1">
+        <v>20</v>
+      </c>
+      <c r="I821" s="3">
+        <v>4</v>
+      </c>
+      <c r="J821" s="3">
+        <v>8</v>
+      </c>
+      <c r="K821" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="822" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A822" s="3">
+        <v>821</v>
+      </c>
+      <c r="B822" s="3">
+        <v>100</v>
+      </c>
+      <c r="C822" s="2">
+        <v>43220</v>
+      </c>
+      <c r="D822" t="s">
+        <v>132</v>
+      </c>
+      <c r="E822">
+        <v>2018</v>
+      </c>
+      <c r="F822" t="s">
+        <v>17</v>
+      </c>
+      <c r="G822" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H822" s="1">
+        <v>45</v>
+      </c>
+      <c r="I822" s="3">
+        <v>4</v>
+      </c>
+      <c r="J822" s="3">
+        <v>8</v>
+      </c>
+      <c r="K822" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="823" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A823" s="3">
+        <v>822</v>
+      </c>
+      <c r="B823" s="3">
+        <v>100</v>
+      </c>
+      <c r="C823" s="2">
+        <v>43220</v>
+      </c>
+      <c r="D823" t="s">
+        <v>132</v>
+      </c>
+      <c r="E823">
+        <v>2018</v>
+      </c>
+      <c r="F823" t="s">
+        <v>17</v>
+      </c>
+      <c r="G823" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H823" s="1">
+        <v>0</v>
+      </c>
+      <c r="I823" s="3">
+        <v>3</v>
+      </c>
+      <c r="J823" s="3">
+        <v>30</v>
+      </c>
+      <c r="K823" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="824" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A824" s="3">
+        <v>823</v>
+      </c>
+      <c r="B824" s="3">
+        <v>100</v>
+      </c>
+      <c r="C824" s="2">
+        <v>43220</v>
+      </c>
+      <c r="D824" t="s">
+        <v>132</v>
+      </c>
+      <c r="E824">
+        <v>2018</v>
+      </c>
+      <c r="F824" t="s">
+        <v>17</v>
+      </c>
+      <c r="G824" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H824" s="1">
+        <v>0</v>
+      </c>
+      <c r="I824" s="3">
+        <v>3</v>
+      </c>
+      <c r="J824" s="3">
+        <v>30</v>
+      </c>
+      <c r="K824" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="825" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A825" s="3">
+        <v>824</v>
+      </c>
+      <c r="B825" s="3">
+        <v>100</v>
+      </c>
+      <c r="C825" s="2">
+        <v>43220</v>
+      </c>
+      <c r="D825" t="s">
+        <v>132</v>
+      </c>
+      <c r="E825">
+        <v>2018</v>
+      </c>
+      <c r="F825" t="s">
+        <v>17</v>
+      </c>
+      <c r="G825" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H825" s="1">
+        <v>0</v>
+      </c>
+      <c r="I825" s="3">
+        <v>3</v>
+      </c>
+      <c r="J825" s="3">
+        <v>30</v>
+      </c>
+      <c r="K825" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="826" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A826" s="3">
+        <v>825</v>
+      </c>
+      <c r="B826" s="3">
+        <v>101</v>
+      </c>
+      <c r="C826" s="2">
+        <v>43222</v>
+      </c>
+      <c r="D826" t="s">
+        <v>137</v>
+      </c>
+      <c r="E826">
+        <v>2018</v>
+      </c>
+      <c r="F826" t="s">
+        <v>18</v>
+      </c>
+      <c r="G826" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H826" s="1">
+        <v>85</v>
+      </c>
+      <c r="I826" s="3">
+        <v>5</v>
+      </c>
+      <c r="J826" s="3">
+        <v>5</v>
+      </c>
+      <c r="K826" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="827" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A827" s="3">
+        <v>826</v>
+      </c>
+      <c r="B827" s="3">
+        <v>101</v>
+      </c>
+      <c r="C827" s="2">
+        <v>43222</v>
+      </c>
+      <c r="D827" t="s">
+        <v>137</v>
+      </c>
+      <c r="E827">
+        <v>2018</v>
+      </c>
+      <c r="F827" t="s">
+        <v>18</v>
+      </c>
+      <c r="G827" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H827" s="1">
+        <v>52.5</v>
+      </c>
+      <c r="I827" s="3">
+        <v>5</v>
+      </c>
+      <c r="J827" s="3">
+        <v>5</v>
+      </c>
+      <c r="K827" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="828" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A828" s="3">
+        <v>827</v>
+      </c>
+      <c r="B828" s="3">
+        <v>101</v>
+      </c>
+      <c r="C828" s="2">
+        <v>43222</v>
+      </c>
+      <c r="D828" t="s">
+        <v>137</v>
+      </c>
+      <c r="E828">
+        <v>2018</v>
+      </c>
+      <c r="F828" t="s">
+        <v>18</v>
+      </c>
+      <c r="G828" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H828" s="1">
+        <v>10</v>
+      </c>
+      <c r="I828" s="3">
+        <v>4</v>
+      </c>
+      <c r="J828" s="3">
+        <v>8</v>
+      </c>
+      <c r="K828" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="829" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A829" s="3">
+        <v>828</v>
+      </c>
+      <c r="B829" s="3">
+        <v>101</v>
+      </c>
+      <c r="C829" s="2">
+        <v>43222</v>
+      </c>
+      <c r="D829" t="s">
+        <v>137</v>
+      </c>
+      <c r="E829">
+        <v>2018</v>
+      </c>
+      <c r="F829" t="s">
+        <v>18</v>
+      </c>
+      <c r="G829" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="H829" s="1">
+        <v>10</v>
+      </c>
+      <c r="I829" s="3">
+        <v>4</v>
+      </c>
+      <c r="J829" s="3">
+        <v>8</v>
+      </c>
+      <c r="K829" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="830" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A830" s="3">
+        <v>829</v>
+      </c>
+      <c r="B830" s="3">
+        <v>101</v>
+      </c>
+      <c r="C830" s="2">
+        <v>43222</v>
+      </c>
+      <c r="D830" t="s">
+        <v>137</v>
+      </c>
+      <c r="E830">
+        <v>2018</v>
+      </c>
+      <c r="F830" t="s">
+        <v>18</v>
+      </c>
+      <c r="G830" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="H830" s="1">
+        <v>30</v>
+      </c>
+      <c r="I830" s="3">
+        <v>4</v>
+      </c>
+      <c r="J830" s="3">
+        <v>12</v>
+      </c>
+      <c r="K830" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="831" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A831" s="3">
+        <v>830</v>
+      </c>
+      <c r="B831" s="3">
+        <v>102</v>
+      </c>
+      <c r="C831" s="2">
+        <v>43224</v>
+      </c>
+      <c r="D831" t="s">
+        <v>137</v>
+      </c>
+      <c r="E831">
+        <v>2018</v>
+      </c>
+      <c r="F831" t="s">
+        <v>49</v>
+      </c>
+      <c r="G831" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H831" s="1">
+        <v>105</v>
+      </c>
+      <c r="I831" s="3">
+        <v>4</v>
+      </c>
+      <c r="J831" s="3">
+        <v>8</v>
+      </c>
+      <c r="K831" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="832" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A832" s="3">
+        <v>831</v>
+      </c>
+      <c r="B832" s="3">
+        <v>102</v>
+      </c>
+      <c r="C832" s="2">
+        <v>43224</v>
+      </c>
+      <c r="D832" t="s">
+        <v>137</v>
+      </c>
+      <c r="E832">
+        <v>2018</v>
+      </c>
+      <c r="F832" t="s">
+        <v>49</v>
+      </c>
+      <c r="G832" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H832" s="1">
+        <v>70</v>
+      </c>
+      <c r="I832" s="3">
+        <v>3</v>
+      </c>
+      <c r="J832" s="3">
+        <v>8</v>
+      </c>
+      <c r="K832" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="833" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A833" s="3">
+        <v>832</v>
+      </c>
+      <c r="B833" s="3">
+        <v>102</v>
+      </c>
+      <c r="C833" s="2">
+        <v>43224</v>
+      </c>
+      <c r="D833" t="s">
+        <v>137</v>
+      </c>
+      <c r="E833">
+        <v>2018</v>
+      </c>
+      <c r="F833" t="s">
+        <v>49</v>
+      </c>
+      <c r="G833" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="H833" s="1">
+        <v>70</v>
+      </c>
+      <c r="I833" s="3">
+        <v>4</v>
+      </c>
+      <c r="J833" s="3">
+        <v>8</v>
+      </c>
+      <c r="K833" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="834" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A834" s="3">
+        <v>833</v>
+      </c>
+      <c r="B834" s="3">
+        <v>102</v>
+      </c>
+      <c r="C834" s="2">
+        <v>43224</v>
+      </c>
+      <c r="D834" t="s">
+        <v>137</v>
+      </c>
+      <c r="E834">
+        <v>2018</v>
+      </c>
+      <c r="F834" t="s">
+        <v>49</v>
+      </c>
+      <c r="G834" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="H834" s="1">
+        <v>30</v>
+      </c>
+      <c r="I834" s="3">
+        <v>4</v>
+      </c>
+      <c r="J834" s="3">
+        <v>8</v>
+      </c>
+      <c r="K834" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="835" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A835" s="3">
+        <v>834</v>
+      </c>
+      <c r="B835" s="3">
+        <v>102</v>
+      </c>
+      <c r="C835" s="2">
+        <v>43224</v>
+      </c>
+      <c r="D835" t="s">
+        <v>137</v>
+      </c>
+      <c r="E835">
+        <v>2018</v>
+      </c>
+      <c r="F835" t="s">
+        <v>49</v>
+      </c>
+      <c r="G835" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H835" s="1">
+        <v>0</v>
+      </c>
+      <c r="I835" s="3">
+        <v>2</v>
+      </c>
+      <c r="J835" s="3">
+        <v>10</v>
+      </c>
+      <c r="K835" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="836" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A836" s="3">
+        <v>835</v>
+      </c>
+      <c r="B836" s="3">
+        <v>102</v>
+      </c>
+      <c r="C836" s="2">
+        <v>43224</v>
+      </c>
+      <c r="D836" t="s">
+        <v>137</v>
+      </c>
+      <c r="E836">
+        <v>2018</v>
+      </c>
+      <c r="F836" t="s">
+        <v>49</v>
+      </c>
+      <c r="G836" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H836" s="1">
+        <v>0</v>
+      </c>
+      <c r="I836" s="3">
+        <v>2</v>
+      </c>
+      <c r="J836" s="3">
+        <v>10</v>
+      </c>
+      <c r="K836" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="837" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A837" s="3">
+        <v>836</v>
+      </c>
+      <c r="B837" s="3">
+        <v>102</v>
+      </c>
+      <c r="C837" s="2">
+        <v>43224</v>
+      </c>
+      <c r="D837" t="s">
+        <v>137</v>
+      </c>
+      <c r="E837">
+        <v>2018</v>
+      </c>
+      <c r="F837" t="s">
+        <v>49</v>
+      </c>
+      <c r="G837" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="H837" s="1">
+        <v>0</v>
+      </c>
+      <c r="I837" s="3">
+        <v>2</v>
+      </c>
+      <c r="J837" s="3">
+        <v>12</v>
+      </c>
+      <c r="K837" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="838" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A838" s="3">
+        <v>837</v>
+      </c>
+      <c r="B838" s="3">
+        <v>102</v>
+      </c>
+      <c r="C838" s="2">
+        <v>43224</v>
+      </c>
+      <c r="D838" t="s">
+        <v>137</v>
+      </c>
+      <c r="E838">
+        <v>2018</v>
+      </c>
+      <c r="F838" t="s">
+        <v>49</v>
+      </c>
+      <c r="G838" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="H838" s="1">
+        <v>0</v>
+      </c>
+      <c r="I838" s="3">
+        <v>2</v>
+      </c>
+      <c r="J838" s="3">
+        <v>10</v>
+      </c>
+      <c r="K838" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="839" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A839" s="3">
+        <v>838</v>
+      </c>
+      <c r="B839" s="3">
+        <v>102</v>
+      </c>
+      <c r="C839" s="2">
+        <v>43224</v>
+      </c>
+      <c r="D839" t="s">
+        <v>137</v>
+      </c>
+      <c r="E839">
+        <v>2018</v>
+      </c>
+      <c r="F839" t="s">
+        <v>49</v>
+      </c>
+      <c r="G839" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="H839" s="1">
+        <v>0</v>
+      </c>
+      <c r="I839" s="3">
+        <v>2</v>
+      </c>
+      <c r="J839" s="3">
+        <v>10</v>
+      </c>
+      <c r="K839" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="840" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A840" s="3">
+        <v>839</v>
+      </c>
+      <c r="B840" s="3">
+        <v>103</v>
+      </c>
+      <c r="C840" s="2">
+        <v>43225</v>
+      </c>
+      <c r="D840" t="s">
+        <v>137</v>
+      </c>
+      <c r="E840">
+        <v>2018</v>
+      </c>
+      <c r="F840" t="s">
+        <v>79</v>
+      </c>
+      <c r="G840" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H840" s="1">
+        <v>25</v>
+      </c>
+      <c r="I840" s="3">
+        <v>4</v>
+      </c>
+      <c r="J840" s="3">
+        <v>8</v>
+      </c>
+      <c r="K840" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="841" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A841" s="3">
+        <v>840</v>
+      </c>
+      <c r="B841" s="3">
+        <v>103</v>
+      </c>
+      <c r="C841" s="2">
+        <v>43225</v>
+      </c>
+      <c r="D841" t="s">
+        <v>137</v>
+      </c>
+      <c r="E841">
+        <v>2018</v>
+      </c>
+      <c r="F841" t="s">
+        <v>79</v>
+      </c>
+      <c r="G841" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H841" s="1">
+        <v>25</v>
+      </c>
+      <c r="I841" s="3">
+        <v>4</v>
+      </c>
+      <c r="J841" s="3">
+        <v>8</v>
+      </c>
+      <c r="K841" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="842" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A842" s="3">
+        <v>841</v>
+      </c>
+      <c r="B842" s="3">
+        <v>103</v>
+      </c>
+      <c r="C842" s="2">
+        <v>43225</v>
+      </c>
+      <c r="D842" t="s">
+        <v>137</v>
+      </c>
+      <c r="E842">
+        <v>2018</v>
+      </c>
+      <c r="F842" t="s">
+        <v>79</v>
+      </c>
+      <c r="G842" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H842" s="1">
+        <v>45</v>
+      </c>
+      <c r="I842" s="3">
+        <v>4</v>
+      </c>
+      <c r="J842" s="3">
+        <v>8</v>
+      </c>
+      <c r="K842" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="843" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A843" s="3">
+        <v>842</v>
+      </c>
+      <c r="B843" s="3">
+        <v>103</v>
+      </c>
+      <c r="C843" s="2">
+        <v>43225</v>
+      </c>
+      <c r="D843" t="s">
+        <v>137</v>
+      </c>
+      <c r="E843">
+        <v>2018</v>
+      </c>
+      <c r="F843" t="s">
+        <v>79</v>
+      </c>
+      <c r="G843" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H843" s="1">
+        <v>20</v>
+      </c>
+      <c r="I843" s="3">
+        <v>4</v>
+      </c>
+      <c r="J843" s="3">
+        <v>8</v>
+      </c>
+      <c r="K843" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="844" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A844" s="3">
+        <v>843</v>
+      </c>
+      <c r="B844" s="3">
+        <v>103</v>
+      </c>
+      <c r="C844" s="2">
+        <v>43225</v>
+      </c>
+      <c r="D844" t="s">
+        <v>137</v>
+      </c>
+      <c r="E844">
+        <v>2018</v>
+      </c>
+      <c r="F844" t="s">
+        <v>79</v>
+      </c>
+      <c r="G844" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="H844" s="1">
+        <v>10</v>
+      </c>
+      <c r="I844" s="3">
+        <v>4</v>
+      </c>
+      <c r="J844" s="3">
+        <v>12</v>
+      </c>
+      <c r="K844" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="845" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A845" s="3">
+        <v>844</v>
+      </c>
+      <c r="B845" s="3">
+        <v>103</v>
+      </c>
+      <c r="C845" s="2">
+        <v>43225</v>
+      </c>
+      <c r="D845" t="s">
+        <v>137</v>
+      </c>
+      <c r="E845">
+        <v>2018</v>
+      </c>
+      <c r="F845" t="s">
+        <v>79</v>
+      </c>
+      <c r="G845" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="H845" s="1">
+        <v>0</v>
+      </c>
+      <c r="I845" s="3">
+        <v>4</v>
+      </c>
+      <c r="J845" s="3">
+        <v>12</v>
+      </c>
+      <c r="K845" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="846" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A846" s="3">
+        <v>845</v>
+      </c>
+      <c r="B846" s="3">
+        <v>103</v>
+      </c>
+      <c r="C846" s="2">
+        <v>43225</v>
+      </c>
+      <c r="D846" t="s">
+        <v>137</v>
+      </c>
+      <c r="E846">
+        <v>2018</v>
+      </c>
+      <c r="F846" t="s">
+        <v>79</v>
+      </c>
+      <c r="G846" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="H846" s="1">
+        <v>0</v>
+      </c>
+      <c r="I846" s="3">
+        <v>4</v>
+      </c>
+      <c r="J846" s="3">
+        <v>12</v>
+      </c>
+      <c r="K846" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="847" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A847" s="3">
+        <v>846</v>
+      </c>
+      <c r="B847" s="3">
+        <v>104</v>
+      </c>
+      <c r="C847" s="2">
+        <v>43226</v>
+      </c>
+      <c r="D847" t="s">
+        <v>137</v>
+      </c>
+      <c r="E847">
+        <v>2018</v>
+      </c>
+      <c r="F847" t="s">
+        <v>44</v>
+      </c>
+      <c r="G847" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H847" s="1">
+        <v>75</v>
+      </c>
+      <c r="I847" s="3">
+        <v>3</v>
+      </c>
+      <c r="J847" s="3">
+        <v>8</v>
+      </c>
+      <c r="K847" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="848" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A848" s="3">
+        <v>847</v>
+      </c>
+      <c r="B848" s="3">
+        <v>104</v>
+      </c>
+      <c r="C848" s="2">
+        <v>43226</v>
+      </c>
+      <c r="D848" t="s">
+        <v>137</v>
+      </c>
+      <c r="E848">
+        <v>2018</v>
+      </c>
+      <c r="F848" t="s">
+        <v>44</v>
+      </c>
+      <c r="G848" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="H848" s="1">
+        <v>45</v>
+      </c>
+      <c r="I848" s="3">
+        <v>3</v>
+      </c>
+      <c r="J848" s="3">
+        <v>8</v>
+      </c>
+      <c r="K848" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="849" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A849" s="3">
+        <v>848</v>
+      </c>
+      <c r="B849" s="3">
+        <v>104</v>
+      </c>
+      <c r="C849" s="2">
+        <v>43226</v>
+      </c>
+      <c r="D849" t="s">
+        <v>137</v>
+      </c>
+      <c r="E849">
+        <v>2018</v>
+      </c>
+      <c r="F849" t="s">
+        <v>44</v>
+      </c>
+      <c r="G849" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H849" s="1">
+        <v>65</v>
+      </c>
+      <c r="I849" s="3">
+        <v>3</v>
+      </c>
+      <c r="J849" s="3">
+        <v>12</v>
+      </c>
+      <c r="K849" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="850" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A850" s="3">
+        <v>849</v>
+      </c>
+      <c r="B850" s="3">
+        <v>104</v>
+      </c>
+      <c r="C850" s="2">
+        <v>43226</v>
+      </c>
+      <c r="D850" t="s">
+        <v>137</v>
+      </c>
+      <c r="E850">
+        <v>2018</v>
+      </c>
+      <c r="F850" t="s">
+        <v>44</v>
+      </c>
+      <c r="G850" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H850" s="1">
+        <v>65</v>
+      </c>
+      <c r="I850" s="3">
+        <v>3</v>
+      </c>
+      <c r="J850" s="3">
+        <v>12</v>
+      </c>
+      <c r="K850" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="851" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A851" s="3">
+        <v>850</v>
+      </c>
+      <c r="B851" s="3">
+        <v>104</v>
+      </c>
+      <c r="C851" s="2">
+        <v>43226</v>
+      </c>
+      <c r="D851" t="s">
+        <v>137</v>
+      </c>
+      <c r="E851">
+        <v>2018</v>
+      </c>
+      <c r="F851" t="s">
+        <v>44</v>
+      </c>
+      <c r="G851" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H851" s="1">
+        <v>108</v>
+      </c>
+      <c r="I851" s="3">
+        <v>4</v>
+      </c>
+      <c r="J851" s="3">
+        <v>8</v>
+      </c>
+      <c r="K851" t="s">
+        <v>87</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updating GymWorkouts file 13/05/2018
</commit_message>
<xml_diff>
--- a/datasets/GymWorkouts.xlsx
+++ b/datasets/GymWorkouts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Will\Documents\Data Science\My Projects\My Data Project\mydata\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{554EA8EF-D7F9-4C6F-A403-316A3CD37E07}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF530E7B-39F9-4A30-AAA2-8876CC7A4296}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="11640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3411" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3463" uniqueCount="140">
   <si>
     <t>Exercise Date</t>
   </si>
@@ -799,11 +799,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K851"/>
+  <dimension ref="A1:K864"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A828" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A852" sqref="A852"/>
+      <pane ySplit="1" topLeftCell="A850" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A866" sqref="A866"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -30606,6 +30606,461 @@
         <v>87</v>
       </c>
     </row>
+    <row r="852" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A852" s="3">
+        <v>851</v>
+      </c>
+      <c r="B852" s="3">
+        <v>105</v>
+      </c>
+      <c r="C852" s="2">
+        <v>43231</v>
+      </c>
+      <c r="D852" t="s">
+        <v>137</v>
+      </c>
+      <c r="E852">
+        <v>2018</v>
+      </c>
+      <c r="F852" t="s">
+        <v>49</v>
+      </c>
+      <c r="G852" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H852" s="1">
+        <v>105</v>
+      </c>
+      <c r="I852" s="3">
+        <v>4</v>
+      </c>
+      <c r="J852" s="3">
+        <v>8</v>
+      </c>
+      <c r="K852" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="853" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A853" s="3">
+        <v>852</v>
+      </c>
+      <c r="B853" s="3">
+        <v>105</v>
+      </c>
+      <c r="C853" s="2">
+        <v>43231</v>
+      </c>
+      <c r="D853" t="s">
+        <v>137</v>
+      </c>
+      <c r="E853">
+        <v>2018</v>
+      </c>
+      <c r="F853" t="s">
+        <v>49</v>
+      </c>
+      <c r="G853" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H853" s="1">
+        <v>60</v>
+      </c>
+      <c r="I853" s="3">
+        <v>4</v>
+      </c>
+      <c r="J853" s="3">
+        <v>12</v>
+      </c>
+      <c r="K853" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="854" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A854" s="3">
+        <v>853</v>
+      </c>
+      <c r="B854" s="3">
+        <v>105</v>
+      </c>
+      <c r="C854" s="2">
+        <v>43231</v>
+      </c>
+      <c r="D854" t="s">
+        <v>137</v>
+      </c>
+      <c r="E854">
+        <v>2018</v>
+      </c>
+      <c r="F854" t="s">
+        <v>49</v>
+      </c>
+      <c r="G854" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H854" s="1">
+        <v>60</v>
+      </c>
+      <c r="I854" s="3">
+        <v>4</v>
+      </c>
+      <c r="J854" s="3">
+        <v>12</v>
+      </c>
+      <c r="K854" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="855" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A855" s="3">
+        <v>854</v>
+      </c>
+      <c r="B855" s="3">
+        <v>105</v>
+      </c>
+      <c r="C855" s="2">
+        <v>43231</v>
+      </c>
+      <c r="D855" t="s">
+        <v>137</v>
+      </c>
+      <c r="E855">
+        <v>2018</v>
+      </c>
+      <c r="F855" t="s">
+        <v>49</v>
+      </c>
+      <c r="G855" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="H855" s="1">
+        <v>30</v>
+      </c>
+      <c r="I855" s="3">
+        <v>4</v>
+      </c>
+      <c r="J855" s="3">
+        <v>12</v>
+      </c>
+      <c r="K855" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="856" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A856" s="3">
+        <v>855</v>
+      </c>
+      <c r="B856" s="3">
+        <v>105</v>
+      </c>
+      <c r="C856" s="2">
+        <v>43231</v>
+      </c>
+      <c r="D856" t="s">
+        <v>137</v>
+      </c>
+      <c r="E856">
+        <v>2018</v>
+      </c>
+      <c r="F856" t="s">
+        <v>49</v>
+      </c>
+      <c r="G856" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H856" s="1">
+        <v>101</v>
+      </c>
+      <c r="I856" s="3">
+        <v>4</v>
+      </c>
+      <c r="J856" s="3">
+        <v>8</v>
+      </c>
+      <c r="K856" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="857" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A857" s="3">
+        <v>856</v>
+      </c>
+      <c r="B857" s="3">
+        <v>105</v>
+      </c>
+      <c r="C857" s="2">
+        <v>43231</v>
+      </c>
+      <c r="D857" t="s">
+        <v>137</v>
+      </c>
+      <c r="E857">
+        <v>2018</v>
+      </c>
+      <c r="F857" t="s">
+        <v>49</v>
+      </c>
+      <c r="G857" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H857" s="1">
+        <v>25</v>
+      </c>
+      <c r="I857" s="3">
+        <v>4</v>
+      </c>
+      <c r="J857" s="3">
+        <v>12</v>
+      </c>
+      <c r="K857" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="858" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A858" s="3">
+        <v>857</v>
+      </c>
+      <c r="B858" s="3">
+        <v>106</v>
+      </c>
+      <c r="C858" s="2">
+        <v>43232</v>
+      </c>
+      <c r="D858" t="s">
+        <v>137</v>
+      </c>
+      <c r="E858">
+        <v>2018</v>
+      </c>
+      <c r="F858" t="s">
+        <v>79</v>
+      </c>
+      <c r="G858" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H858" s="1">
+        <v>85</v>
+      </c>
+      <c r="I858" s="3">
+        <v>5</v>
+      </c>
+      <c r="J858" s="3">
+        <v>5</v>
+      </c>
+      <c r="K858" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="859" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A859" s="3">
+        <v>858</v>
+      </c>
+      <c r="B859" s="3">
+        <v>106</v>
+      </c>
+      <c r="C859" s="2">
+        <v>43232</v>
+      </c>
+      <c r="D859" t="s">
+        <v>137</v>
+      </c>
+      <c r="E859">
+        <v>2018</v>
+      </c>
+      <c r="F859" t="s">
+        <v>79</v>
+      </c>
+      <c r="G859" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H859" s="1">
+        <v>52.5</v>
+      </c>
+      <c r="I859" s="3">
+        <v>5</v>
+      </c>
+      <c r="J859" s="3">
+        <v>5</v>
+      </c>
+      <c r="K859" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="860" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A860" s="3">
+        <v>859</v>
+      </c>
+      <c r="B860" s="3">
+        <v>106</v>
+      </c>
+      <c r="C860" s="2">
+        <v>43232</v>
+      </c>
+      <c r="D860" t="s">
+        <v>137</v>
+      </c>
+      <c r="E860">
+        <v>2018</v>
+      </c>
+      <c r="F860" t="s">
+        <v>79</v>
+      </c>
+      <c r="G860" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H860" s="1">
+        <v>90</v>
+      </c>
+      <c r="I860" s="3">
+        <v>5</v>
+      </c>
+      <c r="J860" s="3">
+        <v>5</v>
+      </c>
+      <c r="K860" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="861" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A861" s="3">
+        <v>860</v>
+      </c>
+      <c r="B861" s="3">
+        <v>106</v>
+      </c>
+      <c r="C861" s="2">
+        <v>43232</v>
+      </c>
+      <c r="D861" t="s">
+        <v>137</v>
+      </c>
+      <c r="E861">
+        <v>2018</v>
+      </c>
+      <c r="F861" t="s">
+        <v>79</v>
+      </c>
+      <c r="G861" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="H861" s="1">
+        <v>10</v>
+      </c>
+      <c r="I861" s="3">
+        <v>4</v>
+      </c>
+      <c r="J861" s="3">
+        <v>8</v>
+      </c>
+      <c r="K861" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="862" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A862" s="3">
+        <v>861</v>
+      </c>
+      <c r="B862" s="3">
+        <v>106</v>
+      </c>
+      <c r="C862" s="2">
+        <v>43232</v>
+      </c>
+      <c r="D862" t="s">
+        <v>137</v>
+      </c>
+      <c r="E862">
+        <v>2018</v>
+      </c>
+      <c r="F862" t="s">
+        <v>79</v>
+      </c>
+      <c r="G862" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H862" s="1">
+        <v>10</v>
+      </c>
+      <c r="I862" s="3">
+        <v>4</v>
+      </c>
+      <c r="J862" s="3">
+        <v>8</v>
+      </c>
+      <c r="K862" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="863" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A863" s="3">
+        <v>862</v>
+      </c>
+      <c r="B863" s="3">
+        <v>106</v>
+      </c>
+      <c r="C863" s="2">
+        <v>43232</v>
+      </c>
+      <c r="D863" t="s">
+        <v>137</v>
+      </c>
+      <c r="E863">
+        <v>2018</v>
+      </c>
+      <c r="F863" t="s">
+        <v>79</v>
+      </c>
+      <c r="G863" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="H863" s="1">
+        <v>10</v>
+      </c>
+      <c r="I863" s="3">
+        <v>4</v>
+      </c>
+      <c r="J863" s="3">
+        <v>8</v>
+      </c>
+      <c r="K863" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="864" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A864" s="3">
+        <v>863</v>
+      </c>
+      <c r="B864" s="3">
+        <v>106</v>
+      </c>
+      <c r="C864" s="2">
+        <v>43232</v>
+      </c>
+      <c r="D864" t="s">
+        <v>137</v>
+      </c>
+      <c r="E864">
+        <v>2018</v>
+      </c>
+      <c r="F864" t="s">
+        <v>79</v>
+      </c>
+      <c r="G864" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H864" s="1">
+        <v>0</v>
+      </c>
+      <c r="I864" s="3">
+        <v>5</v>
+      </c>
+      <c r="J864" s="3">
+        <v>30</v>
+      </c>
+      <c r="K864" t="s">
+        <v>88</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updating GymWorkouts file 27/05/2018
</commit_message>
<xml_diff>
--- a/datasets/GymWorkouts.xlsx
+++ b/datasets/GymWorkouts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Will\Documents\Data Science\My Projects\My Data Project\mydata\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF530E7B-39F9-4A30-AAA2-8876CC7A4296}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D71349E4-D274-4F7F-BD3B-FD1BB9B9B250}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="11640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3463" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3647" uniqueCount="149">
   <si>
     <t>Exercise Date</t>
   </si>
@@ -446,6 +446,33 @@
   <si>
     <t>Right Situp</t>
   </si>
+  <si>
+    <t>Dumbell Fly</t>
+  </si>
+  <si>
+    <t>Machine Shoulder Press</t>
+  </si>
+  <si>
+    <t>Skull Crusher</t>
+  </si>
+  <si>
+    <t>Standing Machine Calf Raise</t>
+  </si>
+  <si>
+    <t>Decline sit-up</t>
+  </si>
+  <si>
+    <t>Close grip push ups</t>
+  </si>
+  <si>
+    <t>Barbell Curl</t>
+  </si>
+  <si>
+    <t>hypertension back</t>
+  </si>
+  <si>
+    <t>One-arm row</t>
+  </si>
 </sst>
 </file>
 
@@ -799,11 +826,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K864"/>
+  <dimension ref="A1:K910"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A850" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A866" sqref="A866"/>
+      <pane ySplit="1" topLeftCell="A886" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D913" sqref="D913"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -31061,6 +31088,1616 @@
         <v>88</v>
       </c>
     </row>
+    <row r="865" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A865" s="3">
+        <v>864</v>
+      </c>
+      <c r="B865" s="3">
+        <v>107</v>
+      </c>
+      <c r="C865" s="2">
+        <v>43235</v>
+      </c>
+      <c r="D865" t="s">
+        <v>137</v>
+      </c>
+      <c r="E865">
+        <v>2018</v>
+      </c>
+      <c r="F865" t="s">
+        <v>73</v>
+      </c>
+      <c r="G865" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H865" s="1">
+        <v>65</v>
+      </c>
+      <c r="I865" s="3">
+        <v>4</v>
+      </c>
+      <c r="J865" s="3">
+        <v>12</v>
+      </c>
+      <c r="K865" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="866" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A866" s="3">
+        <v>865</v>
+      </c>
+      <c r="B866" s="3">
+        <v>107</v>
+      </c>
+      <c r="C866" s="2">
+        <v>43235</v>
+      </c>
+      <c r="D866" t="s">
+        <v>137</v>
+      </c>
+      <c r="E866">
+        <v>2018</v>
+      </c>
+      <c r="F866" t="s">
+        <v>73</v>
+      </c>
+      <c r="G866" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="H866" s="1">
+        <v>45</v>
+      </c>
+      <c r="I866" s="3">
+        <v>3</v>
+      </c>
+      <c r="J866" s="3">
+        <v>12</v>
+      </c>
+      <c r="K866" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="867" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A867" s="3">
+        <v>866</v>
+      </c>
+      <c r="B867" s="3">
+        <v>107</v>
+      </c>
+      <c r="C867" s="2">
+        <v>43235</v>
+      </c>
+      <c r="D867" t="s">
+        <v>137</v>
+      </c>
+      <c r="E867">
+        <v>2018</v>
+      </c>
+      <c r="F867" t="s">
+        <v>73</v>
+      </c>
+      <c r="G867" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="H867" s="1">
+        <v>40</v>
+      </c>
+      <c r="I867" s="3">
+        <v>4</v>
+      </c>
+      <c r="J867" s="3">
+        <v>10</v>
+      </c>
+      <c r="K867" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="868" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A868" s="3">
+        <v>867</v>
+      </c>
+      <c r="B868" s="3">
+        <v>107</v>
+      </c>
+      <c r="C868" s="2">
+        <v>43235</v>
+      </c>
+      <c r="D868" t="s">
+        <v>137</v>
+      </c>
+      <c r="E868">
+        <v>2018</v>
+      </c>
+      <c r="F868" t="s">
+        <v>73</v>
+      </c>
+      <c r="G868" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H868" s="1">
+        <v>20</v>
+      </c>
+      <c r="I868" s="3">
+        <v>3</v>
+      </c>
+      <c r="J868" s="3">
+        <v>10</v>
+      </c>
+      <c r="K868" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="869" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A869" s="3">
+        <v>868</v>
+      </c>
+      <c r="B869" s="3">
+        <v>107</v>
+      </c>
+      <c r="C869" s="2">
+        <v>43235</v>
+      </c>
+      <c r="D869" t="s">
+        <v>137</v>
+      </c>
+      <c r="E869">
+        <v>2018</v>
+      </c>
+      <c r="F869" t="s">
+        <v>73</v>
+      </c>
+      <c r="G869" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H869" s="1">
+        <v>60</v>
+      </c>
+      <c r="I869" s="3">
+        <v>3</v>
+      </c>
+      <c r="J869" s="3">
+        <v>12</v>
+      </c>
+      <c r="K869" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="870" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A870" s="3">
+        <v>869</v>
+      </c>
+      <c r="B870" s="3">
+        <v>107</v>
+      </c>
+      <c r="C870" s="2">
+        <v>43235</v>
+      </c>
+      <c r="D870" t="s">
+        <v>137</v>
+      </c>
+      <c r="E870">
+        <v>2018</v>
+      </c>
+      <c r="F870" t="s">
+        <v>73</v>
+      </c>
+      <c r="G870" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="H870" s="1">
+        <v>25</v>
+      </c>
+      <c r="I870" s="3">
+        <v>2</v>
+      </c>
+      <c r="J870" s="3">
+        <v>12</v>
+      </c>
+      <c r="K870" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="871" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A871" s="3">
+        <v>870</v>
+      </c>
+      <c r="B871" s="3">
+        <v>108</v>
+      </c>
+      <c r="C871" s="2">
+        <v>43236</v>
+      </c>
+      <c r="D871" t="s">
+        <v>137</v>
+      </c>
+      <c r="E871">
+        <v>2018</v>
+      </c>
+      <c r="F871" t="s">
+        <v>18</v>
+      </c>
+      <c r="G871" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H871" s="1">
+        <v>70</v>
+      </c>
+      <c r="I871" s="3">
+        <v>4</v>
+      </c>
+      <c r="J871" s="3">
+        <v>10</v>
+      </c>
+      <c r="K871" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="872" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A872" s="3">
+        <v>871</v>
+      </c>
+      <c r="B872" s="3">
+        <v>108</v>
+      </c>
+      <c r="C872" s="2">
+        <v>43236</v>
+      </c>
+      <c r="D872" t="s">
+        <v>137</v>
+      </c>
+      <c r="E872">
+        <v>2018</v>
+      </c>
+      <c r="F872" t="s">
+        <v>18</v>
+      </c>
+      <c r="G872" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="H872" s="1">
+        <v>110</v>
+      </c>
+      <c r="I872" s="3">
+        <v>3</v>
+      </c>
+      <c r="J872" s="3">
+        <v>12</v>
+      </c>
+      <c r="K872" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="873" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A873" s="3">
+        <v>872</v>
+      </c>
+      <c r="B873" s="3">
+        <v>108</v>
+      </c>
+      <c r="C873" s="2">
+        <v>43236</v>
+      </c>
+      <c r="D873" t="s">
+        <v>137</v>
+      </c>
+      <c r="E873">
+        <v>2018</v>
+      </c>
+      <c r="F873" t="s">
+        <v>18</v>
+      </c>
+      <c r="G873" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="H873" s="1">
+        <v>45</v>
+      </c>
+      <c r="I873" s="3">
+        <v>3</v>
+      </c>
+      <c r="J873" s="3">
+        <v>10</v>
+      </c>
+      <c r="K873" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="874" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A874" s="3">
+        <v>873</v>
+      </c>
+      <c r="B874" s="3">
+        <v>108</v>
+      </c>
+      <c r="C874" s="2">
+        <v>43236</v>
+      </c>
+      <c r="D874" t="s">
+        <v>137</v>
+      </c>
+      <c r="E874">
+        <v>2018</v>
+      </c>
+      <c r="F874" t="s">
+        <v>18</v>
+      </c>
+      <c r="G874" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H874" s="1">
+        <v>108</v>
+      </c>
+      <c r="I874" s="3">
+        <v>3</v>
+      </c>
+      <c r="J874" s="3">
+        <v>10</v>
+      </c>
+      <c r="K874" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="875" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A875" s="3">
+        <v>874</v>
+      </c>
+      <c r="B875" s="3">
+        <v>108</v>
+      </c>
+      <c r="C875" s="2">
+        <v>43236</v>
+      </c>
+      <c r="D875" t="s">
+        <v>137</v>
+      </c>
+      <c r="E875">
+        <v>2018</v>
+      </c>
+      <c r="F875" t="s">
+        <v>18</v>
+      </c>
+      <c r="G875" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="H875" s="1">
+        <v>50</v>
+      </c>
+      <c r="I875" s="3">
+        <v>3</v>
+      </c>
+      <c r="J875" s="3">
+        <v>10</v>
+      </c>
+      <c r="K875" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="876" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A876" s="3">
+        <v>875</v>
+      </c>
+      <c r="B876" s="3">
+        <v>108</v>
+      </c>
+      <c r="C876" s="2">
+        <v>43236</v>
+      </c>
+      <c r="D876" t="s">
+        <v>137</v>
+      </c>
+      <c r="E876">
+        <v>2018</v>
+      </c>
+      <c r="F876" t="s">
+        <v>18</v>
+      </c>
+      <c r="G876" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H876" s="1">
+        <v>0</v>
+      </c>
+      <c r="I876" s="3">
+        <v>3</v>
+      </c>
+      <c r="J876" s="3">
+        <v>30</v>
+      </c>
+      <c r="K876" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="877" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A877" s="3">
+        <v>876</v>
+      </c>
+      <c r="B877" s="3">
+        <v>108</v>
+      </c>
+      <c r="C877" s="2">
+        <v>43236</v>
+      </c>
+      <c r="D877" t="s">
+        <v>137</v>
+      </c>
+      <c r="E877">
+        <v>2018</v>
+      </c>
+      <c r="F877" t="s">
+        <v>18</v>
+      </c>
+      <c r="G877" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="H877" s="1">
+        <v>0</v>
+      </c>
+      <c r="I877" s="3">
+        <v>3</v>
+      </c>
+      <c r="J877" s="3">
+        <v>15</v>
+      </c>
+      <c r="K877" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="878" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A878" s="3">
+        <v>877</v>
+      </c>
+      <c r="B878" s="3">
+        <v>108</v>
+      </c>
+      <c r="C878" s="2">
+        <v>43236</v>
+      </c>
+      <c r="D878" t="s">
+        <v>137</v>
+      </c>
+      <c r="E878">
+        <v>2018</v>
+      </c>
+      <c r="F878" t="s">
+        <v>18</v>
+      </c>
+      <c r="G878" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="H878" s="1">
+        <v>0</v>
+      </c>
+      <c r="I878" s="3">
+        <v>3</v>
+      </c>
+      <c r="J878" s="3">
+        <v>15</v>
+      </c>
+      <c r="K878" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="879" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A879" s="3">
+        <v>878</v>
+      </c>
+      <c r="B879" s="3">
+        <v>109</v>
+      </c>
+      <c r="C879" s="2">
+        <v>43238</v>
+      </c>
+      <c r="D879" t="s">
+        <v>137</v>
+      </c>
+      <c r="E879">
+        <v>2018</v>
+      </c>
+      <c r="F879" t="s">
+        <v>49</v>
+      </c>
+      <c r="G879" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H879" s="1">
+        <v>0</v>
+      </c>
+      <c r="I879" s="3">
+        <v>3</v>
+      </c>
+      <c r="J879" s="3">
+        <v>15</v>
+      </c>
+      <c r="K879" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="880" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A880" s="3">
+        <v>879</v>
+      </c>
+      <c r="B880" s="3">
+        <v>109</v>
+      </c>
+      <c r="C880" s="2">
+        <v>43238</v>
+      </c>
+      <c r="D880" t="s">
+        <v>137</v>
+      </c>
+      <c r="E880">
+        <v>2018</v>
+      </c>
+      <c r="F880" t="s">
+        <v>49</v>
+      </c>
+      <c r="G880" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H880" s="1">
+        <v>0</v>
+      </c>
+      <c r="I880" s="3">
+        <v>3</v>
+      </c>
+      <c r="J880" s="3">
+        <v>30</v>
+      </c>
+      <c r="K880" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="881" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A881" s="3">
+        <v>880</v>
+      </c>
+      <c r="B881" s="3">
+        <v>109</v>
+      </c>
+      <c r="C881" s="2">
+        <v>43238</v>
+      </c>
+      <c r="D881" t="s">
+        <v>137</v>
+      </c>
+      <c r="E881">
+        <v>2018</v>
+      </c>
+      <c r="F881" t="s">
+        <v>49</v>
+      </c>
+      <c r="G881" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H881" s="1">
+        <v>0</v>
+      </c>
+      <c r="I881" s="3">
+        <v>3</v>
+      </c>
+      <c r="J881" s="3">
+        <v>20</v>
+      </c>
+      <c r="K881" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="882" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A882" s="3">
+        <v>881</v>
+      </c>
+      <c r="B882" s="3">
+        <v>109</v>
+      </c>
+      <c r="C882" s="2">
+        <v>43238</v>
+      </c>
+      <c r="D882" t="s">
+        <v>137</v>
+      </c>
+      <c r="E882">
+        <v>2018</v>
+      </c>
+      <c r="F882" t="s">
+        <v>49</v>
+      </c>
+      <c r="G882" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H882" s="1">
+        <v>0</v>
+      </c>
+      <c r="I882" s="3">
+        <v>3</v>
+      </c>
+      <c r="J882" s="3">
+        <v>20</v>
+      </c>
+      <c r="K882" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="883" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A883" s="3">
+        <v>882</v>
+      </c>
+      <c r="B883" s="3">
+        <v>110</v>
+      </c>
+      <c r="C883" s="2">
+        <v>43241</v>
+      </c>
+      <c r="D883" t="s">
+        <v>137</v>
+      </c>
+      <c r="E883">
+        <v>2018</v>
+      </c>
+      <c r="F883" t="s">
+        <v>17</v>
+      </c>
+      <c r="G883" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H883" s="1">
+        <v>25</v>
+      </c>
+      <c r="I883" s="3">
+        <v>4</v>
+      </c>
+      <c r="J883" s="3">
+        <v>8</v>
+      </c>
+      <c r="K883" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="884" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A884" s="3">
+        <v>883</v>
+      </c>
+      <c r="B884" s="3">
+        <v>110</v>
+      </c>
+      <c r="C884" s="2">
+        <v>43241</v>
+      </c>
+      <c r="D884" t="s">
+        <v>137</v>
+      </c>
+      <c r="E884">
+        <v>2018</v>
+      </c>
+      <c r="F884" t="s">
+        <v>17</v>
+      </c>
+      <c r="G884" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="H884" s="1">
+        <v>60</v>
+      </c>
+      <c r="I884" s="3">
+        <v>4</v>
+      </c>
+      <c r="J884" s="3">
+        <v>8</v>
+      </c>
+      <c r="K884" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="885" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A885" s="3">
+        <v>884</v>
+      </c>
+      <c r="B885" s="3">
+        <v>110</v>
+      </c>
+      <c r="C885" s="2">
+        <v>43241</v>
+      </c>
+      <c r="D885" t="s">
+        <v>137</v>
+      </c>
+      <c r="E885">
+        <v>2018</v>
+      </c>
+      <c r="F885" t="s">
+        <v>17</v>
+      </c>
+      <c r="G885" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="H885" s="1">
+        <v>0</v>
+      </c>
+      <c r="I885" s="3">
+        <v>3</v>
+      </c>
+      <c r="J885" s="3">
+        <v>12</v>
+      </c>
+      <c r="K885" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="886" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A886" s="3">
+        <v>885</v>
+      </c>
+      <c r="B886" s="3">
+        <v>110</v>
+      </c>
+      <c r="C886" s="2">
+        <v>43241</v>
+      </c>
+      <c r="D886" t="s">
+        <v>137</v>
+      </c>
+      <c r="E886">
+        <v>2018</v>
+      </c>
+      <c r="F886" t="s">
+        <v>17</v>
+      </c>
+      <c r="G886" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="H886" s="1">
+        <v>0</v>
+      </c>
+      <c r="I886" s="3">
+        <v>3</v>
+      </c>
+      <c r="J886" s="3">
+        <v>8</v>
+      </c>
+      <c r="K886" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="887" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A887" s="3">
+        <v>886</v>
+      </c>
+      <c r="B887" s="3">
+        <v>110</v>
+      </c>
+      <c r="C887" s="2">
+        <v>43241</v>
+      </c>
+      <c r="D887" t="s">
+        <v>137</v>
+      </c>
+      <c r="E887">
+        <v>2018</v>
+      </c>
+      <c r="F887" t="s">
+        <v>17</v>
+      </c>
+      <c r="G887" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H887" s="1">
+        <v>42</v>
+      </c>
+      <c r="I887" s="3">
+        <v>3</v>
+      </c>
+      <c r="J887" s="3">
+        <v>10</v>
+      </c>
+      <c r="K887" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="888" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A888" s="3">
+        <v>887</v>
+      </c>
+      <c r="B888" s="3">
+        <v>110</v>
+      </c>
+      <c r="C888" s="2">
+        <v>43241</v>
+      </c>
+      <c r="D888" t="s">
+        <v>137</v>
+      </c>
+      <c r="E888">
+        <v>2018</v>
+      </c>
+      <c r="F888" t="s">
+        <v>17</v>
+      </c>
+      <c r="G888" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="H888" s="1">
+        <v>30</v>
+      </c>
+      <c r="I888" s="3">
+        <v>4</v>
+      </c>
+      <c r="J888" s="3">
+        <v>12</v>
+      </c>
+      <c r="K888" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="889" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A889" s="3">
+        <v>888</v>
+      </c>
+      <c r="B889" s="3">
+        <v>111</v>
+      </c>
+      <c r="C889" s="2">
+        <v>43243</v>
+      </c>
+      <c r="D889" t="s">
+        <v>137</v>
+      </c>
+      <c r="E889">
+        <v>2018</v>
+      </c>
+      <c r="F889" t="s">
+        <v>18</v>
+      </c>
+      <c r="G889" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H889" s="1">
+        <v>80</v>
+      </c>
+      <c r="I889" s="3">
+        <v>4</v>
+      </c>
+      <c r="J889" s="3">
+        <v>8</v>
+      </c>
+      <c r="K889" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="890" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A890" s="3">
+        <v>889</v>
+      </c>
+      <c r="B890" s="3">
+        <v>111</v>
+      </c>
+      <c r="C890" s="2">
+        <v>43243</v>
+      </c>
+      <c r="D890" t="s">
+        <v>137</v>
+      </c>
+      <c r="E890">
+        <v>2018</v>
+      </c>
+      <c r="F890" t="s">
+        <v>18</v>
+      </c>
+      <c r="G890" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="H890" s="1">
+        <v>30</v>
+      </c>
+      <c r="I890" s="3">
+        <v>3</v>
+      </c>
+      <c r="J890" s="3">
+        <v>12</v>
+      </c>
+      <c r="K890" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="891" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A891" s="3">
+        <v>890</v>
+      </c>
+      <c r="B891" s="3">
+        <v>111</v>
+      </c>
+      <c r="C891" s="2">
+        <v>43243</v>
+      </c>
+      <c r="D891" t="s">
+        <v>137</v>
+      </c>
+      <c r="E891">
+        <v>2018</v>
+      </c>
+      <c r="F891" t="s">
+        <v>18</v>
+      </c>
+      <c r="G891" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="H891" s="1">
+        <v>0</v>
+      </c>
+      <c r="I891" s="3">
+        <v>3</v>
+      </c>
+      <c r="J891" s="3">
+        <v>10</v>
+      </c>
+      <c r="K891" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="892" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A892" s="3">
+        <v>891</v>
+      </c>
+      <c r="B892" s="3">
+        <v>111</v>
+      </c>
+      <c r="C892" s="2">
+        <v>43243</v>
+      </c>
+      <c r="D892" t="s">
+        <v>137</v>
+      </c>
+      <c r="E892">
+        <v>2018</v>
+      </c>
+      <c r="F892" t="s">
+        <v>18</v>
+      </c>
+      <c r="G892" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H892" s="1">
+        <v>0</v>
+      </c>
+      <c r="I892" s="3">
+        <v>3</v>
+      </c>
+      <c r="J892" s="3">
+        <v>30</v>
+      </c>
+      <c r="K892" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="893" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A893" s="3">
+        <v>892</v>
+      </c>
+      <c r="B893" s="3">
+        <v>111</v>
+      </c>
+      <c r="C893" s="2">
+        <v>43243</v>
+      </c>
+      <c r="D893" t="s">
+        <v>137</v>
+      </c>
+      <c r="E893">
+        <v>2018</v>
+      </c>
+      <c r="F893" t="s">
+        <v>18</v>
+      </c>
+      <c r="G893" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="H893" s="1">
+        <v>35</v>
+      </c>
+      <c r="I893" s="3">
+        <v>3</v>
+      </c>
+      <c r="J893" s="3">
+        <v>12</v>
+      </c>
+      <c r="K893" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="894" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A894" s="3">
+        <v>893</v>
+      </c>
+      <c r="B894" s="3">
+        <v>112</v>
+      </c>
+      <c r="C894" s="2">
+        <v>43244</v>
+      </c>
+      <c r="D894" t="s">
+        <v>137</v>
+      </c>
+      <c r="E894">
+        <v>2018</v>
+      </c>
+      <c r="F894" t="s">
+        <v>16</v>
+      </c>
+      <c r="G894" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="H894" s="1">
+        <v>70</v>
+      </c>
+      <c r="I894" s="3">
+        <v>4</v>
+      </c>
+      <c r="J894" s="3">
+        <v>8</v>
+      </c>
+      <c r="K894" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="895" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A895" s="3">
+        <v>894</v>
+      </c>
+      <c r="B895" s="3">
+        <v>112</v>
+      </c>
+      <c r="C895" s="2">
+        <v>43244</v>
+      </c>
+      <c r="D895" t="s">
+        <v>137</v>
+      </c>
+      <c r="E895">
+        <v>2018</v>
+      </c>
+      <c r="F895" t="s">
+        <v>16</v>
+      </c>
+      <c r="G895" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="H895" s="1">
+        <v>30</v>
+      </c>
+      <c r="I895" s="3">
+        <v>4</v>
+      </c>
+      <c r="J895" s="3">
+        <v>8</v>
+      </c>
+      <c r="K895" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="896" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A896" s="3">
+        <v>895</v>
+      </c>
+      <c r="B896" s="3">
+        <v>112</v>
+      </c>
+      <c r="C896" s="2">
+        <v>43244</v>
+      </c>
+      <c r="D896" t="s">
+        <v>137</v>
+      </c>
+      <c r="E896">
+        <v>2018</v>
+      </c>
+      <c r="F896" t="s">
+        <v>16</v>
+      </c>
+      <c r="G896" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H896" s="1">
+        <v>50</v>
+      </c>
+      <c r="I896" s="3">
+        <v>5</v>
+      </c>
+      <c r="J896" s="3">
+        <v>5</v>
+      </c>
+      <c r="K896" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="897" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A897" s="3">
+        <v>896</v>
+      </c>
+      <c r="B897" s="3">
+        <v>112</v>
+      </c>
+      <c r="C897" s="2">
+        <v>43244</v>
+      </c>
+      <c r="D897" t="s">
+        <v>137</v>
+      </c>
+      <c r="E897">
+        <v>2018</v>
+      </c>
+      <c r="F897" t="s">
+        <v>16</v>
+      </c>
+      <c r="G897" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H897" s="1">
+        <v>90</v>
+      </c>
+      <c r="I897" s="3">
+        <v>5</v>
+      </c>
+      <c r="J897" s="3">
+        <v>5</v>
+      </c>
+      <c r="K897" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="898" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A898" s="3">
+        <v>897</v>
+      </c>
+      <c r="B898" s="3">
+        <v>112</v>
+      </c>
+      <c r="C898" s="2">
+        <v>43244</v>
+      </c>
+      <c r="D898" t="s">
+        <v>137</v>
+      </c>
+      <c r="E898">
+        <v>2018</v>
+      </c>
+      <c r="F898" t="s">
+        <v>16</v>
+      </c>
+      <c r="G898" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="H898" s="1">
+        <v>35</v>
+      </c>
+      <c r="I898" s="3">
+        <v>4</v>
+      </c>
+      <c r="J898" s="3">
+        <v>12</v>
+      </c>
+      <c r="K898" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="899" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A899" s="3">
+        <v>898</v>
+      </c>
+      <c r="B899" s="3">
+        <v>113</v>
+      </c>
+      <c r="C899" s="2">
+        <v>43246</v>
+      </c>
+      <c r="D899" t="s">
+        <v>137</v>
+      </c>
+      <c r="E899">
+        <v>2018</v>
+      </c>
+      <c r="F899" t="s">
+        <v>79</v>
+      </c>
+      <c r="G899" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H899" s="1">
+        <v>70</v>
+      </c>
+      <c r="I899" s="3">
+        <v>4</v>
+      </c>
+      <c r="J899" s="3">
+        <v>8</v>
+      </c>
+      <c r="K899" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="900" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A900" s="3">
+        <v>899</v>
+      </c>
+      <c r="B900" s="3">
+        <v>113</v>
+      </c>
+      <c r="C900" s="2">
+        <v>43246</v>
+      </c>
+      <c r="D900" t="s">
+        <v>137</v>
+      </c>
+      <c r="E900">
+        <v>2018</v>
+      </c>
+      <c r="F900" t="s">
+        <v>79</v>
+      </c>
+      <c r="G900" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="H900" s="1">
+        <v>45</v>
+      </c>
+      <c r="I900" s="3">
+        <v>3</v>
+      </c>
+      <c r="J900" s="3">
+        <v>12</v>
+      </c>
+      <c r="K900" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="901" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A901" s="3">
+        <v>900</v>
+      </c>
+      <c r="B901" s="3">
+        <v>113</v>
+      </c>
+      <c r="C901" s="2">
+        <v>43246</v>
+      </c>
+      <c r="D901" t="s">
+        <v>137</v>
+      </c>
+      <c r="E901">
+        <v>2018</v>
+      </c>
+      <c r="F901" t="s">
+        <v>79</v>
+      </c>
+      <c r="G901" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="H901" s="1">
+        <v>40</v>
+      </c>
+      <c r="I901" s="3">
+        <v>4</v>
+      </c>
+      <c r="J901" s="3">
+        <v>10</v>
+      </c>
+      <c r="K901" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="902" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A902" s="3">
+        <v>901</v>
+      </c>
+      <c r="B902" s="3">
+        <v>113</v>
+      </c>
+      <c r="C902" s="2">
+        <v>43246</v>
+      </c>
+      <c r="D902" t="s">
+        <v>137</v>
+      </c>
+      <c r="E902">
+        <v>2018</v>
+      </c>
+      <c r="F902" t="s">
+        <v>79</v>
+      </c>
+      <c r="G902" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H902" s="1">
+        <v>20</v>
+      </c>
+      <c r="I902" s="3">
+        <v>3</v>
+      </c>
+      <c r="J902" s="3">
+        <v>12</v>
+      </c>
+      <c r="K902" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="903" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A903" s="3">
+        <v>902</v>
+      </c>
+      <c r="B903" s="3">
+        <v>113</v>
+      </c>
+      <c r="C903" s="2">
+        <v>43246</v>
+      </c>
+      <c r="D903" t="s">
+        <v>137</v>
+      </c>
+      <c r="E903">
+        <v>2018</v>
+      </c>
+      <c r="F903" t="s">
+        <v>79</v>
+      </c>
+      <c r="G903" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H903" s="1">
+        <v>60</v>
+      </c>
+      <c r="I903" s="3">
+        <v>3</v>
+      </c>
+      <c r="J903" s="3">
+        <v>12</v>
+      </c>
+      <c r="K903" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="904" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A904" s="3">
+        <v>903</v>
+      </c>
+      <c r="B904" s="3">
+        <v>113</v>
+      </c>
+      <c r="C904" s="2">
+        <v>43246</v>
+      </c>
+      <c r="D904" t="s">
+        <v>137</v>
+      </c>
+      <c r="E904">
+        <v>2018</v>
+      </c>
+      <c r="F904" t="s">
+        <v>79</v>
+      </c>
+      <c r="G904" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="H904" s="1">
+        <v>25</v>
+      </c>
+      <c r="I904" s="3">
+        <v>2</v>
+      </c>
+      <c r="J904" s="3">
+        <v>12</v>
+      </c>
+      <c r="K904" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="905" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A905" s="3">
+        <v>904</v>
+      </c>
+      <c r="B905" s="3">
+        <v>113</v>
+      </c>
+      <c r="C905" s="2">
+        <v>43246</v>
+      </c>
+      <c r="D905" t="s">
+        <v>137</v>
+      </c>
+      <c r="E905">
+        <v>2018</v>
+      </c>
+      <c r="F905" t="s">
+        <v>79</v>
+      </c>
+      <c r="G905" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="H905" s="1">
+        <v>35</v>
+      </c>
+      <c r="I905" s="3">
+        <v>3</v>
+      </c>
+      <c r="J905" s="3">
+        <v>12</v>
+      </c>
+      <c r="K905" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="906" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A906" s="3">
+        <v>905</v>
+      </c>
+      <c r="B906" s="3">
+        <v>114</v>
+      </c>
+      <c r="C906" s="2">
+        <v>43247</v>
+      </c>
+      <c r="D906" t="s">
+        <v>137</v>
+      </c>
+      <c r="E906">
+        <v>2018</v>
+      </c>
+      <c r="F906" t="s">
+        <v>44</v>
+      </c>
+      <c r="G906" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H906" s="1">
+        <v>101</v>
+      </c>
+      <c r="I906" s="3">
+        <v>4</v>
+      </c>
+      <c r="J906" s="3">
+        <v>10</v>
+      </c>
+      <c r="K906" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="907" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A907" s="3">
+        <v>906</v>
+      </c>
+      <c r="B907" s="3">
+        <v>114</v>
+      </c>
+      <c r="C907" s="2">
+        <v>43247</v>
+      </c>
+      <c r="D907" t="s">
+        <v>137</v>
+      </c>
+      <c r="E907">
+        <v>2018</v>
+      </c>
+      <c r="F907" t="s">
+        <v>44</v>
+      </c>
+      <c r="G907" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H907" s="1">
+        <v>70</v>
+      </c>
+      <c r="I907" s="3">
+        <v>4</v>
+      </c>
+      <c r="J907" s="3">
+        <v>12</v>
+      </c>
+      <c r="K907" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="908" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A908" s="3">
+        <v>907</v>
+      </c>
+      <c r="B908" s="3">
+        <v>114</v>
+      </c>
+      <c r="C908" s="2">
+        <v>43247</v>
+      </c>
+      <c r="D908" t="s">
+        <v>137</v>
+      </c>
+      <c r="E908">
+        <v>2018</v>
+      </c>
+      <c r="F908" t="s">
+        <v>44</v>
+      </c>
+      <c r="G908" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H908" s="1">
+        <v>70</v>
+      </c>
+      <c r="I908" s="3">
+        <v>4</v>
+      </c>
+      <c r="J908" s="3">
+        <v>12</v>
+      </c>
+      <c r="K908" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="909" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A909" s="3">
+        <v>908</v>
+      </c>
+      <c r="B909" s="3">
+        <v>114</v>
+      </c>
+      <c r="C909" s="2">
+        <v>43247</v>
+      </c>
+      <c r="D909" t="s">
+        <v>137</v>
+      </c>
+      <c r="E909">
+        <v>2018</v>
+      </c>
+      <c r="F909" t="s">
+        <v>44</v>
+      </c>
+      <c r="G909" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H909" s="1">
+        <v>40</v>
+      </c>
+      <c r="I909" s="3">
+        <v>4</v>
+      </c>
+      <c r="J909" s="3">
+        <v>8</v>
+      </c>
+      <c r="K909" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="910" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A910" s="3">
+        <v>909</v>
+      </c>
+      <c r="B910" s="3">
+        <v>114</v>
+      </c>
+      <c r="C910" s="2">
+        <v>43247</v>
+      </c>
+      <c r="D910" t="s">
+        <v>137</v>
+      </c>
+      <c r="E910">
+        <v>2018</v>
+      </c>
+      <c r="F910" t="s">
+        <v>44</v>
+      </c>
+      <c r="G910" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H910" s="1">
+        <v>20</v>
+      </c>
+      <c r="I910" s="3">
+        <v>4</v>
+      </c>
+      <c r="J910" s="3">
+        <v>8</v>
+      </c>
+      <c r="K910" t="s">
+        <v>89</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>